<commit_message>
OOP Interfaces And Abstraction - Exercise Complete
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Solidity" sheetId="5" r:id="rId5"/>
     <sheet name="Git" sheetId="6" r:id="rId6"/>
     <sheet name="Comparators" sheetId="7" r:id="rId7"/>
+    <sheet name="OOP" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -25,7 +26,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0">
+    <comment ref="A21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="230">
   <si>
     <t>Операция</t>
   </si>
@@ -1840,17 +1841,116 @@
   <si>
     <t>Проверка за по-голям елемент</t>
   </si>
+  <si>
+    <t>Принцип</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Process of wrapping code and  data together into a single unit
+- Flexibility and extensibility of the code
+- Reduces complexity
+- Structural changes remain local
+- Allows validation and data binding</t>
+  </si>
+  <si>
+    <t>=&gt; Fields should be private
+=&gt;Properties should be public</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Encapsulation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(Hiding Implementation)
+(Access Modifiers)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Encapsulation:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     - Hides implementation
+     - Reduces complexity
+     - Ensures that structural changes  remain local
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mutable and Immutable objects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2288,36 +2388,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2332,101 +2432,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2531,7 +2649,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2566,7 +2684,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5374,7 +5492,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -5394,7 +5512,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="23" t="s">
         <v>175</v>
       </c>
@@ -5462,10 +5580,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="48"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>
@@ -5620,7 +5738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5632,21 +5750,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="50" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="46" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="46" t="s">
         <v>224</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -5657,4 +5775,45 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="52" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
OOP Polimorphism - Exercise Complete
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="232">
   <si>
     <t>Операция</t>
   </si>
@@ -1883,6 +1883,26 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Polymorphism
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Abstract Classes, Abstract Methods, Override Methods)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ability of an object to take on many forms</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -1919,17 +1939,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Mutable and Immutable objects</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
     </r>
   </si>
 </sst>
@@ -2388,7 +2397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2516,6 +2525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2528,23 +2543,20 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5492,7 +5504,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -5512,7 +5524,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="23" t="s">
         <v>175</v>
       </c>
@@ -5580,10 +5592,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="50"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>
@@ -5779,37 +5791,45 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="52" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="54" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23" style="48" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="56" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="57" t="s">
         <v>227</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
         <v>229</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C# OOP -Exceptions And Error Handling
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Git" sheetId="6" r:id="rId6"/>
     <sheet name="Comparators" sheetId="7" r:id="rId7"/>
     <sheet name="OOP" sheetId="8" r:id="rId8"/>
+    <sheet name="Reflection" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -26,7 +27,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0">
+    <comment ref="A21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="262">
   <si>
     <t>Операция</t>
   </si>
@@ -2055,17 +2056,55 @@
     <t>Fields and constants can't be defined. 
 If we add a new method we have to track down all the implementations of the interface and define implementation for the new method</t>
   </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Activator</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Assembly assembly = Assembly.GetCallingAssembly();</t>
+  </si>
+  <si>
+    <t>Type[] types = assembly
+                .GetTypes();
+Type typeToCreate = types
+                .FirstOrDefault(t =&gt; t.Name == commandName);</t>
+  </si>
+  <si>
+    <t>Object instance = (ICommand)Activator
+                .CreateInstance(typeToCreate);
+ICommand command = (ICommand)instance;
+string result = command.Execute(commandArgs);</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2526,36 +2565,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2570,97 +2609,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2672,24 +2711,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2793,7 +2833,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2828,7 +2868,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5636,7 +5676,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -5656,7 +5696,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
+      <c r="A2" s="56"/>
       <c r="B2" s="23" t="s">
         <v>175</v>
       </c>
@@ -5724,10 +5764,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>
@@ -5925,7 +5965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -5992,7 +6032,7 @@
       <c r="C5" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="54" t="s">
         <v>231</v>
       </c>
       <c r="E5" s="42" t="s">
@@ -6013,7 +6053,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="53" t="s">
         <v>232</v>
       </c>
       <c r="B8" s="51" t="s">
@@ -6056,4 +6096,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B2" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
C# OOP - Demo Exam
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="OOP" sheetId="8" r:id="rId8"/>
     <sheet name="Reflection" sheetId="9" r:id="rId9"/>
     <sheet name="UnitTesting" sheetId="10" r:id="rId10"/>
+    <sheet name="Exceptions" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -28,7 +29,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0">
+    <comment ref="A21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="265">
   <si>
     <t>Операция</t>
   </si>
@@ -2090,11 +2091,17 @@
   <si>
     <t>https://www.automatetheplanet.com/nunit-cheat-sheet/</t>
   </si>
+  <si>
+    <t>throw new ArgumentException(string.Format("MotorcycleExists!", model));</t>
+  </si>
+  <si>
+    <t>throw new ArgumentException("MotorcycleExists!");</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2739,6 +2746,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2751,7 +2759,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2841,7 +2848,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2849,6 +2856,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2902,7 +2920,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2937,7 +2955,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5284,7 +5302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -5294,7 +5312,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="56" t="s">
         <v>262</v>
       </c>
     </row>
@@ -5336,6 +5354,35 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
@@ -5801,7 +5848,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -5821,7 +5868,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="23" t="s">
         <v>175</v>
       </c>
@@ -5889,10 +5936,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="59"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
OOP Exam 11.08.2019 - Complete
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -2104,9 +2104,6 @@
     <t>Inheritance, Encapsulation , Abstraction,Polymorphism</t>
   </si>
   <si>
-    <t xml:space="preserve">  Контструктори</t>
-  </si>
-  <si>
     <t>Абстрактни и виртуални методи</t>
   </si>
   <si>
@@ -2114,6 +2111,9 @@
   </si>
   <si>
     <t>Първо се вика наследника и след това базовия метод. Виртуални и абстрактни методи не се викат в конструктор</t>
+  </si>
+  <si>
+    <t>Базови Контструктори</t>
   </si>
 </sst>
 </file>
@@ -5309,7 +5309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -6145,8 +6145,8 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6164,18 +6164,18 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
C# DB - Exercises
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
-    <sheet name="Regex" sheetId="2" r:id="rId2"/>
-    <sheet name="ShortCuts" sheetId="3" r:id="rId3"/>
+    <sheet name="DB-SQL" sheetId="11" r:id="rId2"/>
+    <sheet name="Regex" sheetId="2" r:id="rId3"/>
     <sheet name="DB" sheetId="4" r:id="rId4"/>
     <sheet name="Solidity" sheetId="5" r:id="rId5"/>
     <sheet name="Git" sheetId="6" r:id="rId6"/>
     <sheet name="Comparators" sheetId="7" r:id="rId7"/>
-    <sheet name="OOP" sheetId="8" r:id="rId8"/>
-    <sheet name="SOLID" sheetId="12" r:id="rId9"/>
-    <sheet name="Reflection" sheetId="9" r:id="rId10"/>
-    <sheet name="UnitTesting" sheetId="10" r:id="rId11"/>
-    <sheet name="Exceptions" sheetId="11" r:id="rId12"/>
+    <sheet name="ShortCuts" sheetId="3" r:id="rId8"/>
+    <sheet name="OOP" sheetId="8" r:id="rId9"/>
+    <sheet name="SOLID" sheetId="12" r:id="rId10"/>
+    <sheet name="Reflection" sheetId="9" r:id="rId11"/>
+    <sheet name="UnitTesting" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -84,39 +84,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="313">
   <si>
     <t>Операция</t>
   </si>
@@ -278,15 +251,6 @@
   </si>
   <si>
     <t>Console.WriteLine(string.Join(Environment.NewLine, namePoints.Select(a =&gt; $"{a.Key} | {a.Value}")));</t>
-  </si>
-  <si>
-    <t>Хвърляне на грешка</t>
-  </si>
-  <si>
-    <t>Throw new Exception("Error message!")</t>
-  </si>
-  <si>
-    <t>Throw exception</t>
   </si>
   <si>
     <t>IndexOf</t>
@@ -2066,12 +2030,6 @@
     <t>https://www.automatetheplanet.com/nunit-cheat-sheet/</t>
   </si>
   <si>
-    <t>throw new ArgumentException(string.Format("MotorcycleExists!", model));</t>
-  </si>
-  <si>
-    <t>throw new ArgumentException("MotorcycleExists!");</t>
-  </si>
-  <si>
     <t>An interface contains only the signatures of methods,
 properties, events or indexers.
 Интерфейса описва функциалността на  конкретен обект.Като класовете имплементиращи интерфейса могат да бъдат ползвани чрез общите им свойства.</t>
@@ -2165,6 +2123,431 @@
   </si>
   <si>
     <t>Type[] currnetUnitType = assembly.GetTypes();</t>
+  </si>
+  <si>
+    <t>Хвърляне на грешка - Throw exception</t>
+  </si>
+  <si>
+    <t>Throw new Exception("Error message!")
+throw new ArgumentException("MotorcycleExists!");
+throw new ArgumentException(string.Format("MotorcycleExists!", model));</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>CREATE DATABASE Employees</t>
+  </si>
+  <si>
+    <t>КОМАНДА</t>
+  </si>
+  <si>
+    <t>Създаване на база данни (DB)</t>
+  </si>
+  <si>
+    <t>Създаване на таблица</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE People(
+Id int NOT NULL,
+Email varchar(50) NOT NULL,
+FirstName varchar(50),
+LastName varchar(50) )
+</t>
+  </si>
+  <si>
+    <t>Взимане на всички данни от таблицата</t>
+  </si>
+  <si>
+    <t>SELECT * FROM Employees</t>
+  </si>
+  <si>
+    <t>SELECT TOP (5) FirstName, LastName
+FROM Employees</t>
+  </si>
+  <si>
+    <t>Взимане на първите 5 реда от таблица</t>
+  </si>
+  <si>
+    <t>Свойства на колоните (Custom Column Properties)</t>
+  </si>
+  <si>
+    <t>Промяна на таблиците след създаването им 
+(Altering Tables - Changing Table Properties After Creation)</t>
+  </si>
+  <si>
+    <t>Deleting from Database
+(Dropping and Truncating)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add check constraint - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE InstrumentReadings
+ADD CONSTRAINT PositiveValue
+CHECK (Kelvin &gt; 0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Set default value -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ALTER TABLE People
+ADD DEFAULT 0
+FOR Balance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add unique constraint -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ALTER TABLE People
+ADD CONSTRAINT uq_Email
+UNIQUE (Email)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modify data type of existing column - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE People
+ALTER COLUMN Email VARCHAR(100)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add primary key to existing column - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE People
+ADD CONSTRAINT PK_Id
+PRIMARY KEY (Id)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Delete existing column - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE People
+DROP COLUMN FullName</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Adding a column - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ADD Salary DECIMAL(15, 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A table can be changed using the keywords - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE Employees</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Value constraint - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kelvin DECIMAL(10,2) CHECK (Kelvin &gt; 0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Default value - if not specified (otherwise set to NULL) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Balance DECIMAL(10,2) DEFAULT 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unique constraint - no repeating values in entire table - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email VARCHAR(50) UNIQUE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Identity (auto-increment) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Id INT PRIMARY KEY IDENTITY</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Primary Key - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Id INT NOT NULL PRIMARY KEY</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To delete all records in a table - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRUNCATE TABLE Employees</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">To drop a table – delete data and structure - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DROP TABLE Employees</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">To drop entire database - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DROP DATABASE AMS</t>
+    </r>
+  </si>
+  <si>
+    <t>Removing constraint from column</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This includes primary keys, check constraints and unique field - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE Employees
+DROP CONSTRAINT PK_Id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To remove default value (if not specified, revert to NULL) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALTER TABLE Employees
+ALTER COLUMN Clients
+DROP DEFAULT</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2423,7 +2806,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -2657,12 +3040,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2827,6 +3234,40 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3233,10 +3674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C395"/>
+  <dimension ref="A1:C394"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -3436,10 +3877,10 @@
     </row>
     <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>48</v>
@@ -3447,10 +3888,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>50</v>
@@ -3458,46 +3899,46 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>128</v>
+        <v>281</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>130</v>
+        <v>279</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5354,11 +5795,6 @@
       <c r="A394" s="8"/>
       <c r="B394" s="6"/>
       <c r="C394" s="6"/>
-    </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A395" s="8"/>
-      <c r="B395" s="6"/>
-      <c r="C395" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5369,9 +5805,68 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -5385,55 +5880,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C3" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>278</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5442,7 +5937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5457,7 +5952,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -5498,36 +5993,227 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.5703125" style="69" customWidth="1"/>
+    <col min="2" max="2" width="95" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>257</v>
-      </c>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="64"/>
+      <c r="B7" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64"/>
+      <c r="B8" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="64"/>
+      <c r="B9" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="65"/>
+      <c r="B10" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
+      <c r="B12" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="70"/>
+    </row>
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
+      <c r="B13" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="62"/>
+      <c r="B14" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="62"/>
+      <c r="B15" s="71" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="62"/>
+      <c r="B16" s="71" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="62"/>
+      <c r="B17" s="71" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="62"/>
+      <c r="B18" s="71" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="64"/>
+      <c r="B20" s="72" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="65"/>
+      <c r="B21" s="72" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="65"/>
+      <c r="B23" s="74" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="66"/>
+      <c r="B24" s="72"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="72"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="72"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="72"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="72"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="72"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="72"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="72"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="72"/>
+    </row>
+    <row r="33" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="72"/>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="72"/>
+    </row>
+    <row r="35" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="72"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A22:A23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -5544,334 +6230,284 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
         <v>96</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
         <v>114</v>
       </c>
-      <c r="B19" t="s">
-        <v>117</v>
-      </c>
       <c r="C19" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5892,75 +6528,75 @@
   <sheetData>
     <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B7" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5993,95 +6629,95 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>159</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="58"/>
       <c r="B2" s="23" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>154</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C4" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>153</v>
-      </c>
       <c r="E4" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="176.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>168</v>
-      </c>
       <c r="D5" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>167</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
       <c r="B6" s="59" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="26"/>
@@ -6089,19 +6725,19 @@
     </row>
     <row r="7" spans="1:6" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B7" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>176</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>179</v>
       </c>
       <c r="F7" s="24"/>
     </row>
@@ -6134,98 +6770,98 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C6" s="38"/>
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C8" s="38"/>
     </row>
     <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -6262,13 +6898,13 @@
     </row>
     <row r="2" spans="1:3" s="46" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -6278,6 +6914,56 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -6301,185 +6987,126 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="42" t="s">
         <v>246</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="53" t="s">
         <v>227</v>
       </c>
-      <c r="B8" s="50" t="s">
-        <v>225</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>230</v>
-      </c>
       <c r="E8" s="42" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="240" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>231</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
C# DB - 02. DB-Basics-Basic-CRUD-Exercises
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="544">
   <si>
     <t>Операция</t>
   </si>
@@ -3238,63 +3238,6 @@
     <t>Опреснява информацията в базата така че след изпълнението на командите да са достъпни за следващата част от кода</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">GO
-GO 10 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- GO execute the related sql commands n times
-Declare @ID nvarchar(5);
-set @ID = 5;
-select @ID </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Not Accesible</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-GO
-select @ID - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ACCESSIBLE</t>
-    </r>
-  </si>
-  <si>
     <t>The IN operator allows you to specify multiple values in a WHERE clause.
 The IN operator is a shorthand for multiple OR conditions.</t>
   </si>
@@ -3338,9 +3281,6 @@
     <t>ISNULL</t>
   </si>
   <si>
-    <t>ISNULL(MiddleName,'') - Ако стойността в колоната е NULL, NULL се замества с ''</t>
-  </si>
-  <si>
     <t>Multiple order</t>
   </si>
   <si>
@@ -4441,57 +4381,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>[Name] LIKE '[^rbd]%'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CREATE VIEW v_EmployeesByDepartment AS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SELECT FirstName + ' ' + LastName AS [Full Name], Salary
-FROM Employees</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-That how is called : SELECT * FROM v_EmployeesByDepartment</t>
     </r>
   </si>
   <si>
@@ -5154,9 +5043,6 @@
     <t>GO</t>
   </si>
   <si>
-    <t>Изпълни кода от GO надолу</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">DISTINCT </t>
     </r>
@@ -5181,6 +5067,139 @@
     <t>SELECT DepartmentID
 FROM Employees
 GROUP BY DepartmentID</t>
+  </si>
+  <si>
+    <t>All T-SQL prior GO will execute "at once"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INSERT INTO mytable DEFAULT VALUES
+GO 10
+GO 10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- GO execute the related sql commands n times
+Declare @ID nvarchar(5);
+set @ID = 5;
+select @ID </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Not Accesible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+GO
+select @ID - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ACCESSIBLE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CREATE VIEW v_EmployeesByDepartment AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT FirstName + ' ' + LastName AS [Full Name], Salary
+FROM Employees</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+That how is called : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT * FROM v_EmployeesByDepartment</t>
+    </r>
+  </si>
+  <si>
+    <t>ISNULL(MiddleName,' ') - Ако стойността в колоната е NULL, NULL се замества с ' '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COALESCE </t>
+  </si>
+  <si>
+    <t>Evaluates the arguments in order and returns the current value of the first expression that initially doesn't evaluate to NULL. For example, SELECT COALESCE(NULL, NULL, 'third_value', 'fourth_value'); returns the third value because the third value is the first value that isn't null.</t>
   </si>
 </sst>
 </file>
@@ -5906,7 +5925,7 @@
     <xf numFmtId="0" fontId="34" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6157,20 +6176,29 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="22" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6190,17 +6218,8 @@
     <xf numFmtId="0" fontId="35" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6212,6 +6231,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8944,10 +8969,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C159"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8966,90 +8991,90 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>343</v>
       </c>
-      <c r="B2" s="104"/>
+      <c r="B2" s="94"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="106" t="s">
-        <v>512</v>
-      </c>
-      <c r="B3" s="105"/>
+      <c r="A3" s="96" t="s">
+        <v>509</v>
+      </c>
+      <c r="B3" s="95"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="105" t="s">
-        <v>524</v>
-      </c>
-      <c r="B7" s="103"/>
+      <c r="A7" s="95" t="s">
+        <v>521</v>
+      </c>
+      <c r="B7" s="92"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="105" t="s">
-        <v>527</v>
-      </c>
-      <c r="B11" s="103"/>
+      <c r="A11" s="95" t="s">
+        <v>524</v>
+      </c>
+      <c r="B11" s="92"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="105" t="s">
-        <v>391</v>
-      </c>
-      <c r="B13" s="105"/>
+      <c r="A13" s="95" t="s">
+        <v>389</v>
+      </c>
+      <c r="B13" s="95"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -9093,45 +9118,45 @@
     </row>
     <row r="19" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="105" t="s">
-        <v>509</v>
-      </c>
-      <c r="B20" s="105"/>
+      <c r="A20" s="95" t="s">
+        <v>506</v>
+      </c>
+      <c r="B20" s="95"/>
     </row>
     <row r="21" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
         <v>341</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="105" t="s">
-        <v>390</v>
-      </c>
-      <c r="B22" s="105"/>
+      <c r="A22" s="95" t="s">
+        <v>388</v>
+      </c>
+      <c r="B22" s="95"/>
     </row>
     <row r="23" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
         <v>342</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="105" t="s">
+      <c r="A24" s="95" t="s">
         <v>353</v>
       </c>
-      <c r="B24" s="105"/>
+      <c r="B24" s="95"/>
     </row>
     <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="57" t="s">
@@ -9158,10 +9183,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="105" t="s">
+      <c r="A28" s="95" t="s">
         <v>353</v>
       </c>
-      <c r="B28" s="105"/>
+      <c r="B28" s="95"/>
     </row>
     <row r="29" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="72" t="s">
@@ -9188,10 +9213,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="103" t="s">
+      <c r="A32" s="92" t="s">
         <v>363</v>
       </c>
-      <c r="B32" s="103"/>
+      <c r="B32" s="92"/>
     </row>
     <row r="33" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="72" t="s">
@@ -9211,17 +9236,17 @@
     </row>
     <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="57" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>383</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="105" t="s">
+      <c r="A36" s="95" t="s">
         <v>360</v>
       </c>
-      <c r="B36" s="105"/>
+      <c r="B36" s="95"/>
     </row>
     <row r="37" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="72" t="s">
@@ -9241,78 +9266,78 @@
     </row>
     <row r="39" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A39" s="57" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B39" s="74" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="103" t="s">
+      <c r="A40" s="92" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="103"/>
+      <c r="B40" s="92"/>
     </row>
     <row r="41" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A41" s="57" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>473</v>
+        <v>540</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
+        <v>379</v>
+      </c>
+      <c r="B42" s="74" t="s">
         <v>380</v>
       </c>
-      <c r="B42" s="74" t="s">
-        <v>381</v>
-      </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="105" t="s">
-        <v>519</v>
-      </c>
-      <c r="B43" s="103"/>
+      <c r="A43" s="95" t="s">
+        <v>516</v>
+      </c>
+      <c r="B43" s="92"/>
     </row>
     <row r="44" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B44" s="74" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B45" s="74" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B46" s="74" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="94" t="s">
+      <c r="A47" s="93" t="s">
         <v>374</v>
       </c>
-      <c r="B47" s="94"/>
+      <c r="B47" s="93"/>
     </row>
     <row r="48" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A48" s="92" t="s">
+      <c r="A48" s="99" t="s">
         <v>312</v>
       </c>
-      <c r="B48" s="93"/>
+      <c r="B48" s="98"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="100" t="s">
+      <c r="A49" s="103" t="s">
         <v>322</v>
       </c>
       <c r="B49" s="62" t="s">
@@ -9320,7 +9345,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="101"/>
+      <c r="A50" s="104"/>
       <c r="B50" s="62" t="s">
         <v>314</v>
       </c>
@@ -9329,13 +9354,13 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="102"/>
+      <c r="A51" s="105"/>
       <c r="B51" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="100" t="s">
+      <c r="A52" s="103" t="s">
         <v>323</v>
       </c>
       <c r="B52" s="62" t="s">
@@ -9343,25 +9368,25 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="101"/>
+      <c r="A53" s="104"/>
       <c r="B53" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="101"/>
+      <c r="A54" s="104"/>
       <c r="B54" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="102"/>
+      <c r="A55" s="105"/>
       <c r="B55" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="100" t="s">
+      <c r="A56" s="103" t="s">
         <v>324</v>
       </c>
       <c r="B56" s="62" t="s">
@@ -9369,13 +9394,13 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="102"/>
+      <c r="A57" s="105"/>
       <c r="B57" s="62" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="103" t="s">
         <v>325</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -9386,23 +9411,23 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="101"/>
+      <c r="A59" s="104"/>
       <c r="B59" s="62" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C59" s="68" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="101"/>
+      <c r="A60" s="104"/>
       <c r="B60" s="62" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C60" s="68"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="102"/>
+      <c r="A61" s="105"/>
       <c r="B61" s="62" t="s">
         <v>327</v>
       </c>
@@ -9420,7 +9445,7 @@
         <v>285</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -9432,7 +9457,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="97" t="s">
+      <c r="A65" s="100" t="s">
         <v>290</v>
       </c>
       <c r="B65" s="62" t="s">
@@ -9440,37 +9465,37 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="98"/>
+      <c r="A66" s="101"/>
       <c r="B66" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="98"/>
+      <c r="A67" s="101"/>
       <c r="B67" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="98"/>
+      <c r="A68" s="101"/>
       <c r="B68" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="98"/>
+      <c r="A69" s="101"/>
       <c r="B69" s="62" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="99"/>
+      <c r="A70" s="102"/>
       <c r="B70" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="97" t="s">
+      <c r="A71" s="100" t="s">
         <v>291</v>
       </c>
       <c r="B71" s="62" t="s">
@@ -9478,62 +9503,62 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="98"/>
+      <c r="A72" s="101"/>
       <c r="B72" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C72" s="67"/>
     </row>
     <row r="73" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="98"/>
+      <c r="A73" s="101"/>
       <c r="B73" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="98"/>
+      <c r="A74" s="101"/>
       <c r="B74" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="98"/>
+      <c r="A75" s="101"/>
       <c r="B75" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="98"/>
+      <c r="A76" s="101"/>
       <c r="B76" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="98"/>
+      <c r="A77" s="101"/>
       <c r="B77" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="98"/>
+      <c r="A78" s="101"/>
       <c r="B78" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="98"/>
+      <c r="A79" s="101"/>
       <c r="B79" s="81" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="99"/>
+      <c r="A80" s="102"/>
       <c r="B80" s="81" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="97" t="s">
+      <c r="A81" s="100" t="s">
         <v>292</v>
       </c>
       <c r="B81" s="82" t="s">
@@ -9541,21 +9566,21 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="98"/>
+      <c r="A82" s="101"/>
       <c r="B82" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C82"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="99"/>
+      <c r="A83" s="102"/>
       <c r="B83" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C83"/>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="97" t="s">
+      <c r="A84" s="100" t="s">
         <v>309</v>
       </c>
       <c r="B84" s="84" t="s">
@@ -9564,7 +9589,7 @@
       <c r="C84"/>
     </row>
     <row r="85" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="99"/>
+      <c r="A85" s="102"/>
       <c r="B85" s="84" t="s">
         <v>311</v>
       </c>
@@ -9590,617 +9615,647 @@
     </row>
     <row r="88" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="61" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B88" s="85" t="s">
         <v>329</v>
       </c>
       <c r="C88"/>
     </row>
-    <row r="89" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A89" s="71" t="s">
         <v>375</v>
       </c>
       <c r="B89" s="84" t="s">
-        <v>376</v>
+        <v>539</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A90" s="91" t="s">
-        <v>537</v>
-      </c>
-      <c r="B90" s="84" t="s">
+        <v>534</v>
+      </c>
+      <c r="B90" s="81" t="s">
         <v>538</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A91" s="73" t="s">
-        <v>378</v>
-      </c>
-      <c r="B91" s="84" t="s">
         <v>377</v>
       </c>
+      <c r="B91" s="81" t="s">
+        <v>376</v>
+      </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="94" t="s">
-        <v>392</v>
-      </c>
-      <c r="B92" s="94"/>
+      <c r="A92" s="93" t="s">
+        <v>390</v>
+      </c>
+      <c r="B92" s="93"/>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A93" s="92" t="s">
-        <v>393</v>
-      </c>
-      <c r="B93" s="93"/>
+      <c r="A93" s="99" t="s">
+        <v>391</v>
+      </c>
+      <c r="B93" s="98"/>
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="70" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B94" s="60" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C94"/>
     </row>
     <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="70" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B95" s="76" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C95"/>
     </row>
     <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="70" t="s">
+        <v>396</v>
+      </c>
+      <c r="B96" s="76" t="s">
+        <v>397</v>
+      </c>
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A97" s="99" t="s">
         <v>398</v>
       </c>
-      <c r="B96" s="76" t="s">
-        <v>399</v>
-      </c>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A97" s="92" t="s">
-        <v>400</v>
-      </c>
-      <c r="B97" s="93"/>
+      <c r="B97" s="98"/>
       <c r="C97"/>
     </row>
     <row r="98" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="57" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B98" s="80" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A99" s="57" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B99" s="80" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="72" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B100" s="80" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="57" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B101" s="80" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="57" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B102" s="80" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A103" s="57" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B103" s="79" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A104" s="57" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B104" s="79" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="57" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B105" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C105"/>
     </row>
     <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="57" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B106" s="80" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A107" s="57" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B107" s="79" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A108" s="57" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B108" s="79" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C108"/>
     </row>
     <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A109" s="57" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B109" s="79" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C109"/>
     </row>
     <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B110" s="79" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C110"/>
     </row>
     <row r="111" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A111" s="57" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B111" s="79" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C111"/>
     </row>
     <row r="112" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
       <c r="A112" s="72" t="s">
+        <v>427</v>
+      </c>
+      <c r="B112" s="80" t="s">
+        <v>428</v>
+      </c>
+      <c r="C112"/>
+    </row>
+    <row r="113" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="112" t="s">
+        <v>542</v>
+      </c>
+      <c r="B113" s="111" t="s">
+        <v>543</v>
+      </c>
+      <c r="C113"/>
+    </row>
+    <row r="114" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A114" s="99" t="s">
         <v>429</v>
       </c>
-      <c r="B112" s="80" t="s">
-        <v>430</v>
-      </c>
-      <c r="C112"/>
-    </row>
-    <row r="113" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A113" s="92" t="s">
-        <v>431</v>
-      </c>
-      <c r="B113" s="93"/>
-      <c r="C113"/>
-    </row>
-    <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="57" t="s">
-        <v>436</v>
-      </c>
-      <c r="B114" s="79" t="s">
-        <v>435</v>
-      </c>
+      <c r="B114" s="98"/>
       <c r="C114"/>
     </row>
     <row r="115" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A115" s="57" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B115" s="79" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C115"/>
     </row>
     <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A116" s="57" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B116" s="79" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C116"/>
     </row>
     <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
+        <v>436</v>
+      </c>
+      <c r="B117" s="79" t="s">
+        <v>431</v>
+      </c>
+      <c r="C117"/>
+    </row>
+    <row r="118" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="57" t="s">
+        <v>437</v>
+      </c>
+      <c r="B118" s="79" t="s">
+        <v>430</v>
+      </c>
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="70" t="s">
+        <v>441</v>
+      </c>
+      <c r="B119" s="79" t="s">
+        <v>438</v>
+      </c>
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="57" t="s">
+        <v>440</v>
+      </c>
+      <c r="B120" s="79" t="s">
         <v>439</v>
       </c>
-      <c r="B117" s="79" t="s">
-        <v>432</v>
-      </c>
-      <c r="C117"/>
-    </row>
-    <row r="118" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="70" t="s">
+      <c r="C120"/>
+    </row>
+    <row r="121" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A121" s="70" t="s">
+        <v>442</v>
+      </c>
+      <c r="B121" s="80" t="s">
         <v>443</v>
       </c>
-      <c r="B118" s="79" t="s">
-        <v>440</v>
-      </c>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
-        <v>442</v>
-      </c>
-      <c r="B119" s="79" t="s">
-        <v>441</v>
-      </c>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="70" t="s">
+      <c r="C121"/>
+    </row>
+    <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="B120" s="80" t="s">
+      <c r="B122" s="79" t="s">
         <v>445</v>
       </c>
-      <c r="C120"/>
-    </row>
-    <row r="121" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="57" t="s">
+      <c r="C122"/>
+    </row>
+    <row r="123" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A123" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="B121" s="79" t="s">
+      <c r="B123" s="80" t="s">
         <v>447</v>
       </c>
-      <c r="C121"/>
-    </row>
-    <row r="122" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A122" s="57" t="s">
+      <c r="C123"/>
+    </row>
+    <row r="124" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A124" s="99" t="s">
+        <v>503</v>
+      </c>
+      <c r="B124" s="98"/>
+      <c r="C124"/>
+    </row>
+    <row r="125" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A125" s="57" t="s">
         <v>448</v>
       </c>
-      <c r="B122" s="80" t="s">
+      <c r="B125" s="80" t="s">
+        <v>502</v>
+      </c>
+      <c r="C125"/>
+    </row>
+    <row r="126" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A126" s="57" t="s">
         <v>449</v>
       </c>
-      <c r="C122"/>
-    </row>
-    <row r="123" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A123" s="92" t="s">
-        <v>506</v>
-      </c>
-      <c r="B123" s="93"/>
-      <c r="C123"/>
-    </row>
-    <row r="124" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
+      <c r="B126" s="80" t="s">
         <v>450</v>
-      </c>
-      <c r="B124" s="80" t="s">
-        <v>505</v>
-      </c>
-      <c r="C124"/>
-    </row>
-    <row r="125" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A125" s="57" t="s">
-        <v>451</v>
-      </c>
-      <c r="B125" s="80" t="s">
-        <v>452</v>
-      </c>
-      <c r="C125"/>
-    </row>
-    <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="57" t="s">
-        <v>453</v>
-      </c>
-      <c r="B126" s="79" t="s">
-        <v>454</v>
       </c>
       <c r="C126"/>
     </row>
     <row r="127" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A127" s="57" t="s">
+        <v>451</v>
+      </c>
+      <c r="B127" s="79" t="s">
+        <v>452</v>
+      </c>
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="57" t="s">
+        <v>453</v>
+      </c>
+      <c r="B128" s="79" t="s">
+        <v>454</v>
+      </c>
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="70" t="s">
         <v>455</v>
       </c>
-      <c r="B127" s="79" t="s">
+      <c r="B129" s="79" t="s">
         <v>456</v>
       </c>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A128" s="70" t="s">
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
+      <c r="A130" s="77" t="s">
+        <v>458</v>
+      </c>
+      <c r="B130" s="80" t="s">
         <v>457</v>
       </c>
-      <c r="B128" s="79" t="s">
-        <v>458</v>
-      </c>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
-      <c r="A129" s="77" t="s">
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A131" s="78" t="s">
+        <v>459</v>
+      </c>
+      <c r="B131" s="80" t="s">
         <v>460</v>
       </c>
-      <c r="B129" s="80" t="s">
-        <v>459</v>
-      </c>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A130" s="78" t="s">
-        <v>461</v>
-      </c>
-      <c r="B130" s="80" t="s">
-        <v>462</v>
-      </c>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A131" s="78" t="s">
-        <v>463</v>
-      </c>
-      <c r="B131" s="79"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A132" s="78" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B132" s="79"/>
       <c r="C132"/>
     </row>
-    <row r="133" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A133" s="78" t="s">
+        <v>462</v>
+      </c>
+      <c r="B133" s="79"/>
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+      <c r="A134" s="78" t="s">
+        <v>463</v>
+      </c>
+      <c r="B134" s="80" t="s">
+        <v>474</v>
+      </c>
+      <c r="C134"/>
+    </row>
+    <row r="135" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A135" s="97" t="s">
+        <v>464</v>
+      </c>
+      <c r="B135" s="98"/>
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A136" s="78" t="s">
+        <v>466</v>
+      </c>
+      <c r="B136" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="B133" s="80" t="s">
-        <v>477</v>
-      </c>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="95" t="s">
-        <v>466</v>
-      </c>
-      <c r="B134" s="93"/>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A135" s="78" t="s">
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A137" s="70" t="s">
+        <v>467</v>
+      </c>
+      <c r="B137" s="86" t="s">
+        <v>470</v>
+      </c>
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A138" s="78" t="s">
         <v>468</v>
       </c>
-      <c r="B135" s="80" t="s">
-        <v>467</v>
-      </c>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A136" s="70" t="s">
+      <c r="B138" s="80" t="s">
         <v>469</v>
       </c>
-      <c r="B136" s="86" t="s">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A139" s="97" t="s">
         <v>472</v>
       </c>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A137" s="78" t="s">
-        <v>470</v>
-      </c>
-      <c r="B137" s="80" t="s">
+      <c r="B139" s="98"/>
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A140" s="70" t="s">
         <v>471</v>
       </c>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A138" s="95" t="s">
+      <c r="B140" s="87" t="s">
+        <v>473</v>
+      </c>
+      <c r="C140"/>
+    </row>
+    <row r="141" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A141" s="93" t="s">
         <v>475</v>
-      </c>
-      <c r="B138" s="93"/>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A139" s="70" t="s">
-        <v>474</v>
-      </c>
-      <c r="B139" s="87" t="s">
-        <v>476</v>
-      </c>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="94" t="s">
-        <v>478</v>
-      </c>
-      <c r="B140" s="94"/>
-      <c r="C140"/>
-    </row>
-    <row r="141" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A141" s="92" t="s">
-        <v>481</v>
       </c>
       <c r="B141" s="93"/>
       <c r="C141"/>
     </row>
-    <row r="142" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A142" s="57" t="s">
+    <row r="142" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A142" s="99" t="s">
+        <v>478</v>
+      </c>
+      <c r="B142" s="98"/>
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A143" s="57" t="s">
+        <v>479</v>
+      </c>
+      <c r="B143" s="76" t="s">
+        <v>537</v>
+      </c>
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A144" s="57" t="s">
+        <v>535</v>
+      </c>
+      <c r="B144" s="80" t="s">
+        <v>536</v>
+      </c>
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A145" s="70"/>
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A146" s="97" t="s">
         <v>482</v>
       </c>
-      <c r="B142" s="76" t="s">
-        <v>541</v>
-      </c>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A143" s="57" t="s">
-        <v>539</v>
-      </c>
-      <c r="B143" s="80" t="s">
-        <v>540</v>
-      </c>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="70"/>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A145" s="95" t="s">
-        <v>485</v>
-      </c>
-      <c r="B145" s="96"/>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A146" s="57" t="s">
-        <v>484</v>
-      </c>
-      <c r="B146" s="76" t="s">
-        <v>483</v>
-      </c>
+      <c r="B146" s="106"/>
       <c r="C146"/>
     </row>
-    <row r="147" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A147" s="57" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="B147" s="76" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="C147"/>
     </row>
     <row r="148" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="57" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B148" s="76" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A149" s="57" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B149" s="76" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A150" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="B150" s="76" t="s">
+        <v>480</v>
+      </c>
+      <c r="C150"/>
+    </row>
+    <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A151" s="57" t="s">
+        <v>488</v>
+      </c>
+      <c r="B151" s="76" t="s">
+        <v>489</v>
+      </c>
+      <c r="C151"/>
+    </row>
+    <row r="152" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A152" s="57" t="s">
+        <v>490</v>
+      </c>
+      <c r="B152" s="76" t="s">
         <v>491</v>
       </c>
-      <c r="B150" s="76" t="s">
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="57" t="s">
+        <v>500</v>
+      </c>
+      <c r="B153" s="88" t="s">
+        <v>501</v>
+      </c>
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A154" s="99" t="s">
+        <v>476</v>
+      </c>
+      <c r="B154" s="98"/>
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A155" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A151" s="57" t="s">
+      <c r="B155" s="76" t="s">
         <v>493</v>
       </c>
-      <c r="B151" s="76" t="s">
+      <c r="C155"/>
+    </row>
+    <row r="156" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A156" s="57" t="s">
+        <v>495</v>
+      </c>
+      <c r="B156" s="76" t="s">
         <v>494</v>
       </c>
-      <c r="C151"/>
-    </row>
-    <row r="152" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="57" t="s">
-        <v>503</v>
-      </c>
-      <c r="B152" s="88" t="s">
-        <v>504</v>
-      </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A153" s="92" t="s">
-        <v>479</v>
-      </c>
-      <c r="B153" s="93"/>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A154" s="57" t="s">
-        <v>495</v>
-      </c>
-      <c r="B154" s="76" t="s">
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A157" s="99" t="s">
+        <v>477</v>
+      </c>
+      <c r="B157" s="98"/>
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A158" s="57" t="s">
         <v>496</v>
       </c>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A155" s="57" t="s">
+      <c r="B158" s="76" t="s">
+        <v>497</v>
+      </c>
+      <c r="C158"/>
+    </row>
+    <row r="159" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A159" s="57" t="s">
         <v>498</v>
       </c>
-      <c r="B155" s="76" t="s">
-        <v>497</v>
-      </c>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A156" s="92" t="s">
-        <v>480</v>
-      </c>
-      <c r="B156" s="93"/>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A157" s="57" t="s">
+      <c r="B159" s="76" t="s">
         <v>499</v>
       </c>
-      <c r="B157" s="76" t="s">
-        <v>500</v>
-      </c>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A158" s="57" t="s">
-        <v>501</v>
-      </c>
-      <c r="B158" s="76" t="s">
-        <v>502</v>
-      </c>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="57"/>
-      <c r="B159" s="76"/>
       <c r="C159"/>
+    </row>
+    <row r="160" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A160" s="57"/>
+      <c r="B160" s="76"/>
+      <c r="C160"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A71:A80"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A124:B124"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A2:B2"/>
@@ -10215,27 +10270,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A71:A80"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A153:B153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# DB - EXERCISE 23.09.2019
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="554">
   <si>
     <t>Операция</t>
   </si>
@@ -4436,23 +4436,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">GROUP BY </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>allows you to get each separate group and use
-an "aggregate" function over it (like Average, Min or Max):</t>
-    </r>
-  </si>
-  <si>
     <t>SELECT e.DepartmentID,
 MIN(e.Salary) AS MinSalary
 FROM Employees AS e
@@ -5064,11 +5047,6 @@
 FROM Employees</t>
   </si>
   <si>
-    <t>SELECT DepartmentID
-FROM Employees
-GROUP BY DepartmentID</t>
-  </si>
-  <si>
     <t>All T-SQL prior GO will execute "at once"</t>
   </si>
   <si>
@@ -5200,6 +5178,203 @@
   </si>
   <si>
     <t>Evaluates the arguments in order and returns the current value of the first expression that initially doesn't evaluate to NULL. For example, SELECT COALESCE(NULL, NULL, 'third_value', 'fourth_value'); returns the third value because the third value is the first value that isn't null.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT DepartmentID
+FROM Employees
+GROUP BY DepartmentID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  DepositGroup ,MagicWandCreator , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MIN(DepositCharge)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> WizzardDeposits
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GROUP BY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DepositGroup, MagicWandCreator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GROUP BY </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>allows you to get each separate group and use
+an "aggregate" function over it (like Average, Min or Max)
+Колоните които не се агрегират трябва да участват задължително в GROUP BY - GROUP BY DepositGroup, MagicWandCreator</t>
+    </r>
+  </si>
+  <si>
+    <t>Сумиране на клетка от ред със стойност на клетка от следващия ред</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SELECT SUM(dif.[Difference]) AS SumDifference FROM(
+      SELECT wd.DepositAmount ,
+       (SELECT wd.DepositAmount - w.DepositAmount FROM WizzardDeposits AS w WHERE w.Id = wd.Id+1) AS      [Difference] 
+      FROM WizzardDeposits AS wd
+ ) AS dif</t>
+  </si>
+  <si>
+    <t>OTHER Functions</t>
+  </si>
+  <si>
+    <r>
+      <t>LEAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - or example, by using the LEAD() function, from the current row, you can access data of the next row, or the row after the next row, and so on.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LAG </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-  by using the LAG() function, from the current row, you can access data of the previous row, or the row before the previous row, and so on. </t>
+    </r>
+  </si>
+  <si>
+    <t>LAG(return_value ,offset [,default]) 
+OVER (
+    [PARTITION BY partition_expression, ... ]
+    ORDER BY sort_expression [ASC | DESC], ...)</t>
+  </si>
+  <si>
+    <t>LEAD(return_value ,offset [,default]) 
+OVER (
+    [PARTITION BY partition_expression, ... ]
+    ORDER BY sort_expression [ASC | DESC], ...)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To delete rows - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DELETE FROM table_name WHERE condition;</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT * INTO NewTable
+FROM Employees 
+WHERE Salary &gt; 30000</t>
+  </si>
+  <si>
+    <t>Създаване на таблица от съществуваща чрез SELECT</t>
   </si>
 </sst>
 </file>
@@ -5925,7 +6100,7 @@
     <xf numFmtId="0" fontId="34" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6176,29 +6351,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6218,8 +6390,17 @@
     <xf numFmtId="0" fontId="35" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6233,11 +6414,17 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -8969,10 +9156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C160"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8991,90 +9178,90 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="96" t="s">
         <v>343</v>
       </c>
-      <c r="B2" s="94"/>
+      <c r="B2" s="106"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="96" t="s">
-        <v>509</v>
-      </c>
-      <c r="B3" s="95"/>
+      <c r="A3" s="108" t="s">
+        <v>508</v>
+      </c>
+      <c r="B3" s="107"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4" s="74" t="s">
         <v>510</v>
-      </c>
-      <c r="B4" s="74" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" s="74" t="s">
         <v>512</v>
-      </c>
-      <c r="B5" s="74" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
+        <v>513</v>
+      </c>
+      <c r="B6" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="B6" s="74" t="s">
-        <v>515</v>
-      </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="95" t="s">
-        <v>521</v>
-      </c>
-      <c r="B7" s="92"/>
+      <c r="A7" s="107" t="s">
+        <v>520</v>
+      </c>
+      <c r="B7" s="105"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
+        <v>521</v>
+      </c>
+      <c r="B8" s="89" t="s">
         <v>522</v>
-      </c>
-      <c r="B8" s="89" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
+        <v>526</v>
+      </c>
+      <c r="B9" s="116" t="s">
         <v>527</v>
-      </c>
-      <c r="B9" s="89" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
+        <v>528</v>
+      </c>
+      <c r="B10" s="89" t="s">
         <v>529</v>
       </c>
-      <c r="B10" s="89" t="s">
-        <v>530</v>
-      </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="95" t="s">
-        <v>524</v>
-      </c>
-      <c r="B11" s="92"/>
+      <c r="A11" s="107" t="s">
+        <v>523</v>
+      </c>
+      <c r="B11" s="105"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
+        <v>524</v>
+      </c>
+      <c r="B12" s="90" t="s">
         <v>525</v>
       </c>
-      <c r="B12" s="90" t="s">
-        <v>526</v>
-      </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="107" t="s">
         <v>389</v>
       </c>
-      <c r="B13" s="95"/>
+      <c r="B13" s="107"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -9118,31 +9305,31 @@
     </row>
     <row r="19" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="B19" s="74" t="s">
         <v>504</v>
       </c>
-      <c r="B19" s="74" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="107" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="95" t="s">
-        <v>506</v>
-      </c>
-      <c r="B20" s="95"/>
+      <c r="B20" s="107"/>
     </row>
     <row r="21" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
         <v>341</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="107" t="s">
         <v>388</v>
       </c>
-      <c r="B22" s="95"/>
+      <c r="B22" s="107"/>
     </row>
     <row r="23" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
@@ -9153,10 +9340,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="95" t="s">
+      <c r="A24" s="107" t="s">
         <v>353</v>
       </c>
-      <c r="B24" s="95"/>
+      <c r="B24" s="107"/>
     </row>
     <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="57" t="s">
@@ -9183,10 +9370,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="95" t="s">
+      <c r="A28" s="107" t="s">
         <v>353</v>
       </c>
-      <c r="B28" s="95"/>
+      <c r="B28" s="107"/>
     </row>
     <row r="29" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="72" t="s">
@@ -9213,10 +9400,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="92" t="s">
+      <c r="A32" s="105" t="s">
         <v>363</v>
       </c>
-      <c r="B32" s="92"/>
+      <c r="B32" s="105"/>
     </row>
     <row r="33" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="72" t="s">
@@ -9239,14 +9426,14 @@
         <v>381</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="95" t="s">
+      <c r="A36" s="107" t="s">
         <v>360</v>
       </c>
-      <c r="B36" s="95"/>
+      <c r="B36" s="107"/>
     </row>
     <row r="37" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="72" t="s">
@@ -9273,17 +9460,17 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="92" t="s">
+      <c r="A40" s="105" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="92"/>
+      <c r="B40" s="105"/>
     </row>
     <row r="41" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A41" s="57" t="s">
         <v>378</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
@@ -9295,10 +9482,10 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="95" t="s">
-        <v>516</v>
-      </c>
-      <c r="B43" s="92"/>
+      <c r="A43" s="107" t="s">
+        <v>515</v>
+      </c>
+      <c r="B43" s="105"/>
     </row>
     <row r="44" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
@@ -9310,34 +9497,34 @@
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
+        <v>516</v>
+      </c>
+      <c r="B45" s="74" t="s">
         <v>517</v>
-      </c>
-      <c r="B45" s="74" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
+        <v>518</v>
+      </c>
+      <c r="B46" s="74" t="s">
         <v>519</v>
       </c>
-      <c r="B46" s="74" t="s">
-        <v>520</v>
-      </c>
     </row>
     <row r="47" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="96" t="s">
         <v>374</v>
       </c>
-      <c r="B47" s="93"/>
+      <c r="B47" s="96"/>
     </row>
     <row r="48" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A48" s="99" t="s">
+      <c r="A48" s="94" t="s">
         <v>312</v>
       </c>
-      <c r="B48" s="98"/>
+      <c r="B48" s="95"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="103" t="s">
+      <c r="A49" s="102" t="s">
         <v>322</v>
       </c>
       <c r="B49" s="62" t="s">
@@ -9345,7 +9532,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="104"/>
+      <c r="A50" s="103"/>
       <c r="B50" s="62" t="s">
         <v>314</v>
       </c>
@@ -9354,13 +9541,13 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="105"/>
+      <c r="A51" s="104"/>
       <c r="B51" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="103" t="s">
+      <c r="A52" s="102" t="s">
         <v>323</v>
       </c>
       <c r="B52" s="62" t="s">
@@ -9368,25 +9555,25 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="104"/>
+      <c r="A53" s="103"/>
       <c r="B53" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="104"/>
+      <c r="A54" s="103"/>
       <c r="B54" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="105"/>
+      <c r="A55" s="104"/>
       <c r="B55" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="103" t="s">
+      <c r="A56" s="102" t="s">
         <v>324</v>
       </c>
       <c r="B56" s="62" t="s">
@@ -9394,13 +9581,13 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="105"/>
+      <c r="A57" s="104"/>
       <c r="B57" s="62" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="103" t="s">
+      <c r="A58" s="102" t="s">
         <v>325</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -9411,23 +9598,23 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="104"/>
+      <c r="A59" s="103"/>
       <c r="B59" s="62" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C59" s="68" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="104"/>
+      <c r="A60" s="103"/>
       <c r="B60" s="62" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C60" s="68"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="105"/>
+      <c r="A61" s="104"/>
       <c r="B61" s="62" t="s">
         <v>327</v>
       </c>
@@ -9445,817 +9632,861 @@
         <v>285</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="57" t="s">
+        <v>553</v>
+      </c>
+      <c r="B64" s="62" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="57" t="s">
         <v>286</v>
       </c>
-      <c r="B64" s="62" t="s">
+      <c r="B65" s="62" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="100" t="s">
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="B65" s="62" t="s">
+      <c r="B66" s="62" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="101"/>
-      <c r="B66" s="62" t="s">
+    <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="100"/>
+      <c r="B67" s="62" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="101"/>
-      <c r="B67" s="62" t="s">
+    <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="100"/>
+      <c r="B68" s="62" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="101"/>
-      <c r="B68" s="62" t="s">
+    <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="100"/>
+      <c r="B69" s="62" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="101"/>
-      <c r="B69" s="62" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="102"/>
+    <row r="70" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="100"/>
       <c r="B70" s="62" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="101"/>
+      <c r="B71" s="62" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="100" t="s">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="99" t="s">
         <v>291</v>
       </c>
-      <c r="B71" s="62" t="s">
+      <c r="B72" s="62" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="101"/>
-      <c r="B72" s="62" t="s">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="100"/>
+      <c r="B73" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="C72" s="67"/>
-    </row>
-    <row r="73" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="101"/>
-      <c r="B73" s="62" t="s">
+      <c r="C73" s="67"/>
+    </row>
+    <row r="74" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="100"/>
+      <c r="B74" s="62" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="101"/>
-      <c r="B74" s="62" t="s">
+    <row r="75" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="100"/>
+      <c r="B75" s="62" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="101"/>
-      <c r="B75" s="81" t="s">
+    <row r="76" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A76" s="100"/>
+      <c r="B76" s="81" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="101"/>
-      <c r="B76" s="81" t="s">
+    <row r="77" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="100"/>
+      <c r="B77" s="81" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="101"/>
-      <c r="B77" s="81" t="s">
+    <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="100"/>
+      <c r="B78" s="81" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="101"/>
-      <c r="B78" s="81" t="s">
+    <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="100"/>
+      <c r="B79" s="81" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="101"/>
-      <c r="B79" s="81" t="s">
+    <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="100"/>
+      <c r="B80" s="81" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="102"/>
-      <c r="B80" s="81" t="s">
+    <row r="81" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="101"/>
+      <c r="B81" s="81" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="100" t="s">
+    <row r="82" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="99" t="s">
         <v>292</v>
       </c>
-      <c r="B81" s="82" t="s">
+      <c r="B82" s="82" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="101"/>
-      <c r="B82" s="83" t="s">
+    <row r="83" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="100"/>
+      <c r="B83" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="C82"/>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="102"/>
-      <c r="B83" s="83" t="s">
+      <c r="C83"/>
+    </row>
+    <row r="84" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="100"/>
+      <c r="B84" s="83" t="s">
         <v>308</v>
       </c>
-      <c r="C83"/>
-    </row>
-    <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="100" t="s">
+      <c r="C84"/>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="101"/>
+      <c r="B85" s="82" t="s">
+        <v>551</v>
+      </c>
+      <c r="C85"/>
+    </row>
+    <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="99" t="s">
         <v>309</v>
       </c>
-      <c r="B84" s="84" t="s">
+      <c r="B86" s="84" t="s">
         <v>310</v>
       </c>
-      <c r="C84"/>
-    </row>
-    <row r="85" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="102"/>
-      <c r="B85" s="84" t="s">
+      <c r="C86"/>
+    </row>
+    <row r="87" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A87" s="101"/>
+      <c r="B87" s="84" t="s">
         <v>311</v>
       </c>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="69" t="s">
+      <c r="C87"/>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="69" t="s">
         <v>337</v>
       </c>
-      <c r="B86" s="83" t="s">
+      <c r="B88" s="83" t="s">
         <v>338</v>
       </c>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="65" t="s">
+      <c r="C88"/>
+    </row>
+    <row r="89" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="65" t="s">
         <v>336</v>
       </c>
-      <c r="B87" s="84" t="s">
+      <c r="B89" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="61" t="s">
+      <c r="C89"/>
+    </row>
+    <row r="90" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="61" t="s">
         <v>387</v>
       </c>
-      <c r="B88" s="85" t="s">
+      <c r="B90" s="85" t="s">
         <v>329</v>
       </c>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="71" t="s">
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="71" t="s">
         <v>375</v>
       </c>
-      <c r="B89" s="84" t="s">
-        <v>539</v>
-      </c>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="91" t="s">
-        <v>534</v>
-      </c>
-      <c r="B90" s="81" t="s">
-        <v>538</v>
-      </c>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="73" t="s">
+      <c r="B91" s="84" t="s">
+        <v>537</v>
+      </c>
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="91" t="s">
+        <v>533</v>
+      </c>
+      <c r="B92" s="81" t="s">
+        <v>536</v>
+      </c>
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="73" t="s">
         <v>377</v>
       </c>
-      <c r="B91" s="81" t="s">
+      <c r="B93" s="81" t="s">
         <v>376</v>
       </c>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="93" t="s">
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="96" t="s">
         <v>390</v>
       </c>
-      <c r="B92" s="93"/>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A93" s="99" t="s">
+      <c r="B94" s="96"/>
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A95" s="94" t="s">
         <v>391</v>
       </c>
-      <c r="B93" s="98"/>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="70" t="s">
+      <c r="B95" s="95"/>
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="70" t="s">
         <v>392</v>
       </c>
-      <c r="B94" s="60" t="s">
+      <c r="B96" s="60" t="s">
         <v>393</v>
       </c>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="70" t="s">
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="70" t="s">
         <v>394</v>
       </c>
-      <c r="B95" s="76" t="s">
+      <c r="B97" s="76" t="s">
         <v>395</v>
       </c>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="70" t="s">
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="70" t="s">
         <v>396</v>
       </c>
-      <c r="B96" s="76" t="s">
+      <c r="B98" s="76" t="s">
         <v>397</v>
       </c>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A97" s="99" t="s">
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A99" s="94" t="s">
         <v>398</v>
       </c>
-      <c r="B97" s="98"/>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A98" s="57" t="s">
+      <c r="B99" s="95"/>
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A100" s="57" t="s">
         <v>400</v>
       </c>
-      <c r="B98" s="80" t="s">
+      <c r="B100" s="80" t="s">
         <v>399</v>
       </c>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="57" t="s">
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="B99" s="80" t="s">
+      <c r="B101" s="80" t="s">
         <v>402</v>
       </c>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A100" s="72" t="s">
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A102" s="72" t="s">
         <v>403</v>
       </c>
-      <c r="B100" s="80" t="s">
+      <c r="B102" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A101" s="57" t="s">
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="B101" s="80" t="s">
+      <c r="B103" s="80" t="s">
         <v>406</v>
       </c>
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="57" t="s">
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="B102" s="80" t="s">
+      <c r="B104" s="80" t="s">
         <v>408</v>
       </c>
-      <c r="C102"/>
-    </row>
-    <row r="103" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="57" t="s">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="B103" s="79" t="s">
+      <c r="B105" s="79" t="s">
         <v>410</v>
       </c>
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="57" t="s">
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="B104" s="79" t="s">
+      <c r="B106" s="79" t="s">
         <v>412</v>
       </c>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A105" s="57" t="s">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A107" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="B105" s="86" t="s">
+      <c r="B107" s="86" t="s">
         <v>414</v>
       </c>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="57" t="s">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="B106" s="80" t="s">
+      <c r="B108" s="80" t="s">
         <v>415</v>
-      </c>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="57" t="s">
-        <v>422</v>
-      </c>
-      <c r="B107" s="79" t="s">
-        <v>416</v>
-      </c>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="B108" s="79" t="s">
-        <v>417</v>
       </c>
       <c r="C108"/>
     </row>
     <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A109" s="57" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B109" s="79" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C109"/>
     </row>
     <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="B110" s="79" t="s">
+        <v>417</v>
+      </c>
+      <c r="C110"/>
+    </row>
+    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="B111" s="79" t="s">
+        <v>419</v>
+      </c>
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="57" t="s">
         <v>420</v>
       </c>
-      <c r="B110" s="79" t="s">
+      <c r="B112" s="79" t="s">
         <v>424</v>
       </c>
-      <c r="C110"/>
-    </row>
-    <row r="111" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
+      <c r="C112"/>
+    </row>
+    <row r="113" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A113" s="57" t="s">
         <v>425</v>
       </c>
-      <c r="B111" s="79" t="s">
+      <c r="B113" s="79" t="s">
         <v>426</v>
       </c>
-      <c r="C111"/>
-    </row>
-    <row r="112" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="72" t="s">
+      <c r="C113"/>
+    </row>
+    <row r="114" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="72" t="s">
         <v>427</v>
       </c>
-      <c r="B112" s="80" t="s">
+      <c r="B114" s="80" t="s">
         <v>428</v>
       </c>
-      <c r="C112"/>
-    </row>
-    <row r="113" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="112" t="s">
-        <v>542</v>
-      </c>
-      <c r="B113" s="111" t="s">
-        <v>543</v>
-      </c>
-      <c r="C113"/>
-    </row>
-    <row r="114" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A114" s="99" t="s">
+      <c r="C114"/>
+    </row>
+    <row r="115" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="93" t="s">
+        <v>540</v>
+      </c>
+      <c r="B115" s="92" t="s">
+        <v>541</v>
+      </c>
+      <c r="C115"/>
+    </row>
+    <row r="116" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A116" s="94" t="s">
         <v>429</v>
       </c>
-      <c r="B114" s="98"/>
-      <c r="C114"/>
-    </row>
-    <row r="115" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
-        <v>434</v>
-      </c>
-      <c r="B115" s="79" t="s">
-        <v>433</v>
-      </c>
-      <c r="C115"/>
-    </row>
-    <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="57" t="s">
-        <v>435</v>
-      </c>
-      <c r="B116" s="79" t="s">
-        <v>432</v>
-      </c>
+      <c r="B116" s="95"/>
       <c r="C116"/>
     </row>
     <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B117" s="79" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C117"/>
     </row>
     <row r="118" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
+        <v>435</v>
+      </c>
+      <c r="B118" s="79" t="s">
+        <v>432</v>
+      </c>
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="57" t="s">
+        <v>436</v>
+      </c>
+      <c r="B119" s="79" t="s">
+        <v>431</v>
+      </c>
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="57" t="s">
         <v>437</v>
       </c>
-      <c r="B118" s="79" t="s">
+      <c r="B120" s="79" t="s">
         <v>430</v>
       </c>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="70" t="s">
+      <c r="C120"/>
+    </row>
+    <row r="121" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="70" t="s">
         <v>441</v>
       </c>
-      <c r="B119" s="79" t="s">
+      <c r="B121" s="79" t="s">
         <v>438</v>
       </c>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
+      <c r="C121"/>
+    </row>
+    <row r="122" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A122" s="57" t="s">
         <v>440</v>
       </c>
-      <c r="B120" s="79" t="s">
+      <c r="B122" s="79" t="s">
         <v>439</v>
       </c>
-      <c r="C120"/>
-    </row>
-    <row r="121" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A121" s="70" t="s">
+      <c r="C122"/>
+    </row>
+    <row r="123" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="70" t="s">
         <v>442</v>
       </c>
-      <c r="B121" s="80" t="s">
+      <c r="B123" s="80" t="s">
         <v>443</v>
       </c>
-      <c r="C121"/>
-    </row>
-    <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="57" t="s">
+      <c r="C123"/>
+    </row>
+    <row r="124" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="B122" s="79" t="s">
+      <c r="B124" s="79" t="s">
         <v>445</v>
       </c>
-      <c r="C122"/>
-    </row>
-    <row r="123" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
+      <c r="C124"/>
+    </row>
+    <row r="125" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A125" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="B123" s="80" t="s">
+      <c r="B125" s="80" t="s">
         <v>447</v>
       </c>
-      <c r="C123"/>
-    </row>
-    <row r="124" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A124" s="99" t="s">
-        <v>503</v>
-      </c>
-      <c r="B124" s="98"/>
-      <c r="C124"/>
-    </row>
-    <row r="125" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A125" s="57" t="s">
+      <c r="C125"/>
+    </row>
+    <row r="126" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A126" s="94" t="s">
+        <v>502</v>
+      </c>
+      <c r="B126" s="95"/>
+      <c r="C126"/>
+    </row>
+    <row r="127" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A127" s="57" t="s">
         <v>448</v>
       </c>
-      <c r="B125" s="80" t="s">
-        <v>502</v>
-      </c>
-      <c r="C125"/>
-    </row>
-    <row r="126" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A126" s="57" t="s">
+      <c r="B127" s="80" t="s">
+        <v>501</v>
+      </c>
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A128" s="57" t="s">
         <v>449</v>
       </c>
-      <c r="B126" s="80" t="s">
+      <c r="B128" s="80" t="s">
         <v>450</v>
       </c>
-      <c r="C126"/>
-    </row>
-    <row r="127" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="57" t="s">
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="57" t="s">
         <v>451</v>
       </c>
-      <c r="B127" s="79" t="s">
+      <c r="B129" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="57" t="s">
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="57" t="s">
         <v>453</v>
       </c>
-      <c r="B128" s="79" t="s">
+      <c r="B130" s="79" t="s">
         <v>454</v>
       </c>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A129" s="70" t="s">
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="70" t="s">
         <v>455</v>
       </c>
-      <c r="B129" s="79" t="s">
+      <c r="B131" s="79" t="s">
         <v>456</v>
       </c>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
-      <c r="A130" s="77" t="s">
+      <c r="C131"/>
+    </row>
+    <row r="132" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
+      <c r="A132" s="77" t="s">
         <v>458</v>
       </c>
-      <c r="B130" s="80" t="s">
+      <c r="B132" s="80" t="s">
         <v>457</v>
       </c>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A131" s="78" t="s">
+      <c r="C132"/>
+    </row>
+    <row r="133" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A133" s="78" t="s">
         <v>459</v>
       </c>
-      <c r="B131" s="80" t="s">
+      <c r="B133" s="80" t="s">
         <v>460</v>
       </c>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A132" s="78" t="s">
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A134" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="B132" s="79"/>
-      <c r="C132"/>
-    </row>
-    <row r="133" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A133" s="78" t="s">
+      <c r="B134" s="79"/>
+      <c r="C134"/>
+    </row>
+    <row r="135" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A135" s="78" t="s">
         <v>462</v>
       </c>
-      <c r="B133" s="79"/>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" ht="105" x14ac:dyDescent="0.3">
-      <c r="A134" s="78" t="s">
+      <c r="B135" s="79"/>
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+      <c r="A136" s="78" t="s">
         <v>463</v>
       </c>
-      <c r="B134" s="80" t="s">
+      <c r="B136" s="80" t="s">
         <v>474</v>
       </c>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="97" t="s">
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A137" s="97" t="s">
         <v>464</v>
       </c>
-      <c r="B135" s="98"/>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A136" s="78" t="s">
+      <c r="B137" s="95"/>
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A138" s="78" t="s">
         <v>466</v>
       </c>
-      <c r="B136" s="80" t="s">
+      <c r="B138" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A137" s="70" t="s">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A139" s="70" t="s">
         <v>467</v>
       </c>
-      <c r="B137" s="86" t="s">
+      <c r="B139" s="86" t="s">
         <v>470</v>
       </c>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A138" s="78" t="s">
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A140" s="78" t="s">
         <v>468</v>
       </c>
-      <c r="B138" s="80" t="s">
+      <c r="B140" s="80" t="s">
         <v>469</v>
       </c>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A139" s="97" t="s">
+      <c r="C140"/>
+    </row>
+    <row r="141" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A141" s="97" t="s">
         <v>472</v>
       </c>
-      <c r="B139" s="98"/>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A140" s="70" t="s">
+      <c r="B141" s="95"/>
+      <c r="C141"/>
+    </row>
+    <row r="142" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A142" s="70" t="s">
         <v>471</v>
       </c>
-      <c r="B140" s="87" t="s">
+      <c r="B142" s="87" t="s">
         <v>473</v>
       </c>
-      <c r="C140"/>
-    </row>
-    <row r="141" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A141" s="93" t="s">
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A143" s="114" t="s">
+        <v>544</v>
+      </c>
+      <c r="B143" s="113" t="s">
+        <v>545</v>
+      </c>
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A144" s="97" t="s">
+        <v>546</v>
+      </c>
+      <c r="B144" s="95"/>
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A145" s="57" t="s">
+        <v>547</v>
+      </c>
+      <c r="B145" s="80" t="s">
+        <v>550</v>
+      </c>
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A146" s="57" t="s">
+        <v>548</v>
+      </c>
+      <c r="B146" s="76" t="s">
+        <v>549</v>
+      </c>
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="57"/>
+      <c r="B147" s="115"/>
+      <c r="C147"/>
+    </row>
+    <row r="148" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A148" s="96" t="s">
         <v>475</v>
       </c>
-      <c r="B141" s="93"/>
-      <c r="C141"/>
-    </row>
-    <row r="142" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A142" s="99" t="s">
+      <c r="B148" s="96"/>
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A149" s="94" t="s">
         <v>478</v>
       </c>
-      <c r="B142" s="98"/>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A143" s="57" t="s">
-        <v>479</v>
-      </c>
-      <c r="B143" s="76" t="s">
-        <v>537</v>
-      </c>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A144" s="57" t="s">
+      <c r="B149" s="95"/>
+      <c r="C149"/>
+    </row>
+    <row r="150" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A150" s="57" t="s">
+        <v>543</v>
+      </c>
+      <c r="B150" s="76" t="s">
+        <v>542</v>
+      </c>
+      <c r="C150"/>
+    </row>
+    <row r="151" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A151" s="57" t="s">
+        <v>534</v>
+      </c>
+      <c r="B151" s="80" t="s">
         <v>535</v>
       </c>
-      <c r="B144" s="80" t="s">
-        <v>536</v>
-      </c>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="70"/>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="97" t="s">
-        <v>482</v>
-      </c>
-      <c r="B146" s="106"/>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A147" s="57" t="s">
+      <c r="C151"/>
+    </row>
+    <row r="152" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A152" s="57"/>
+      <c r="B152" s="80"/>
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="57"/>
+      <c r="B153" s="80"/>
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A154" s="70"/>
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="97" t="s">
         <v>481</v>
       </c>
-      <c r="B147" s="76" t="s">
-        <v>480</v>
-      </c>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A148" s="57" t="s">
-        <v>487</v>
-      </c>
-      <c r="B148" s="76" t="s">
-        <v>483</v>
-      </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A149" s="57" t="s">
-        <v>485</v>
-      </c>
-      <c r="B149" s="76" t="s">
-        <v>484</v>
-      </c>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A150" s="57" t="s">
-        <v>486</v>
-      </c>
-      <c r="B150" s="76" t="s">
-        <v>480</v>
-      </c>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A151" s="57" t="s">
-        <v>488</v>
-      </c>
-      <c r="B151" s="76" t="s">
-        <v>489</v>
-      </c>
-      <c r="C151"/>
-    </row>
-    <row r="152" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A152" s="57" t="s">
-        <v>490</v>
-      </c>
-      <c r="B152" s="76" t="s">
-        <v>491</v>
-      </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="57" t="s">
-        <v>500</v>
-      </c>
-      <c r="B153" s="88" t="s">
-        <v>501</v>
-      </c>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="99" t="s">
-        <v>476</v>
-      </c>
-      <c r="B154" s="98"/>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A155" s="57" t="s">
-        <v>492</v>
-      </c>
-      <c r="B155" s="76" t="s">
-        <v>493</v>
-      </c>
+      <c r="B155" s="98"/>
       <c r="C155"/>
     </row>
     <row r="156" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="57" t="s">
+        <v>480</v>
+      </c>
+      <c r="B156" s="76" t="s">
+        <v>479</v>
+      </c>
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A157" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="B157" s="76" t="s">
+        <v>482</v>
+      </c>
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A158" s="57" t="s">
+        <v>484</v>
+      </c>
+      <c r="B158" s="76" t="s">
+        <v>483</v>
+      </c>
+      <c r="C158"/>
+    </row>
+    <row r="159" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A159" s="57" t="s">
+        <v>485</v>
+      </c>
+      <c r="B159" s="76" t="s">
+        <v>479</v>
+      </c>
+      <c r="C159"/>
+    </row>
+    <row r="160" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A160" s="57" t="s">
+        <v>487</v>
+      </c>
+      <c r="B160" s="76" t="s">
+        <v>488</v>
+      </c>
+      <c r="C160"/>
+    </row>
+    <row r="161" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A161" s="57" t="s">
+        <v>489</v>
+      </c>
+      <c r="B161" s="76" t="s">
+        <v>490</v>
+      </c>
+      <c r="C161"/>
+    </row>
+    <row r="162" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="57" t="s">
+        <v>499</v>
+      </c>
+      <c r="B162" s="88" t="s">
+        <v>500</v>
+      </c>
+      <c r="C162"/>
+    </row>
+    <row r="163" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A163" s="94" t="s">
+        <v>476</v>
+      </c>
+      <c r="B163" s="95"/>
+      <c r="C163"/>
+    </row>
+    <row r="164" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A164" s="57" t="s">
+        <v>491</v>
+      </c>
+      <c r="B164" s="76" t="s">
+        <v>492</v>
+      </c>
+      <c r="C164"/>
+    </row>
+    <row r="165" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A165" s="57" t="s">
+        <v>494</v>
+      </c>
+      <c r="B165" s="76" t="s">
+        <v>493</v>
+      </c>
+      <c r="C165"/>
+    </row>
+    <row r="166" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A166" s="94" t="s">
+        <v>477</v>
+      </c>
+      <c r="B166" s="95"/>
+      <c r="C166"/>
+    </row>
+    <row r="167" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A167" s="57" t="s">
         <v>495</v>
       </c>
-      <c r="B156" s="76" t="s">
-        <v>494</v>
-      </c>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A157" s="99" t="s">
-        <v>477</v>
-      </c>
-      <c r="B157" s="98"/>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A158" s="57" t="s">
+      <c r="B167" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="B158" s="76" t="s">
+      <c r="C167"/>
+    </row>
+    <row r="168" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A168" s="57" t="s">
         <v>497</v>
       </c>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A159" s="57" t="s">
+      <c r="B168" s="76" t="s">
         <v>498</v>
       </c>
-      <c r="B159" s="76" t="s">
-        <v>499</v>
-      </c>
-      <c r="C159"/>
-    </row>
-    <row r="160" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="57"/>
-      <c r="B160" s="76"/>
-      <c r="C160"/>
+      <c r="C168"/>
+    </row>
+    <row r="169" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A169" s="57"/>
+      <c r="B169" s="76"/>
+      <c r="C169"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A71:A80"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A124:B124"/>
+  <mergeCells count="36">
+    <mergeCell ref="A144:B144"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A2:B2"/>
@@ -10270,6 +10501,27 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A72:A81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A163:B163"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10691,7 +10943,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="109" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -10711,7 +10963,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="108"/>
+      <c r="A2" s="110"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -10779,10 +11031,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="111" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="110"/>
+      <c r="C6" s="112"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - EXERCISE 24.09.2019
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="556">
   <si>
     <t>Операция</t>
   </si>
@@ -4401,15 +4401,6 @@
       WHERE SubTable.Rank = 2 </t>
   </si>
   <si>
-    <t xml:space="preserve">SELECT *
- FROM (
-     SELECT EmployeeID, FirstName,LastName, Salary, 
-     DENSE_RANK() OVER (PARTITION BY Salary ORDER BY EmployeeID) AS Rank
-     FROM Employees 
-     WHERE Salary BETWEEN 10000 AND 50000 ) AS SubTable
- WHERE SubTable.Rank = 2 </t>
-  </si>
-  <si>
     <t>Data Aggregation - COUNT, SUM, MAX, MIN, AVG…</t>
   </si>
   <si>
@@ -5376,17 +5367,49 @@
   <si>
     <t>Създаване на таблица от съществуваща чрез SELECT</t>
   </si>
+  <si>
+    <t xml:space="preserve">DENSE_RANK again gives you the ranking within your ordered partition, but the ranks are consecutive. No ranks are skipped if there are ranks with multiple items.
+SELECT *
+ FROM (
+     SELECT EmployeeID, FirstName,LastName, Salary, 
+     DENSE_RANK() OVER (PARTITION BY Salary ORDER BY EmployeeID) AS Rank
+     FROM Employees 
+     WHERE Salary BETWEEN 10000 AND 50000 ) AS SubTable
+ WHERE SubTable.Rank = 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANK gives you the ranking within your ordered partition. Ties are assigned the same rank, with the next ranking(s) skipped. So, if you have 3 items at rank 2, the next rank listed would be ranked 5.
+SELECT *
+ FROM (
+     SELECT EmployeeID, FirstName,LastName, Salary, 
+     RANK() OVER (PARTITION BY Salary ORDER BY EmployeeID) AS Rank
+     FROM Employees 
+     WHERE Salary BETWEEN 10000 AND 50000 ) AS SubTable
+ WHERE SubTable.Rank = 2 </t>
+  </si>
+  <si>
+    <t>SELECT ROW_NUMBER() OVER (Order by Id) AS RowNumber, Field1, Field2, Field3
+FROM User</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6094,42 +6117,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6144,91 +6167,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6243,73 +6266,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6318,113 +6341,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -9158,8 +9181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9178,90 +9201,90 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="101" t="s">
         <v>343</v>
       </c>
-      <c r="B2" s="106"/>
+      <c r="B2" s="102"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="108" t="s">
-        <v>508</v>
-      </c>
-      <c r="B3" s="107"/>
+      <c r="A3" s="104" t="s">
+        <v>507</v>
+      </c>
+      <c r="B3" s="103"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
+        <v>508</v>
+      </c>
+      <c r="B4" s="74" t="s">
         <v>509</v>
-      </c>
-      <c r="B4" s="74" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
+        <v>510</v>
+      </c>
+      <c r="B5" s="74" t="s">
         <v>511</v>
-      </c>
-      <c r="B5" s="74" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
+        <v>512</v>
+      </c>
+      <c r="B6" s="74" t="s">
         <v>513</v>
       </c>
-      <c r="B6" s="74" t="s">
-        <v>514</v>
-      </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
-        <v>520</v>
-      </c>
-      <c r="B7" s="105"/>
+      <c r="A7" s="103" t="s">
+        <v>519</v>
+      </c>
+      <c r="B7" s="100"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
+        <v>520</v>
+      </c>
+      <c r="B8" s="89" t="s">
         <v>521</v>
-      </c>
-      <c r="B8" s="89" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
+        <v>525</v>
+      </c>
+      <c r="B9" s="97" t="s">
         <v>526</v>
-      </c>
-      <c r="B9" s="116" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
+        <v>527</v>
+      </c>
+      <c r="B10" s="89" t="s">
         <v>528</v>
       </c>
-      <c r="B10" s="89" t="s">
-        <v>529</v>
-      </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="107" t="s">
-        <v>523</v>
-      </c>
-      <c r="B11" s="105"/>
+      <c r="A11" s="103" t="s">
+        <v>522</v>
+      </c>
+      <c r="B11" s="100"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
+        <v>523</v>
+      </c>
+      <c r="B12" s="90" t="s">
         <v>524</v>
       </c>
-      <c r="B12" s="90" t="s">
-        <v>525</v>
-      </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="103" t="s">
         <v>389</v>
       </c>
-      <c r="B13" s="107"/>
+      <c r="B13" s="103"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -9305,31 +9328,31 @@
     </row>
     <row r="19" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
+        <v>502</v>
+      </c>
+      <c r="B19" s="74" t="s">
         <v>503</v>
       </c>
-      <c r="B19" s="74" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="103" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="107" t="s">
-        <v>505</v>
-      </c>
-      <c r="B20" s="107"/>
+      <c r="B20" s="103"/>
     </row>
     <row r="21" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
         <v>341</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="107" t="s">
+      <c r="A22" s="103" t="s">
         <v>388</v>
       </c>
-      <c r="B22" s="107"/>
+      <c r="B22" s="103"/>
     </row>
     <row r="23" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
@@ -9340,10 +9363,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="103" t="s">
         <v>353</v>
       </c>
-      <c r="B24" s="107"/>
+      <c r="B24" s="103"/>
     </row>
     <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="57" t="s">
@@ -9370,10 +9393,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="103" t="s">
         <v>353</v>
       </c>
-      <c r="B28" s="107"/>
+      <c r="B28" s="103"/>
     </row>
     <row r="29" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="72" t="s">
@@ -9400,10 +9423,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="100" t="s">
         <v>363</v>
       </c>
-      <c r="B32" s="105"/>
+      <c r="B32" s="100"/>
     </row>
     <row r="33" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="72" t="s">
@@ -9426,14 +9449,14 @@
         <v>381</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="107" t="s">
+      <c r="A36" s="103" t="s">
         <v>360</v>
       </c>
-      <c r="B36" s="107"/>
+      <c r="B36" s="103"/>
     </row>
     <row r="37" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="72" t="s">
@@ -9460,17 +9483,17 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="105" t="s">
+      <c r="A40" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="B40" s="105"/>
+      <c r="B40" s="100"/>
     </row>
     <row r="41" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A41" s="57" t="s">
         <v>378</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
@@ -9482,10 +9505,10 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="107" t="s">
-        <v>515</v>
-      </c>
-      <c r="B43" s="105"/>
+      <c r="A43" s="103" t="s">
+        <v>514</v>
+      </c>
+      <c r="B43" s="100"/>
     </row>
     <row r="44" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
@@ -9497,34 +9520,34 @@
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
+        <v>515</v>
+      </c>
+      <c r="B45" s="74" t="s">
         <v>516</v>
-      </c>
-      <c r="B45" s="74" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
+        <v>517</v>
+      </c>
+      <c r="B46" s="74" t="s">
         <v>518</v>
       </c>
-      <c r="B46" s="74" t="s">
-        <v>519</v>
-      </c>
     </row>
     <row r="47" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="B47" s="96"/>
+      <c r="B47" s="101"/>
     </row>
     <row r="48" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A48" s="94" t="s">
+      <c r="A48" s="105" t="s">
         <v>312</v>
       </c>
-      <c r="B48" s="95"/>
+      <c r="B48" s="99"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="102" t="s">
+      <c r="A49" s="109" t="s">
         <v>322</v>
       </c>
       <c r="B49" s="62" t="s">
@@ -9532,7 +9555,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="103"/>
+      <c r="A50" s="110"/>
       <c r="B50" s="62" t="s">
         <v>314</v>
       </c>
@@ -9541,13 +9564,13 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="104"/>
+      <c r="A51" s="111"/>
       <c r="B51" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="109" t="s">
         <v>323</v>
       </c>
       <c r="B52" s="62" t="s">
@@ -9555,25 +9578,25 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="103"/>
+      <c r="A53" s="110"/>
       <c r="B53" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="103"/>
+      <c r="A54" s="110"/>
       <c r="B54" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="104"/>
+      <c r="A55" s="111"/>
       <c r="B55" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="102" t="s">
+      <c r="A56" s="109" t="s">
         <v>324</v>
       </c>
       <c r="B56" s="62" t="s">
@@ -9581,13 +9604,13 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="104"/>
+      <c r="A57" s="111"/>
       <c r="B57" s="62" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="102" t="s">
+      <c r="A58" s="109" t="s">
         <v>325</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -9598,23 +9621,23 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="103"/>
+      <c r="A59" s="110"/>
       <c r="B59" s="62" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C59" s="68" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="103"/>
+      <c r="A60" s="110"/>
       <c r="B60" s="62" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C60" s="68"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="104"/>
+      <c r="A61" s="111"/>
       <c r="B61" s="62" t="s">
         <v>327</v>
       </c>
@@ -9632,15 +9655,15 @@
         <v>285</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="57" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -9652,7 +9675,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="99" t="s">
+      <c r="A66" s="106" t="s">
         <v>290</v>
       </c>
       <c r="B66" s="62" t="s">
@@ -9660,37 +9683,37 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="100"/>
+      <c r="A67" s="107"/>
       <c r="B67" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="100"/>
+      <c r="A68" s="107"/>
       <c r="B68" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="100"/>
+      <c r="A69" s="107"/>
       <c r="B69" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="100"/>
+      <c r="A70" s="107"/>
       <c r="B70" s="62" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="101"/>
+      <c r="A71" s="108"/>
       <c r="B71" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="99" t="s">
+      <c r="A72" s="106" t="s">
         <v>291</v>
       </c>
       <c r="B72" s="62" t="s">
@@ -9698,62 +9721,62 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="100"/>
+      <c r="A73" s="107"/>
       <c r="B73" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C73" s="67"/>
     </row>
     <row r="74" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="100"/>
+      <c r="A74" s="107"/>
       <c r="B74" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="100"/>
+      <c r="A75" s="107"/>
       <c r="B75" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="100"/>
+      <c r="A76" s="107"/>
       <c r="B76" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="100"/>
+      <c r="A77" s="107"/>
       <c r="B77" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="100"/>
+      <c r="A78" s="107"/>
       <c r="B78" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="100"/>
+      <c r="A79" s="107"/>
       <c r="B79" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="100"/>
+      <c r="A80" s="107"/>
       <c r="B80" s="81" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="101"/>
+      <c r="A81" s="108"/>
       <c r="B81" s="81" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="99" t="s">
+      <c r="A82" s="106" t="s">
         <v>292</v>
       </c>
       <c r="B82" s="82" t="s">
@@ -9761,28 +9784,28 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="100"/>
+      <c r="A83" s="107"/>
       <c r="B83" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C83"/>
     </row>
     <row r="84" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="100"/>
+      <c r="A84" s="107"/>
       <c r="B84" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C84"/>
     </row>
     <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="101"/>
+      <c r="A85" s="108"/>
       <c r="B85" s="82" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C85"/>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="99" t="s">
+      <c r="A86" s="106" t="s">
         <v>309</v>
       </c>
       <c r="B86" s="84" t="s">
@@ -9791,7 +9814,7 @@
       <c r="C86"/>
     </row>
     <row r="87" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A87" s="101"/>
+      <c r="A87" s="108"/>
       <c r="B87" s="84" t="s">
         <v>311</v>
       </c>
@@ -9829,16 +9852,16 @@
         <v>375</v>
       </c>
       <c r="B91" s="84" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A92" s="91" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B92" s="81" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C92"/>
     </row>
@@ -9852,17 +9875,17 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="96" t="s">
+      <c r="A94" s="101" t="s">
         <v>390</v>
       </c>
-      <c r="B94" s="96"/>
+      <c r="B94" s="101"/>
       <c r="C94"/>
     </row>
     <row r="95" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A95" s="94" t="s">
+      <c r="A95" s="105" t="s">
         <v>391</v>
       </c>
-      <c r="B95" s="95"/>
+      <c r="B95" s="99"/>
       <c r="C95"/>
     </row>
     <row r="96" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -9893,10 +9916,10 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A99" s="94" t="s">
+      <c r="A99" s="105" t="s">
         <v>398</v>
       </c>
-      <c r="B99" s="95"/>
+      <c r="B99" s="99"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -10036,18 +10059,18 @@
     </row>
     <row r="115" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="93" t="s">
+        <v>539</v>
+      </c>
+      <c r="B115" s="92" t="s">
         <v>540</v>
       </c>
-      <c r="B115" s="92" t="s">
-        <v>541</v>
-      </c>
       <c r="C115"/>
     </row>
     <row r="116" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A116" s="94" t="s">
+      <c r="A116" s="105" t="s">
         <v>429</v>
       </c>
-      <c r="B116" s="95"/>
+      <c r="B116" s="99"/>
       <c r="C116"/>
     </row>
     <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -10132,10 +10155,10 @@
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A126" s="94" t="s">
-        <v>502</v>
-      </c>
-      <c r="B126" s="95"/>
+      <c r="A126" s="105" t="s">
+        <v>501</v>
+      </c>
+      <c r="B126" s="99"/>
       <c r="C126"/>
     </row>
     <row r="127" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -10143,7 +10166,7 @@
         <v>448</v>
       </c>
       <c r="B127" s="80" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C127"/>
     </row>
@@ -10205,30 +10228,34 @@
       <c r="A134" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="B134" s="79"/>
+      <c r="B134" s="80" t="s">
+        <v>555</v>
+      </c>
       <c r="C134"/>
     </row>
-    <row r="135" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A135" s="78" t="s">
         <v>462</v>
       </c>
-      <c r="B135" s="79"/>
+      <c r="B135" s="80" t="s">
+        <v>554</v>
+      </c>
       <c r="C135"/>
     </row>
-    <row r="136" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A136" s="78" t="s">
         <v>463</v>
       </c>
       <c r="B136" s="80" t="s">
-        <v>474</v>
+        <v>553</v>
       </c>
       <c r="C136"/>
     </row>
     <row r="137" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A137" s="97" t="s">
+      <c r="A137" s="98" t="s">
         <v>464</v>
       </c>
-      <c r="B137" s="95"/>
+      <c r="B137" s="99"/>
       <c r="C137"/>
     </row>
     <row r="138" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -10259,10 +10286,10 @@
       <c r="C140"/>
     </row>
     <row r="141" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A141" s="97" t="s">
+      <c r="A141" s="98" t="s">
         <v>472</v>
       </c>
-      <c r="B141" s="95"/>
+      <c r="B141" s="99"/>
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -10275,73 +10302,73 @@
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A143" s="114" t="s">
+      <c r="A143" s="95" t="s">
+        <v>543</v>
+      </c>
+      <c r="B143" s="94" t="s">
         <v>544</v>
       </c>
-      <c r="B143" s="113" t="s">
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A144" s="98" t="s">
         <v>545</v>
       </c>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A144" s="97" t="s">
-        <v>546</v>
-      </c>
-      <c r="B144" s="95"/>
+      <c r="B144" s="99"/>
       <c r="C144"/>
     </row>
     <row r="145" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A145" s="57" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B145" s="80" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" s="57" t="s">
+        <v>547</v>
+      </c>
+      <c r="B146" s="76" t="s">
         <v>548</v>
-      </c>
-      <c r="B146" s="76" t="s">
-        <v>549</v>
       </c>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A147" s="57"/>
-      <c r="B147" s="115"/>
+      <c r="B147" s="96"/>
       <c r="C147"/>
     </row>
     <row r="148" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="96" t="s">
-        <v>475</v>
-      </c>
-      <c r="B148" s="96"/>
+      <c r="A148" s="101" t="s">
+        <v>474</v>
+      </c>
+      <c r="B148" s="101"/>
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A149" s="94" t="s">
-        <v>478</v>
-      </c>
-      <c r="B149" s="95"/>
+      <c r="A149" s="105" t="s">
+        <v>477</v>
+      </c>
+      <c r="B149" s="99"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A150" s="57" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B150" s="76" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
       <c r="A151" s="57" t="s">
+        <v>533</v>
+      </c>
+      <c r="B151" s="80" t="s">
         <v>534</v>
-      </c>
-      <c r="B151" s="80" t="s">
-        <v>535</v>
       </c>
       <c r="C151"/>
     </row>
@@ -10360,122 +10387,122 @@
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A155" s="97" t="s">
-        <v>481</v>
-      </c>
-      <c r="B155" s="98"/>
+      <c r="A155" s="98" t="s">
+        <v>480</v>
+      </c>
+      <c r="B155" s="112"/>
       <c r="C155"/>
     </row>
     <row r="156" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="57" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B156" s="76" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C156"/>
     </row>
     <row r="157" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A157" s="57" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B157" s="76" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A158" s="57" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B158" s="76" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" s="57" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B159" s="76" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="B160" s="76" t="s">
         <v>487</v>
-      </c>
-      <c r="B160" s="76" t="s">
-        <v>488</v>
       </c>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A161" s="57" t="s">
+        <v>488</v>
+      </c>
+      <c r="B161" s="76" t="s">
         <v>489</v>
-      </c>
-      <c r="B161" s="76" t="s">
-        <v>490</v>
       </c>
       <c r="C161"/>
     </row>
     <row r="162" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A162" s="57" t="s">
+        <v>498</v>
+      </c>
+      <c r="B162" s="88" t="s">
         <v>499</v>
       </c>
-      <c r="B162" s="88" t="s">
-        <v>500</v>
-      </c>
       <c r="C162"/>
     </row>
     <row r="163" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A163" s="94" t="s">
-        <v>476</v>
-      </c>
-      <c r="B163" s="95"/>
+      <c r="A163" s="105" t="s">
+        <v>475</v>
+      </c>
+      <c r="B163" s="99"/>
       <c r="C163"/>
     </row>
     <row r="164" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="57" t="s">
+        <v>490</v>
+      </c>
+      <c r="B164" s="76" t="s">
         <v>491</v>
-      </c>
-      <c r="B164" s="76" t="s">
-        <v>492</v>
       </c>
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A165" s="57" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B165" s="76" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A166" s="94" t="s">
-        <v>477</v>
-      </c>
-      <c r="B166" s="95"/>
+      <c r="A166" s="105" t="s">
+        <v>476</v>
+      </c>
+      <c r="B166" s="99"/>
       <c r="C166"/>
     </row>
     <row r="167" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A167" s="57" t="s">
+        <v>494</v>
+      </c>
+      <c r="B167" s="76" t="s">
         <v>495</v>
-      </c>
-      <c r="B167" s="76" t="s">
-        <v>496</v>
       </c>
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A168" s="57" t="s">
+        <v>496</v>
+      </c>
+      <c r="B168" s="76" t="s">
         <v>497</v>
-      </c>
-      <c r="B168" s="76" t="s">
-        <v>498</v>
       </c>
       <c r="C168"/>
     </row>
@@ -10486,6 +10513,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A72:A81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A61"/>
     <mergeCell ref="A144:B144"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A47:B47"/>
@@ -10502,26 +10549,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A72:A81"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A66:A71"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A163:B163"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10943,7 +10970,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="113" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -10963,7 +10990,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="110"/>
+      <c r="A2" s="114"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -11031,10 +11058,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="115" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="112"/>
+      <c r="C6" s="116"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - EXERCISE 28.09.2019
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" activeTab="1"/>
@@ -30,7 +30,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="602">
   <si>
     <t>Операция</t>
   </si>
@@ -5737,11 +5737,62 @@
 ADD CONSTRAINT PK_User PRIMARY KEY (Id,Username);</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">SELECT name FROM (SELECT name FROM agentinformation) a  </t>
+  </si>
+  <si>
+    <t>SELECT FROM SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SELECT DepositAmount - LEAD(DepositAmount) OVER (ORDER BY ID ) AS Diff
+   FROM   WizzardDeposits</t>
+  </si>
+  <si>
+    <t>SELECT wd.DepositAmount ,
+  (SELECT wd.DepositAmount - w.DepositAmount FROM WizzardDeposits AS w WHERE w.Id = wd.Id+1) AS [Difference] 
+ FROM WizzardDeposits AS wd</t>
+  </si>
+  <si>
+    <t>SEELCT NEXT ROW DATA</t>
+  </si>
+  <si>
+    <t>CREATE TABLE PTable (
+     Key1 varchar(20) not null,
+     Key2 date not null,
+     CONSTRAINT PK_PTable PRIMARY KEY (Key1,Key2)
+)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>КОМПОЗИТЕН КЛЮЧ ПРИ СЪЗДАВАНЕ НА ТАБЛИЦАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+COPOSITE KEY ON CREATE</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6491,7 +6542,7 @@
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6748,15 +6799,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6772,29 +6814,20 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6814,8 +6847,17 @@
     <xf numFmtId="0" fontId="36" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6828,6 +6870,9 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -6922,7 +6967,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -6930,6 +6975,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -6983,7 +7039,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7018,7 +7074,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9548,10 +9604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9570,16 +9626,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="101" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="107"/>
+      <c r="B2" s="111"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="113" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="108"/>
+      <c r="B3" s="112"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -9606,10 +9662,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="112" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="106"/>
+      <c r="B7" s="110"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -9623,7 +9679,7 @@
       <c r="A9" s="72" t="s">
         <v>523</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="94" t="s">
         <v>524</v>
       </c>
     </row>
@@ -9636,10 +9692,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="112" t="s">
         <v>520</v>
       </c>
-      <c r="B11" s="106"/>
+      <c r="B11" s="110"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -9650,10 +9706,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="112" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="108"/>
+      <c r="B13" s="112"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -9703,1373 +9759,1387 @@
         <v>501</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="108" t="s">
+    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="72" t="s">
+        <v>596</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="112" t="s">
         <v>502</v>
       </c>
-      <c r="B20" s="108"/>
-    </row>
-    <row r="21" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="70" t="s">
+      <c r="B21" s="112"/>
+    </row>
+    <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="70" t="s">
         <v>339</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B22" s="74" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="108" t="s">
+    <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="112" t="s">
         <v>386</v>
       </c>
-      <c r="B22" s="108"/>
-    </row>
-    <row r="23" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A23" s="70" t="s">
+      <c r="B23" s="112"/>
+    </row>
+    <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="70" t="s">
         <v>340</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B24" s="74" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="108" t="s">
+    <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="112" t="s">
         <v>351</v>
       </c>
-      <c r="B24" s="108"/>
-    </row>
-    <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="B25" s="112"/>
+    </row>
+    <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="57" t="s">
         <v>345</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B26" s="81" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+    <row r="27" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B27" s="81" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+    <row r="28" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B28" s="81" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="108" t="s">
+    <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="112" t="s">
         <v>351</v>
       </c>
-      <c r="B28" s="108"/>
-    </row>
-    <row r="29" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="72" t="s">
+      <c r="B29" s="112"/>
+    </row>
+    <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="B29" s="74" t="s">
+      <c r="B30" s="74" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+    <row r="31" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="57" t="s">
         <v>364</v>
       </c>
-      <c r="B30" s="74" t="s">
+      <c r="B31" s="74" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+    <row r="32" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B32" s="74" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="106" t="s">
+    <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="110" t="s">
         <v>361</v>
       </c>
-      <c r="B32" s="106"/>
-    </row>
-    <row r="33" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="72" t="s">
-        <v>368</v>
-      </c>
-      <c r="B33" s="74" t="s">
-        <v>356</v>
-      </c>
+      <c r="B33" s="110"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
+        <v>368</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="72" t="s">
         <v>355</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B35" s="74" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+    <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="B35" s="74" t="s">
+      <c r="B36" s="74" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="108" t="s">
+    <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="112" t="s">
         <v>358</v>
       </c>
-      <c r="B36" s="108"/>
-    </row>
-    <row r="37" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="72" t="s">
-        <v>370</v>
-      </c>
-      <c r="B37" s="74" t="s">
-        <v>359</v>
-      </c>
+      <c r="B37" s="112"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
+        <v>370</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="72" t="s">
         <v>369</v>
       </c>
-      <c r="B38" s="74" t="s">
+      <c r="B39" s="74" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
+    <row r="40" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="57" t="s">
         <v>380</v>
       </c>
-      <c r="B39" s="74" t="s">
+      <c r="B40" s="74" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="106" t="s">
+    <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="110" t="s">
         <v>362</v>
       </c>
-      <c r="B40" s="106"/>
-    </row>
-    <row r="41" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
+      <c r="B41" s="110"/>
+    </row>
+    <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="B41" s="74" t="s">
+      <c r="B42" s="74" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="57" t="s">
+    <row r="43" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="B42" s="74" t="s">
+      <c r="B43" s="74" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="108" t="s">
+    <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="112" t="s">
         <v>512</v>
       </c>
-      <c r="B43" s="106"/>
-    </row>
-    <row r="44" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="57" t="s">
+      <c r="B44" s="110"/>
+    </row>
+    <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="B44" s="74" t="s">
+      <c r="B45" s="74" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="s">
-        <v>513</v>
-      </c>
-      <c r="B45" s="74" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
+        <v>513</v>
+      </c>
+      <c r="B46" s="74" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="57" t="s">
         <v>515</v>
       </c>
-      <c r="B46" s="74" t="s">
+      <c r="B47" s="74" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="102" t="s">
+    <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="101" t="s">
         <v>372</v>
       </c>
-      <c r="B47" s="102"/>
-    </row>
-    <row r="48" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A48" s="103" t="s">
+      <c r="B48" s="101"/>
+    </row>
+    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A49" s="99" t="s">
         <v>312</v>
       </c>
-      <c r="B48" s="104"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="113" t="s">
+      <c r="B49" s="100"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="107" t="s">
         <v>321</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B50" s="62" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="114"/>
-      <c r="B50" s="62" t="s">
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="108"/>
+      <c r="B51" s="62" t="s">
         <v>593</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C51" s="66" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="115"/>
-      <c r="B51" s="62" t="s">
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="109"/>
+      <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="113" t="s">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="107" t="s">
         <v>322</v>
       </c>
-      <c r="B52" s="62" t="s">
+      <c r="B53" s="62" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="114"/>
-      <c r="B53" s="62" t="s">
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="108"/>
+      <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="114"/>
-      <c r="B54" s="62" t="s">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="108"/>
+      <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="115"/>
-      <c r="B55" s="62" t="s">
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="109"/>
+      <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="113" t="s">
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="107" t="s">
         <v>323</v>
       </c>
-      <c r="B56" s="62" t="s">
+      <c r="B57" s="62" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="115"/>
-      <c r="B57" s="62" t="s">
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="109"/>
+      <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="113" t="s">
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="107" t="s">
         <v>324</v>
       </c>
-      <c r="B58" s="62" t="s">
+      <c r="B59" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="C58" s="66" t="s">
+      <c r="C59" s="66" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="114"/>
-      <c r="B59" s="62" t="s">
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="108"/>
+      <c r="B60" s="62" t="s">
         <v>528</v>
       </c>
-      <c r="C59" s="68" t="s">
+      <c r="C60" s="68" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="114"/>
-      <c r="B60" s="62" t="s">
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="108"/>
+      <c r="B61" s="62" t="s">
         <v>590</v>
       </c>
-      <c r="C60" s="68"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="115"/>
-      <c r="B61" s="62" t="s">
+      <c r="C61" s="68"/>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="109"/>
+      <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="63" t="s">
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="63" t="s">
         <v>284</v>
       </c>
-      <c r="B62" s="62" t="s">
+      <c r="B63" s="62" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="57" t="s">
+    <row r="64" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="57" t="s">
         <v>285</v>
       </c>
-      <c r="B63" s="62" t="s">
+      <c r="B64" s="62" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="57" t="s">
+    <row r="65" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="57" t="s">
+        <v>601</v>
+      </c>
+      <c r="B65" s="62" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="57" t="s">
         <v>549</v>
       </c>
-      <c r="B64" s="62" t="s">
+      <c r="B66" s="62" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="57" t="s">
+    <row r="67" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="57" t="s">
         <v>286</v>
       </c>
-      <c r="B65" s="62" t="s">
+      <c r="B67" s="62" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="110" t="s">
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="104" t="s">
         <v>290</v>
       </c>
-      <c r="B66" s="62" t="s">
+      <c r="B68" s="62" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="111"/>
-      <c r="B67" s="62" t="s">
+    <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="105"/>
+      <c r="B69" s="62" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="111"/>
-      <c r="B68" s="62" t="s">
+    <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="105"/>
+      <c r="B70" s="62" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="111"/>
-      <c r="B69" s="62" t="s">
+    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="105"/>
+      <c r="B71" s="62" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="111"/>
-      <c r="B70" s="62" t="s">
+    <row r="72" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="105"/>
+      <c r="B72" s="62" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="112"/>
-      <c r="B71" s="62" t="s">
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="106"/>
+      <c r="B73" s="62" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="110" t="s">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="104" t="s">
         <v>291</v>
       </c>
-      <c r="B72" s="62" t="s">
+      <c r="B74" s="62" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="111"/>
-      <c r="B73" s="62" t="s">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="105"/>
+      <c r="B75" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="C73" s="67"/>
-    </row>
-    <row r="74" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
-      <c r="B74" s="62" t="s">
+      <c r="C75" s="67"/>
+    </row>
+    <row r="76" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="105"/>
+      <c r="B76" s="62" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="111"/>
-      <c r="B75" s="62" t="s">
+    <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="105"/>
+      <c r="B77" s="62" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="111"/>
-      <c r="B76" s="81" t="s">
+    <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="105"/>
+      <c r="B78" s="81" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="111"/>
-      <c r="B77" s="81" t="s">
+    <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="105"/>
+      <c r="B79" s="81" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="111"/>
-      <c r="B78" s="81" t="s">
+    <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="105"/>
+      <c r="B80" s="81" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="111"/>
-      <c r="B79" s="81" t="s">
+    <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="105"/>
+      <c r="B81" s="81" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A80" s="111"/>
-      <c r="B80" s="81" t="s">
+    <row r="82" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A82" s="105"/>
+      <c r="B82" s="81" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="111"/>
-      <c r="B81" s="81" t="s">
+    <row r="83" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="105"/>
+      <c r="B83" s="81" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="111"/>
-      <c r="B82" s="81" t="s">
+    <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="105"/>
+      <c r="B84" s="81" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="112"/>
-      <c r="B83" s="81" t="s">
+    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="106"/>
+      <c r="B85" s="81" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="110" t="s">
+    <row r="86" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="104" t="s">
         <v>292</v>
       </c>
-      <c r="B84" s="82" t="s">
+      <c r="B86" s="82" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="111"/>
-      <c r="B85" s="83" t="s">
+    <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="105"/>
+      <c r="B87" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="111"/>
-      <c r="B86" s="83" t="s">
+      <c r="C87"/>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="105"/>
+      <c r="B88" s="83" t="s">
         <v>308</v>
       </c>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="112"/>
-      <c r="B87" s="82" t="s">
+      <c r="C88"/>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="106"/>
+      <c r="B89" s="82" t="s">
         <v>547</v>
       </c>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="110" t="s">
+      <c r="C89"/>
+    </row>
+    <row r="90" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="104" t="s">
         <v>309</v>
       </c>
-      <c r="B88" s="84" t="s">
+      <c r="B90" s="84" t="s">
         <v>310</v>
       </c>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A89" s="112"/>
-      <c r="B89" s="84" t="s">
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A91" s="106"/>
+      <c r="B91" s="84" t="s">
         <v>311</v>
       </c>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A90" s="69" t="s">
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="69" t="s">
         <v>335</v>
       </c>
-      <c r="B90" s="83" t="s">
+      <c r="B92" s="83" t="s">
         <v>336</v>
       </c>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="65" t="s">
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="B91" s="84" t="s">
+      <c r="B93" s="84" t="s">
         <v>333</v>
       </c>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A92" s="61" t="s">
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A94" s="61" t="s">
         <v>385</v>
       </c>
-      <c r="B92" s="85" t="s">
+      <c r="B94" s="85" t="s">
         <v>328</v>
       </c>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="71" t="s">
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="71" t="s">
         <v>373</v>
       </c>
-      <c r="B93" s="84" t="s">
+      <c r="B95" s="84" t="s">
         <v>533</v>
       </c>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="91" t="s">
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="91" t="s">
         <v>529</v>
       </c>
-      <c r="B94" s="81" t="s">
+      <c r="B96" s="81" t="s">
         <v>532</v>
       </c>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="73" t="s">
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="73" t="s">
         <v>375</v>
       </c>
-      <c r="B95" s="81" t="s">
+      <c r="B97" s="81" t="s">
         <v>374</v>
       </c>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="102" t="s">
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="101" t="s">
         <v>388</v>
       </c>
-      <c r="B96" s="102"/>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A97" s="103" t="s">
+      <c r="B98" s="101"/>
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A99" s="99" t="s">
         <v>389</v>
       </c>
-      <c r="B97" s="104"/>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="70" t="s">
+      <c r="B99" s="100"/>
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="70" t="s">
         <v>390</v>
       </c>
-      <c r="B98" s="60" t="s">
+      <c r="B100" s="60" t="s">
         <v>391</v>
       </c>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="70" t="s">
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="70" t="s">
         <v>392</v>
       </c>
-      <c r="B99" s="76" t="s">
+      <c r="B101" s="76" t="s">
         <v>393</v>
       </c>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="70" t="s">
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="70" t="s">
         <v>394</v>
       </c>
-      <c r="B100" s="76" t="s">
+      <c r="B102" s="76" t="s">
         <v>395</v>
       </c>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A101" s="103" t="s">
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A103" s="99" t="s">
         <v>396</v>
       </c>
-      <c r="B101" s="104"/>
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A102" s="57" t="s">
+      <c r="B103" s="100"/>
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A104" s="57" t="s">
         <v>398</v>
       </c>
-      <c r="B102" s="80" t="s">
+      <c r="B104" s="80" t="s">
         <v>397</v>
       </c>
-      <c r="C102"/>
-    </row>
-    <row r="103" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="57" t="s">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="57" t="s">
         <v>399</v>
       </c>
-      <c r="B103" s="80" t="s">
+      <c r="B105" s="80" t="s">
         <v>400</v>
       </c>
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A104" s="72" t="s">
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A106" s="72" t="s">
         <v>401</v>
       </c>
-      <c r="B104" s="80" t="s">
+      <c r="B106" s="80" t="s">
         <v>402</v>
       </c>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A105" s="57" t="s">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A107" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="B105" s="80" t="s">
+      <c r="B107" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="57" t="s">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="B106" s="80" t="s">
+      <c r="B108" s="80" t="s">
         <v>406</v>
       </c>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="57" t="s">
+      <c r="C108"/>
+    </row>
+    <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="B107" s="79" t="s">
+      <c r="B109" s="79" t="s">
         <v>408</v>
       </c>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="57" t="s">
+      <c r="C109"/>
+    </row>
+    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A110" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="B108" s="79" t="s">
+      <c r="B110" s="79" t="s">
         <v>410</v>
       </c>
-      <c r="C108"/>
-    </row>
-    <row r="109" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A109" s="57" t="s">
+      <c r="C110"/>
+    </row>
+    <row r="111" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A111" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="B109" s="86" t="s">
+      <c r="B111" s="86" t="s">
         <v>412</v>
       </c>
-      <c r="C109"/>
-    </row>
-    <row r="110" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="57" t="s">
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="57" t="s">
         <v>421</v>
       </c>
-      <c r="B110" s="80" t="s">
+      <c r="B112" s="80" t="s">
         <v>413</v>
-      </c>
-      <c r="C110"/>
-    </row>
-    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
-        <v>420</v>
-      </c>
-      <c r="B111" s="79" t="s">
-        <v>414</v>
-      </c>
-      <c r="C111"/>
-    </row>
-    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="B112" s="79" t="s">
-        <v>415</v>
       </c>
       <c r="C112"/>
     </row>
     <row r="113" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B113" s="79" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C113"/>
     </row>
     <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
+        <v>419</v>
+      </c>
+      <c r="B114" s="79" t="s">
+        <v>415</v>
+      </c>
+      <c r="C114"/>
+    </row>
+    <row r="115" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="57" t="s">
+        <v>416</v>
+      </c>
+      <c r="B115" s="79" t="s">
+        <v>417</v>
+      </c>
+      <c r="C115"/>
+    </row>
+    <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="57" t="s">
         <v>418</v>
       </c>
-      <c r="B114" s="79" t="s">
+      <c r="B116" s="79" t="s">
         <v>422</v>
       </c>
-      <c r="C114"/>
-    </row>
-    <row r="115" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
+      <c r="C116"/>
+    </row>
+    <row r="117" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A117" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="B115" s="79" t="s">
+      <c r="B117" s="79" t="s">
         <v>424</v>
       </c>
-      <c r="C115"/>
-    </row>
-    <row r="116" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="72" t="s">
+      <c r="C117"/>
+    </row>
+    <row r="118" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="72" t="s">
         <v>425</v>
       </c>
-      <c r="B116" s="80" t="s">
+      <c r="B118" s="80" t="s">
         <v>426</v>
       </c>
-      <c r="C116"/>
-    </row>
-    <row r="117" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="93" t="s">
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="93" t="s">
         <v>536</v>
       </c>
-      <c r="B117" s="92" t="s">
+      <c r="B119" s="92" t="s">
         <v>537</v>
       </c>
-      <c r="C117"/>
-    </row>
-    <row r="118" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A118" s="103" t="s">
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A120" s="99" t="s">
         <v>427</v>
       </c>
-      <c r="B118" s="104"/>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
-        <v>432</v>
-      </c>
-      <c r="B119" s="79" t="s">
-        <v>431</v>
-      </c>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
-        <v>433</v>
-      </c>
-      <c r="B120" s="79" t="s">
-        <v>430</v>
-      </c>
+      <c r="B120" s="100"/>
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B121" s="79" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
+        <v>433</v>
+      </c>
+      <c r="B122" s="79" t="s">
+        <v>430</v>
+      </c>
+      <c r="C122"/>
+    </row>
+    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="57" t="s">
+        <v>434</v>
+      </c>
+      <c r="B123" s="79" t="s">
+        <v>429</v>
+      </c>
+      <c r="C123"/>
+    </row>
+    <row r="124" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="B122" s="79" t="s">
+      <c r="B124" s="79" t="s">
         <v>428</v>
       </c>
-      <c r="C122"/>
-    </row>
-    <row r="123" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="70" t="s">
+      <c r="C124"/>
+    </row>
+    <row r="125" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="70" t="s">
         <v>439</v>
       </c>
-      <c r="B123" s="79" t="s">
+      <c r="B125" s="79" t="s">
         <v>436</v>
       </c>
-      <c r="C123"/>
-    </row>
-    <row r="124" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
+      <c r="C125"/>
+    </row>
+    <row r="126" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A126" s="57" t="s">
         <v>438</v>
       </c>
-      <c r="B124" s="79" t="s">
+      <c r="B126" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="C124"/>
-    </row>
-    <row r="125" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="70" t="s">
+      <c r="C126"/>
+    </row>
+    <row r="127" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" s="70" t="s">
         <v>440</v>
       </c>
-      <c r="B125" s="80" t="s">
+      <c r="B127" s="80" t="s">
         <v>441</v>
       </c>
-      <c r="C125"/>
-    </row>
-    <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="57" t="s">
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="57" t="s">
         <v>442</v>
       </c>
-      <c r="B126" s="79" t="s">
+      <c r="B128" s="79" t="s">
         <v>443</v>
       </c>
-      <c r="C126"/>
-    </row>
-    <row r="127" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A127" s="57" t="s">
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A129" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="B127" s="80" t="s">
+      <c r="B129" s="80" t="s">
         <v>445</v>
       </c>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A128" s="103" t="s">
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A130" s="99" t="s">
         <v>499</v>
       </c>
-      <c r="B128" s="104"/>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A129" s="57" t="s">
+      <c r="B130" s="100"/>
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A131" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="B129" s="80" t="s">
+      <c r="B131" s="80" t="s">
         <v>498</v>
       </c>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A130" s="57" t="s">
+      <c r="C131"/>
+    </row>
+    <row r="132" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A132" s="57" t="s">
         <v>447</v>
       </c>
-      <c r="B130" s="80" t="s">
+      <c r="B132" s="80" t="s">
         <v>448</v>
       </c>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
+      <c r="C132"/>
+    </row>
+    <row r="133" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="57" t="s">
         <v>449</v>
       </c>
-      <c r="B131" s="79" t="s">
+      <c r="B133" s="79" t="s">
         <v>450</v>
       </c>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="57" t="s">
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="57" t="s">
         <v>451</v>
       </c>
-      <c r="B132" s="79" t="s">
+      <c r="B134" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="C132"/>
-    </row>
-    <row r="133" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="70" t="s">
+      <c r="C134"/>
+    </row>
+    <row r="135" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A135" s="70" t="s">
         <v>453</v>
       </c>
-      <c r="B133" s="79" t="s">
+      <c r="B135" s="79" t="s">
         <v>454</v>
       </c>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
-      <c r="A134" s="77" t="s">
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
+      <c r="A136" s="77" t="s">
         <v>456</v>
       </c>
-      <c r="B134" s="80" t="s">
+      <c r="B136" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:3" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="A135" s="78" t="s">
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="1:3" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="A137" s="78" t="s">
         <v>457</v>
       </c>
-      <c r="B135" s="101" t="s">
+      <c r="B137" s="98" t="s">
         <v>458</v>
       </c>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A136" s="78" t="s">
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A138" s="78" t="s">
         <v>459</v>
       </c>
-      <c r="B136" s="101" t="s">
+      <c r="B138" s="98" t="s">
         <v>552</v>
       </c>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
-      <c r="A137" s="78" t="s">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
+      <c r="A139" s="78" t="s">
         <v>460</v>
       </c>
-      <c r="B137" s="101" t="s">
+      <c r="B139" s="98" t="s">
         <v>551</v>
       </c>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
-      <c r="A138" s="78" t="s">
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
+      <c r="A140" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="B138" s="101" t="s">
+      <c r="B140" s="98" t="s">
         <v>550</v>
       </c>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A139" s="105" t="s">
+      <c r="C140"/>
+    </row>
+    <row r="141" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A141" s="102" t="s">
         <v>462</v>
       </c>
-      <c r="B139" s="104"/>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A140" s="78" t="s">
+      <c r="B141" s="100"/>
+      <c r="C141"/>
+    </row>
+    <row r="142" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A142" s="78" t="s">
         <v>464</v>
       </c>
-      <c r="B140" s="80" t="s">
+      <c r="B142" s="80" t="s">
         <v>463</v>
       </c>
-      <c r="C140"/>
-    </row>
-    <row r="141" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A141" s="70" t="s">
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A143" s="70" t="s">
         <v>465</v>
       </c>
-      <c r="B141" s="86" t="s">
+      <c r="B143" s="86" t="s">
         <v>468</v>
       </c>
-      <c r="C141"/>
-    </row>
-    <row r="142" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A142" s="78" t="s">
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A144" s="78" t="s">
         <v>466</v>
       </c>
-      <c r="B142" s="80" t="s">
+      <c r="B144" s="80" t="s">
         <v>467</v>
       </c>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="105" t="s">
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A145" s="102" t="s">
         <v>470</v>
       </c>
-      <c r="B143" s="104"/>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A144" s="70" t="s">
+      <c r="B145" s="100"/>
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A146" s="70" t="s">
         <v>469</v>
       </c>
-      <c r="B144" s="87" t="s">
+      <c r="B146" s="87" t="s">
         <v>471</v>
       </c>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A145" s="95" t="s">
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A147" s="57" t="s">
         <v>540</v>
       </c>
-      <c r="B145" s="94" t="s">
+      <c r="B147" s="87" t="s">
         <v>541</v>
       </c>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="105" t="s">
+      <c r="C147"/>
+    </row>
+    <row r="148" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A148" s="102" t="s">
         <v>542</v>
       </c>
-      <c r="B146" s="104"/>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A147" s="57" t="s">
+      <c r="B148" s="100"/>
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A149" s="57" t="s">
         <v>543</v>
       </c>
-      <c r="B147" s="80" t="s">
+      <c r="B149" s="80" t="s">
         <v>546</v>
       </c>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A148" s="57" t="s">
+      <c r="C149" s="11" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A150" s="57" t="s">
         <v>544</v>
       </c>
-      <c r="B148" s="76" t="s">
+      <c r="B150" s="76" t="s">
         <v>545</v>
       </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="57"/>
-      <c r="B149" s="96"/>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="102" t="s">
+      <c r="C150"/>
+    </row>
+    <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A151" s="57" t="s">
+        <v>599</v>
+      </c>
+      <c r="B151" s="118" t="s">
+        <v>598</v>
+      </c>
+      <c r="C151"/>
+    </row>
+    <row r="152" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A152" s="101" t="s">
         <v>472</v>
       </c>
-      <c r="B150" s="102"/>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A151" s="103" t="s">
+      <c r="B152" s="101"/>
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A153" s="99" t="s">
         <v>475</v>
       </c>
-      <c r="B151" s="104"/>
-      <c r="C151"/>
-    </row>
-    <row r="152" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A152" s="57" t="s">
+      <c r="B153" s="100"/>
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A154" s="57" t="s">
         <v>539</v>
       </c>
-      <c r="B152" s="76" t="s">
+      <c r="B154" s="76" t="s">
         <v>538</v>
       </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A153" s="57" t="s">
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A155" s="57" t="s">
         <v>530</v>
       </c>
-      <c r="B153" s="80" t="s">
+      <c r="B155" s="80" t="s">
         <v>531</v>
       </c>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="57"/>
-      <c r="B154" s="80"/>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="57"/>
-      <c r="B155" s="80"/>
       <c r="C155"/>
     </row>
     <row r="156" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="70"/>
+      <c r="A156" s="57"/>
+      <c r="B156" s="80"/>
       <c r="C156"/>
     </row>
-    <row r="157" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A157" s="105" t="s">
+    <row r="157" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="57"/>
+      <c r="B157" s="80"/>
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A158" s="70"/>
+      <c r="C158"/>
+    </row>
+    <row r="159" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A159" s="102" t="s">
         <v>478</v>
       </c>
-      <c r="B157" s="116"/>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A158" s="57" t="s">
+      <c r="B159" s="103"/>
+      <c r="C159"/>
+    </row>
+    <row r="160" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A160" s="57" t="s">
         <v>477</v>
       </c>
-      <c r="B158" s="76" t="s">
+      <c r="B160" s="76" t="s">
         <v>476</v>
-      </c>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A159" s="57" t="s">
-        <v>483</v>
-      </c>
-      <c r="B159" s="76" t="s">
-        <v>479</v>
-      </c>
-      <c r="C159"/>
-    </row>
-    <row r="160" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A160" s="57" t="s">
-        <v>481</v>
-      </c>
-      <c r="B160" s="76" t="s">
-        <v>480</v>
       </c>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" s="57" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B161" s="76" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C161"/>
     </row>
     <row r="162" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A162" s="57" t="s">
+        <v>481</v>
+      </c>
+      <c r="B162" s="76" t="s">
+        <v>480</v>
+      </c>
+      <c r="C162"/>
+    </row>
+    <row r="163" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A163" s="57" t="s">
+        <v>482</v>
+      </c>
+      <c r="B163" s="76" t="s">
+        <v>476</v>
+      </c>
+      <c r="C163"/>
+    </row>
+    <row r="164" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A164" s="57" t="s">
         <v>484</v>
       </c>
-      <c r="B162" s="76" t="s">
+      <c r="B164" s="76" t="s">
         <v>485</v>
       </c>
-      <c r="C162"/>
-    </row>
-    <row r="163" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A163" s="57" t="s">
+      <c r="C164"/>
+    </row>
+    <row r="165" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A165" s="57" t="s">
         <v>486</v>
       </c>
-      <c r="B163" s="76" t="s">
+      <c r="B165" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="C163"/>
-    </row>
-    <row r="164" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A164" s="57" t="s">
+      <c r="C165"/>
+    </row>
+    <row r="166" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="57" t="s">
         <v>496</v>
       </c>
-      <c r="B164" s="88" t="s">
+      <c r="B166" s="88" t="s">
         <v>497</v>
       </c>
-      <c r="C164"/>
-    </row>
-    <row r="165" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A165" s="103" t="s">
+      <c r="C166"/>
+    </row>
+    <row r="167" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A167" s="99" t="s">
         <v>473</v>
       </c>
-      <c r="B165" s="104"/>
-      <c r="C165"/>
-    </row>
-    <row r="166" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A166" s="57" t="s">
+      <c r="B167" s="100"/>
+      <c r="C167"/>
+    </row>
+    <row r="168" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A168" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="B166" s="76" t="s">
+      <c r="B168" s="76" t="s">
         <v>489</v>
       </c>
-      <c r="C166"/>
-    </row>
-    <row r="167" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A167" s="57" t="s">
+      <c r="C168"/>
+    </row>
+    <row r="169" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A169" s="57" t="s">
         <v>491</v>
       </c>
-      <c r="B167" s="76" t="s">
+      <c r="B169" s="76" t="s">
         <v>490</v>
       </c>
-      <c r="C167"/>
-    </row>
-    <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="103" t="s">
+      <c r="C169"/>
+    </row>
+    <row r="170" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A170" s="99" t="s">
         <v>474</v>
       </c>
-      <c r="B168" s="104"/>
-      <c r="C168"/>
-    </row>
-    <row r="169" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A169" s="57" t="s">
+      <c r="B170" s="100"/>
+      <c r="C170"/>
+    </row>
+    <row r="171" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A171" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="B169" s="76" t="s">
+      <c r="B171" s="76" t="s">
         <v>493</v>
       </c>
-      <c r="C169"/>
-    </row>
-    <row r="170" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A170" s="57" t="s">
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A172" s="57" t="s">
         <v>494</v>
       </c>
-      <c r="B170" s="76" t="s">
+      <c r="B172" s="76" t="s">
         <v>495</v>
       </c>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A171" s="102" t="s">
+      <c r="C172"/>
+    </row>
+    <row r="173" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A173" s="101" t="s">
         <v>553</v>
       </c>
-      <c r="B171" s="102"/>
-      <c r="C171"/>
-    </row>
-    <row r="172" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A172" s="103" t="s">
+      <c r="B173" s="101"/>
+      <c r="C173"/>
+    </row>
+    <row r="174" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A174" s="99" t="s">
         <v>554</v>
       </c>
-      <c r="B172" s="104"/>
-      <c r="C172"/>
-    </row>
-    <row r="173" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A173" s="57" t="s">
+      <c r="B174" s="100"/>
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A175" s="57" t="s">
         <v>556</v>
       </c>
-      <c r="B173" s="76" t="s">
+      <c r="B175" s="76" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A174" s="57"/>
-      <c r="B174" s="76"/>
-    </row>
-    <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="103" t="s">
+    <row r="176" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A176" s="57"/>
+      <c r="B176" s="76"/>
+    </row>
+    <row r="177" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A177" s="99" t="s">
         <v>553</v>
       </c>
-      <c r="B175" s="104"/>
-      <c r="C175"/>
-    </row>
-    <row r="176" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A176" s="57" t="s">
+      <c r="B177" s="100"/>
+      <c r="C177"/>
+    </row>
+    <row r="178" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A178" s="57" t="s">
         <v>558</v>
       </c>
-      <c r="B176" s="76" t="s">
+      <c r="B178" s="76" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A177" s="57" t="s">
+    <row r="179" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A179" s="57" t="s">
         <v>560</v>
       </c>
-      <c r="B177" s="76" t="s">
+      <c r="B179" s="76" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A178" s="57" t="s">
+    <row r="180" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A180" s="57" t="s">
         <v>562</v>
       </c>
-      <c r="B178" s="76" t="s">
+      <c r="B180" s="76" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A179" s="57" t="s">
+    <row r="181" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A181" s="57" t="s">
         <v>565</v>
       </c>
-      <c r="B179" s="76" t="s">
+      <c r="B181" s="76" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="57" t="s">
+    <row r="182" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="57" t="s">
         <v>567</v>
       </c>
-      <c r="B180" s="76" t="s">
+      <c r="B182" s="76" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
-      <c r="A181" s="57" t="s">
+    <row r="183" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
+      <c r="A183" s="57" t="s">
         <v>568</v>
       </c>
-      <c r="B181" s="80" t="s">
+      <c r="B183" s="80" t="s">
         <v>569</v>
       </c>
-      <c r="C181" s="99" t="s">
+      <c r="C183" s="96" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
-      <c r="A182" s="57" t="s">
+    <row r="184" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
+      <c r="A184" s="57" t="s">
         <v>570</v>
       </c>
-      <c r="B182" s="80" t="s">
+      <c r="B184" s="80" t="s">
         <v>571</v>
       </c>
-      <c r="C182" s="99" t="s">
+      <c r="C184" s="96" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A183" s="57" t="s">
+    <row r="185" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A185" s="57" t="s">
         <v>572</v>
       </c>
-      <c r="B183" s="76" t="s">
+      <c r="B185" s="76" t="s">
         <v>573</v>
       </c>
-      <c r="C183" s="98" t="s">
+      <c r="C185" s="95" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="57"/>
-      <c r="B184" s="76"/>
-    </row>
-    <row r="185" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A185" s="103" t="s">
+    <row r="186" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A186" s="57"/>
+      <c r="B186" s="76"/>
+    </row>
+    <row r="187" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A187" s="99" t="s">
         <v>577</v>
       </c>
-      <c r="B185" s="104"/>
-      <c r="C185"/>
-    </row>
-    <row r="186" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A186" s="57" t="s">
+      <c r="B187" s="100"/>
+      <c r="C187"/>
+    </row>
+    <row r="188" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A188" s="57" t="s">
         <v>578</v>
       </c>
-      <c r="B186" s="76" t="s">
+      <c r="B188" s="76" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A187" s="57"/>
-      <c r="B187" s="76" t="s">
+    <row r="189" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A189" s="57"/>
+      <c r="B189" s="76" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A188" s="105" t="s">
+    <row r="190" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A190" s="102" t="s">
         <v>581</v>
       </c>
-      <c r="B188" s="104"/>
-    </row>
-    <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A189" s="57" t="s">
+      <c r="B190" s="100"/>
+    </row>
+    <row r="191" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A191" s="57" t="s">
         <v>582</v>
       </c>
-      <c r="B189" s="76" t="s">
+      <c r="B191" s="76" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A190" s="57" t="s">
+    <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A192" s="57" t="s">
         <v>584</v>
       </c>
-      <c r="B190" s="76" t="s">
+      <c r="B192" s="76" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A191" s="57" t="s">
+    <row r="193" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A193" s="57" t="s">
         <v>588</v>
       </c>
-      <c r="B191" s="100" t="s">
+      <c r="B193" s="97" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A192" s="57" t="s">
+    <row r="194" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A194" s="57" t="s">
         <v>586</v>
       </c>
-      <c r="B192" s="100" t="s">
+      <c r="B194" s="97" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="103" t="s">
+    <row r="195" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A195" s="99" t="s">
         <v>555</v>
       </c>
-      <c r="B193" s="104"/>
-      <c r="C193"/>
-    </row>
-    <row r="194" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="57"/>
-      <c r="B194" s="76"/>
-    </row>
-    <row r="195" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="57"/>
-      <c r="B195" s="76"/>
+      <c r="B195" s="100"/>
+      <c r="C195"/>
     </row>
     <row r="196" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A196" s="57"/>
@@ -11171,50 +11241,58 @@
       <c r="A220" s="57"/>
       <c r="B220" s="76"/>
     </row>
+    <row r="221" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A221" s="57"/>
+      <c r="B221" s="76"/>
+    </row>
+    <row r="222" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A222" s="57"/>
+      <c r="B222" s="76"/>
+    </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A72:A83"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="A66:A71"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A47:B47"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A74:A85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A167:B167"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11636,7 +11714,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="114" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -11656,7 +11734,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="118"/>
+      <c r="A2" s="115"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -11724,10 +11802,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="116" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="120"/>
+      <c r="C6" s="117"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - EXERCISE 29.09.2019 - Table Relations
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="631">
   <si>
     <t>Операция</t>
   </si>
@@ -5366,9 +5366,6 @@
     <t>Database Design</t>
   </si>
   <si>
-    <t>E/R Diagrams</t>
-  </si>
-  <si>
     <t>Steps in Database Design</t>
   </si>
   <si>
@@ -5787,6 +5784,221 @@
       <t xml:space="preserve">
 COPOSITE KEY ON CREATE</t>
     </r>
+  </si>
+  <si>
+    <t>Joins, Subqueries, CTEs and Indices</t>
+  </si>
+  <si>
+    <t>Indices</t>
+  </si>
+  <si>
+    <t>JOINS
+Gathering Data From Multiple Tables</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Inner joins
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Join of two tables returning only rows matching the join condition)</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT * FROM Employees AS e
+INNER JOIN Departments AS d
+ON e.DepartmentID = d.DepartmentID</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Left (or right) outer join
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Returns the results of the inner join as well as unmatched rows
+from the left (or right) table)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Full outer join
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Returns the results of an inner join along with all unmatched rows)</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT * FROM Employees AS e
+LEFT OUTER JOIN Departments AS d
+ON e.DepartmentID = d.DepartmentID
+SELECT * FROM Employees AS e
+RIGHT OUTER JOIN Departments AS d
+ON e.DepartmentID = d.DepartmentID</t>
+  </si>
+  <si>
+    <t>SELECT * FROM Employees AS e
+FULL JOIN Departments AS d
+ON e.DepartmentID = d.DepartmentID</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SELECT LastName, Name AS
+DepartmentName
+FROM Employees, Departments
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+A Cartesian product is formed when:
+A join condition is omitted
+A join condition is invalid
+All rows in the first table are joined to all rows in the second table
+To avoid a Cartesian product, always include a valid join condition</t>
+    </r>
+  </si>
+  <si>
+    <t>Cartesian Product</t>
+  </si>
+  <si>
+    <t>SELECT * FROM Employees AS e
+CROSS JOIN Departments AS d</t>
+  </si>
+  <si>
+    <t>Cross Join</t>
+  </si>
+  <si>
+    <t>Subqueries
+Query Manipulation on Multiple Levels</t>
+  </si>
+  <si>
+    <t>Subqueries use a query’s result as data for another query</t>
+  </si>
+  <si>
+    <t>SELECT FROM Employees AS e
+WHERE e.DepartmentID IN
+(SELECT d.DepartmentID
+FROM Deparments AS d
+WHERE d.Name = 'Finance')</t>
+  </si>
+  <si>
+    <t>Common Table Expressions (CTE)
+Reusable Subqueries</t>
+  </si>
+  <si>
+    <t>Common Table Expressions (CTE) can be considered as
+"named subqueries".
+They could be used to improve code readability and code
+reuse.
+Usually they are positioned in the beginning of the query.</t>
+  </si>
+  <si>
+    <t>WITH Employees_CTE
+(FirstName, LastName, DepartmentName)
+AS
+(SELECT e.FirstName, e.LastName, d.Name
+FROM Employees AS e
+LEFT JOIN Departments AS d ON
+d.DepartmentID = e.DepartmentID)
+SELECT FirstName, LastName, DepartmentName
+FROM Employees_CTE</t>
+  </si>
+  <si>
+    <t>Indexes
+Clustered and Non-Clustered Indexes</t>
+  </si>
+  <si>
+    <t>Temporary Tables</t>
+  </si>
+  <si>
+    <t>Temporary tables are stored in tempdb.
+Automatically deleted when they are no longer used.</t>
+  </si>
+  <si>
+    <t>CREATE TABLE #TempTable
+(
+-- Add columns here.
+)
+SELECT * FROM #TempTable</t>
+  </si>
+  <si>
+    <t>CREATE TABLE #Employees
+(Id INT PRIMARY KEY,
+FirstName VARCHAR(50) NOT NULL,
+LastName VARCHAR(50),
+Address VARCHAR(50))
+SELECT * FROM #Employees</t>
+  </si>
+  <si>
+    <t>Temporary Table Syntax</t>
+  </si>
+  <si>
+    <t>Clustered Indexes</t>
+  </si>
+  <si>
+    <t>Non-Clustered Indexes</t>
+  </si>
+  <si>
+    <t>Useful for fast retrieving of a single record or a range of records
+Maintained in a separate structure in the DB
+Tend to be much narrower than the base table
+Can locate the exact record(s) with less I/O
+Has at least one more intermediate level than the clustered index
+Much less valuable if a table doesn’t have a clustered index
+A non-clustered index has pointers to the actual data rows (pointers to the clustered index if there is one).</t>
+  </si>
+  <si>
+    <t>Clustered index is actually the data itself
+Very useful for fast execution of WHERE, ORDER BY and GROUP BY clauses.
+Maximum 1 clustered index per table
+If a table has no clustered index, its data rows are stored in an unordered structure (heap).</t>
+  </si>
+  <si>
+    <t>Indices speed up the searching of values in a certain column or group of columns
+Usually implemented as B-trees
+Indices can be built-in the table (clustered) or stored externally (non-clustered)
+Adding and deleting records in indexed tables is slower!
+Indices should be used for big tables only (e.g. 50 000 rows).</t>
   </si>
 </sst>
 </file>
@@ -6542,7 +6754,7 @@
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6814,20 +7026,32 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6847,17 +7071,8 @@
     <xf numFmtId="0" fontId="36" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6871,8 +7086,14 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -9604,15 +9825,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A217" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.7109375" style="64" customWidth="1"/>
+    <col min="1" max="1" width="66.42578125" style="64" customWidth="1"/>
     <col min="2" max="2" width="95" style="58" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" style="66" customWidth="1"/>
   </cols>
@@ -9626,16 +9847,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="100" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="111"/>
+      <c r="B2" s="105"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="107" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="112"/>
+      <c r="B3" s="106"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -9662,10 +9883,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="106" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="110"/>
+      <c r="B7" s="104"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -9692,10 +9913,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="106" t="s">
         <v>520</v>
       </c>
-      <c r="B11" s="110"/>
+      <c r="B11" s="104"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -9706,10 +9927,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="106" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="112"/>
+      <c r="B13" s="106"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -9761,17 +9982,17 @@
     </row>
     <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="106" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="112"/>
+      <c r="B21" s="106"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -9782,10 +10003,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112" t="s">
+      <c r="A23" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="112"/>
+      <c r="B23" s="106"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -9796,10 +10017,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="112" t="s">
+      <c r="A25" s="106" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="112"/>
+      <c r="B25" s="106"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -9826,10 +10047,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="112" t="s">
+      <c r="A29" s="106" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="112"/>
+      <c r="B29" s="106"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -9856,10 +10077,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="110" t="s">
+      <c r="A33" s="104" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="110"/>
+      <c r="B33" s="104"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -9886,10 +10107,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="112" t="s">
+      <c r="A37" s="106" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="112"/>
+      <c r="B37" s="106"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -9916,10 +10137,10 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="110" t="s">
+      <c r="A41" s="104" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="110"/>
+      <c r="B41" s="104"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
@@ -9938,10 +10159,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="112" t="s">
+      <c r="A44" s="106" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="110"/>
+      <c r="B44" s="104"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -9968,19 +10189,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="101" t="s">
+      <c r="A48" s="100" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="101"/>
+      <c r="B48" s="100"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="99" t="s">
+      <c r="A49" s="101" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="100"/>
+      <c r="B49" s="102"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="107" t="s">
+      <c r="A50" s="111" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -9988,22 +10209,22 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="108"/>
+      <c r="A51" s="112"/>
       <c r="B51" s="62" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C51" s="66" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="109"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="107" t="s">
+      <c r="A53" s="111" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -10011,25 +10232,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="108"/>
+      <c r="A54" s="112"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="108"/>
+      <c r="A55" s="112"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="109"/>
+      <c r="A56" s="113"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="107" t="s">
+      <c r="A57" s="111" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -10037,13 +10258,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="109"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="107" t="s">
+      <c r="A59" s="111" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -10054,7 +10275,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="108"/>
+      <c r="A60" s="112"/>
       <c r="B60" s="62" t="s">
         <v>528</v>
       </c>
@@ -10063,14 +10284,14 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="108"/>
+      <c r="A61" s="112"/>
       <c r="B61" s="62" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="109"/>
+      <c r="A62" s="113"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
@@ -10093,10 +10314,10 @@
     </row>
     <row r="65" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A65" s="57" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B65" s="62" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -10116,7 +10337,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="104" t="s">
+      <c r="A68" s="108" t="s">
         <v>290</v>
       </c>
       <c r="B68" s="62" t="s">
@@ -10124,37 +10345,37 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="105"/>
+      <c r="A69" s="109"/>
       <c r="B69" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="105"/>
+      <c r="A70" s="109"/>
       <c r="B70" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="105"/>
+      <c r="A71" s="109"/>
       <c r="B71" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="105"/>
+      <c r="A72" s="109"/>
       <c r="B72" s="62" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="106"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="104" t="s">
+      <c r="A74" s="108" t="s">
         <v>291</v>
       </c>
       <c r="B74" s="62" t="s">
@@ -10162,74 +10383,74 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="105"/>
+      <c r="A75" s="109"/>
       <c r="B75" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C75" s="67"/>
     </row>
     <row r="76" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="105"/>
+      <c r="A76" s="109"/>
       <c r="B76" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="105"/>
+      <c r="A77" s="109"/>
       <c r="B77" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="105"/>
+      <c r="A78" s="109"/>
       <c r="B78" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="105"/>
+      <c r="A79" s="109"/>
       <c r="B79" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="105"/>
+      <c r="A80" s="109"/>
       <c r="B80" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="105"/>
+      <c r="A81" s="109"/>
       <c r="B81" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A82" s="105"/>
+      <c r="A82" s="109"/>
       <c r="B82" s="81" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="105"/>
+      <c r="A83" s="109"/>
       <c r="B83" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="105"/>
+      <c r="A84" s="109"/>
       <c r="B84" s="81" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="106"/>
+      <c r="A85" s="110"/>
       <c r="B85" s="81" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="104" t="s">
+      <c r="A86" s="108" t="s">
         <v>292</v>
       </c>
       <c r="B86" s="82" t="s">
@@ -10237,28 +10458,28 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="105"/>
+      <c r="A87" s="109"/>
       <c r="B87" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C87"/>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="105"/>
+      <c r="A88" s="109"/>
       <c r="B88" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="106"/>
+      <c r="A89" s="110"/>
       <c r="B89" s="82" t="s">
         <v>547</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="104" t="s">
+      <c r="A90" s="108" t="s">
         <v>309</v>
       </c>
       <c r="B90" s="84" t="s">
@@ -10267,7 +10488,7 @@
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A91" s="106"/>
+      <c r="A91" s="110"/>
       <c r="B91" s="84" t="s">
         <v>311</v>
       </c>
@@ -10328,17 +10549,17 @@
       <c r="C97"/>
     </row>
     <row r="98" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="101" t="s">
+      <c r="A98" s="100" t="s">
         <v>388</v>
       </c>
-      <c r="B98" s="101"/>
+      <c r="B98" s="100"/>
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A99" s="99" t="s">
+      <c r="A99" s="101" t="s">
         <v>389</v>
       </c>
-      <c r="B99" s="100"/>
+      <c r="B99" s="102"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -10369,10 +10590,10 @@
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="99" t="s">
+      <c r="A103" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="B103" s="100"/>
+      <c r="B103" s="102"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -10520,10 +10741,10 @@
       <c r="C119"/>
     </row>
     <row r="120" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A120" s="99" t="s">
+      <c r="A120" s="101" t="s">
         <v>427</v>
       </c>
-      <c r="B120" s="100"/>
+      <c r="B120" s="102"/>
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -10608,10 +10829,10 @@
       <c r="C129"/>
     </row>
     <row r="130" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A130" s="99" t="s">
+      <c r="A130" s="101" t="s">
         <v>499</v>
       </c>
-      <c r="B130" s="100"/>
+      <c r="B130" s="102"/>
       <c r="C130"/>
     </row>
     <row r="131" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -10705,10 +10926,10 @@
       <c r="C140"/>
     </row>
     <row r="141" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A141" s="102" t="s">
+      <c r="A141" s="103" t="s">
         <v>462</v>
       </c>
-      <c r="B141" s="100"/>
+      <c r="B141" s="102"/>
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -10739,10 +10960,10 @@
       <c r="C144"/>
     </row>
     <row r="145" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A145" s="102" t="s">
+      <c r="A145" s="103" t="s">
         <v>470</v>
       </c>
-      <c r="B145" s="100"/>
+      <c r="B145" s="102"/>
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -10764,10 +10985,10 @@
       <c r="C147"/>
     </row>
     <row r="148" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="102" t="s">
+      <c r="A148" s="103" t="s">
         <v>542</v>
       </c>
-      <c r="B148" s="100"/>
+      <c r="B148" s="102"/>
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -10778,7 +10999,7 @@
         <v>546</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -10792,25 +11013,25 @@
     </row>
     <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" s="57" t="s">
-        <v>599</v>
-      </c>
-      <c r="B151" s="118" t="s">
         <v>598</v>
       </c>
+      <c r="B151" s="99" t="s">
+        <v>597</v>
+      </c>
       <c r="C151"/>
     </row>
     <row r="152" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A152" s="101" t="s">
+      <c r="A152" s="100" t="s">
         <v>472</v>
       </c>
-      <c r="B152" s="101"/>
+      <c r="B152" s="100"/>
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A153" s="99" t="s">
+      <c r="A153" s="101" t="s">
         <v>475</v>
       </c>
-      <c r="B153" s="100"/>
+      <c r="B153" s="102"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -10846,10 +11067,10 @@
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A159" s="102" t="s">
+      <c r="A159" s="103" t="s">
         <v>478</v>
       </c>
-      <c r="B159" s="103"/>
+      <c r="B159" s="114"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -10916,10 +11137,10 @@
       <c r="C166"/>
     </row>
     <row r="167" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A167" s="99" t="s">
+      <c r="A167" s="101" t="s">
         <v>473</v>
       </c>
-      <c r="B167" s="100"/>
+      <c r="B167" s="102"/>
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -10941,10 +11162,10 @@
       <c r="C169"/>
     </row>
     <row r="170" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A170" s="99" t="s">
+      <c r="A170" s="101" t="s">
         <v>474</v>
       </c>
-      <c r="B170" s="100"/>
+      <c r="B170" s="102"/>
       <c r="C170"/>
     </row>
     <row r="171" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -10966,25 +11187,25 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A173" s="101" t="s">
+      <c r="A173" s="100" t="s">
         <v>553</v>
       </c>
-      <c r="B173" s="101"/>
+      <c r="B173" s="100"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A174" s="99" t="s">
+      <c r="A174" s="101" t="s">
         <v>554</v>
       </c>
-      <c r="B174" s="100"/>
+      <c r="B174" s="102"/>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A175" s="57" t="s">
+        <v>555</v>
+      </c>
+      <c r="B175" s="76" t="s">
         <v>556</v>
-      </c>
-      <c r="B175" s="76" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -10992,83 +11213,83 @@
       <c r="B176" s="76"/>
     </row>
     <row r="177" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A177" s="99" t="s">
+      <c r="A177" s="101" t="s">
         <v>553</v>
       </c>
-      <c r="B177" s="100"/>
+      <c r="B177" s="102"/>
       <c r="C177"/>
     </row>
     <row r="178" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A178" s="57" t="s">
+        <v>557</v>
+      </c>
+      <c r="B178" s="76" t="s">
         <v>558</v>
-      </c>
-      <c r="B178" s="76" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A179" s="57" t="s">
+        <v>559</v>
+      </c>
+      <c r="B179" s="76" t="s">
         <v>560</v>
-      </c>
-      <c r="B179" s="76" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="57" t="s">
+        <v>561</v>
+      </c>
+      <c r="B180" s="76" t="s">
         <v>562</v>
-      </c>
-      <c r="B180" s="76" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="57" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B181" s="76" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="57" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B182" s="76" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A183" s="57" t="s">
+        <v>567</v>
+      </c>
+      <c r="B183" s="80" t="s">
         <v>568</v>
       </c>
-      <c r="B183" s="80" t="s">
-        <v>569</v>
-      </c>
       <c r="C183" s="96" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
       <c r="A184" s="57" t="s">
+        <v>569</v>
+      </c>
+      <c r="B184" s="80" t="s">
         <v>570</v>
       </c>
-      <c r="B184" s="80" t="s">
-        <v>571</v>
-      </c>
       <c r="C184" s="96" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A185" s="57" t="s">
+        <v>571</v>
+      </c>
+      <c r="B185" s="76" t="s">
         <v>572</v>
       </c>
-      <c r="B185" s="76" t="s">
-        <v>573</v>
-      </c>
       <c r="C185" s="95" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -11076,106 +11297,134 @@
       <c r="B186" s="76"/>
     </row>
     <row r="187" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A187" s="99" t="s">
-        <v>577</v>
-      </c>
-      <c r="B187" s="100"/>
+      <c r="A187" s="101" t="s">
+        <v>576</v>
+      </c>
+      <c r="B187" s="102"/>
       <c r="C187"/>
     </row>
     <row r="188" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A188" s="57" t="s">
+        <v>577</v>
+      </c>
+      <c r="B188" s="76" t="s">
         <v>578</v>
-      </c>
-      <c r="B188" s="76" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A189" s="57"/>
       <c r="B189" s="76" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A190" s="103" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A190" s="102" t="s">
-        <v>581</v>
-      </c>
-      <c r="B190" s="100"/>
+      <c r="B190" s="102"/>
     </row>
     <row r="191" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A191" s="57" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B191" s="76" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B192" s="76" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A193" s="57" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B193" s="97" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A194" s="57" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B194" s="97" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A195" s="99" t="s">
-        <v>555</v>
+      <c r="A195" s="100" t="s">
+        <v>601</v>
       </c>
       <c r="B195" s="100"/>
       <c r="C195"/>
     </row>
-    <row r="196" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="57"/>
-      <c r="B196" s="76"/>
-    </row>
-    <row r="197" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="57"/>
-      <c r="B197" s="76"/>
-    </row>
-    <row r="198" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="57"/>
-      <c r="B198" s="76"/>
-    </row>
-    <row r="199" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="57"/>
-      <c r="B199" s="76"/>
-    </row>
-    <row r="200" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="57"/>
-      <c r="B200" s="76"/>
-    </row>
-    <row r="201" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="57"/>
-      <c r="B201" s="76"/>
+    <row r="196" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A196" s="103" t="s">
+        <v>603</v>
+      </c>
+      <c r="B196" s="102"/>
+    </row>
+    <row r="197" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A197" s="57" t="s">
+        <v>604</v>
+      </c>
+      <c r="B197" s="120" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A198" s="57" t="s">
+        <v>606</v>
+      </c>
+      <c r="B198" s="120" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A199" s="57" t="s">
+        <v>607</v>
+      </c>
+      <c r="B199" s="120" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A200" s="57" t="s">
+        <v>611</v>
+      </c>
+      <c r="B200" s="121" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="57" t="s">
+        <v>613</v>
+      </c>
+      <c r="B201" s="120" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="202" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A202" s="57"/>
-      <c r="B202" s="76"/>
-    </row>
-    <row r="203" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="57"/>
-      <c r="B203" s="76"/>
-    </row>
-    <row r="204" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="57"/>
-      <c r="B204" s="76"/>
+      <c r="B202" s="119"/>
+    </row>
+    <row r="203" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A203" s="103" t="s">
+        <v>614</v>
+      </c>
+      <c r="B203" s="102"/>
+    </row>
+    <row r="204" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A204" s="57" t="s">
+        <v>615</v>
+      </c>
+      <c r="B204" s="76" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="205" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A205" s="57"/>
@@ -11205,41 +11454,71 @@
       <c r="A211" s="57"/>
       <c r="B211" s="76"/>
     </row>
-    <row r="212" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="57"/>
-      <c r="B212" s="76"/>
-    </row>
-    <row r="213" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A213" s="57"/>
-      <c r="B213" s="76"/>
-    </row>
-    <row r="214" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="57"/>
-      <c r="B214" s="76"/>
-    </row>
-    <row r="215" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A215" s="57"/>
-      <c r="B215" s="76"/>
-    </row>
-    <row r="216" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A216" s="57"/>
-      <c r="B216" s="76"/>
-    </row>
-    <row r="217" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A217" s="57"/>
-      <c r="B217" s="76"/>
-    </row>
-    <row r="218" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="57"/>
-      <c r="B218" s="76"/>
-    </row>
-    <row r="219" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="57"/>
-      <c r="B219" s="76"/>
-    </row>
-    <row r="220" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="57"/>
-      <c r="B220" s="76"/>
+    <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A212" s="103" t="s">
+        <v>617</v>
+      </c>
+      <c r="B212" s="102"/>
+    </row>
+    <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A213" s="72" t="s">
+        <v>618</v>
+      </c>
+      <c r="B213" s="76" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A214" s="103" t="s">
+        <v>621</v>
+      </c>
+      <c r="B214" s="102"/>
+    </row>
+    <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A215" s="57" t="s">
+        <v>622</v>
+      </c>
+      <c r="B215" s="76" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A216" s="57" t="s">
+        <v>625</v>
+      </c>
+      <c r="B216" s="76" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A217" s="103" t="s">
+        <v>620</v>
+      </c>
+      <c r="B217" s="102"/>
+    </row>
+    <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A218" s="57" t="s">
+        <v>602</v>
+      </c>
+      <c r="B218" s="80" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A219" s="57" t="s">
+        <v>626</v>
+      </c>
+      <c r="B219" s="76" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A220" s="57" t="s">
+        <v>627</v>
+      </c>
+      <c r="B220" s="76" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="221" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A221" s="57"/>
@@ -11249,14 +11528,337 @@
       <c r="A222" s="57"/>
       <c r="B222" s="76"/>
     </row>
+    <row r="223" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A223" s="57"/>
+      <c r="B223" s="76"/>
+    </row>
+    <row r="224" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A224" s="57"/>
+      <c r="B224" s="76"/>
+    </row>
+    <row r="225" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A225" s="57"/>
+      <c r="B225" s="76"/>
+    </row>
+    <row r="226" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A226" s="57"/>
+      <c r="B226" s="76"/>
+    </row>
+    <row r="227" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A227" s="57"/>
+      <c r="B227" s="76"/>
+    </row>
+    <row r="228" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A228" s="57"/>
+      <c r="B228" s="76"/>
+    </row>
+    <row r="229" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A229" s="57"/>
+      <c r="B229" s="76"/>
+    </row>
+    <row r="230" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A230" s="57"/>
+      <c r="B230" s="76"/>
+    </row>
+    <row r="231" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A231" s="57"/>
+      <c r="B231" s="76"/>
+    </row>
+    <row r="232" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A232" s="57"/>
+      <c r="B232" s="76"/>
+    </row>
+    <row r="233" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A233" s="57"/>
+      <c r="B233" s="76"/>
+    </row>
+    <row r="234" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A234" s="57"/>
+      <c r="B234" s="76"/>
+    </row>
+    <row r="235" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A235" s="57"/>
+      <c r="B235" s="76"/>
+    </row>
+    <row r="236" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A236" s="57"/>
+      <c r="B236" s="76"/>
+    </row>
+    <row r="237" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A237" s="57"/>
+      <c r="B237" s="76"/>
+    </row>
+    <row r="238" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A238" s="57"/>
+      <c r="B238" s="76"/>
+    </row>
+    <row r="239" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A239" s="57"/>
+      <c r="B239" s="76"/>
+    </row>
+    <row r="240" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A240" s="57"/>
+      <c r="B240" s="76"/>
+    </row>
+    <row r="241" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A241" s="57"/>
+      <c r="B241" s="76"/>
+    </row>
+    <row r="242" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A242" s="57"/>
+      <c r="B242" s="76"/>
+    </row>
+    <row r="243" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A243" s="57"/>
+      <c r="B243" s="76"/>
+    </row>
+    <row r="244" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A244" s="57"/>
+      <c r="B244" s="76"/>
+    </row>
+    <row r="245" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A245" s="57"/>
+      <c r="B245" s="76"/>
+    </row>
+    <row r="246" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A246" s="57"/>
+      <c r="B246" s="76"/>
+    </row>
+    <row r="247" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A247" s="57"/>
+      <c r="B247" s="76"/>
+    </row>
+    <row r="248" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A248" s="57"/>
+      <c r="B248" s="76"/>
+    </row>
+    <row r="249" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A249" s="57"/>
+      <c r="B249" s="76"/>
+    </row>
+    <row r="250" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A250" s="57"/>
+      <c r="B250" s="76"/>
+    </row>
+    <row r="251" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A251" s="57"/>
+      <c r="B251" s="76"/>
+    </row>
+    <row r="252" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A252" s="57"/>
+      <c r="B252" s="76"/>
+    </row>
+    <row r="253" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A253" s="57"/>
+      <c r="B253" s="76"/>
+    </row>
+    <row r="254" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A254" s="57"/>
+      <c r="B254" s="76"/>
+    </row>
+    <row r="255" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A255" s="57"/>
+      <c r="B255" s="76"/>
+    </row>
+    <row r="256" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A256" s="57"/>
+      <c r="B256" s="76"/>
+    </row>
+    <row r="257" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A257" s="57"/>
+      <c r="B257" s="76"/>
+    </row>
+    <row r="258" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A258" s="57"/>
+      <c r="B258" s="76"/>
+    </row>
+    <row r="259" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A259" s="57"/>
+      <c r="B259" s="76"/>
+    </row>
+    <row r="260" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A260" s="57"/>
+      <c r="B260" s="76"/>
+    </row>
+    <row r="261" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A261" s="57"/>
+      <c r="B261" s="76"/>
+    </row>
+    <row r="262" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A262" s="57"/>
+      <c r="B262" s="76"/>
+    </row>
+    <row r="263" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A263" s="57"/>
+      <c r="B263" s="76"/>
+    </row>
+    <row r="264" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A264" s="57"/>
+      <c r="B264" s="76"/>
+    </row>
+    <row r="265" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A265" s="57"/>
+      <c r="B265" s="76"/>
+    </row>
+    <row r="266" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A266" s="57"/>
+      <c r="B266" s="76"/>
+    </row>
+    <row r="267" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A267" s="57"/>
+      <c r="B267" s="76"/>
+    </row>
+    <row r="268" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A268" s="57"/>
+      <c r="B268" s="76"/>
+    </row>
+    <row r="269" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A269" s="57"/>
+      <c r="B269" s="76"/>
+    </row>
+    <row r="270" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A270" s="57"/>
+      <c r="B270" s="76"/>
+    </row>
+    <row r="271" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A271" s="57"/>
+      <c r="B271" s="76"/>
+    </row>
+    <row r="272" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A272" s="57"/>
+      <c r="B272" s="76"/>
+    </row>
+    <row r="273" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A273" s="57"/>
+      <c r="B273" s="76"/>
+    </row>
+    <row r="274" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A274" s="57"/>
+      <c r="B274" s="76"/>
+    </row>
+    <row r="275" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A275" s="57"/>
+      <c r="B275" s="76"/>
+    </row>
+    <row r="276" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A276" s="57"/>
+      <c r="B276" s="76"/>
+    </row>
+    <row r="277" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A277" s="57"/>
+      <c r="B277" s="76"/>
+    </row>
+    <row r="278" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A278" s="57"/>
+      <c r="B278" s="76"/>
+    </row>
+    <row r="279" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A279" s="57"/>
+      <c r="B279" s="76"/>
+    </row>
+    <row r="280" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A280" s="57"/>
+      <c r="B280" s="76"/>
+    </row>
+    <row r="281" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A281" s="57"/>
+      <c r="B281" s="76"/>
+    </row>
+    <row r="282" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A282" s="57"/>
+      <c r="B282" s="76"/>
+    </row>
+    <row r="283" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A283" s="57"/>
+      <c r="B283" s="76"/>
+    </row>
+    <row r="284" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A284" s="57"/>
+      <c r="B284" s="76"/>
+    </row>
+    <row r="285" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A285" s="57"/>
+      <c r="B285" s="76"/>
+    </row>
+    <row r="286" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A286" s="57"/>
+      <c r="B286" s="76"/>
+    </row>
+    <row r="287" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A287" s="57"/>
+      <c r="B287" s="76"/>
+    </row>
+    <row r="288" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A288" s="57"/>
+      <c r="B288" s="76"/>
+    </row>
+    <row r="289" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A289" s="57"/>
+      <c r="B289" s="76"/>
+    </row>
+    <row r="290" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A290" s="57"/>
+      <c r="B290" s="76"/>
+    </row>
+    <row r="291" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A291" s="57"/>
+      <c r="B291" s="76"/>
+    </row>
+    <row r="292" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A292" s="57"/>
+      <c r="B292" s="76"/>
+    </row>
+    <row r="293" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A293" s="57"/>
+      <c r="B293" s="76"/>
+    </row>
+    <row r="294" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A294" s="57"/>
+      <c r="B294" s="76"/>
+    </row>
+    <row r="295" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A295" s="57"/>
+      <c r="B295" s="76"/>
+    </row>
+    <row r="296" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A296" s="57"/>
+      <c r="B296" s="76"/>
+    </row>
+    <row r="297" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A297" s="57"/>
+      <c r="B297" s="76"/>
+    </row>
+    <row r="298" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A298" s="57"/>
+      <c r="B298" s="76"/>
+    </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="A195:B195"/>
-    <mergeCell ref="A190:B190"/>
+  <mergeCells count="47">
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A74:A85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
     <mergeCell ref="A148:B148"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
@@ -11273,26 +11875,12 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A74:A85"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="A190:B190"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11714,7 +12302,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="115" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -11734,7 +12322,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115"/>
+      <c r="A2" s="116"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -11802,10 +12390,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="116" t="s">
+      <c r="B6" s="117" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="117"/>
+      <c r="C6" s="118"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - EXERCISE 30.09.2019 - Table Relations
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -6019,12 +6019,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6776,42 +6784,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6826,91 +6834,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6925,73 +6933,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7000,119 +7008,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7120,10 +7071,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9859,7 +9867,7 @@
   <dimension ref="A1:C299"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9878,16 +9886,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="107" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="105"/>
+      <c r="B2" s="116"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="118" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="106"/>
+      <c r="B3" s="117"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -9914,10 +9922,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="117" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="104"/>
+      <c r="B7" s="115"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -9944,10 +9952,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="117" t="s">
         <v>520</v>
       </c>
-      <c r="B11" s="104"/>
+      <c r="B11" s="115"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -9958,10 +9966,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="117" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="106"/>
+      <c r="B13" s="117"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -10020,10 +10028,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="106" t="s">
+      <c r="A21" s="117" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="106"/>
+      <c r="B21" s="117"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -10034,10 +10042,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="106" t="s">
+      <c r="A23" s="117" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="106"/>
+      <c r="B23" s="117"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -10048,10 +10056,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="106" t="s">
+      <c r="A25" s="117" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="106"/>
+      <c r="B25" s="117"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -10069,7 +10077,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>349</v>
       </c>
@@ -10078,10 +10086,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="117" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="106"/>
+      <c r="B29" s="117"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -10108,10 +10116,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="115" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="104"/>
+      <c r="B33" s="115"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -10138,10 +10146,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="106" t="s">
+      <c r="A37" s="117" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="106"/>
+      <c r="B37" s="117"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -10168,10 +10176,10 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="104" t="s">
+      <c r="A41" s="115" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="104"/>
+      <c r="B41" s="115"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
@@ -10190,10 +10198,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="106" t="s">
+      <c r="A44" s="117" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="104"/>
+      <c r="B44" s="115"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -10220,19 +10228,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="100" t="s">
+      <c r="A48" s="107" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="100"/>
+      <c r="B48" s="107"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="101" t="s">
+      <c r="A49" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="102"/>
+      <c r="B49" s="105"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="111" t="s">
+      <c r="A50" s="112" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10240,7 +10248,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="112"/>
+      <c r="A51" s="113"/>
       <c r="B51" s="62" t="s">
         <v>592</v>
       </c>
@@ -10249,13 +10257,13 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="113"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="111" t="s">
+      <c r="A53" s="112" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -10263,25 +10271,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="112"/>
+      <c r="A54" s="113"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="112"/>
+      <c r="A55" s="113"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="113"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="111" t="s">
+      <c r="A57" s="112" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -10289,13 +10297,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="113"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="111" t="s">
+      <c r="A59" s="112" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -10306,7 +10314,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="112"/>
+      <c r="A60" s="113"/>
       <c r="B60" s="62" t="s">
         <v>528</v>
       </c>
@@ -10315,20 +10323,20 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="112"/>
+      <c r="A61" s="113"/>
       <c r="B61" s="62" t="s">
         <v>589</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="113"/>
+      <c r="A62" s="114"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="122" t="s">
+      <c r="A63" s="103" t="s">
         <v>633</v>
       </c>
       <c r="B63" s="62" t="s">
@@ -10376,7 +10384,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="108" t="s">
+      <c r="A69" s="109" t="s">
         <v>290</v>
       </c>
       <c r="B69" s="62" t="s">
@@ -10384,37 +10392,37 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="109"/>
+      <c r="A70" s="110"/>
       <c r="B70" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="109"/>
+      <c r="A71" s="110"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="109"/>
+      <c r="A72" s="110"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="109"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="62" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="110"/>
+      <c r="A74" s="111"/>
       <c r="B74" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="108" t="s">
+      <c r="A75" s="109" t="s">
         <v>291</v>
       </c>
       <c r="B75" s="62" t="s">
@@ -10422,74 +10430,74 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="109"/>
+      <c r="A76" s="110"/>
       <c r="B76" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C76" s="67"/>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="109"/>
+      <c r="A77" s="110"/>
       <c r="B77" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="109"/>
+      <c r="A78" s="110"/>
       <c r="B78" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="109"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="109"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="109"/>
+      <c r="A81" s="110"/>
       <c r="B81" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="109"/>
+      <c r="A82" s="110"/>
       <c r="B82" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="109"/>
+      <c r="A83" s="110"/>
       <c r="B83" s="81" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="109"/>
+      <c r="A84" s="110"/>
       <c r="B84" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="109"/>
+      <c r="A85" s="110"/>
       <c r="B85" s="81" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="110"/>
+      <c r="A86" s="111"/>
       <c r="B86" s="81" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="108" t="s">
+      <c r="A87" s="109" t="s">
         <v>292</v>
       </c>
       <c r="B87" s="82" t="s">
@@ -10497,28 +10505,28 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="109"/>
+      <c r="A88" s="110"/>
       <c r="B88" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="109"/>
+      <c r="A89" s="110"/>
       <c r="B89" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="110"/>
+      <c r="A90" s="111"/>
       <c r="B90" s="82" t="s">
         <v>547</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="108" t="s">
+      <c r="A91" s="109" t="s">
         <v>309</v>
       </c>
       <c r="B91" s="84" t="s">
@@ -10527,7 +10535,7 @@
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="110"/>
+      <c r="A92" s="111"/>
       <c r="B92" s="84" t="s">
         <v>311</v>
       </c>
@@ -10551,7 +10559,7 @@
       </c>
       <c r="C94"/>
     </row>
-    <row r="95" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A95" s="61" t="s">
         <v>385</v>
       </c>
@@ -10588,17 +10596,17 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="100" t="s">
+      <c r="A99" s="107" t="s">
         <v>388</v>
       </c>
-      <c r="B99" s="100"/>
+      <c r="B99" s="107"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="101" t="s">
+      <c r="A100" s="106" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="102"/>
+      <c r="B100" s="105"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -10629,10 +10637,10 @@
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A104" s="101" t="s">
+      <c r="A104" s="106" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="102"/>
+      <c r="B104" s="105"/>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -10780,10 +10788,10 @@
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A121" s="101" t="s">
+      <c r="A121" s="106" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="102"/>
+      <c r="B121" s="105"/>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -10868,10 +10876,10 @@
       <c r="C130"/>
     </row>
     <row r="131" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A131" s="101" t="s">
+      <c r="A131" s="106" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="102"/>
+      <c r="B131" s="105"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -10919,7 +10927,7 @@
       </c>
       <c r="C136"/>
     </row>
-    <row r="137" spans="1:3" ht="119.25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="103.5" x14ac:dyDescent="0.25">
       <c r="A137" s="77" t="s">
         <v>456</v>
       </c>
@@ -10965,10 +10973,10 @@
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="103" t="s">
+      <c r="A142" s="104" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="102"/>
+      <c r="B142" s="105"/>
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -10999,10 +11007,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="103" t="s">
+      <c r="A146" s="104" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="102"/>
+      <c r="B146" s="105"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11024,10 +11032,10 @@
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="103" t="s">
+      <c r="A149" s="104" t="s">
         <v>542</v>
       </c>
-      <c r="B149" s="102"/>
+      <c r="B149" s="105"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -11060,17 +11068,17 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="100" t="s">
+      <c r="A153" s="107" t="s">
         <v>472</v>
       </c>
-      <c r="B153" s="100"/>
+      <c r="B153" s="107"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="101" t="s">
+      <c r="A154" s="106" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="102"/>
+      <c r="B154" s="105"/>
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -11106,10 +11114,10 @@
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="103" t="s">
+      <c r="A160" s="104" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="114"/>
+      <c r="B160" s="108"/>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -11176,10 +11184,10 @@
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="101" t="s">
+      <c r="A168" s="106" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="102"/>
+      <c r="B168" s="105"/>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -11201,10 +11209,10 @@
       <c r="C170"/>
     </row>
     <row r="171" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A171" s="101" t="s">
+      <c r="A171" s="106" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="102"/>
+      <c r="B171" s="105"/>
       <c r="C171"/>
     </row>
     <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -11226,17 +11234,17 @@
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A174" s="100" t="s">
+      <c r="A174" s="107" t="s">
         <v>553</v>
       </c>
-      <c r="B174" s="100"/>
+      <c r="B174" s="107"/>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="101" t="s">
+      <c r="A175" s="106" t="s">
         <v>554</v>
       </c>
-      <c r="B175" s="102"/>
+      <c r="B175" s="105"/>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11252,10 +11260,10 @@
       <c r="B177" s="76"/>
     </row>
     <row r="178" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A178" s="101" t="s">
+      <c r="A178" s="106" t="s">
         <v>553</v>
       </c>
-      <c r="B178" s="102"/>
+      <c r="B178" s="105"/>
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11336,10 +11344,10 @@
       <c r="B187" s="76"/>
     </row>
     <row r="188" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A188" s="101" t="s">
+      <c r="A188" s="106" t="s">
         <v>576</v>
       </c>
-      <c r="B188" s="102"/>
+      <c r="B188" s="105"/>
       <c r="C188"/>
     </row>
     <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11357,10 +11365,10 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="103" t="s">
+      <c r="A191" s="104" t="s">
         <v>580</v>
       </c>
-      <c r="B191" s="102"/>
+      <c r="B191" s="105"/>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
@@ -11395,23 +11403,23 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A196" s="100" t="s">
+      <c r="A196" s="107" t="s">
         <v>601</v>
       </c>
-      <c r="B196" s="100"/>
+      <c r="B196" s="107"/>
       <c r="C196"/>
     </row>
     <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="103" t="s">
+      <c r="A197" s="104" t="s">
         <v>603</v>
       </c>
-      <c r="B197" s="102"/>
+      <c r="B197" s="105"/>
     </row>
     <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A198" s="57" t="s">
         <v>604</v>
       </c>
-      <c r="B198" s="120" t="s">
+      <c r="B198" s="101" t="s">
         <v>605</v>
       </c>
     </row>
@@ -11419,7 +11427,7 @@
       <c r="A199" s="57" t="s">
         <v>606</v>
       </c>
-      <c r="B199" s="120" t="s">
+      <c r="B199" s="101" t="s">
         <v>608</v>
       </c>
     </row>
@@ -11427,7 +11435,7 @@
       <c r="A200" s="57" t="s">
         <v>607</v>
       </c>
-      <c r="B200" s="120" t="s">
+      <c r="B200" s="101" t="s">
         <v>609</v>
       </c>
     </row>
@@ -11435,7 +11443,7 @@
       <c r="A201" s="57" t="s">
         <v>611</v>
       </c>
-      <c r="B201" s="121" t="s">
+      <c r="B201" s="102" t="s">
         <v>610</v>
       </c>
     </row>
@@ -11443,19 +11451,19 @@
       <c r="A202" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="B202" s="120" t="s">
+      <c r="B202" s="101" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A203" s="57"/>
-      <c r="B203" s="119"/>
+      <c r="B203" s="100"/>
     </row>
     <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="103" t="s">
+      <c r="A204" s="104" t="s">
         <v>614</v>
       </c>
-      <c r="B204" s="102"/>
+      <c r="B204" s="105"/>
     </row>
     <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="57" t="s">
@@ -11494,10 +11502,10 @@
       <c r="B212" s="76"/>
     </row>
     <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="103" t="s">
+      <c r="A213" s="104" t="s">
         <v>616</v>
       </c>
-      <c r="B213" s="102"/>
+      <c r="B213" s="105"/>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="72" t="s">
@@ -11508,10 +11516,10 @@
       </c>
     </row>
     <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="103" t="s">
+      <c r="A215" s="104" t="s">
         <v>620</v>
       </c>
-      <c r="B215" s="102"/>
+      <c r="B215" s="105"/>
     </row>
     <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="57" t="s">
@@ -11530,10 +11538,10 @@
       </c>
     </row>
     <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="103" t="s">
+      <c r="A218" s="104" t="s">
         <v>619</v>
       </c>
-      <c r="B218" s="102"/>
+      <c r="B218" s="105"/>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A219" s="57" t="s">
@@ -11877,31 +11885,12 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A75:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A191:B191"/>
     <mergeCell ref="A149:B149"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
@@ -11918,12 +11907,31 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A75:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A215:B215"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12345,7 +12353,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="119" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -12365,7 +12373,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116"/>
+      <c r="A2" s="120"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -12433,10 +12441,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="121" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="118"/>
+      <c r="C6" s="122"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - EXERCISE 03.09.2019 - Table Relations
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -7518,6 +7518,12 @@
     <xf numFmtId="0" fontId="50" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7525,22 +7531,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7560,8 +7551,17 @@
     <xf numFmtId="0" fontId="37" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10308,7 +10308,7 @@
   <dimension ref="A1:C297"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C250" sqref="C250"/>
+      <selection activeCell="C248" sqref="C248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10327,16 +10327,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="106" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="109"/>
+      <c r="B2" s="116"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="118" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="110"/>
+      <c r="B3" s="117"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -10363,10 +10363,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="117" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="108"/>
+      <c r="B7" s="115"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -10393,10 +10393,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="117" t="s">
         <v>520</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="115"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -10407,10 +10407,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="117" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="110"/>
+      <c r="B13" s="117"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -10469,10 +10469,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="117" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="110"/>
+      <c r="B21" s="117"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -10483,10 +10483,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="117" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="110"/>
+      <c r="B23" s="117"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -10497,10 +10497,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="117" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="110"/>
+      <c r="B25" s="117"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -10527,10 +10527,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="110" t="s">
+      <c r="A29" s="117" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="110"/>
+      <c r="B29" s="117"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -10557,10 +10557,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="108" t="s">
+      <c r="A33" s="115" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="108"/>
+      <c r="B33" s="115"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -10587,10 +10587,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="110" t="s">
+      <c r="A37" s="117" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="110"/>
+      <c r="B37" s="117"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -10617,10 +10617,10 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="108" t="s">
+      <c r="A41" s="115" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="108"/>
+      <c r="B41" s="115"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
@@ -10639,10 +10639,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="110" t="s">
+      <c r="A44" s="117" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="108"/>
+      <c r="B44" s="115"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -10669,19 +10669,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="104" t="s">
+      <c r="A48" s="106" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="104"/>
+      <c r="B48" s="106"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="105" t="s">
+      <c r="A49" s="107" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="106"/>
+      <c r="B49" s="105"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="115" t="s">
+      <c r="A50" s="112" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10689,7 +10689,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="116"/>
+      <c r="A51" s="113"/>
       <c r="B51" s="62" t="s">
         <v>592</v>
       </c>
@@ -10698,13 +10698,13 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="117"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="115" t="s">
+      <c r="A53" s="112" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -10712,25 +10712,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
+      <c r="A54" s="113"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="116"/>
+      <c r="A55" s="113"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="117"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="112" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -10738,13 +10738,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="117"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="115" t="s">
+      <c r="A59" s="112" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -10755,7 +10755,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="116"/>
+      <c r="A60" s="113"/>
       <c r="B60" s="62" t="s">
         <v>528</v>
       </c>
@@ -10764,14 +10764,14 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="116"/>
+      <c r="A61" s="113"/>
       <c r="B61" s="62" t="s">
         <v>589</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="117"/>
+      <c r="A62" s="114"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
@@ -10825,7 +10825,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="112" t="s">
+      <c r="A69" s="109" t="s">
         <v>290</v>
       </c>
       <c r="B69" s="62" t="s">
@@ -10833,37 +10833,37 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="113"/>
+      <c r="A70" s="110"/>
       <c r="B70" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="113"/>
+      <c r="A71" s="110"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="113"/>
+      <c r="A72" s="110"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="113"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="62" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="114"/>
+      <c r="A74" s="111"/>
       <c r="B74" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="112" t="s">
+      <c r="A75" s="109" t="s">
         <v>291</v>
       </c>
       <c r="B75" s="62" t="s">
@@ -10871,74 +10871,74 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="113"/>
+      <c r="A76" s="110"/>
       <c r="B76" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C76" s="67"/>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="113"/>
+      <c r="A77" s="110"/>
       <c r="B77" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="113"/>
+      <c r="A78" s="110"/>
       <c r="B78" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="113"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="113"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="113"/>
+      <c r="A81" s="110"/>
       <c r="B81" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="113"/>
+      <c r="A82" s="110"/>
       <c r="B82" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="113"/>
+      <c r="A83" s="110"/>
       <c r="B83" s="81" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="113"/>
+      <c r="A84" s="110"/>
       <c r="B84" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="113"/>
+      <c r="A85" s="110"/>
       <c r="B85" s="81" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="114"/>
+      <c r="A86" s="111"/>
       <c r="B86" s="81" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="112" t="s">
+      <c r="A87" s="109" t="s">
         <v>292</v>
       </c>
       <c r="B87" s="82" t="s">
@@ -10946,28 +10946,28 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="113"/>
+      <c r="A88" s="110"/>
       <c r="B88" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="113"/>
+      <c r="A89" s="110"/>
       <c r="B89" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="114"/>
+      <c r="A90" s="111"/>
       <c r="B90" s="82" t="s">
         <v>547</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="112" t="s">
+      <c r="A91" s="109" t="s">
         <v>309</v>
       </c>
       <c r="B91" s="84" t="s">
@@ -10976,7 +10976,7 @@
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="114"/>
+      <c r="A92" s="111"/>
       <c r="B92" s="84" t="s">
         <v>311</v>
       </c>
@@ -11037,17 +11037,17 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="104" t="s">
+      <c r="A99" s="106" t="s">
         <v>388</v>
       </c>
-      <c r="B99" s="104"/>
+      <c r="B99" s="106"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="105" t="s">
+      <c r="A100" s="107" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="106"/>
+      <c r="B100" s="105"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -11078,10 +11078,10 @@
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A104" s="105" t="s">
+      <c r="A104" s="107" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="106"/>
+      <c r="B104" s="105"/>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -11229,10 +11229,10 @@
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A121" s="105" t="s">
+      <c r="A121" s="107" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="106"/>
+      <c r="B121" s="105"/>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -11317,10 +11317,10 @@
       <c r="C130"/>
     </row>
     <row r="131" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A131" s="105" t="s">
+      <c r="A131" s="107" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="106"/>
+      <c r="B131" s="105"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11414,10 +11414,10 @@
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="107" t="s">
+      <c r="A142" s="104" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="106"/>
+      <c r="B142" s="105"/>
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -11448,10 +11448,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="107" t="s">
+      <c r="A146" s="104" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="106"/>
+      <c r="B146" s="105"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11473,10 +11473,10 @@
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="107" t="s">
+      <c r="A149" s="104" t="s">
         <v>542</v>
       </c>
-      <c r="B149" s="106"/>
+      <c r="B149" s="105"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -11509,17 +11509,17 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="104" t="s">
+      <c r="A153" s="106" t="s">
         <v>472</v>
       </c>
-      <c r="B153" s="104"/>
+      <c r="B153" s="106"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="105" t="s">
+      <c r="A154" s="107" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="106"/>
+      <c r="B154" s="105"/>
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -11555,10 +11555,10 @@
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="107" t="s">
+      <c r="A160" s="104" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="118"/>
+      <c r="B160" s="108"/>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -11625,10 +11625,10 @@
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="105" t="s">
+      <c r="A168" s="107" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="106"/>
+      <c r="B168" s="105"/>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -11650,10 +11650,10 @@
       <c r="C170"/>
     </row>
     <row r="171" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A171" s="105" t="s">
+      <c r="A171" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="106"/>
+      <c r="B171" s="105"/>
       <c r="C171"/>
     </row>
     <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -11675,17 +11675,17 @@
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A174" s="104" t="s">
+      <c r="A174" s="106" t="s">
         <v>553</v>
       </c>
-      <c r="B174" s="104"/>
+      <c r="B174" s="106"/>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="105" t="s">
+      <c r="A175" s="107" t="s">
         <v>554</v>
       </c>
-      <c r="B175" s="106"/>
+      <c r="B175" s="105"/>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11701,10 +11701,10 @@
       <c r="B177" s="76"/>
     </row>
     <row r="178" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A178" s="105" t="s">
+      <c r="A178" s="107" t="s">
         <v>553</v>
       </c>
-      <c r="B178" s="106"/>
+      <c r="B178" s="105"/>
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11785,10 +11785,10 @@
       <c r="B187" s="76"/>
     </row>
     <row r="188" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A188" s="105" t="s">
+      <c r="A188" s="107" t="s">
         <v>576</v>
       </c>
-      <c r="B188" s="106"/>
+      <c r="B188" s="105"/>
       <c r="C188"/>
     </row>
     <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11806,10 +11806,10 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="107" t="s">
+      <c r="A191" s="104" t="s">
         <v>580</v>
       </c>
-      <c r="B191" s="106"/>
+      <c r="B191" s="105"/>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
@@ -11844,17 +11844,17 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A196" s="104" t="s">
+      <c r="A196" s="106" t="s">
         <v>601</v>
       </c>
-      <c r="B196" s="104"/>
+      <c r="B196" s="106"/>
       <c r="C196"/>
     </row>
     <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="107" t="s">
+      <c r="A197" s="104" t="s">
         <v>603</v>
       </c>
-      <c r="B197" s="106"/>
+      <c r="B197" s="105"/>
     </row>
     <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A198" s="57" t="s">
@@ -11901,10 +11901,10 @@
       <c r="B203" s="100"/>
     </row>
     <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="107" t="s">
+      <c r="A204" s="104" t="s">
         <v>614</v>
       </c>
-      <c r="B204" s="106"/>
+      <c r="B204" s="105"/>
     </row>
     <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="57" t="s">
@@ -11943,10 +11943,10 @@
       <c r="B212" s="76"/>
     </row>
     <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="107" t="s">
+      <c r="A213" s="104" t="s">
         <v>616</v>
       </c>
-      <c r="B213" s="106"/>
+      <c r="B213" s="105"/>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="72" t="s">
@@ -11957,10 +11957,10 @@
       </c>
     </row>
     <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="107" t="s">
+      <c r="A215" s="104" t="s">
         <v>620</v>
       </c>
-      <c r="B215" s="106"/>
+      <c r="B215" s="105"/>
     </row>
     <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="57" t="s">
@@ -11979,10 +11979,10 @@
       </c>
     </row>
     <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="107" t="s">
+      <c r="A218" s="104" t="s">
         <v>619</v>
       </c>
-      <c r="B218" s="106"/>
+      <c r="B218" s="105"/>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A219" s="57" t="s">
@@ -12017,22 +12017,22 @@
       </c>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="104" t="s">
+      <c r="A223" s="106" t="s">
         <v>635</v>
       </c>
-      <c r="B223" s="104"/>
+      <c r="B223" s="106"/>
     </row>
     <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A224" s="107" t="s">
+      <c r="A224" s="104" t="s">
         <v>637</v>
       </c>
-      <c r="B224" s="106"/>
+      <c r="B224" s="105"/>
     </row>
     <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A225" s="107" t="s">
+      <c r="A225" s="104" t="s">
         <v>636</v>
       </c>
-      <c r="B225" s="106"/>
+      <c r="B225" s="105"/>
     </row>
     <row r="226" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A226" s="57" t="s">
@@ -12043,10 +12043,10 @@
       </c>
     </row>
     <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A227" s="107" t="s">
+      <c r="A227" s="104" t="s">
         <v>640</v>
       </c>
-      <c r="B227" s="106"/>
+      <c r="B227" s="105"/>
     </row>
     <row r="228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="57" t="s">
@@ -12089,10 +12089,10 @@
       </c>
     </row>
     <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A233" s="107" t="s">
+      <c r="A233" s="104" t="s">
         <v>650</v>
       </c>
-      <c r="B233" s="106"/>
+      <c r="B233" s="105"/>
     </row>
     <row r="234" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="57" t="s">
@@ -12103,10 +12103,10 @@
       </c>
     </row>
     <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="107" t="s">
+      <c r="A235" s="104" t="s">
         <v>653</v>
       </c>
-      <c r="B235" s="106"/>
+      <c r="B235" s="105"/>
     </row>
     <row r="236" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A236" s="57" t="s">
@@ -12123,10 +12123,10 @@
       </c>
     </row>
     <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A238" s="107" t="s">
+      <c r="A238" s="104" t="s">
         <v>657</v>
       </c>
-      <c r="B238" s="106"/>
+      <c r="B238" s="105"/>
     </row>
     <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="57" t="s">
@@ -12273,10 +12273,10 @@
       </c>
     </row>
     <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A257" s="107" t="s">
+      <c r="A257" s="104" t="s">
         <v>694</v>
       </c>
-      <c r="B257" s="106"/>
+      <c r="B257" s="105"/>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="57" t="s">
@@ -12452,39 +12452,12 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="A257:B257"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A225:B225"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A233:B233"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A75:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A191:B191"/>
     <mergeCell ref="A149:B149"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
@@ -12501,12 +12474,39 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A75:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A225:B225"/>
+    <mergeCell ref="A227:B227"/>
+    <mergeCell ref="A233:B233"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DB - Exercises 04.01.2019
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" activeTab="1"/>
@@ -30,7 +30,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="704">
   <si>
     <t>Операция</t>
   </si>
@@ -4793,65 +4793,6 @@
 int, called @ClientID and return a DECIMAL. It could look like this:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CREATE FUNCTION f_CalculateTotalBalance (@ClientID INT)
-RETURNS DECIMAL(15, 2)
-BEGIN
-     DECLARE @result AS DECIMAL(15, 2) = (
-     SELECT SUM(Balance)
-     FROM Accounts WHERE ClientId = @ClientID
-     )
-     RETURN @result
-END</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Now try and select the function, giving it an existing client ID as the parameter, example for client ID -&gt; 4: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">SELECT dbo.f_CalculateTotalBalance(4) AS Balance </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Notice the dbo. before the function name – this is the name of the schema which we must type when callingfunctions.</t>
-    </r>
-  </si>
-  <si>
     <t>Create Procedures</t>
   </si>
   <si>
@@ -6447,25 +6388,113 @@
   <si>
     <t xml:space="preserve">Error Handling - EXAMPLE </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CREATE FUNCTION f_CalculateTotalBalance (@ClientID INT)
+RETURNS DECIMAL(15, 2)
+BEGIN
+     DECLARE @result AS DECIMAL(15, 2) = (
+     SELECT SUM(Balance)
+     FROM Accounts WHERE ClientId = @ClientID
+     )
+     RETURN @result
+END</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Now try and select the function, giving it an existing client ID as the parameter, example for client ID -&gt; 4: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SELECT dbo.f_CalculateTotalBalance(4) AS Balance </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Notice the dbo. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>before the function name – this is the name of the schema which we must type when callingfunctions.</t>
+    </r>
+  </si>
+  <si>
+    <t>LOOPS</t>
+  </si>
+  <si>
+    <t>WHILE LOOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECLARE @Count INT =  0
+WHILE(@Count &lt; 5)
+BEGIN
+ SET @Count += 1
+ SELECT @Count
+END </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="52" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -7225,42 +7254,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7275,91 +7304,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7374,73 +7403,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7449,43 +7478,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7494,13 +7520,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7515,65 +7541,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7668,7 +7697,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -7676,17 +7705,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -7740,7 +7758,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7775,7 +7793,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10307,8 +10325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C248" sqref="C248"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B262" sqref="B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10327,16 +10345,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="105" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="116"/>
+      <c r="B2" s="115"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="117" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="117"/>
+      <c r="B3" s="116"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -10363,54 +10381,54 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="116" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="114"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
         <v>518</v>
       </c>
-      <c r="B8" s="89" t="s">
-        <v>519</v>
+      <c r="B8" s="122" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
+        <v>522</v>
+      </c>
+      <c r="B9" s="93" t="s">
         <v>523</v>
-      </c>
-      <c r="B9" s="94" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
+        <v>524</v>
+      </c>
+      <c r="B10" s="122" t="s">
         <v>525</v>
       </c>
-      <c r="B10" s="89" t="s">
-        <v>526</v>
-      </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="117" t="s">
-        <v>520</v>
-      </c>
-      <c r="B11" s="115"/>
+      <c r="A11" s="116" t="s">
+        <v>519</v>
+      </c>
+      <c r="B11" s="114"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
+        <v>520</v>
+      </c>
+      <c r="B12" s="89" t="s">
         <v>521</v>
       </c>
-      <c r="B12" s="90" t="s">
-        <v>522</v>
-      </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="116" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="117"/>
+      <c r="B13" s="116"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -10462,17 +10480,17 @@
     </row>
     <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="117" t="s">
+      <c r="A21" s="116" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="117"/>
+      <c r="B21" s="116"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -10483,10 +10501,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="116" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="117"/>
+      <c r="B23" s="116"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -10497,10 +10515,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="116" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="117"/>
+      <c r="B25" s="116"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -10527,10 +10545,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="116" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="117"/>
+      <c r="B29" s="116"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -10557,10 +10575,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="115" t="s">
+      <c r="A33" s="114" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="115"/>
+      <c r="B33" s="114"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -10583,14 +10601,14 @@
         <v>379</v>
       </c>
       <c r="B36" s="74" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="117" t="s">
+      <c r="A37" s="116" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="117"/>
+      <c r="B37" s="116"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -10617,17 +10635,17 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="115" t="s">
+      <c r="A41" s="114" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="115"/>
+      <c r="B41" s="114"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
         <v>376</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
@@ -10639,10 +10657,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="117" t="s">
+      <c r="A44" s="116" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="115"/>
+      <c r="B44" s="114"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -10669,19 +10687,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="106" t="s">
+      <c r="A48" s="105" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="106"/>
+      <c r="B48" s="105"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="107" t="s">
+      <c r="A49" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="105"/>
+      <c r="B49" s="104"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="112" t="s">
+      <c r="A50" s="111" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10689,22 +10707,22 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="113"/>
+      <c r="A51" s="112"/>
       <c r="B51" s="62" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C51" s="66" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="114"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="112" t="s">
+      <c r="A53" s="111" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -10712,25 +10730,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="113"/>
+      <c r="A54" s="112"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="113"/>
+      <c r="A55" s="112"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="114"/>
+      <c r="A56" s="113"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="112" t="s">
+      <c r="A57" s="111" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -10738,13 +10756,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="114"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="112" t="s">
+      <c r="A59" s="111" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -10755,33 +10773,33 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="113"/>
+      <c r="A60" s="112"/>
       <c r="B60" s="62" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C60" s="68" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="113"/>
+      <c r="A61" s="112"/>
       <c r="B61" s="62" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="114"/>
+      <c r="A62" s="113"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="103" t="s">
-        <v>633</v>
+      <c r="A63" s="102" t="s">
+        <v>632</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -10802,18 +10820,18 @@
     </row>
     <row r="66" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A66" s="57" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B66" s="62" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A67" s="57" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -10825,7 +10843,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="109" t="s">
+      <c r="A69" s="108" t="s">
         <v>290</v>
       </c>
       <c r="B69" s="62" t="s">
@@ -10833,37 +10851,37 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="110"/>
+      <c r="A70" s="109"/>
       <c r="B70" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="110"/>
+      <c r="A71" s="109"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="110"/>
+      <c r="A72" s="109"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="110"/>
+      <c r="A73" s="109"/>
       <c r="B73" s="62" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
+      <c r="A74" s="110"/>
       <c r="B74" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="109" t="s">
+      <c r="A75" s="108" t="s">
         <v>291</v>
       </c>
       <c r="B75" s="62" t="s">
@@ -10871,74 +10889,74 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="110"/>
+      <c r="A76" s="109"/>
       <c r="B76" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C76" s="67"/>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="110"/>
+      <c r="A77" s="109"/>
       <c r="B77" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="110"/>
+      <c r="A78" s="109"/>
       <c r="B78" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="110"/>
+      <c r="A79" s="109"/>
       <c r="B79" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="110"/>
+      <c r="A80" s="109"/>
       <c r="B80" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="110"/>
+      <c r="A81" s="109"/>
       <c r="B81" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="110"/>
+      <c r="A82" s="109"/>
       <c r="B82" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="110"/>
+      <c r="A83" s="109"/>
       <c r="B83" s="81" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="110"/>
+      <c r="A84" s="109"/>
       <c r="B84" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="110"/>
+      <c r="A85" s="109"/>
       <c r="B85" s="81" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="111"/>
+      <c r="A86" s="110"/>
       <c r="B86" s="81" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="109" t="s">
+      <c r="A87" s="108" t="s">
         <v>292</v>
       </c>
       <c r="B87" s="82" t="s">
@@ -10946,28 +10964,28 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="110"/>
+      <c r="A88" s="109"/>
       <c r="B88" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="110"/>
+      <c r="A89" s="109"/>
       <c r="B89" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="111"/>
+      <c r="A90" s="110"/>
       <c r="B90" s="82" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="109" t="s">
+      <c r="A91" s="108" t="s">
         <v>309</v>
       </c>
       <c r="B91" s="84" t="s">
@@ -10976,7 +10994,7 @@
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="111"/>
+      <c r="A92" s="110"/>
       <c r="B92" s="84" t="s">
         <v>311</v>
       </c>
@@ -11014,16 +11032,16 @@
         <v>373</v>
       </c>
       <c r="B96" s="84" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C96"/>
     </row>
     <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="91" t="s">
-        <v>529</v>
+      <c r="A97" s="90" t="s">
+        <v>528</v>
       </c>
       <c r="B97" s="81" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C97"/>
     </row>
@@ -11037,17 +11055,17 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="106" t="s">
+      <c r="A99" s="105" t="s">
         <v>388</v>
       </c>
-      <c r="B99" s="106"/>
+      <c r="B99" s="105"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="107" t="s">
+      <c r="A100" s="106" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="105"/>
+      <c r="B100" s="104"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -11078,10 +11096,10 @@
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A104" s="107" t="s">
+      <c r="A104" s="106" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="105"/>
+      <c r="B104" s="104"/>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -11220,19 +11238,19 @@
       <c r="C119"/>
     </row>
     <row r="120" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="93" t="s">
+      <c r="A120" s="92" t="s">
+        <v>535</v>
+      </c>
+      <c r="B120" s="91" t="s">
         <v>536</v>
       </c>
-      <c r="B120" s="92" t="s">
-        <v>537</v>
-      </c>
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A121" s="107" t="s">
+      <c r="A121" s="106" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="105"/>
+      <c r="B121" s="104"/>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -11317,10 +11335,10 @@
       <c r="C130"/>
     </row>
     <row r="131" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A131" s="107" t="s">
+      <c r="A131" s="106" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="105"/>
+      <c r="B131" s="104"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11381,7 +11399,7 @@
       <c r="A138" s="78" t="s">
         <v>457</v>
       </c>
-      <c r="B138" s="98" t="s">
+      <c r="B138" s="97" t="s">
         <v>458</v>
       </c>
       <c r="C138"/>
@@ -11390,8 +11408,8 @@
       <c r="A139" s="78" t="s">
         <v>459</v>
       </c>
-      <c r="B139" s="98" t="s">
-        <v>552</v>
+      <c r="B139" s="97" t="s">
+        <v>551</v>
       </c>
       <c r="C139"/>
     </row>
@@ -11399,8 +11417,8 @@
       <c r="A140" s="78" t="s">
         <v>460</v>
       </c>
-      <c r="B140" s="98" t="s">
-        <v>551</v>
+      <c r="B140" s="97" t="s">
+        <v>550</v>
       </c>
       <c r="C140"/>
     </row>
@@ -11408,16 +11426,16 @@
       <c r="A141" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="B141" s="98" t="s">
-        <v>550</v>
+      <c r="B141" s="97" t="s">
+        <v>549</v>
       </c>
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="104" t="s">
+      <c r="A142" s="103" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="105"/>
+      <c r="B142" s="104"/>
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -11448,10 +11466,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="104" t="s">
+      <c r="A146" s="103" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="105"/>
+      <c r="B146" s="104"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11465,78 +11483,78 @@
     </row>
     <row r="148" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A148" s="57" t="s">
+        <v>539</v>
+      </c>
+      <c r="B148" s="87" t="s">
         <v>540</v>
       </c>
-      <c r="B148" s="87" t="s">
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="103" t="s">
         <v>541</v>
       </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="104" t="s">
-        <v>542</v>
-      </c>
-      <c r="B149" s="105"/>
+      <c r="B149" s="104"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A150" s="57" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B150" s="80" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" s="57" t="s">
+        <v>543</v>
+      </c>
+      <c r="B151" s="76" t="s">
         <v>544</v>
-      </c>
-      <c r="B151" s="76" t="s">
-        <v>545</v>
       </c>
       <c r="C151"/>
     </row>
     <row r="152" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A152" s="57" t="s">
-        <v>598</v>
-      </c>
-      <c r="B152" s="99" t="s">
         <v>597</v>
       </c>
+      <c r="B152" s="98" t="s">
+        <v>596</v>
+      </c>
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="106" t="s">
+      <c r="A153" s="105" t="s">
         <v>472</v>
       </c>
-      <c r="B153" s="106"/>
+      <c r="B153" s="105"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="107" t="s">
+      <c r="A154" s="106" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="105"/>
+      <c r="B154" s="104"/>
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A155" s="57" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B155" s="76" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C155"/>
     </row>
     <row r="156" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
       <c r="A156" s="57" t="s">
+        <v>529</v>
+      </c>
+      <c r="B156" s="80" t="s">
         <v>530</v>
-      </c>
-      <c r="B156" s="80" t="s">
-        <v>531</v>
       </c>
       <c r="C156"/>
     </row>
@@ -11555,10 +11573,10 @@
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="104" t="s">
+      <c r="A160" s="103" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="108"/>
+      <c r="B160" s="107"/>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -11625,10 +11643,10 @@
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="107" t="s">
+      <c r="A168" s="106" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="105"/>
+      <c r="B168" s="104"/>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -11650,10 +11668,10 @@
       <c r="C170"/>
     </row>
     <row r="171" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A171" s="107" t="s">
+      <c r="A171" s="106" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="105"/>
+      <c r="B171" s="104"/>
       <c r="C171"/>
     </row>
     <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -11675,25 +11693,25 @@
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A174" s="106" t="s">
+      <c r="A174" s="105" t="s">
+        <v>552</v>
+      </c>
+      <c r="B174" s="105"/>
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A175" s="106" t="s">
         <v>553</v>
       </c>
-      <c r="B174" s="106"/>
-      <c r="C174"/>
-    </row>
-    <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="107" t="s">
-        <v>554</v>
-      </c>
-      <c r="B175" s="105"/>
+      <c r="B175" s="104"/>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A176" s="57" t="s">
+        <v>554</v>
+      </c>
+      <c r="B176" s="76" t="s">
         <v>555</v>
-      </c>
-      <c r="B176" s="76" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -11701,83 +11719,83 @@
       <c r="B177" s="76"/>
     </row>
     <row r="178" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A178" s="107" t="s">
-        <v>553</v>
-      </c>
-      <c r="B178" s="105"/>
+      <c r="A178" s="106" t="s">
+        <v>552</v>
+      </c>
+      <c r="B178" s="104"/>
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A179" s="57" t="s">
+        <v>556</v>
+      </c>
+      <c r="B179" s="76" t="s">
         <v>557</v>
-      </c>
-      <c r="B179" s="76" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A180" s="57" t="s">
+        <v>558</v>
+      </c>
+      <c r="B180" s="76" t="s">
         <v>559</v>
-      </c>
-      <c r="B180" s="76" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="57" t="s">
+        <v>560</v>
+      </c>
+      <c r="B181" s="76" t="s">
         <v>561</v>
-      </c>
-      <c r="B181" s="76" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="57" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B182" s="76" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="57" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B183" s="76" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A184" s="57" t="s">
+        <v>566</v>
+      </c>
+      <c r="B184" s="80" t="s">
         <v>567</v>
       </c>
-      <c r="B184" s="80" t="s">
-        <v>568</v>
-      </c>
-      <c r="C184" s="96" t="s">
-        <v>574</v>
+      <c r="C184" s="95" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
       <c r="A185" s="57" t="s">
+        <v>568</v>
+      </c>
+      <c r="B185" s="80" t="s">
         <v>569</v>
       </c>
-      <c r="B185" s="80" t="s">
-        <v>570</v>
-      </c>
-      <c r="C185" s="96" t="s">
-        <v>573</v>
+      <c r="C185" s="95" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A186" s="57" t="s">
+        <v>570</v>
+      </c>
+      <c r="B186" s="76" t="s">
         <v>571</v>
       </c>
-      <c r="B186" s="76" t="s">
-        <v>572</v>
-      </c>
-      <c r="C186" s="95" t="s">
-        <v>575</v>
+      <c r="C186" s="94" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -11785,133 +11803,133 @@
       <c r="B187" s="76"/>
     </row>
     <row r="188" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A188" s="107" t="s">
-        <v>576</v>
-      </c>
-      <c r="B188" s="105"/>
+      <c r="A188" s="106" t="s">
+        <v>575</v>
+      </c>
+      <c r="B188" s="104"/>
       <c r="C188"/>
     </row>
     <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A189" s="57" t="s">
+        <v>576</v>
+      </c>
+      <c r="B189" s="76" t="s">
         <v>577</v>
-      </c>
-      <c r="B189" s="76" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A190" s="57"/>
       <c r="B190" s="76" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A191" s="103" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="104" t="s">
-        <v>580</v>
-      </c>
-      <c r="B191" s="105"/>
+      <c r="B191" s="104"/>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B192" s="76" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A193" s="57" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B193" s="76" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A194" s="57" t="s">
-        <v>587</v>
-      </c>
-      <c r="B194" s="97" t="s">
         <v>586</v>
+      </c>
+      <c r="B194" s="96" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A195" s="57" t="s">
-        <v>585</v>
-      </c>
-      <c r="B195" s="97" t="s">
         <v>584</v>
       </c>
+      <c r="B195" s="96" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A196" s="106" t="s">
-        <v>601</v>
-      </c>
-      <c r="B196" s="106"/>
+      <c r="A196" s="105" t="s">
+        <v>600</v>
+      </c>
+      <c r="B196" s="105"/>
       <c r="C196"/>
     </row>
     <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="104" t="s">
-        <v>603</v>
-      </c>
-      <c r="B197" s="105"/>
+      <c r="A197" s="103" t="s">
+        <v>602</v>
+      </c>
+      <c r="B197" s="104"/>
     </row>
     <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A198" s="57" t="s">
+        <v>603</v>
+      </c>
+      <c r="B198" s="100" t="s">
         <v>604</v>
-      </c>
-      <c r="B198" s="101" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A199" s="57" t="s">
-        <v>606</v>
-      </c>
-      <c r="B199" s="101" t="s">
-        <v>608</v>
+        <v>605</v>
+      </c>
+      <c r="B199" s="100" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A200" s="57" t="s">
-        <v>607</v>
-      </c>
-      <c r="B200" s="101" t="s">
-        <v>609</v>
+        <v>606</v>
+      </c>
+      <c r="B200" s="100" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A201" s="57" t="s">
-        <v>611</v>
-      </c>
-      <c r="B201" s="102" t="s">
         <v>610</v>
+      </c>
+      <c r="B201" s="101" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="57" t="s">
-        <v>613</v>
-      </c>
-      <c r="B202" s="101" t="s">
         <v>612</v>
+      </c>
+      <c r="B202" s="100" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A203" s="57"/>
-      <c r="B203" s="100"/>
+      <c r="B203" s="99"/>
     </row>
     <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="104" t="s">
-        <v>614</v>
-      </c>
-      <c r="B204" s="105"/>
+      <c r="A204" s="103" t="s">
+        <v>613</v>
+      </c>
+      <c r="B204" s="104"/>
     </row>
     <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="57" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B205" s="76" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -11943,372 +11961,378 @@
       <c r="B212" s="76"/>
     </row>
     <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="104" t="s">
-        <v>616</v>
-      </c>
-      <c r="B213" s="105"/>
+      <c r="A213" s="103" t="s">
+        <v>615</v>
+      </c>
+      <c r="B213" s="104"/>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="72" t="s">
+        <v>616</v>
+      </c>
+      <c r="B214" s="76" t="s">
         <v>617</v>
       </c>
-      <c r="B214" s="76" t="s">
-        <v>618</v>
-      </c>
     </row>
     <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="104" t="s">
-        <v>620</v>
-      </c>
-      <c r="B215" s="105"/>
+      <c r="A215" s="103" t="s">
+        <v>619</v>
+      </c>
+      <c r="B215" s="104"/>
     </row>
     <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="57" t="s">
+        <v>620</v>
+      </c>
+      <c r="B216" s="76" t="s">
         <v>621</v>
-      </c>
-      <c r="B216" s="76" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A217" s="57" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B217" s="76" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="104" t="s">
-        <v>619</v>
-      </c>
-      <c r="B218" s="105"/>
+      <c r="A218" s="103" t="s">
+        <v>618</v>
+      </c>
+      <c r="B218" s="104"/>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A219" s="57" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B219" s="80" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A220" s="57" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B220" s="76" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A221" s="57" t="s">
+        <v>625</v>
+      </c>
+      <c r="B221" s="76" t="s">
         <v>626</v>
-      </c>
-      <c r="B221" s="76" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="57" t="s">
+        <v>629</v>
+      </c>
+      <c r="B222" s="76" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="76" t="s">
-        <v>631</v>
-      </c>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="106" t="s">
+      <c r="A223" s="105" t="s">
+        <v>634</v>
+      </c>
+      <c r="B223" s="105"/>
+    </row>
+    <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A224" s="103" t="s">
+        <v>636</v>
+      </c>
+      <c r="B224" s="104"/>
+    </row>
+    <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A225" s="103" t="s">
         <v>635</v>
       </c>
-      <c r="B223" s="106"/>
-    </row>
-    <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A224" s="104" t="s">
-        <v>637</v>
-      </c>
-      <c r="B224" s="105"/>
-    </row>
-    <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A225" s="104" t="s">
-        <v>636</v>
-      </c>
-      <c r="B225" s="105"/>
+      <c r="B225" s="104"/>
     </row>
     <row r="226" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A226" s="57" t="s">
+        <v>637</v>
+      </c>
+      <c r="B226" s="76" t="s">
         <v>638</v>
       </c>
-      <c r="B226" s="76" t="s">
+    </row>
+    <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A227" s="103" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A227" s="104" t="s">
-        <v>640</v>
-      </c>
-      <c r="B227" s="105"/>
+      <c r="B227" s="104"/>
     </row>
     <row r="228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="57" t="s">
         <v>394</v>
       </c>
       <c r="B228" s="76" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A229" s="57" t="s">
+        <v>641</v>
+      </c>
+      <c r="B229" s="76" t="s">
         <v>642</v>
-      </c>
-      <c r="B229" s="76" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A230" s="57" t="s">
+        <v>643</v>
+      </c>
+      <c r="B230" s="76" t="s">
         <v>644</v>
-      </c>
-      <c r="B230" s="76" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="57" t="s">
+        <v>645</v>
+      </c>
+      <c r="B231" s="76" t="s">
         <v>646</v>
-      </c>
-      <c r="B231" s="76" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A232" s="57" t="s">
+        <v>647</v>
+      </c>
+      <c r="B232" s="76" t="s">
         <v>648</v>
       </c>
-      <c r="B232" s="76" t="s">
+    </row>
+    <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A233" s="103" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A233" s="104" t="s">
-        <v>650</v>
-      </c>
-      <c r="B233" s="105"/>
+      <c r="B233" s="104"/>
     </row>
     <row r="234" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="57" t="s">
+        <v>650</v>
+      </c>
+      <c r="B234" s="76" t="s">
         <v>651</v>
       </c>
-      <c r="B234" s="76" t="s">
+    </row>
+    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A235" s="103" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="104" t="s">
-        <v>653</v>
-      </c>
-      <c r="B235" s="105"/>
+      <c r="B235" s="104"/>
     </row>
     <row r="236" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A236" s="57" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B236" s="76"/>
     </row>
     <row r="237" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A237" s="57" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B237" s="76" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A238" s="103" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A238" s="104" t="s">
-        <v>657</v>
-      </c>
-      <c r="B238" s="105"/>
+      <c r="B238" s="104"/>
     </row>
     <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="57" t="s">
+        <v>657</v>
+      </c>
+      <c r="B239" s="76" t="s">
         <v>658</v>
-      </c>
-      <c r="B239" s="76" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A240" s="57" t="s">
+        <v>659</v>
+      </c>
+      <c r="B240" s="76" t="s">
         <v>660</v>
-      </c>
-      <c r="B240" s="76" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="57" t="s">
+        <v>661</v>
+      </c>
+      <c r="B241" s="76" t="s">
         <v>662</v>
-      </c>
-      <c r="B241" s="76" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A242" s="57" t="s">
+        <v>663</v>
+      </c>
+      <c r="B242" s="76" t="s">
         <v>664</v>
-      </c>
-      <c r="B242" s="76" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A243" s="57" t="s">
+        <v>665</v>
+      </c>
+      <c r="B243" s="76" t="s">
         <v>666</v>
-      </c>
-      <c r="B243" s="76" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="57" t="s">
+        <v>667</v>
+      </c>
+      <c r="B244" s="76" t="s">
         <v>668</v>
-      </c>
-      <c r="B244" s="76" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A245" s="57" t="s">
+        <v>669</v>
+      </c>
+      <c r="B245" s="76" t="s">
         <v>670</v>
-      </c>
-      <c r="B245" s="76" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A246" s="57" t="s">
+        <v>671</v>
+      </c>
+      <c r="B246" s="76" t="s">
         <v>672</v>
-      </c>
-      <c r="B246" s="76" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A247" s="57" t="s">
+        <v>673</v>
+      </c>
+      <c r="B247" s="76" t="s">
         <v>674</v>
-      </c>
-      <c r="B247" s="76" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A248" s="57" t="s">
+        <v>675</v>
+      </c>
+      <c r="B248" s="76" t="s">
         <v>676</v>
-      </c>
-      <c r="B248" s="76" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A249" s="57" t="s">
+        <v>677</v>
+      </c>
+      <c r="B249" s="76" t="s">
         <v>678</v>
-      </c>
-      <c r="B249" s="76" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A250" s="57" t="s">
+        <v>679</v>
+      </c>
+      <c r="B250" s="76" t="s">
         <v>680</v>
-      </c>
-      <c r="B250" s="76" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" s="57" t="s">
+        <v>681</v>
+      </c>
+      <c r="B251" s="76" t="s">
         <v>682</v>
-      </c>
-      <c r="B251" s="76" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A252" s="57" t="s">
+        <v>683</v>
+      </c>
+      <c r="B252" s="76" t="s">
         <v>684</v>
-      </c>
-      <c r="B252" s="76" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A253" s="57" t="s">
+        <v>685</v>
+      </c>
+      <c r="B253" s="76" t="s">
         <v>686</v>
-      </c>
-      <c r="B253" s="76" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="57" t="s">
+        <v>687</v>
+      </c>
+      <c r="B254" s="76" t="s">
         <v>688</v>
-      </c>
-      <c r="B254" s="76" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A255" s="57" t="s">
+        <v>689</v>
+      </c>
+      <c r="B255" s="76" t="s">
         <v>690</v>
-      </c>
-      <c r="B255" s="76" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A256" s="57" t="s">
+        <v>691</v>
+      </c>
+      <c r="B256" s="76" t="s">
         <v>692</v>
       </c>
-      <c r="B256" s="76" t="s">
+    </row>
+    <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A257" s="103" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A257" s="104" t="s">
-        <v>694</v>
-      </c>
-      <c r="B257" s="105"/>
+      <c r="B257" s="104"/>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="57" t="s">
+        <v>694</v>
+      </c>
+      <c r="B258" s="76" t="s">
         <v>695</v>
-      </c>
-      <c r="B258" s="76" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="57" t="s">
+        <v>696</v>
+      </c>
+      <c r="B259" s="76" t="s">
         <v>697</v>
-      </c>
-      <c r="B259" s="76" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A260" s="57" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B260" s="76" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A261" s="57"/>
-      <c r="B261" s="76"/>
-    </row>
-    <row r="262" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A262" s="57"/>
-      <c r="B262" s="76"/>
+        <v>698</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A261" s="103" t="s">
+        <v>701</v>
+      </c>
+      <c r="B261" s="104"/>
+    </row>
+    <row r="262" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A262" s="57" t="s">
+        <v>702</v>
+      </c>
+      <c r="B262" s="76" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="263" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A263" s="57"/>
@@ -12451,7 +12475,8 @@
       <c r="B297" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="56">
+    <mergeCell ref="A261:B261"/>
     <mergeCell ref="A174:B174"/>
     <mergeCell ref="A175:B175"/>
     <mergeCell ref="A178:B178"/>
@@ -12928,7 +12953,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="118" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -12948,7 +12973,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120"/>
+      <c r="A2" s="119"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -13016,10 +13041,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="120" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="122"/>
+      <c r="C6" s="121"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - 06.09.2019 - Triggers and Transactions
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" activeTab="1"/>
@@ -30,7 +30,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="742">
   <si>
     <t>Операция</t>
   </si>
@@ -6484,17 +6484,840 @@
  SELECT @Count
 END </t>
   </si>
+  <si>
+    <t>Triggers and Transactions</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>Triggers</t>
+  </si>
+  <si>
+    <t>A Transaction is a sequence of actions (database operations) executed as a whole:
+Either all of them complete successfully or none of them do
+Examples:
+A bank transfer from one account into another (withdrawal + deposit)
+If either the withdrawal or the deposit fails the whole operation is cancelled</t>
+  </si>
+  <si>
+    <t>Transactions Behavior</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transactions guarantee the consistency and the integrity of the database:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt; All changes in a transaction are temporary
+&gt; Changes are persisted when a COMMIT is executed
+&gt; At any time, all changes can be canceled by ROLLBACK
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All changes are persisted at once</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt; As long as COMMIT is called</t>
+    </r>
+  </si>
+  <si>
+    <t>Transactions: What Can Go Wrong?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Some actions fail to complete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt; The application software or database server crashes
+&gt; The user cancels the action while it’s in progress
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Interference from another transaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt; What happens if several transfers run for the same account at the same time?</t>
+    </r>
+  </si>
+  <si>
+    <t>Transactions Syntax</t>
+  </si>
+  <si>
+    <t>CREATE PROC usp_Withdraw @withdrawAmount DECIMAL(18,2), @accountId INT
+AS
+BEGIN TRANSACTION
+UPDATE Accounts SET Balance = Balance - @withdrawAmount
+WHERE Id = @accountId
+IF @@ROWCOUNT &lt;&gt; 1 -- Didn’t affect exactly one row
+BEGIN
+ROLLBACK
+RAISERROR('Invalid account!', 16, 1)
+RETURN
+END
+COMMIT</t>
+  </si>
+  <si>
+    <t>ACID Model : Atomicity, Consistency, Isolation, Durability</t>
+  </si>
+  <si>
+    <t>Atomicity means that:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transactions execute as a whole</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+DBMS/DataBase Management System/ guarantees that either all of the operations are performed or none of them
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Example: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transferring funds between bank accounts
+Either withdraw + deposit both succeed, or none of them do
+In case of failure, the database stays unchanged</t>
+    </r>
+  </si>
+  <si>
+    <t>Consistency</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Consistency means that:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The database has a legal state in both the transaction’s beginning and its end
+Only valid data will be written to the DB
+Transaction cannot break the rules of the database - Primary keys, foreign keys, check constraints…
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Consistency example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Transaction cannot end with a duplicate primary key in a table</t>
+    </r>
+  </si>
+  <si>
+    <t>Isolation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Isolation means that:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Multiple transactions running at the same time do not impact each other’s execution
+Transactions don’t see other transactions’ uncommitted changes
+Isolation level defines how deep transactions isolate from one another
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Isolation example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If two or more people try to buy the last copy of a product, only one of them will succeed</t>
+    </r>
+  </si>
+  <si>
+    <t>Durability</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Durability means that:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If a transaction is committed it becomes persistent - Cannot be lost or undone
+Ensured by the use of database transaction logs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Durability example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After funds are transferred and committed, the power supply at the DB server is lost
+Transaction stays persistent (no data is lost)</t>
+    </r>
+  </si>
+  <si>
+    <t>What Are Triggers?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Triggers are very much like stored procedures -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Called in case of a specific event
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">We do not call triggers explicitly 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; Triggers are attached to a table
+&gt; Triggers are fired when a certain SQL statement is executed against the contents of the table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Syntax:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+AFTER INSERT/UPDATE/DELETE
+INSTEAD OF INSERT/UPDATE/DELETE</t>
+    </r>
+  </si>
+  <si>
+    <t>After Trigger</t>
+  </si>
+  <si>
+    <t>AFTER Trigger is executed right after an event is fired</t>
+  </si>
+  <si>
+    <t>Instead of Trigger</t>
+  </si>
+  <si>
+    <t>INSTEAD OF Trigger completely replaces an event action from happening
+&gt; You can apply totally different logic</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There are three different events that can be applied within a trigger: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Insert, Update, Delete</t>
+    </r>
+  </si>
+  <si>
+    <t>After Triggers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Defined by the keyword FOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CREATE TRIGGER tr_TownsUpdate ON Towns FOR UPDATE
+AS
+IF (EXISTS(
+     SELECT * FROM inserted
+     WHERE Name IS NULL OR LEN(Name) = 0))
+BEGIN
+     RAISERROR('Town name cannot be empty.', 16, 1)
+     ROLLBACK
+     RETURN
+END
+UPDATE Towns SET Name='' WHERE TownId=1</t>
+    </r>
+  </si>
+  <si>
+    <t>Instead Of Triggers</t>
+  </si>
+  <si>
+    <t>Defined by using INSTEAD OF :
+CREATE TABLE Accounts(
+Username varchar(10) NOT NULL PRIMARY KEY,
+[Password] varchar(20) NOT NULL,
+Active char(1) NOT NULL DEFAULT 'Y’)
+CREATE TRIGGER tr_AccountsDelete ON Accounts
+INSTEAD OF DELETE
+AS
+UPDATE a SET Active = 'N'
+FROM Accounts AS a JOIN DELETED d
+ON d.Username = a.Username
+WHERE a.Active = 'Y'</t>
+  </si>
+  <si>
+    <t>Database Security
+Fixed Server Roles, Fixed Database Roles</t>
+  </si>
+  <si>
+    <t>Database Security: SQL Server</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SQL Server has two layers of database security:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fixed Server Roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+sysadmin, bulkadmin, dbcreator, securityadmin
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fixed Database Roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+db_owner, db_securityadmin, db_accessadmin
+db_backupoperator, db_ddladmin
+db_datareader/db_datawriter</t>
+    </r>
+  </si>
+  <si>
+    <t>Custom Roles</t>
+  </si>
+  <si>
+    <t>SQL Server lets us create custom roles - Collection of privileges (permissions)
+Fine control over permissions - Can use one role for multiple users (groups)
+Makes auditing operations easier</t>
+  </si>
+  <si>
+    <t>Custom Role Permissions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CONTROL SERVER/DATABASE - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Gives all permissions on the server/database
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TAKE OWNERSHIP - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Enables the grantee to take ownership of a securable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VIEW CHANGE TRACKING -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Manage change tracking on schemas and tables
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">VIEW DEFINITION - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Enables the grantee to access metadata
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EXECUTE -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> To run procedures, scalar and aggregate functions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ALTER - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lets a role create, alter, and drop objects from the schema
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">REFERENCES - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lets the role create FOREIGN KEY constraints
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SELECT/DELETE/INSERT/UPDATE : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Grant access to CRUD Operations
+Can be granted on database, schema and object level
+Individual tables, views and columns can be targeted</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="51" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -7254,42 +8077,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7304,91 +8127,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7403,73 +8226,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7478,55 +8301,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7538,71 +8361,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7697,7 +8523,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -7705,6 +8531,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -7758,7 +8595,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7793,7 +8630,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10323,10 +11160,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C297"/>
+  <dimension ref="A1:C291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B262" sqref="B262"/>
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B284" sqref="B284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10345,16 +11182,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="106" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="109"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="111" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="116"/>
+      <c r="B3" s="110"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -10381,16 +11218,16 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="110" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="114"/>
+      <c r="B7" s="108"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
         <v>518</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="103" t="s">
         <v>700</v>
       </c>
     </row>
@@ -10406,15 +11243,15 @@
       <c r="A10" s="72" t="s">
         <v>524</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="103" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="110" t="s">
         <v>519</v>
       </c>
-      <c r="B11" s="114"/>
+      <c r="B11" s="108"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -10425,10 +11262,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="110" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="116"/>
+      <c r="B13" s="110"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -10487,10 +11324,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="110" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="116"/>
+      <c r="B21" s="110"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -10501,10 +11338,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="110" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="116"/>
+      <c r="B23" s="110"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -10515,10 +11352,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="116" t="s">
+      <c r="A25" s="110" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="116"/>
+      <c r="B25" s="110"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -10545,10 +11382,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="110" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="116"/>
+      <c r="B29" s="110"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -10575,10 +11412,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="114" t="s">
+      <c r="A33" s="108" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="114"/>
+      <c r="B33" s="108"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -10605,10 +11442,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="116" t="s">
+      <c r="A37" s="110" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="116"/>
+      <c r="B37" s="110"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -10635,10 +11472,10 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="114" t="s">
+      <c r="A41" s="108" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="114"/>
+      <c r="B41" s="108"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
@@ -10657,10 +11494,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="110" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="114"/>
+      <c r="B44" s="108"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -10687,19 +11524,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="106" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="105"/>
+      <c r="B48" s="106"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="106" t="s">
+      <c r="A49" s="107" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="104"/>
+      <c r="B49" s="105"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="111" t="s">
+      <c r="A50" s="115" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -10707,7 +11544,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="112"/>
+      <c r="A51" s="116"/>
       <c r="B51" s="62" t="s">
         <v>591</v>
       </c>
@@ -10716,13 +11553,13 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="113"/>
+      <c r="A52" s="117"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="111" t="s">
+      <c r="A53" s="115" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -10730,25 +11567,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="112"/>
+      <c r="A54" s="116"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="112"/>
+      <c r="A55" s="116"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="113"/>
+      <c r="A56" s="117"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="111" t="s">
+      <c r="A57" s="115" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -10756,13 +11593,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="113"/>
+      <c r="A58" s="117"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="111" t="s">
+      <c r="A59" s="115" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -10773,7 +11610,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="112"/>
+      <c r="A60" s="116"/>
       <c r="B60" s="62" t="s">
         <v>527</v>
       </c>
@@ -10782,14 +11619,14 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="112"/>
+      <c r="A61" s="116"/>
       <c r="B61" s="62" t="s">
         <v>588</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="113"/>
+      <c r="A62" s="117"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
@@ -10843,7 +11680,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="108" t="s">
+      <c r="A69" s="112" t="s">
         <v>290</v>
       </c>
       <c r="B69" s="62" t="s">
@@ -10851,37 +11688,37 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="109"/>
+      <c r="A70" s="113"/>
       <c r="B70" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="109"/>
+      <c r="A71" s="113"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="109"/>
+      <c r="A72" s="113"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="109"/>
+      <c r="A73" s="113"/>
       <c r="B73" s="62" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="110"/>
+      <c r="A74" s="114"/>
       <c r="B74" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="108" t="s">
+      <c r="A75" s="112" t="s">
         <v>291</v>
       </c>
       <c r="B75" s="62" t="s">
@@ -10889,74 +11726,74 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="109"/>
+      <c r="A76" s="113"/>
       <c r="B76" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C76" s="67"/>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="109"/>
+      <c r="A77" s="113"/>
       <c r="B77" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="109"/>
+      <c r="A78" s="113"/>
       <c r="B78" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="109"/>
+      <c r="A79" s="113"/>
       <c r="B79" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="109"/>
+      <c r="A80" s="113"/>
       <c r="B80" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="109"/>
+      <c r="A81" s="113"/>
       <c r="B81" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="109"/>
+      <c r="A82" s="113"/>
       <c r="B82" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="109"/>
+      <c r="A83" s="113"/>
       <c r="B83" s="81" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="109"/>
+      <c r="A84" s="113"/>
       <c r="B84" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="109"/>
+      <c r="A85" s="113"/>
       <c r="B85" s="81" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="110"/>
+      <c r="A86" s="114"/>
       <c r="B86" s="81" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="108" t="s">
+      <c r="A87" s="112" t="s">
         <v>292</v>
       </c>
       <c r="B87" s="82" t="s">
@@ -10964,28 +11801,28 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="109"/>
+      <c r="A88" s="113"/>
       <c r="B88" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="109"/>
+      <c r="A89" s="113"/>
       <c r="B89" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="110"/>
+      <c r="A90" s="114"/>
       <c r="B90" s="82" t="s">
         <v>546</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="108" t="s">
+      <c r="A91" s="112" t="s">
         <v>309</v>
       </c>
       <c r="B91" s="84" t="s">
@@ -10994,7 +11831,7 @@
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="110"/>
+      <c r="A92" s="114"/>
       <c r="B92" s="84" t="s">
         <v>311</v>
       </c>
@@ -11055,17 +11892,17 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="105" t="s">
+      <c r="A99" s="106" t="s">
         <v>388</v>
       </c>
-      <c r="B99" s="105"/>
+      <c r="B99" s="106"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="106" t="s">
+      <c r="A100" s="107" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="104"/>
+      <c r="B100" s="105"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -11096,10 +11933,10 @@
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A104" s="106" t="s">
+      <c r="A104" s="107" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="104"/>
+      <c r="B104" s="105"/>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -11247,10 +12084,10 @@
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A121" s="106" t="s">
+      <c r="A121" s="107" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="104"/>
+      <c r="B121" s="105"/>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -11335,10 +12172,10 @@
       <c r="C130"/>
     </row>
     <row r="131" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A131" s="106" t="s">
+      <c r="A131" s="107" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="104"/>
+      <c r="B131" s="105"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11432,10 +12269,10 @@
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="103" t="s">
+      <c r="A142" s="104" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="104"/>
+      <c r="B142" s="105"/>
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -11466,10 +12303,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="103" t="s">
+      <c r="A146" s="104" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="104"/>
+      <c r="B146" s="105"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11491,10 +12328,10 @@
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="103" t="s">
+      <c r="A149" s="104" t="s">
         <v>541</v>
       </c>
-      <c r="B149" s="104"/>
+      <c r="B149" s="105"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -11527,17 +12364,17 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="105" t="s">
+      <c r="A153" s="106" t="s">
         <v>472</v>
       </c>
-      <c r="B153" s="105"/>
+      <c r="B153" s="106"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="106" t="s">
+      <c r="A154" s="107" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="104"/>
+      <c r="B154" s="105"/>
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -11573,10 +12410,10 @@
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="103" t="s">
+      <c r="A160" s="104" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="107"/>
+      <c r="B160" s="118"/>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -11643,10 +12480,10 @@
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="106" t="s">
+      <c r="A168" s="107" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="104"/>
+      <c r="B168" s="105"/>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -11668,10 +12505,10 @@
       <c r="C170"/>
     </row>
     <row r="171" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A171" s="106" t="s">
+      <c r="A171" s="107" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="104"/>
+      <c r="B171" s="105"/>
       <c r="C171"/>
     </row>
     <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -11693,17 +12530,17 @@
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A174" s="105" t="s">
+      <c r="A174" s="106" t="s">
         <v>552</v>
       </c>
-      <c r="B174" s="105"/>
+      <c r="B174" s="106"/>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="106" t="s">
+      <c r="A175" s="107" t="s">
         <v>553</v>
       </c>
-      <c r="B175" s="104"/>
+      <c r="B175" s="105"/>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11719,10 +12556,10 @@
       <c r="B177" s="76"/>
     </row>
     <row r="178" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A178" s="106" t="s">
+      <c r="A178" s="107" t="s">
         <v>552</v>
       </c>
-      <c r="B178" s="104"/>
+      <c r="B178" s="105"/>
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -11803,10 +12640,10 @@
       <c r="B187" s="76"/>
     </row>
     <row r="188" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A188" s="106" t="s">
+      <c r="A188" s="107" t="s">
         <v>575</v>
       </c>
-      <c r="B188" s="104"/>
+      <c r="B188" s="105"/>
       <c r="C188"/>
     </row>
     <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -11824,10 +12661,10 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="103" t="s">
+      <c r="A191" s="104" t="s">
         <v>579</v>
       </c>
-      <c r="B191" s="104"/>
+      <c r="B191" s="105"/>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
@@ -11862,17 +12699,17 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A196" s="105" t="s">
+      <c r="A196" s="106" t="s">
         <v>600</v>
       </c>
-      <c r="B196" s="105"/>
+      <c r="B196" s="106"/>
       <c r="C196"/>
     </row>
     <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="103" t="s">
+      <c r="A197" s="104" t="s">
         <v>602</v>
       </c>
-      <c r="B197" s="104"/>
+      <c r="B197" s="105"/>
     </row>
     <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A198" s="57" t="s">
@@ -11919,10 +12756,10 @@
       <c r="B203" s="99"/>
     </row>
     <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="103" t="s">
+      <c r="A204" s="104" t="s">
         <v>613</v>
       </c>
-      <c r="B204" s="104"/>
+      <c r="B204" s="105"/>
     </row>
     <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="57" t="s">
@@ -11961,10 +12798,10 @@
       <c r="B212" s="76"/>
     </row>
     <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="103" t="s">
+      <c r="A213" s="104" t="s">
         <v>615</v>
       </c>
-      <c r="B213" s="104"/>
+      <c r="B213" s="105"/>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="72" t="s">
@@ -11975,10 +12812,10 @@
       </c>
     </row>
     <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="103" t="s">
+      <c r="A215" s="104" t="s">
         <v>619</v>
       </c>
-      <c r="B215" s="104"/>
+      <c r="B215" s="105"/>
     </row>
     <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="57" t="s">
@@ -11997,10 +12834,10 @@
       </c>
     </row>
     <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="103" t="s">
+      <c r="A218" s="104" t="s">
         <v>618</v>
       </c>
-      <c r="B218" s="104"/>
+      <c r="B218" s="105"/>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A219" s="57" t="s">
@@ -12035,22 +12872,22 @@
       </c>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="105" t="s">
+      <c r="A223" s="106" t="s">
         <v>634</v>
       </c>
-      <c r="B223" s="105"/>
+      <c r="B223" s="106"/>
     </row>
     <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A224" s="103" t="s">
+      <c r="A224" s="104" t="s">
         <v>636</v>
       </c>
-      <c r="B224" s="104"/>
+      <c r="B224" s="105"/>
     </row>
     <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A225" s="103" t="s">
+      <c r="A225" s="104" t="s">
         <v>635</v>
       </c>
-      <c r="B225" s="104"/>
+      <c r="B225" s="105"/>
     </row>
     <row r="226" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A226" s="57" t="s">
@@ -12061,10 +12898,10 @@
       </c>
     </row>
     <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A227" s="103" t="s">
+      <c r="A227" s="104" t="s">
         <v>639</v>
       </c>
-      <c r="B227" s="104"/>
+      <c r="B227" s="105"/>
     </row>
     <row r="228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="57" t="s">
@@ -12107,10 +12944,10 @@
       </c>
     </row>
     <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A233" s="103" t="s">
+      <c r="A233" s="104" t="s">
         <v>649</v>
       </c>
-      <c r="B233" s="104"/>
+      <c r="B233" s="105"/>
     </row>
     <row r="234" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="57" t="s">
@@ -12121,10 +12958,10 @@
       </c>
     </row>
     <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="103" t="s">
+      <c r="A235" s="104" t="s">
         <v>652</v>
       </c>
-      <c r="B235" s="104"/>
+      <c r="B235" s="105"/>
     </row>
     <row r="236" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A236" s="57" t="s">
@@ -12141,10 +12978,10 @@
       </c>
     </row>
     <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A238" s="103" t="s">
+      <c r="A238" s="104" t="s">
         <v>656</v>
       </c>
-      <c r="B238" s="104"/>
+      <c r="B238" s="105"/>
     </row>
     <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="57" t="s">
@@ -12291,10 +13128,10 @@
       </c>
     </row>
     <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A257" s="103" t="s">
+      <c r="A257" s="104" t="s">
         <v>693</v>
       </c>
-      <c r="B257" s="104"/>
+      <c r="B257" s="105"/>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="57" t="s">
@@ -12321,10 +13158,10 @@
       </c>
     </row>
     <row r="261" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A261" s="103" t="s">
+      <c r="A261" s="104" t="s">
         <v>701</v>
       </c>
-      <c r="B261" s="104"/>
+      <c r="B261" s="105"/>
     </row>
     <row r="262" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A262" s="57" t="s">
@@ -12334,93 +13171,171 @@
         <v>703</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A263" s="57"/>
-      <c r="B263" s="76"/>
-    </row>
-    <row r="264" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A264" s="57"/>
-      <c r="B264" s="76"/>
-    </row>
-    <row r="265" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A265" s="57"/>
-      <c r="B265" s="76"/>
-    </row>
-    <row r="266" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A266" s="57"/>
-      <c r="B266" s="76"/>
-    </row>
-    <row r="267" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A267" s="57"/>
-      <c r="B267" s="76"/>
-    </row>
-    <row r="268" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A268" s="57"/>
-      <c r="B268" s="76"/>
-    </row>
-    <row r="269" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A269" s="57"/>
-      <c r="B269" s="76"/>
-    </row>
-    <row r="270" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A270" s="57"/>
-      <c r="B270" s="76"/>
-    </row>
-    <row r="271" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A271" s="57"/>
-      <c r="B271" s="76"/>
-    </row>
-    <row r="272" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A272" s="57"/>
-      <c r="B272" s="76"/>
-    </row>
-    <row r="273" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A273" s="57"/>
-      <c r="B273" s="76"/>
-    </row>
-    <row r="274" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A274" s="57"/>
-      <c r="B274" s="76"/>
-    </row>
-    <row r="275" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A275" s="57"/>
-      <c r="B275" s="76"/>
+    <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A263" s="106" t="s">
+        <v>704</v>
+      </c>
+      <c r="B263" s="106"/>
+    </row>
+    <row r="264" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A264" s="104" t="s">
+        <v>705</v>
+      </c>
+      <c r="B264" s="105"/>
+    </row>
+    <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A265" s="57" t="s">
+        <v>705</v>
+      </c>
+      <c r="B265" s="76" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A266" s="57" t="s">
+        <v>708</v>
+      </c>
+      <c r="B266" s="123" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A267" s="57" t="s">
+        <v>710</v>
+      </c>
+      <c r="B267" s="123" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A268" s="57" t="s">
+        <v>712</v>
+      </c>
+      <c r="B268" s="76" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A269" s="104" t="s">
+        <v>714</v>
+      </c>
+      <c r="B269" s="105"/>
+    </row>
+    <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A270" s="57" t="s">
+        <v>715</v>
+      </c>
+      <c r="B270" s="123" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A271" s="57" t="s">
+        <v>717</v>
+      </c>
+      <c r="B271" s="123" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A272" s="57" t="s">
+        <v>719</v>
+      </c>
+      <c r="B272" s="123" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A273" s="57" t="s">
+        <v>721</v>
+      </c>
+      <c r="B273" s="123" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A274" s="104" t="s">
+        <v>706</v>
+      </c>
+      <c r="B274" s="105"/>
+    </row>
+    <row r="275" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A275" s="57" t="s">
+        <v>723</v>
+      </c>
+      <c r="B275" s="123" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="276" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A276" s="57"/>
-      <c r="B276" s="76"/>
-    </row>
-    <row r="277" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A277" s="57"/>
-      <c r="B277" s="76"/>
+      <c r="A276" s="57" t="s">
+        <v>725</v>
+      </c>
+      <c r="B276" s="76" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A277" s="57" t="s">
+        <v>727</v>
+      </c>
+      <c r="B277" s="76" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="278" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A278" s="57"/>
-      <c r="B278" s="76"/>
-    </row>
-    <row r="279" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A279" s="57"/>
-      <c r="B279" s="76"/>
-    </row>
-    <row r="280" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A280" s="57"/>
-      <c r="B280" s="76"/>
-    </row>
-    <row r="281" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A281" s="57"/>
-      <c r="B281" s="76"/>
-    </row>
-    <row r="282" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A282" s="57"/>
-      <c r="B282" s="76"/>
-    </row>
-    <row r="283" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A283" s="57"/>
-      <c r="B283" s="76"/>
-    </row>
-    <row r="284" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A284" s="57"/>
-      <c r="B284" s="76"/>
+      <c r="A278" s="57" t="s">
+        <v>729</v>
+      </c>
+      <c r="B278" s="76" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A279" s="57" t="s">
+        <v>731</v>
+      </c>
+      <c r="B279" s="123" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A280" s="57" t="s">
+        <v>733</v>
+      </c>
+      <c r="B280" s="76" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A281" s="104" t="s">
+        <v>735</v>
+      </c>
+      <c r="B281" s="105"/>
+    </row>
+    <row r="282" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A282" s="57" t="s">
+        <v>736</v>
+      </c>
+      <c r="B282" s="123" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A283" s="57" t="s">
+        <v>738</v>
+      </c>
+      <c r="B283" s="76" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A284" s="57" t="s">
+        <v>740</v>
+      </c>
+      <c r="B284" s="123" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="285" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A285" s="57"/>
@@ -12450,39 +13365,37 @@
       <c r="A291" s="57"/>
       <c r="B291" s="76"/>
     </row>
-    <row r="292" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A292" s="57"/>
-      <c r="B292" s="76"/>
-    </row>
-    <row r="293" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A293" s="57"/>
-      <c r="B293" s="76"/>
-    </row>
-    <row r="294" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A294" s="57"/>
-      <c r="B294" s="76"/>
-    </row>
-    <row r="295" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A295" s="57"/>
-      <c r="B295" s="76"/>
-    </row>
-    <row r="296" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A296" s="57"/>
-      <c r="B296" s="76"/>
-    </row>
-    <row r="297" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A297" s="57"/>
-      <c r="B297" s="76"/>
-    </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A191:B191"/>
+  <mergeCells count="61">
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="A269:B269"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A281:B281"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A225:B225"/>
+    <mergeCell ref="A227:B227"/>
+    <mergeCell ref="A233:B233"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A75:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
     <mergeCell ref="A149:B149"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
@@ -12499,26 +13412,13 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A75:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A261:B261"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A191:B191"/>
     <mergeCell ref="A197:B197"/>
     <mergeCell ref="A204:B204"/>
     <mergeCell ref="A213:B213"/>
@@ -12528,10 +13428,6 @@
     <mergeCell ref="A238:B238"/>
     <mergeCell ref="A257:B257"/>
     <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A225:B225"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A233:B233"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12953,7 +13849,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -12973,7 +13869,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119"/>
+      <c r="A2" s="120"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -13041,10 +13937,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="121" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="121"/>
+      <c r="C6" s="122"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
DB - Exercises 10.10.2019
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" activeTab="1"/>
@@ -30,7 +30,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -4947,9 +4947,6 @@
 FROM Employees</t>
   </si>
   <si>
-    <t>All T-SQL prior GO will execute "at once"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">INSERT INTO mytable DEFAULT VALUES
 GO 10
@@ -7308,17 +7305,28 @@
 INSERT INTO Logs (AccountId, NewSum, OldSum)
 VALUES(@AccountId,@NewSum, @OldSum)</t>
   </si>
+  <si>
+    <t>All T-SQL prior GO will execute "at once" - Изпълнява кода преди GO и тогава продължи надолу по кода</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="53" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8094,42 +8102,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8144,91 +8152,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8243,73 +8251,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8318,55 +8326,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8378,80 +8386,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -8546,7 +8554,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -8554,17 +8562,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -8618,7 +8615,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8653,7 +8650,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11185,8 +11182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C279" sqref="C279"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11208,13 +11205,13 @@
       <c r="A2" s="107" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="117"/>
+      <c r="B2" s="112"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="114" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="118"/>
+      <c r="B3" s="113"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11241,17 +11238,17 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="113" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="111"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
         <v>518</v>
       </c>
       <c r="B8" s="103" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11271,10 +11268,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="113" t="s">
         <v>519</v>
       </c>
-      <c r="B11" s="116"/>
+      <c r="B11" s="111"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11285,10 +11282,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="113" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="118"/>
+      <c r="B13" s="113"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11340,17 +11337,17 @@
     </row>
     <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="113" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="118"/>
+      <c r="B21" s="113"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11361,10 +11358,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="118" t="s">
+      <c r="A23" s="113" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="118"/>
+      <c r="B23" s="113"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11375,10 +11372,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="118" t="s">
+      <c r="A25" s="113" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="118"/>
+      <c r="B25" s="113"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -11405,10 +11402,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="113" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="118"/>
+      <c r="B29" s="113"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -11435,10 +11432,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="111" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="116"/>
+      <c r="B33" s="111"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -11461,14 +11458,14 @@
         <v>379</v>
       </c>
       <c r="B36" s="74" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="118" t="s">
+      <c r="A37" s="113" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="118"/>
+      <c r="B37" s="113"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -11495,17 +11492,17 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="116" t="s">
+      <c r="A41" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="116"/>
+      <c r="B41" s="111"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
         <v>376</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
@@ -11517,10 +11514,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="118" t="s">
+      <c r="A44" s="113" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="116"/>
+      <c r="B44" s="111"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -11553,13 +11550,13 @@
       <c r="B48" s="107"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="108" t="s">
+      <c r="A49" s="110" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="106"/>
+      <c r="B49" s="109"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="113" t="s">
+      <c r="A50" s="118" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -11567,22 +11564,22 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="114"/>
+      <c r="A51" s="119"/>
       <c r="B51" s="62" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C51" s="66" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="115"/>
+      <c r="A52" s="120"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="113" t="s">
+      <c r="A53" s="118" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -11590,25 +11587,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="114"/>
+      <c r="A54" s="119"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="114"/>
+      <c r="A55" s="119"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="115"/>
+      <c r="A56" s="120"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="113" t="s">
+      <c r="A57" s="118" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -11616,13 +11613,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="115"/>
+      <c r="A58" s="120"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="113" t="s">
+      <c r="A59" s="118" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -11633,7 +11630,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="114"/>
+      <c r="A60" s="119"/>
       <c r="B60" s="62" t="s">
         <v>527</v>
       </c>
@@ -11642,24 +11639,24 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="114"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="62" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="115"/>
+      <c r="A62" s="120"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="102" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11680,18 +11677,18 @@
     </row>
     <row r="66" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A66" s="57" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B66" s="62" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A67" s="57" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -11703,7 +11700,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="110" t="s">
+      <c r="A69" s="115" t="s">
         <v>290</v>
       </c>
       <c r="B69" s="62" t="s">
@@ -11711,37 +11708,37 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="111"/>
+      <c r="A70" s="116"/>
       <c r="B70" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="111"/>
+      <c r="A71" s="116"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="111"/>
+      <c r="A72" s="116"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="111"/>
+      <c r="A73" s="116"/>
       <c r="B73" s="62" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="112"/>
+      <c r="A74" s="117"/>
       <c r="B74" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="110" t="s">
+      <c r="A75" s="115" t="s">
         <v>291</v>
       </c>
       <c r="B75" s="62" t="s">
@@ -11749,74 +11746,74 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="111"/>
+      <c r="A76" s="116"/>
       <c r="B76" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C76" s="67"/>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="111"/>
+      <c r="A77" s="116"/>
       <c r="B77" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="111"/>
+      <c r="A78" s="116"/>
       <c r="B78" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="111"/>
+      <c r="A79" s="116"/>
       <c r="B79" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="111"/>
+      <c r="A80" s="116"/>
       <c r="B80" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="111"/>
+      <c r="A81" s="116"/>
       <c r="B81" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="111"/>
+      <c r="A82" s="116"/>
       <c r="B82" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="111"/>
+      <c r="A83" s="116"/>
       <c r="B83" s="81" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="111"/>
+      <c r="A84" s="116"/>
       <c r="B84" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="111"/>
+      <c r="A85" s="116"/>
       <c r="B85" s="81" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="112"/>
+      <c r="A86" s="117"/>
       <c r="B86" s="81" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="110" t="s">
+      <c r="A87" s="115" t="s">
         <v>292</v>
       </c>
       <c r="B87" s="82" t="s">
@@ -11824,28 +11821,28 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="111"/>
+      <c r="A88" s="116"/>
       <c r="B88" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="111"/>
+      <c r="A89" s="116"/>
       <c r="B89" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="112"/>
+      <c r="A90" s="117"/>
       <c r="B90" s="82" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="110" t="s">
+      <c r="A91" s="115" t="s">
         <v>309</v>
       </c>
       <c r="B91" s="84" t="s">
@@ -11854,7 +11851,7 @@
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="112"/>
+      <c r="A92" s="117"/>
       <c r="B92" s="84" t="s">
         <v>311</v>
       </c>
@@ -11892,16 +11889,16 @@
         <v>373</v>
       </c>
       <c r="B96" s="84" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C96"/>
     </row>
-    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A97" s="90" t="s">
         <v>528</v>
       </c>
       <c r="B97" s="81" t="s">
-        <v>531</v>
+        <v>742</v>
       </c>
       <c r="C97"/>
     </row>
@@ -11922,10 +11919,10 @@
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="108" t="s">
+      <c r="A100" s="110" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="106"/>
+      <c r="B100" s="109"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -11956,10 +11953,10 @@
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A104" s="108" t="s">
+      <c r="A104" s="110" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="106"/>
+      <c r="B104" s="109"/>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12099,18 +12096,18 @@
     </row>
     <row r="120" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="92" t="s">
+        <v>534</v>
+      </c>
+      <c r="B120" s="91" t="s">
         <v>535</v>
       </c>
-      <c r="B120" s="91" t="s">
-        <v>536</v>
-      </c>
       <c r="C120"/>
     </row>
     <row r="121" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A121" s="108" t="s">
+      <c r="A121" s="110" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="106"/>
+      <c r="B121" s="109"/>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12195,10 +12192,10 @@
       <c r="C130"/>
     </row>
     <row r="131" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A131" s="108" t="s">
+      <c r="A131" s="110" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="106"/>
+      <c r="B131" s="109"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12269,7 +12266,7 @@
         <v>459</v>
       </c>
       <c r="B139" s="97" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C139"/>
     </row>
@@ -12278,7 +12275,7 @@
         <v>460</v>
       </c>
       <c r="B140" s="97" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C140"/>
     </row>
@@ -12287,15 +12284,15 @@
         <v>461</v>
       </c>
       <c r="B141" s="97" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="105" t="s">
+      <c r="A142" s="108" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="106"/>
+      <c r="B142" s="109"/>
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12326,10 +12323,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="105" t="s">
+      <c r="A146" s="108" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="106"/>
+      <c r="B146" s="109"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12343,46 +12340,46 @@
     </row>
     <row r="148" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A148" s="57" t="s">
+        <v>538</v>
+      </c>
+      <c r="B148" s="87" t="s">
         <v>539</v>
       </c>
-      <c r="B148" s="87" t="s">
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="108" t="s">
         <v>540</v>
       </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="105" t="s">
-        <v>541</v>
-      </c>
-      <c r="B149" s="106"/>
+      <c r="B149" s="109"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A150" s="57" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B150" s="80" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" s="57" t="s">
+        <v>542</v>
+      </c>
+      <c r="B151" s="76" t="s">
         <v>543</v>
-      </c>
-      <c r="B151" s="76" t="s">
-        <v>544</v>
       </c>
       <c r="C151"/>
     </row>
     <row r="152" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A152" s="57" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B152" s="98" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C152"/>
     </row>
@@ -12394,18 +12391,18 @@
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="108" t="s">
+      <c r="A154" s="110" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="106"/>
+      <c r="B154" s="109"/>
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A155" s="57" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B155" s="76" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C155"/>
     </row>
@@ -12433,10 +12430,10 @@
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="105" t="s">
+      <c r="A160" s="108" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="109"/>
+      <c r="B160" s="121"/>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12503,10 +12500,10 @@
       <c r="C167"/>
     </row>
     <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="108" t="s">
+      <c r="A168" s="110" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="106"/>
+      <c r="B168" s="109"/>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12528,10 +12525,10 @@
       <c r="C170"/>
     </row>
     <row r="171" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A171" s="108" t="s">
+      <c r="A171" s="110" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="106"/>
+      <c r="B171" s="109"/>
       <c r="C171"/>
     </row>
     <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12554,24 +12551,24 @@
     </row>
     <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A174" s="107" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B174" s="107"/>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="108" t="s">
-        <v>553</v>
-      </c>
-      <c r="B175" s="106"/>
+      <c r="A175" s="110" t="s">
+        <v>552</v>
+      </c>
+      <c r="B175" s="109"/>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A176" s="57" t="s">
+        <v>553</v>
+      </c>
+      <c r="B176" s="76" t="s">
         <v>554</v>
-      </c>
-      <c r="B176" s="76" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -12579,83 +12576,83 @@
       <c r="B177" s="76"/>
     </row>
     <row r="178" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A178" s="108" t="s">
-        <v>552</v>
-      </c>
-      <c r="B178" s="106"/>
+      <c r="A178" s="110" t="s">
+        <v>551</v>
+      </c>
+      <c r="B178" s="109"/>
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A179" s="57" t="s">
+        <v>555</v>
+      </c>
+      <c r="B179" s="76" t="s">
         <v>556</v>
-      </c>
-      <c r="B179" s="76" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A180" s="57" t="s">
+        <v>557</v>
+      </c>
+      <c r="B180" s="76" t="s">
         <v>558</v>
-      </c>
-      <c r="B180" s="76" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="57" t="s">
+        <v>559</v>
+      </c>
+      <c r="B181" s="76" t="s">
         <v>560</v>
-      </c>
-      <c r="B181" s="76" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="57" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B182" s="76" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="57" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B183" s="76" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A184" s="57" t="s">
+        <v>565</v>
+      </c>
+      <c r="B184" s="80" t="s">
         <v>566</v>
       </c>
-      <c r="B184" s="80" t="s">
-        <v>567</v>
-      </c>
       <c r="C184" s="95" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
       <c r="A185" s="57" t="s">
+        <v>567</v>
+      </c>
+      <c r="B185" s="80" t="s">
         <v>568</v>
       </c>
-      <c r="B185" s="80" t="s">
-        <v>569</v>
-      </c>
       <c r="C185" s="95" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A186" s="57" t="s">
+        <v>569</v>
+      </c>
+      <c r="B186" s="76" t="s">
         <v>570</v>
       </c>
-      <c r="B186" s="76" t="s">
-        <v>571</v>
-      </c>
       <c r="C186" s="94" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -12663,115 +12660,115 @@
       <c r="B187" s="76"/>
     </row>
     <row r="188" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A188" s="108" t="s">
-        <v>575</v>
-      </c>
-      <c r="B188" s="106"/>
+      <c r="A188" s="110" t="s">
+        <v>574</v>
+      </c>
+      <c r="B188" s="109"/>
       <c r="C188"/>
     </row>
     <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A189" s="57" t="s">
+        <v>575</v>
+      </c>
+      <c r="B189" s="76" t="s">
         <v>576</v>
-      </c>
-      <c r="B189" s="76" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A190" s="57"/>
       <c r="B190" s="76" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A191" s="108" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="105" t="s">
-        <v>579</v>
-      </c>
-      <c r="B191" s="106"/>
+      <c r="B191" s="109"/>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B192" s="76" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A193" s="57" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B193" s="76" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A194" s="57" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B194" s="96" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A195" s="57" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B195" s="96" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A196" s="107" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B196" s="107"/>
       <c r="C196"/>
     </row>
     <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="105" t="s">
-        <v>602</v>
-      </c>
-      <c r="B197" s="106"/>
+      <c r="A197" s="108" t="s">
+        <v>601</v>
+      </c>
+      <c r="B197" s="109"/>
     </row>
     <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A198" s="57" t="s">
+        <v>602</v>
+      </c>
+      <c r="B198" s="100" t="s">
         <v>603</v>
-      </c>
-      <c r="B198" s="100" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A199" s="57" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B199" s="100" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A200" s="57" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B200" s="100" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A201" s="57" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B201" s="101" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="57" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B202" s="100" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -12779,17 +12776,17 @@
       <c r="B203" s="99"/>
     </row>
     <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="105" t="s">
-        <v>613</v>
-      </c>
-      <c r="B204" s="106"/>
+      <c r="A204" s="108" t="s">
+        <v>612</v>
+      </c>
+      <c r="B204" s="109"/>
     </row>
     <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="57" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B205" s="76" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -12821,546 +12818,546 @@
       <c r="B212" s="76"/>
     </row>
     <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="105" t="s">
-        <v>615</v>
-      </c>
-      <c r="B213" s="106"/>
+      <c r="A213" s="108" t="s">
+        <v>614</v>
+      </c>
+      <c r="B213" s="109"/>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="72" t="s">
+        <v>615</v>
+      </c>
+      <c r="B214" s="76" t="s">
         <v>616</v>
       </c>
-      <c r="B214" s="76" t="s">
-        <v>617</v>
-      </c>
     </row>
     <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="105" t="s">
-        <v>619</v>
-      </c>
-      <c r="B215" s="106"/>
+      <c r="A215" s="108" t="s">
+        <v>618</v>
+      </c>
+      <c r="B215" s="109"/>
     </row>
     <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="57" t="s">
+        <v>619</v>
+      </c>
+      <c r="B216" s="76" t="s">
         <v>620</v>
-      </c>
-      <c r="B216" s="76" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A217" s="57" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B217" s="76" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="105" t="s">
-        <v>618</v>
-      </c>
-      <c r="B218" s="106"/>
+      <c r="A218" s="108" t="s">
+        <v>617</v>
+      </c>
+      <c r="B218" s="109"/>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A219" s="57" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B219" s="80" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A220" s="57" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B220" s="76" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A221" s="57" t="s">
+        <v>624</v>
+      </c>
+      <c r="B221" s="76" t="s">
         <v>625</v>
-      </c>
-      <c r="B221" s="76" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="57" t="s">
+        <v>628</v>
+      </c>
+      <c r="B222" s="76" t="s">
         <v>629</v>
-      </c>
-      <c r="B222" s="76" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A223" s="107" t="s">
+        <v>633</v>
+      </c>
+      <c r="B223" s="107"/>
+    </row>
+    <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A224" s="108" t="s">
+        <v>635</v>
+      </c>
+      <c r="B224" s="109"/>
+    </row>
+    <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A225" s="108" t="s">
         <v>634</v>
       </c>
-      <c r="B223" s="107"/>
-    </row>
-    <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A224" s="105" t="s">
-        <v>636</v>
-      </c>
-      <c r="B224" s="106"/>
-    </row>
-    <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A225" s="105" t="s">
-        <v>635</v>
-      </c>
-      <c r="B225" s="106"/>
+      <c r="B225" s="109"/>
     </row>
     <row r="226" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A226" s="57" t="s">
+        <v>636</v>
+      </c>
+      <c r="B226" s="76" t="s">
         <v>637</v>
       </c>
-      <c r="B226" s="76" t="s">
+    </row>
+    <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A227" s="108" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A227" s="105" t="s">
-        <v>639</v>
-      </c>
-      <c r="B227" s="106"/>
+      <c r="B227" s="109"/>
     </row>
     <row r="228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="57" t="s">
         <v>394</v>
       </c>
       <c r="B228" s="76" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A229" s="57" t="s">
+        <v>640</v>
+      </c>
+      <c r="B229" s="76" t="s">
         <v>641</v>
-      </c>
-      <c r="B229" s="76" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A230" s="57" t="s">
+        <v>642</v>
+      </c>
+      <c r="B230" s="76" t="s">
         <v>643</v>
-      </c>
-      <c r="B230" s="76" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="57" t="s">
+        <v>644</v>
+      </c>
+      <c r="B231" s="76" t="s">
         <v>645</v>
-      </c>
-      <c r="B231" s="76" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A232" s="57" t="s">
+        <v>646</v>
+      </c>
+      <c r="B232" s="76" t="s">
         <v>647</v>
       </c>
-      <c r="B232" s="76" t="s">
+    </row>
+    <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A233" s="108" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A233" s="105" t="s">
-        <v>649</v>
-      </c>
-      <c r="B233" s="106"/>
+      <c r="B233" s="109"/>
     </row>
     <row r="234" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="57" t="s">
+        <v>649</v>
+      </c>
+      <c r="B234" s="76" t="s">
         <v>650</v>
       </c>
-      <c r="B234" s="76" t="s">
+    </row>
+    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A235" s="108" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="105" t="s">
-        <v>652</v>
-      </c>
-      <c r="B235" s="106"/>
+      <c r="B235" s="109"/>
     </row>
     <row r="236" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A236" s="57" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B236" s="76"/>
     </row>
     <row r="237" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A237" s="57" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B237" s="76" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A238" s="108" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A238" s="105" t="s">
-        <v>656</v>
-      </c>
-      <c r="B238" s="106"/>
+      <c r="B238" s="109"/>
     </row>
     <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="57" t="s">
+        <v>656</v>
+      </c>
+      <c r="B239" s="76" t="s">
         <v>657</v>
-      </c>
-      <c r="B239" s="76" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A240" s="57" t="s">
+        <v>658</v>
+      </c>
+      <c r="B240" s="76" t="s">
         <v>659</v>
-      </c>
-      <c r="B240" s="76" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" s="57" t="s">
+        <v>660</v>
+      </c>
+      <c r="B241" s="76" t="s">
         <v>661</v>
-      </c>
-      <c r="B241" s="76" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A242" s="57" t="s">
+        <v>662</v>
+      </c>
+      <c r="B242" s="76" t="s">
         <v>663</v>
-      </c>
-      <c r="B242" s="76" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A243" s="57" t="s">
+        <v>664</v>
+      </c>
+      <c r="B243" s="76" t="s">
         <v>665</v>
-      </c>
-      <c r="B243" s="76" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="57" t="s">
+        <v>666</v>
+      </c>
+      <c r="B244" s="76" t="s">
         <v>667</v>
-      </c>
-      <c r="B244" s="76" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A245" s="57" t="s">
+        <v>668</v>
+      </c>
+      <c r="B245" s="76" t="s">
         <v>669</v>
-      </c>
-      <c r="B245" s="76" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A246" s="57" t="s">
+        <v>670</v>
+      </c>
+      <c r="B246" s="76" t="s">
         <v>671</v>
-      </c>
-      <c r="B246" s="76" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A247" s="57" t="s">
+        <v>672</v>
+      </c>
+      <c r="B247" s="76" t="s">
         <v>673</v>
-      </c>
-      <c r="B247" s="76" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A248" s="57" t="s">
+        <v>674</v>
+      </c>
+      <c r="B248" s="76" t="s">
         <v>675</v>
-      </c>
-      <c r="B248" s="76" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A249" s="57" t="s">
+        <v>676</v>
+      </c>
+      <c r="B249" s="76" t="s">
         <v>677</v>
-      </c>
-      <c r="B249" s="76" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A250" s="57" t="s">
+        <v>678</v>
+      </c>
+      <c r="B250" s="76" t="s">
         <v>679</v>
-      </c>
-      <c r="B250" s="76" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" s="57" t="s">
+        <v>680</v>
+      </c>
+      <c r="B251" s="76" t="s">
         <v>681</v>
-      </c>
-      <c r="B251" s="76" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A252" s="57" t="s">
+        <v>682</v>
+      </c>
+      <c r="B252" s="76" t="s">
         <v>683</v>
-      </c>
-      <c r="B252" s="76" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A253" s="57" t="s">
+        <v>684</v>
+      </c>
+      <c r="B253" s="76" t="s">
         <v>685</v>
-      </c>
-      <c r="B253" s="76" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="57" t="s">
+        <v>686</v>
+      </c>
+      <c r="B254" s="76" t="s">
         <v>687</v>
-      </c>
-      <c r="B254" s="76" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A255" s="57" t="s">
+        <v>688</v>
+      </c>
+      <c r="B255" s="76" t="s">
         <v>689</v>
-      </c>
-      <c r="B255" s="76" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A256" s="57" t="s">
+        <v>690</v>
+      </c>
+      <c r="B256" s="76" t="s">
         <v>691</v>
       </c>
-      <c r="B256" s="76" t="s">
+    </row>
+    <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A257" s="108" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A257" s="105" t="s">
-        <v>693</v>
-      </c>
-      <c r="B257" s="106"/>
+      <c r="B257" s="109"/>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="57" t="s">
+        <v>693</v>
+      </c>
+      <c r="B258" s="76" t="s">
         <v>694</v>
-      </c>
-      <c r="B258" s="76" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="57" t="s">
+        <v>695</v>
+      </c>
+      <c r="B259" s="76" t="s">
         <v>696</v>
-      </c>
-      <c r="B259" s="76" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A260" s="57" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B260" s="76" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A261" s="105" t="s">
-        <v>701</v>
-      </c>
-      <c r="B261" s="106"/>
+      <c r="A261" s="108" t="s">
+        <v>700</v>
+      </c>
+      <c r="B261" s="109"/>
     </row>
     <row r="262" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A262" s="57" t="s">
+        <v>701</v>
+      </c>
+      <c r="B262" s="76" t="s">
         <v>702</v>
-      </c>
-      <c r="B262" s="76" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A263" s="107" t="s">
+        <v>703</v>
+      </c>
+      <c r="B263" s="107"/>
+    </row>
+    <row r="264" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A264" s="108" t="s">
         <v>704</v>
       </c>
-      <c r="B263" s="107"/>
-    </row>
-    <row r="264" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A264" s="105" t="s">
-        <v>705</v>
-      </c>
-      <c r="B264" s="106"/>
+      <c r="B264" s="109"/>
     </row>
     <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A265" s="57" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B265" s="76" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A266" s="57" t="s">
+        <v>707</v>
+      </c>
+      <c r="B266" s="104" t="s">
         <v>708</v>
-      </c>
-      <c r="B266" s="104" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A267" s="57" t="s">
+        <v>709</v>
+      </c>
+      <c r="B267" s="104" t="s">
         <v>710</v>
-      </c>
-      <c r="B267" s="104" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A268" s="57" t="s">
+        <v>711</v>
+      </c>
+      <c r="B268" s="76" t="s">
         <v>712</v>
       </c>
-      <c r="B268" s="76" t="s">
+    </row>
+    <row r="269" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A269" s="108" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A269" s="105" t="s">
-        <v>714</v>
-      </c>
-      <c r="B269" s="106"/>
+      <c r="B269" s="109"/>
     </row>
     <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A270" s="57" t="s">
+        <v>714</v>
+      </c>
+      <c r="B270" s="104" t="s">
         <v>715</v>
-      </c>
-      <c r="B270" s="104" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A271" s="57" t="s">
+        <v>716</v>
+      </c>
+      <c r="B271" s="104" t="s">
         <v>717</v>
-      </c>
-      <c r="B271" s="104" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A272" s="57" t="s">
+        <v>718</v>
+      </c>
+      <c r="B272" s="104" t="s">
         <v>719</v>
-      </c>
-      <c r="B272" s="104" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A273" s="57" t="s">
+        <v>720</v>
+      </c>
+      <c r="B273" s="104" t="s">
         <v>721</v>
       </c>
-      <c r="B273" s="104" t="s">
-        <v>722</v>
-      </c>
     </row>
     <row r="274" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A274" s="105" t="s">
-        <v>706</v>
-      </c>
-      <c r="B274" s="106"/>
+      <c r="A274" s="108" t="s">
+        <v>705</v>
+      </c>
+      <c r="B274" s="109"/>
     </row>
     <row r="275" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A275" s="57" t="s">
+        <v>722</v>
+      </c>
+      <c r="B275" s="105" t="s">
         <v>723</v>
-      </c>
-      <c r="B275" s="124" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A276" s="57" t="s">
+        <v>724</v>
+      </c>
+      <c r="B276" s="76" t="s">
         <v>725</v>
-      </c>
-      <c r="B276" s="76" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="57" t="s">
+        <v>726</v>
+      </c>
+      <c r="B277" s="76" t="s">
         <v>727</v>
-      </c>
-      <c r="B277" s="76" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A278" s="57" t="s">
+        <v>728</v>
+      </c>
+      <c r="B278" s="76" t="s">
         <v>729</v>
-      </c>
-      <c r="B278" s="76" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A279" s="57" t="s">
+        <v>730</v>
+      </c>
+      <c r="B279" s="105" t="s">
         <v>731</v>
       </c>
-      <c r="B279" s="124" t="s">
-        <v>732</v>
-      </c>
-      <c r="C279" s="125" t="s">
-        <v>742</v>
+      <c r="C279" s="106" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A280" s="57" t="s">
+        <v>732</v>
+      </c>
+      <c r="B280" s="76" t="s">
         <v>733</v>
       </c>
-      <c r="B280" s="76" t="s">
+    </row>
+    <row r="281" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A281" s="108" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A281" s="105" t="s">
-        <v>735</v>
-      </c>
-      <c r="B281" s="106"/>
+      <c r="B281" s="109"/>
     </row>
     <row r="282" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A282" s="57" t="s">
+        <v>735</v>
+      </c>
+      <c r="B282" s="104" t="s">
         <v>736</v>
-      </c>
-      <c r="B282" s="104" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A283" s="57" t="s">
+        <v>737</v>
+      </c>
+      <c r="B283" s="76" t="s">
         <v>738</v>
-      </c>
-      <c r="B283" s="76" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A284" s="57" t="s">
+        <v>739</v>
+      </c>
+      <c r="B284" s="104" t="s">
         <v>740</v>
-      </c>
-      <c r="B284" s="104" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="285" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -13393,18 +13390,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="A269:B269"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A281:B281"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A225:B225"/>
+    <mergeCell ref="A227:B227"/>
+    <mergeCell ref="A233:B233"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A261:B261"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A75:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
     <mergeCell ref="A149:B149"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
@@ -13421,39 +13439,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A75:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="A269:B269"/>
-    <mergeCell ref="A274:B274"/>
-    <mergeCell ref="A281:B281"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A225:B225"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A233:B233"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A215:B215"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13875,7 +13872,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -13895,7 +13892,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121"/>
+      <c r="A2" s="123"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -13963,10 +13960,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="124" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="123"/>
+      <c r="C6" s="125"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - 10.09.2019 - Triggers and Transactions
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" activeTab="1"/>
@@ -30,7 +30,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -7312,7 +7312,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8404,29 +8404,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8446,8 +8437,17 @@
     <xf numFmtId="0" fontId="39" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8554,7 +8554,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -8562,6 +8562,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -8615,7 +8626,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8650,7 +8661,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11183,7 +11194,7 @@
   <dimension ref="A1:C291"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11202,16 +11213,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="109" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="112"/>
+      <c r="B2" s="119"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="121" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="113"/>
+      <c r="B3" s="120"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11238,10 +11249,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="120" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="111"/>
+      <c r="B7" s="118"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11268,10 +11279,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="113" t="s">
+      <c r="A11" s="120" t="s">
         <v>519</v>
       </c>
-      <c r="B11" s="111"/>
+      <c r="B11" s="118"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11282,10 +11293,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="120" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="113"/>
+      <c r="B13" s="120"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11344,10 +11355,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="113" t="s">
+      <c r="A21" s="120" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="113"/>
+      <c r="B21" s="120"/>
     </row>
     <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11358,10 +11369,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="113" t="s">
+      <c r="A23" s="120" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="113"/>
+      <c r="B23" s="120"/>
     </row>
     <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11372,10 +11383,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="113" t="s">
+      <c r="A25" s="120" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="113"/>
+      <c r="B25" s="120"/>
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
@@ -11402,10 +11413,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="113" t="s">
+      <c r="A29" s="120" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="113"/>
+      <c r="B29" s="120"/>
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
@@ -11432,10 +11443,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111" t="s">
+      <c r="A33" s="118" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="111"/>
+      <c r="B33" s="118"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="72" t="s">
@@ -11462,10 +11473,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="113" t="s">
+      <c r="A37" s="120" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="113"/>
+      <c r="B37" s="120"/>
     </row>
     <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="72" t="s">
@@ -11492,10 +11503,10 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="111" t="s">
+      <c r="A41" s="118" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="111"/>
+      <c r="B41" s="118"/>
     </row>
     <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
@@ -11514,10 +11525,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="113" t="s">
+      <c r="A44" s="120" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="111"/>
+      <c r="B44" s="118"/>
     </row>
     <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
@@ -11544,19 +11555,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="107" t="s">
+      <c r="A48" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="107"/>
+      <c r="B48" s="109"/>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A49" s="110" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="109"/>
+      <c r="B49" s="108"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="118" t="s">
+      <c r="A50" s="115" t="s">
         <v>321</v>
       </c>
       <c r="B50" s="62" t="s">
@@ -11564,7 +11575,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="119"/>
+      <c r="A51" s="116"/>
       <c r="B51" s="62" t="s">
         <v>590</v>
       </c>
@@ -11573,13 +11584,13 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="120"/>
+      <c r="A52" s="117"/>
       <c r="B52" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="118" t="s">
+      <c r="A53" s="115" t="s">
         <v>322</v>
       </c>
       <c r="B53" s="62" t="s">
@@ -11587,25 +11598,25 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="119"/>
+      <c r="A54" s="116"/>
       <c r="B54" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="119"/>
+      <c r="A55" s="116"/>
       <c r="B55" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="120"/>
+      <c r="A56" s="117"/>
       <c r="B56" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="118" t="s">
+      <c r="A57" s="115" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="62" t="s">
@@ -11613,13 +11624,13 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="120"/>
+      <c r="A58" s="117"/>
       <c r="B58" s="62" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="118" t="s">
+      <c r="A59" s="115" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="62" t="s">
@@ -11630,7 +11641,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="119"/>
+      <c r="A60" s="116"/>
       <c r="B60" s="62" t="s">
         <v>527</v>
       </c>
@@ -11639,14 +11650,14 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="119"/>
+      <c r="A61" s="116"/>
       <c r="B61" s="62" t="s">
         <v>587</v>
       </c>
       <c r="C61" s="68"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="120"/>
+      <c r="A62" s="117"/>
       <c r="B62" s="62" t="s">
         <v>326</v>
       </c>
@@ -11700,7 +11711,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="115" t="s">
+      <c r="A69" s="112" t="s">
         <v>290</v>
       </c>
       <c r="B69" s="62" t="s">
@@ -11708,37 +11719,37 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="116"/>
+      <c r="A70" s="113"/>
       <c r="B70" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="116"/>
+      <c r="A71" s="113"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="116"/>
+      <c r="A72" s="113"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="116"/>
+      <c r="A73" s="113"/>
       <c r="B73" s="62" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="117"/>
+      <c r="A74" s="114"/>
       <c r="B74" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="115" t="s">
+      <c r="A75" s="112" t="s">
         <v>291</v>
       </c>
       <c r="B75" s="62" t="s">
@@ -11746,74 +11757,74 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="116"/>
+      <c r="A76" s="113"/>
       <c r="B76" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C76" s="67"/>
     </row>
     <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="116"/>
+      <c r="A77" s="113"/>
       <c r="B77" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="116"/>
+      <c r="A78" s="113"/>
       <c r="B78" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="116"/>
+      <c r="A79" s="113"/>
       <c r="B79" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="116"/>
+      <c r="A80" s="113"/>
       <c r="B80" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="116"/>
+      <c r="A81" s="113"/>
       <c r="B81" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="116"/>
+      <c r="A82" s="113"/>
       <c r="B82" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
+      <c r="A83" s="113"/>
       <c r="B83" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="116"/>
+      <c r="A84" s="113"/>
       <c r="B84" s="81" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="116"/>
+      <c r="A85" s="113"/>
       <c r="B85" s="81" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="117"/>
+      <c r="A86" s="114"/>
       <c r="B86" s="81" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="115" t="s">
+      <c r="A87" s="112" t="s">
         <v>292</v>
       </c>
       <c r="B87" s="82" t="s">
@@ -11821,28 +11832,28 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="116"/>
+      <c r="A88" s="113"/>
       <c r="B88" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="116"/>
+      <c r="A89" s="113"/>
       <c r="B89" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="117"/>
+      <c r="A90" s="114"/>
       <c r="B90" s="82" t="s">
         <v>545</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="115" t="s">
+      <c r="A91" s="112" t="s">
         <v>309</v>
       </c>
       <c r="B91" s="84" t="s">
@@ -11851,7 +11862,7 @@
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="117"/>
+      <c r="A92" s="114"/>
       <c r="B92" s="84" t="s">
         <v>311</v>
       </c>
@@ -11912,17 +11923,17 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="107" t="s">
+      <c r="A99" s="109" t="s">
         <v>388</v>
       </c>
-      <c r="B99" s="107"/>
+      <c r="B99" s="109"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A100" s="110" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="109"/>
+      <c r="B100" s="108"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -11956,7 +11967,7 @@
       <c r="A104" s="110" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="109"/>
+      <c r="B104" s="108"/>
       <c r="C104"/>
     </row>
     <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12107,7 +12118,7 @@
       <c r="A121" s="110" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="109"/>
+      <c r="B121" s="108"/>
       <c r="C121"/>
     </row>
     <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12195,7 +12206,7 @@
       <c r="A131" s="110" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="109"/>
+      <c r="B131" s="108"/>
       <c r="C131"/>
     </row>
     <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12289,10 +12300,10 @@
       <c r="C141"/>
     </row>
     <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="108" t="s">
+      <c r="A142" s="107" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="109"/>
+      <c r="B142" s="108"/>
       <c r="C142"/>
     </row>
     <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12323,10 +12334,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="108" t="s">
+      <c r="A146" s="107" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="109"/>
+      <c r="B146" s="108"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12348,10 +12359,10 @@
       <c r="C148"/>
     </row>
     <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="108" t="s">
+      <c r="A149" s="107" t="s">
         <v>540</v>
       </c>
-      <c r="B149" s="109"/>
+      <c r="B149" s="108"/>
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12384,17 +12395,17 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="107" t="s">
+      <c r="A153" s="109" t="s">
         <v>472</v>
       </c>
-      <c r="B153" s="107"/>
+      <c r="B153" s="109"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A154" s="110" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="109"/>
+      <c r="B154" s="108"/>
       <c r="C154"/>
     </row>
     <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12430,10 +12441,10 @@
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="108" t="s">
+      <c r="A160" s="107" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="121"/>
+      <c r="B160" s="111"/>
       <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12503,7 +12514,7 @@
       <c r="A168" s="110" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="109"/>
+      <c r="B168" s="108"/>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12528,7 +12539,7 @@
       <c r="A171" s="110" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="109"/>
+      <c r="B171" s="108"/>
       <c r="C171"/>
     </row>
     <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12550,17 +12561,17 @@
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A174" s="107" t="s">
+      <c r="A174" s="109" t="s">
         <v>551</v>
       </c>
-      <c r="B174" s="107"/>
+      <c r="B174" s="109"/>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A175" s="110" t="s">
         <v>552</v>
       </c>
-      <c r="B175" s="109"/>
+      <c r="B175" s="108"/>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12579,7 +12590,7 @@
       <c r="A178" s="110" t="s">
         <v>551</v>
       </c>
-      <c r="B178" s="109"/>
+      <c r="B178" s="108"/>
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12663,7 +12674,7 @@
       <c r="A188" s="110" t="s">
         <v>574</v>
       </c>
-      <c r="B188" s="109"/>
+      <c r="B188" s="108"/>
       <c r="C188"/>
     </row>
     <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12681,10 +12692,10 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="108" t="s">
+      <c r="A191" s="107" t="s">
         <v>578</v>
       </c>
-      <c r="B191" s="109"/>
+      <c r="B191" s="108"/>
     </row>
     <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A192" s="57" t="s">
@@ -12719,17 +12730,17 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A196" s="107" t="s">
+      <c r="A196" s="109" t="s">
         <v>599</v>
       </c>
-      <c r="B196" s="107"/>
+      <c r="B196" s="109"/>
       <c r="C196"/>
     </row>
     <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="108" t="s">
+      <c r="A197" s="107" t="s">
         <v>601</v>
       </c>
-      <c r="B197" s="109"/>
+      <c r="B197" s="108"/>
     </row>
     <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A198" s="57" t="s">
@@ -12776,10 +12787,10 @@
       <c r="B203" s="99"/>
     </row>
     <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="108" t="s">
+      <c r="A204" s="107" t="s">
         <v>612</v>
       </c>
-      <c r="B204" s="109"/>
+      <c r="B204" s="108"/>
     </row>
     <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="57" t="s">
@@ -12818,10 +12829,10 @@
       <c r="B212" s="76"/>
     </row>
     <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="108" t="s">
+      <c r="A213" s="107" t="s">
         <v>614</v>
       </c>
-      <c r="B213" s="109"/>
+      <c r="B213" s="108"/>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="72" t="s">
@@ -12832,10 +12843,10 @@
       </c>
     </row>
     <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="108" t="s">
+      <c r="A215" s="107" t="s">
         <v>618</v>
       </c>
-      <c r="B215" s="109"/>
+      <c r="B215" s="108"/>
     </row>
     <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="57" t="s">
@@ -12854,10 +12865,10 @@
       </c>
     </row>
     <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="108" t="s">
+      <c r="A218" s="107" t="s">
         <v>617</v>
       </c>
-      <c r="B218" s="109"/>
+      <c r="B218" s="108"/>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A219" s="57" t="s">
@@ -12892,22 +12903,22 @@
       </c>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="107" t="s">
+      <c r="A223" s="109" t="s">
         <v>633</v>
       </c>
-      <c r="B223" s="107"/>
+      <c r="B223" s="109"/>
     </row>
     <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A224" s="108" t="s">
+      <c r="A224" s="107" t="s">
         <v>635</v>
       </c>
-      <c r="B224" s="109"/>
+      <c r="B224" s="108"/>
     </row>
     <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A225" s="108" t="s">
+      <c r="A225" s="107" t="s">
         <v>634</v>
       </c>
-      <c r="B225" s="109"/>
+      <c r="B225" s="108"/>
     </row>
     <row r="226" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A226" s="57" t="s">
@@ -12918,10 +12929,10 @@
       </c>
     </row>
     <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A227" s="108" t="s">
+      <c r="A227" s="107" t="s">
         <v>638</v>
       </c>
-      <c r="B227" s="109"/>
+      <c r="B227" s="108"/>
     </row>
     <row r="228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="57" t="s">
@@ -12964,10 +12975,10 @@
       </c>
     </row>
     <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A233" s="108" t="s">
+      <c r="A233" s="107" t="s">
         <v>648</v>
       </c>
-      <c r="B233" s="109"/>
+      <c r="B233" s="108"/>
     </row>
     <row r="234" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="57" t="s">
@@ -12978,10 +12989,10 @@
       </c>
     </row>
     <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="108" t="s">
+      <c r="A235" s="107" t="s">
         <v>651</v>
       </c>
-      <c r="B235" s="109"/>
+      <c r="B235" s="108"/>
     </row>
     <row r="236" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A236" s="57" t="s">
@@ -12998,10 +13009,10 @@
       </c>
     </row>
     <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A238" s="108" t="s">
+      <c r="A238" s="107" t="s">
         <v>655</v>
       </c>
-      <c r="B238" s="109"/>
+      <c r="B238" s="108"/>
     </row>
     <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="57" t="s">
@@ -13148,10 +13159,10 @@
       </c>
     </row>
     <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A257" s="108" t="s">
+      <c r="A257" s="107" t="s">
         <v>692</v>
       </c>
-      <c r="B257" s="109"/>
+      <c r="B257" s="108"/>
     </row>
     <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A258" s="57" t="s">
@@ -13178,10 +13189,10 @@
       </c>
     </row>
     <row r="261" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A261" s="108" t="s">
+      <c r="A261" s="107" t="s">
         <v>700</v>
       </c>
-      <c r="B261" s="109"/>
+      <c r="B261" s="108"/>
     </row>
     <row r="262" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A262" s="57" t="s">
@@ -13192,16 +13203,16 @@
       </c>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="107" t="s">
+      <c r="A263" s="109" t="s">
         <v>703</v>
       </c>
-      <c r="B263" s="107"/>
+      <c r="B263" s="109"/>
     </row>
     <row r="264" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A264" s="108" t="s">
+      <c r="A264" s="107" t="s">
         <v>704</v>
       </c>
-      <c r="B264" s="109"/>
+      <c r="B264" s="108"/>
     </row>
     <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A265" s="57" t="s">
@@ -13236,10 +13247,10 @@
       </c>
     </row>
     <row r="269" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A269" s="108" t="s">
+      <c r="A269" s="107" t="s">
         <v>713</v>
       </c>
-      <c r="B269" s="109"/>
+      <c r="B269" s="108"/>
     </row>
     <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A270" s="57" t="s">
@@ -13274,10 +13285,10 @@
       </c>
     </row>
     <row r="274" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A274" s="108" t="s">
+      <c r="A274" s="107" t="s">
         <v>705</v>
       </c>
-      <c r="B274" s="109"/>
+      <c r="B274" s="108"/>
     </row>
     <row r="275" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A275" s="57" t="s">
@@ -13331,10 +13342,10 @@
       </c>
     </row>
     <row r="281" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A281" s="108" t="s">
+      <c r="A281" s="107" t="s">
         <v>734</v>
       </c>
-      <c r="B281" s="109"/>
+      <c r="B281" s="108"/>
     </row>
     <row r="282" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A282" s="57" t="s">
@@ -13390,39 +13401,18 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="A269:B269"/>
-    <mergeCell ref="A274:B274"/>
-    <mergeCell ref="A281:B281"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A225:B225"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A233:B233"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="A257:B257"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A75:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A191:B191"/>
     <mergeCell ref="A149:B149"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A48:B48"/>
@@ -13439,18 +13429,39 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A75:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="A269:B269"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A281:B281"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A225:B225"/>
+    <mergeCell ref="A227:B227"/>
+    <mergeCell ref="A233:B233"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A261:B261"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A257:B257"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# DB - 12.09.2019 - Triggers and Transactions
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="748">
   <si>
     <t>Операция</t>
   </si>
@@ -7307,6 +7307,43 @@
   </si>
   <si>
     <t>All T-SQL prior GO will execute "at once" - Изпълнява кода преди GO и тогава продължи надолу по кода</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TRIGGER tr_OnDeleteEmployee ON Employees
+FOR DELETE
+AS
+INSERT INTO 
+ Deleted_Employees (FirstName, LastName, MiddleName, JobTitle, DepartmentId, Salary)
+SELECT FirstName, LastName, MiddleName, JobTitle, DepartmentId, Salary FROM deleted </t>
+  </si>
+  <si>
+    <t>CAST</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The CAST() function converts a value (of any type) into a specified datatype.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT CAST(25.65 AS int);</t>
+    </r>
+  </si>
+  <si>
+    <t>UPDATE Flights
+ SET DepartureTime = NULL, ArrivalTime = NULL
+ WHERE DepartureTime &lt; ArrivalTime</t>
+  </si>
+  <si>
+    <t>Обновяване на повече от един запис</t>
   </si>
 </sst>
 </file>
@@ -8108,7 +8145,7 @@
     <xf numFmtId="0" fontId="38" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8404,20 +8441,29 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8437,17 +8483,8 @@
     <xf numFmtId="0" fontId="39" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8460,6 +8497,15 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11191,10 +11237,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C291"/>
+  <dimension ref="A1:C293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11213,16 +11259,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="107" t="s">
         <v>341</v>
       </c>
-      <c r="B2" s="119"/>
+      <c r="B2" s="112"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="114" t="s">
         <v>505</v>
       </c>
-      <c r="B3" s="120"/>
+      <c r="B3" s="113"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11249,10 +11295,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="113" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="111"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11279,10 +11325,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="113" t="s">
         <v>519</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="111"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11293,10 +11339,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="120" t="s">
+      <c r="A13" s="113" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="120"/>
+      <c r="B13" s="113"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11322,7 +11368,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>366</v>
       </c>
@@ -11330,7 +11376,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
         <v>289</v>
       </c>
@@ -11338,7 +11384,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
         <v>500</v>
       </c>
@@ -11346,7 +11392,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
         <v>593</v>
       </c>
@@ -11354,13 +11400,13 @@
         <v>592</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="120" t="s">
+    <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="113" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="120"/>
-    </row>
-    <row r="22" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="113"/>
+    </row>
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
         <v>339</v>
       </c>
@@ -11368,1445 +11414,1456 @@
         <v>503</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="120" t="s">
+    <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="113" t="s">
         <v>386</v>
       </c>
-      <c r="B23" s="120"/>
-    </row>
-    <row r="24" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="B23" s="113"/>
+    </row>
+    <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
         <v>340</v>
       </c>
       <c r="B24" s="74" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="120" t="s">
+      <c r="C24" s="94"/>
+    </row>
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="127" t="s">
+        <v>747</v>
+      </c>
+      <c r="B25" s="128" t="s">
+        <v>746</v>
+      </c>
+      <c r="C25" s="94"/>
+    </row>
+    <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="113" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="120"/>
-    </row>
-    <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+      <c r="B26" s="113"/>
+    </row>
+    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="57" t="s">
         <v>345</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B27" s="81" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+    <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B28" s="81" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="B28" s="81" t="s">
+      <c r="B29" s="81" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="120" t="s">
+    <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="113" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="120"/>
-    </row>
-    <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
+      <c r="B30" s="113"/>
+    </row>
+    <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="B30" s="74" t="s">
+      <c r="B31" s="74" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
         <v>364</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B32" s="74" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+    <row r="33" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="B32" s="74" t="s">
+      <c r="B33" s="74" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="118" t="s">
+    <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="111" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="118"/>
-    </row>
-    <row r="34" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="72" t="s">
-        <v>368</v>
-      </c>
-      <c r="B34" s="74" t="s">
-        <v>356</v>
-      </c>
+      <c r="B34" s="111"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
+        <v>368</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="72" t="s">
         <v>355</v>
       </c>
-      <c r="B35" s="74" t="s">
+      <c r="B36" s="74" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+    <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="B36" s="74" t="s">
+      <c r="B37" s="74" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="120" t="s">
+    <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="113" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="120"/>
-    </row>
-    <row r="38" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="72" t="s">
-        <v>370</v>
-      </c>
-      <c r="B38" s="74" t="s">
-        <v>359</v>
-      </c>
+      <c r="B38" s="113"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
+        <v>370</v>
+      </c>
+      <c r="B39" s="74" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="72" t="s">
         <v>369</v>
       </c>
-      <c r="B39" s="74" t="s">
+      <c r="B40" s="74" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
+    <row r="41" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="57" t="s">
         <v>380</v>
       </c>
-      <c r="B40" s="74" t="s">
+      <c r="B41" s="74" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="118" t="s">
+    <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="B41" s="118"/>
-    </row>
-    <row r="42" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="57" t="s">
+      <c r="B42" s="111"/>
+    </row>
+    <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="B42" s="74" t="s">
+      <c r="B43" s="74" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="57" t="s">
+    <row r="44" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="B43" s="74" t="s">
+      <c r="B44" s="74" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="120" t="s">
+    <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="113" t="s">
         <v>512</v>
       </c>
-      <c r="B44" s="118"/>
-    </row>
-    <row r="45" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="s">
+      <c r="B45" s="111"/>
+    </row>
+    <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="57" t="s">
         <v>383</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="B46" s="74" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="57" t="s">
-        <v>513</v>
-      </c>
-      <c r="B46" s="74" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="57" t="s">
+        <v>513</v>
+      </c>
+      <c r="B47" s="74" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="57" t="s">
         <v>515</v>
       </c>
-      <c r="B47" s="74" t="s">
+      <c r="B48" s="74" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="109" t="s">
+    <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="107" t="s">
         <v>372</v>
       </c>
-      <c r="B48" s="109"/>
-    </row>
-    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A49" s="110" t="s">
+      <c r="B49" s="107"/>
+    </row>
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A50" s="110" t="s">
         <v>312</v>
       </c>
-      <c r="B49" s="108"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="115" t="s">
+      <c r="B50" s="109"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="118" t="s">
         <v>321</v>
       </c>
-      <c r="B50" s="62" t="s">
+      <c r="B51" s="62" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="116"/>
-      <c r="B51" s="62" t="s">
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="119"/>
+      <c r="B52" s="62" t="s">
         <v>590</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C52" s="66" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="117"/>
-      <c r="B52" s="62" t="s">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="120"/>
+      <c r="B53" s="62" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="115" t="s">
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="118" t="s">
         <v>322</v>
       </c>
-      <c r="B53" s="62" t="s">
+      <c r="B54" s="62" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
-      <c r="B54" s="62" t="s">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="119"/>
+      <c r="B55" s="62" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="116"/>
-      <c r="B55" s="62" t="s">
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="119"/>
+      <c r="B56" s="62" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="117"/>
-      <c r="B56" s="62" t="s">
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="120"/>
+      <c r="B57" s="62" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="115" t="s">
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="118" t="s">
         <v>323</v>
       </c>
-      <c r="B57" s="62" t="s">
+      <c r="B58" s="62" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="117"/>
-      <c r="B58" s="62" t="s">
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="120"/>
+      <c r="B59" s="62" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="115" t="s">
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="118" t="s">
         <v>324</v>
       </c>
-      <c r="B59" s="62" t="s">
+      <c r="B60" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="C59" s="66" t="s">
+      <c r="C60" s="66" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="116"/>
-      <c r="B60" s="62" t="s">
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="119"/>
+      <c r="B61" s="62" t="s">
         <v>527</v>
       </c>
-      <c r="C60" s="68" t="s">
+      <c r="C61" s="68" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="116"/>
-      <c r="B61" s="62" t="s">
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="119"/>
+      <c r="B62" s="62" t="s">
         <v>587</v>
       </c>
-      <c r="C61" s="68"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="117"/>
-      <c r="B62" s="62" t="s">
+      <c r="C62" s="68"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="120"/>
+      <c r="B63" s="62" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="102" t="s">
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="102" t="s">
         <v>631</v>
       </c>
-      <c r="B63" s="62" t="s">
+      <c r="B64" s="62" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="63" t="s">
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="63" t="s">
         <v>284</v>
       </c>
-      <c r="B64" s="62" t="s">
+      <c r="B65" s="62" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="57" t="s">
+    <row r="66" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="57" t="s">
         <v>285</v>
       </c>
-      <c r="B65" s="62" t="s">
+      <c r="B66" s="62" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="57" t="s">
+    <row r="67" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="57" t="s">
         <v>598</v>
       </c>
-      <c r="B66" s="62" t="s">
+      <c r="B67" s="62" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="57" t="s">
+    <row r="68" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="57" t="s">
         <v>547</v>
       </c>
-      <c r="B67" s="62" t="s">
+      <c r="B68" s="62" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="57" t="s">
+    <row r="69" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="57" t="s">
         <v>286</v>
       </c>
-      <c r="B68" s="62" t="s">
+      <c r="B69" s="62" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="112" t="s">
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="115" t="s">
         <v>290</v>
       </c>
-      <c r="B69" s="62" t="s">
+      <c r="B70" s="62" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="113"/>
-      <c r="B70" s="62" t="s">
+    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="116"/>
+      <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="113"/>
-      <c r="B71" s="62" t="s">
+    <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="116"/>
+      <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="113"/>
-      <c r="B72" s="62" t="s">
+    <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="116"/>
+      <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="113"/>
-      <c r="B73" s="62" t="s">
+    <row r="74" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="116"/>
+      <c r="B74" s="62" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="114"/>
-      <c r="B74" s="62" t="s">
+    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="117"/>
+      <c r="B75" s="62" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="112" t="s">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="115" t="s">
         <v>291</v>
       </c>
-      <c r="B75" s="62" t="s">
+      <c r="B76" s="62" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="113"/>
-      <c r="B76" s="62" t="s">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="116"/>
+      <c r="B77" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="C76" s="67"/>
-    </row>
-    <row r="77" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="113"/>
-      <c r="B77" s="62" t="s">
+      <c r="C77" s="67"/>
+    </row>
+    <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="116"/>
+      <c r="B78" s="62" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="113"/>
-      <c r="B78" s="62" t="s">
+    <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="116"/>
+      <c r="B79" s="62" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="113"/>
-      <c r="B79" s="81" t="s">
+    <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="116"/>
+      <c r="B80" s="81" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="113"/>
-      <c r="B80" s="81" t="s">
+    <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="116"/>
+      <c r="B81" s="81" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="113"/>
-      <c r="B81" s="81" t="s">
+    <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="116"/>
+      <c r="B82" s="81" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="113"/>
-      <c r="B82" s="81" t="s">
+    <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="116"/>
+      <c r="B83" s="81" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A83" s="113"/>
-      <c r="B83" s="81" t="s">
+    <row r="84" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A84" s="116"/>
+      <c r="B84" s="81" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="113"/>
-      <c r="B84" s="81" t="s">
+    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="116"/>
+      <c r="B85" s="81" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="113"/>
-      <c r="B85" s="81" t="s">
+    <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="116"/>
+      <c r="B86" s="81" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="114"/>
-      <c r="B86" s="81" t="s">
+    <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="117"/>
+      <c r="B87" s="81" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="112" t="s">
+    <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="115" t="s">
         <v>292</v>
       </c>
-      <c r="B87" s="82" t="s">
+      <c r="B88" s="82" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="113"/>
-      <c r="B88" s="83" t="s">
+    <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="116"/>
+      <c r="B89" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="113"/>
-      <c r="B89" s="83" t="s">
+      <c r="C89"/>
+    </row>
+    <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="116"/>
+      <c r="B90" s="83" t="s">
         <v>308</v>
       </c>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="114"/>
-      <c r="B90" s="82" t="s">
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="117"/>
+      <c r="B91" s="82" t="s">
         <v>545</v>
       </c>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="112" t="s">
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="115" t="s">
         <v>309</v>
       </c>
-      <c r="B91" s="84" t="s">
+      <c r="B92" s="84" t="s">
         <v>310</v>
       </c>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="114"/>
-      <c r="B92" s="84" t="s">
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A93" s="117"/>
+      <c r="B93" s="84" t="s">
         <v>311</v>
       </c>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="69" t="s">
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="69" t="s">
         <v>335</v>
       </c>
-      <c r="B93" s="83" t="s">
+      <c r="B94" s="83" t="s">
         <v>336</v>
       </c>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="65" t="s">
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="65" t="s">
         <v>334</v>
       </c>
-      <c r="B94" s="84" t="s">
+      <c r="B95" s="84" t="s">
         <v>333</v>
       </c>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="61" t="s">
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A96" s="61" t="s">
         <v>385</v>
       </c>
-      <c r="B95" s="85" t="s">
+      <c r="B96" s="85" t="s">
         <v>328</v>
       </c>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="71" t="s">
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="71" t="s">
         <v>373</v>
       </c>
-      <c r="B96" s="84" t="s">
+      <c r="B97" s="84" t="s">
         <v>531</v>
       </c>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="90" t="s">
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="90" t="s">
         <v>528</v>
       </c>
-      <c r="B97" s="81" t="s">
+      <c r="B98" s="81" t="s">
         <v>742</v>
       </c>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="73" t="s">
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="73" t="s">
         <v>375</v>
       </c>
-      <c r="B98" s="81" t="s">
+      <c r="B99" s="81" t="s">
         <v>374</v>
       </c>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="109" t="s">
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="107" t="s">
         <v>388</v>
       </c>
-      <c r="B99" s="109"/>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="110" t="s">
+      <c r="B100" s="107"/>
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A101" s="110" t="s">
         <v>389</v>
       </c>
-      <c r="B100" s="108"/>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="70" t="s">
+      <c r="B101" s="109"/>
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="70" t="s">
         <v>390</v>
       </c>
-      <c r="B101" s="60" t="s">
+      <c r="B102" s="60" t="s">
         <v>391</v>
-      </c>
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="70" t="s">
-        <v>392</v>
-      </c>
-      <c r="B102" s="76" t="s">
-        <v>393</v>
       </c>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="70" t="s">
+        <v>392</v>
+      </c>
+      <c r="B103" s="76" t="s">
+        <v>393</v>
+      </c>
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="70" t="s">
         <v>394</v>
       </c>
-      <c r="B103" s="76" t="s">
+      <c r="B104" s="76" t="s">
         <v>395</v>
       </c>
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A104" s="110" t="s">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A105" s="110" t="s">
         <v>396</v>
       </c>
-      <c r="B104" s="108"/>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="57" t="s">
+      <c r="B105" s="109"/>
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A106" s="57" t="s">
         <v>398</v>
       </c>
-      <c r="B105" s="80" t="s">
+      <c r="B106" s="80" t="s">
         <v>397</v>
       </c>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="57" t="s">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="57" t="s">
         <v>399</v>
       </c>
-      <c r="B106" s="80" t="s">
+      <c r="B107" s="80" t="s">
         <v>400</v>
       </c>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A107" s="72" t="s">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A108" s="72" t="s">
         <v>401</v>
       </c>
-      <c r="B107" s="80" t="s">
+      <c r="B108" s="80" t="s">
         <v>402</v>
       </c>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A108" s="57" t="s">
+      <c r="C108"/>
+    </row>
+    <row r="109" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A109" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="B108" s="80" t="s">
+      <c r="B109" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="C108"/>
-    </row>
-    <row r="109" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="57" t="s">
+      <c r="C109"/>
+    </row>
+    <row r="110" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="B109" s="80" t="s">
+      <c r="B110" s="80" t="s">
         <v>406</v>
-      </c>
-      <c r="C109"/>
-    </row>
-    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="57" t="s">
-        <v>407</v>
-      </c>
-      <c r="B110" s="79" t="s">
-        <v>408</v>
       </c>
       <c r="C110"/>
     </row>
     <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A111" s="57" t="s">
+        <v>407</v>
+      </c>
+      <c r="B111" s="79" t="s">
+        <v>408</v>
+      </c>
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="B111" s="79" t="s">
+      <c r="B112" s="79" t="s">
         <v>410</v>
       </c>
-      <c r="C111"/>
-    </row>
-    <row r="112" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A112" s="57" t="s">
+      <c r="C112"/>
+    </row>
+    <row r="113" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A113" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="B112" s="86" t="s">
+      <c r="B113" s="86" t="s">
         <v>412</v>
       </c>
-      <c r="C112"/>
-    </row>
-    <row r="113" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="57" t="s">
+      <c r="C113"/>
+    </row>
+    <row r="114" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="57" t="s">
         <v>421</v>
       </c>
-      <c r="B113" s="80" t="s">
+      <c r="B114" s="80" t="s">
         <v>413</v>
-      </c>
-      <c r="C113"/>
-    </row>
-    <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="57" t="s">
-        <v>420</v>
-      </c>
-      <c r="B114" s="79" t="s">
-        <v>414</v>
       </c>
       <c r="C114"/>
     </row>
     <row r="115" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A115" s="57" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B115" s="79" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C115"/>
     </row>
     <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A116" s="57" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B116" s="79" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C116"/>
     </row>
     <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
+        <v>416</v>
+      </c>
+      <c r="B117" s="79" t="s">
+        <v>417</v>
+      </c>
+      <c r="C117"/>
+    </row>
+    <row r="118" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="57" t="s">
         <v>418</v>
       </c>
-      <c r="B117" s="79" t="s">
+      <c r="B118" s="79" t="s">
         <v>422</v>
       </c>
-      <c r="C117"/>
-    </row>
-    <row r="118" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A118" s="57" t="s">
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A119" s="57" t="s">
         <v>423</v>
       </c>
-      <c r="B118" s="79" t="s">
+      <c r="B119" s="79" t="s">
         <v>424</v>
       </c>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="72" t="s">
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="72" t="s">
         <v>425</v>
       </c>
-      <c r="B119" s="80" t="s">
+      <c r="B120" s="80" t="s">
         <v>426</v>
       </c>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="92" t="s">
+      <c r="C120"/>
+    </row>
+    <row r="121" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A121" s="92" t="s">
         <v>534</v>
       </c>
-      <c r="B120" s="91" t="s">
+      <c r="B121" s="91" t="s">
         <v>535</v>
       </c>
-      <c r="C120"/>
-    </row>
-    <row r="121" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A121" s="110" t="s">
+      <c r="C121"/>
+    </row>
+    <row r="122" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A122" s="110" t="s">
         <v>427</v>
       </c>
-      <c r="B121" s="108"/>
-      <c r="C121"/>
-    </row>
-    <row r="122" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="57" t="s">
-        <v>432</v>
-      </c>
-      <c r="B122" s="79" t="s">
-        <v>431</v>
-      </c>
+      <c r="B122" s="109"/>
       <c r="C122"/>
     </row>
     <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A123" s="57" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B123" s="79" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C123"/>
     </row>
     <row r="124" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A124" s="57" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B124" s="79" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
+        <v>434</v>
+      </c>
+      <c r="B125" s="79" t="s">
+        <v>429</v>
+      </c>
+      <c r="C125"/>
+    </row>
+    <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="B125" s="79" t="s">
+      <c r="B126" s="79" t="s">
         <v>428</v>
       </c>
-      <c r="C125"/>
-    </row>
-    <row r="126" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="70" t="s">
+      <c r="C126"/>
+    </row>
+    <row r="127" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="70" t="s">
         <v>439</v>
       </c>
-      <c r="B126" s="79" t="s">
+      <c r="B127" s="79" t="s">
         <v>436</v>
       </c>
-      <c r="C126"/>
-    </row>
-    <row r="127" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A127" s="57" t="s">
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A128" s="57" t="s">
         <v>438</v>
       </c>
-      <c r="B127" s="79" t="s">
+      <c r="B128" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A128" s="70" t="s">
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A129" s="70" t="s">
         <v>440</v>
       </c>
-      <c r="B128" s="80" t="s">
+      <c r="B129" s="80" t="s">
         <v>441</v>
       </c>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="57" t="s">
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="57" t="s">
         <v>442</v>
       </c>
-      <c r="B129" s="79" t="s">
+      <c r="B130" s="79" t="s">
         <v>443</v>
       </c>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A130" s="57" t="s">
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A131" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="B130" s="80" t="s">
+      <c r="B131" s="80" t="s">
         <v>445</v>
       </c>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A131" s="110" t="s">
+      <c r="C131"/>
+    </row>
+    <row r="132" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A132" s="110" t="s">
         <v>499</v>
       </c>
-      <c r="B131" s="108"/>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A132" s="57" t="s">
+      <c r="B132" s="109"/>
+      <c r="C132"/>
+    </row>
+    <row r="133" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A133" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="B132" s="80" t="s">
+      <c r="B133" s="80" t="s">
         <v>498</v>
       </c>
-      <c r="C132"/>
-    </row>
-    <row r="133" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A133" s="57" t="s">
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A134" s="57" t="s">
         <v>447</v>
       </c>
-      <c r="B133" s="80" t="s">
+      <c r="B134" s="80" t="s">
         <v>448</v>
-      </c>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="57" t="s">
-        <v>449</v>
-      </c>
-      <c r="B134" s="79" t="s">
-        <v>450</v>
       </c>
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A135" s="57" t="s">
+        <v>449</v>
+      </c>
+      <c r="B135" s="79" t="s">
+        <v>450</v>
+      </c>
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="57" t="s">
         <v>451</v>
       </c>
-      <c r="B135" s="79" t="s">
+      <c r="B136" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="70" t="s">
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A137" s="70" t="s">
         <v>453</v>
       </c>
-      <c r="B136" s="79" t="s">
+      <c r="B137" s="79" t="s">
         <v>454</v>
       </c>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" ht="103.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="77" t="s">
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="1:3" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="77" t="s">
         <v>456</v>
       </c>
-      <c r="B137" s="80" t="s">
+      <c r="B138" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="A138" s="78" t="s">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="1:3" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="A139" s="78" t="s">
         <v>457</v>
       </c>
-      <c r="B138" s="97" t="s">
+      <c r="B139" s="97" t="s">
         <v>458</v>
       </c>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A139" s="78" t="s">
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A140" s="78" t="s">
         <v>459</v>
       </c>
-      <c r="B139" s="97" t="s">
+      <c r="B140" s="97" t="s">
         <v>550</v>
-      </c>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
-      <c r="A140" s="78" t="s">
-        <v>460</v>
-      </c>
-      <c r="B140" s="97" t="s">
-        <v>549</v>
       </c>
       <c r="C140"/>
     </row>
     <row r="141" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
       <c r="A141" s="78" t="s">
+        <v>460</v>
+      </c>
+      <c r="B141" s="97" t="s">
+        <v>549</v>
+      </c>
+      <c r="C141"/>
+    </row>
+    <row r="142" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
+      <c r="A142" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="B141" s="97" t="s">
+      <c r="B142" s="97" t="s">
         <v>548</v>
       </c>
-      <c r="C141"/>
-    </row>
-    <row r="142" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="107" t="s">
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A143" s="108" t="s">
         <v>462</v>
       </c>
-      <c r="B142" s="108"/>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A143" s="78" t="s">
+      <c r="B143" s="109"/>
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A144" s="78" t="s">
         <v>464</v>
       </c>
-      <c r="B143" s="80" t="s">
+      <c r="B144" s="80" t="s">
         <v>463</v>
       </c>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A144" s="70" t="s">
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A145" s="70" t="s">
         <v>465</v>
       </c>
-      <c r="B144" s="86" t="s">
+      <c r="B145" s="86" t="s">
         <v>468</v>
       </c>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A145" s="78" t="s">
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A146" s="78" t="s">
         <v>466</v>
       </c>
-      <c r="B145" s="80" t="s">
+      <c r="B146" s="80" t="s">
         <v>467</v>
       </c>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="107" t="s">
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A147" s="108" t="s">
         <v>470</v>
       </c>
-      <c r="B146" s="108"/>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A147" s="70" t="s">
+      <c r="B147" s="109"/>
+      <c r="C147"/>
+    </row>
+    <row r="148" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A148" s="70" t="s">
         <v>469</v>
       </c>
-      <c r="B147" s="87" t="s">
+      <c r="B148" s="87" t="s">
         <v>471</v>
       </c>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A148" s="57" t="s">
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A149" s="57" t="s">
         <v>538</v>
       </c>
-      <c r="B148" s="87" t="s">
+      <c r="B149" s="87" t="s">
         <v>539</v>
       </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A149" s="107" t="s">
+      <c r="C149"/>
+    </row>
+    <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="108" t="s">
         <v>540</v>
       </c>
-      <c r="B149" s="108"/>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A150" s="57" t="s">
-        <v>541</v>
-      </c>
-      <c r="B150" s="80" t="s">
-        <v>544</v>
-      </c>
-      <c r="C150" s="11" t="s">
-        <v>594</v>
-      </c>
+      <c r="B150" s="109"/>
+      <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" s="57" t="s">
-        <v>542</v>
-      </c>
-      <c r="B151" s="76" t="s">
-        <v>543</v>
-      </c>
-      <c r="C151"/>
+        <v>541</v>
+      </c>
+      <c r="B151" s="80" t="s">
+        <v>544</v>
+      </c>
+      <c r="C151" s="11" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="152" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A152" s="57" t="s">
+        <v>542</v>
+      </c>
+      <c r="B152" s="76" t="s">
+        <v>543</v>
+      </c>
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A153" s="57" t="s">
         <v>596</v>
       </c>
-      <c r="B152" s="98" t="s">
+      <c r="B153" s="98" t="s">
         <v>595</v>
       </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="109" t="s">
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="57" t="s">
+        <v>744</v>
+      </c>
+      <c r="B154" s="98" t="s">
+        <v>745</v>
+      </c>
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="107" t="s">
         <v>472</v>
       </c>
-      <c r="B153" s="109"/>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A154" s="110" t="s">
+      <c r="B155" s="107"/>
+      <c r="C155"/>
+    </row>
+    <row r="156" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A156" s="110" t="s">
         <v>475</v>
       </c>
-      <c r="B154" s="108"/>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A155" s="57" t="s">
+      <c r="B156" s="109"/>
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A157" s="57" t="s">
         <v>537</v>
       </c>
-      <c r="B155" s="76" t="s">
+      <c r="B157" s="76" t="s">
         <v>536</v>
       </c>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A156" s="57" t="s">
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A158" s="57" t="s">
         <v>529</v>
       </c>
-      <c r="B156" s="80" t="s">
+      <c r="B158" s="80" t="s">
         <v>530</v>
       </c>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="57"/>
-      <c r="B157" s="80"/>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="57"/>
-      <c r="B158" s="80"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="70"/>
+      <c r="A159" s="57"/>
+      <c r="B159" s="80"/>
       <c r="C159"/>
     </row>
-    <row r="160" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A160" s="107" t="s">
+    <row r="160" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A160" s="57"/>
+      <c r="B160" s="80"/>
+      <c r="C160"/>
+    </row>
+    <row r="161" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A161" s="70"/>
+      <c r="C161"/>
+    </row>
+    <row r="162" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A162" s="108" t="s">
         <v>478</v>
       </c>
-      <c r="B160" s="111"/>
-      <c r="C160"/>
-    </row>
-    <row r="161" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A161" s="57" t="s">
+      <c r="B162" s="121"/>
+      <c r="C162"/>
+    </row>
+    <row r="163" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A163" s="57" t="s">
         <v>477</v>
       </c>
-      <c r="B161" s="76" t="s">
+      <c r="B163" s="76" t="s">
         <v>476</v>
-      </c>
-      <c r="C161"/>
-    </row>
-    <row r="162" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A162" s="57" t="s">
-        <v>483</v>
-      </c>
-      <c r="B162" s="76" t="s">
-        <v>479</v>
-      </c>
-      <c r="C162"/>
-    </row>
-    <row r="163" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A163" s="57" t="s">
-        <v>481</v>
-      </c>
-      <c r="B163" s="76" t="s">
-        <v>480</v>
       </c>
       <c r="C163"/>
     </row>
     <row r="164" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A164" s="57" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B164" s="76" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A165" s="57" t="s">
+        <v>481</v>
+      </c>
+      <c r="B165" s="76" t="s">
+        <v>480</v>
+      </c>
+      <c r="C165"/>
+    </row>
+    <row r="166" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A166" s="57" t="s">
+        <v>482</v>
+      </c>
+      <c r="B166" s="76" t="s">
+        <v>476</v>
+      </c>
+      <c r="C166"/>
+    </row>
+    <row r="167" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A167" s="57" t="s">
         <v>484</v>
       </c>
-      <c r="B165" s="76" t="s">
+      <c r="B167" s="76" t="s">
         <v>485</v>
       </c>
-      <c r="C165"/>
-    </row>
-    <row r="166" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A166" s="57" t="s">
+      <c r="C167"/>
+    </row>
+    <row r="168" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A168" s="57" t="s">
         <v>486</v>
       </c>
-      <c r="B166" s="76" t="s">
+      <c r="B168" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="C166"/>
-    </row>
-    <row r="167" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="57" t="s">
+      <c r="C168"/>
+    </row>
+    <row r="169" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A169" s="57" t="s">
         <v>496</v>
       </c>
-      <c r="B167" s="88" t="s">
+      <c r="B169" s="88" t="s">
         <v>497</v>
       </c>
-      <c r="C167"/>
-    </row>
-    <row r="168" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A168" s="110" t="s">
+      <c r="C169"/>
+    </row>
+    <row r="170" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A170" s="110" t="s">
         <v>473</v>
       </c>
-      <c r="B168" s="108"/>
-      <c r="C168"/>
-    </row>
-    <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A169" s="57" t="s">
+      <c r="B170" s="109"/>
+      <c r="C170"/>
+    </row>
+    <row r="171" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A171" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="B169" s="76" t="s">
+      <c r="B171" s="76" t="s">
         <v>489</v>
       </c>
-      <c r="C169"/>
-    </row>
-    <row r="170" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A170" s="57" t="s">
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A172" s="57" t="s">
         <v>491</v>
       </c>
-      <c r="B170" s="76" t="s">
+      <c r="B172" s="76" t="s">
         <v>490</v>
       </c>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A171" s="110" t="s">
+      <c r="C172"/>
+    </row>
+    <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A173" s="110" t="s">
         <v>474</v>
       </c>
-      <c r="B171" s="108"/>
-      <c r="C171"/>
-    </row>
-    <row r="172" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A172" s="57" t="s">
+      <c r="B173" s="109"/>
+      <c r="C173"/>
+    </row>
+    <row r="174" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A174" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="B172" s="76" t="s">
+      <c r="B174" s="76" t="s">
         <v>493</v>
       </c>
-      <c r="C172"/>
-    </row>
-    <row r="173" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A173" s="57" t="s">
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A175" s="57" t="s">
         <v>494</v>
       </c>
-      <c r="B173" s="76" t="s">
+      <c r="B175" s="76" t="s">
         <v>495</v>
       </c>
-      <c r="C173"/>
-    </row>
-    <row r="174" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A174" s="109" t="s">
+      <c r="C175"/>
+    </row>
+    <row r="176" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A176" s="107" t="s">
         <v>551</v>
       </c>
-      <c r="B174" s="109"/>
-      <c r="C174"/>
-    </row>
-    <row r="175" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A175" s="110" t="s">
+      <c r="B176" s="107"/>
+      <c r="C176"/>
+    </row>
+    <row r="177" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A177" s="110" t="s">
         <v>552</v>
       </c>
-      <c r="B175" s="108"/>
-      <c r="C175"/>
-    </row>
-    <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A176" s="57" t="s">
+      <c r="B177" s="109"/>
+      <c r="C177"/>
+    </row>
+    <row r="178" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A178" s="57" t="s">
         <v>553</v>
       </c>
-      <c r="B176" s="76" t="s">
+      <c r="B178" s="76" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A177" s="57"/>
-      <c r="B177" s="76"/>
-    </row>
-    <row r="178" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A178" s="110" t="s">
+    <row r="179" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A179" s="57"/>
+      <c r="B179" s="76"/>
+    </row>
+    <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A180" s="110" t="s">
         <v>551</v>
       </c>
-      <c r="B178" s="108"/>
-      <c r="C178"/>
-    </row>
-    <row r="179" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A179" s="57" t="s">
+      <c r="B180" s="109"/>
+      <c r="C180"/>
+    </row>
+    <row r="181" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A181" s="57" t="s">
         <v>555</v>
       </c>
-      <c r="B179" s="76" t="s">
+      <c r="B181" s="76" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A180" s="57" t="s">
+    <row r="182" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A182" s="57" t="s">
         <v>557</v>
       </c>
-      <c r="B180" s="76" t="s">
+      <c r="B182" s="76" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A181" s="57" t="s">
+    <row r="183" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A183" s="57" t="s">
         <v>559</v>
       </c>
-      <c r="B181" s="76" t="s">
+      <c r="B183" s="76" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="57" t="s">
+    <row r="184" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A184" s="57" t="s">
         <v>562</v>
       </c>
-      <c r="B182" s="76" t="s">
+      <c r="B184" s="76" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A183" s="57" t="s">
+    <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" s="57" t="s">
         <v>564</v>
       </c>
-      <c r="B183" s="76" t="s">
+      <c r="B185" s="76" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="57" t="s">
+    <row r="186" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
+      <c r="A186" s="57" t="s">
         <v>565</v>
       </c>
-      <c r="B184" s="80" t="s">
+      <c r="B186" s="80" t="s">
         <v>566</v>
       </c>
-      <c r="C184" s="95" t="s">
+      <c r="C186" s="95" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
-      <c r="A185" s="57" t="s">
+    <row r="187" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
+      <c r="A187" s="57" t="s">
         <v>567</v>
       </c>
-      <c r="B185" s="80" t="s">
+      <c r="B187" s="80" t="s">
         <v>568</v>
       </c>
-      <c r="C185" s="95" t="s">
+      <c r="C187" s="95" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A186" s="57" t="s">
+    <row r="188" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A188" s="57" t="s">
         <v>569</v>
       </c>
-      <c r="B186" s="76" t="s">
+      <c r="B188" s="76" t="s">
         <v>570</v>
       </c>
-      <c r="C186" s="94" t="s">
+      <c r="C188" s="94" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="57"/>
-      <c r="B187" s="76"/>
-    </row>
-    <row r="188" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A188" s="110" t="s">
+    <row r="189" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A189" s="57"/>
+      <c r="B189" s="76"/>
+    </row>
+    <row r="190" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A190" s="110" t="s">
         <v>574</v>
       </c>
-      <c r="B188" s="108"/>
-      <c r="C188"/>
-    </row>
-    <row r="189" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A189" s="57" t="s">
+      <c r="B190" s="109"/>
+      <c r="C190"/>
+    </row>
+    <row r="191" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A191" s="57" t="s">
         <v>575</v>
       </c>
-      <c r="B189" s="76" t="s">
+      <c r="B191" s="76" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A190" s="57"/>
-      <c r="B190" s="76" t="s">
+    <row r="192" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A192" s="57"/>
+      <c r="B192" s="76" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A191" s="107" t="s">
+    <row r="193" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A193" s="108" t="s">
         <v>578</v>
       </c>
-      <c r="B191" s="108"/>
-    </row>
-    <row r="192" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A192" s="57" t="s">
+      <c r="B193" s="109"/>
+    </row>
+    <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A194" s="57" t="s">
         <v>579</v>
       </c>
-      <c r="B192" s="76" t="s">
+      <c r="B194" s="76" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A193" s="57" t="s">
+    <row r="195" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A195" s="57" t="s">
         <v>581</v>
       </c>
-      <c r="B193" s="76" t="s">
+      <c r="B195" s="76" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A194" s="57" t="s">
+    <row r="196" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A196" s="57" t="s">
         <v>585</v>
       </c>
-      <c r="B194" s="96" t="s">
+      <c r="B196" s="96" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A195" s="57" t="s">
+    <row r="197" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A197" s="57" t="s">
         <v>583</v>
       </c>
-      <c r="B195" s="96" t="s">
+      <c r="B197" s="96" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A196" s="109" t="s">
+    <row r="198" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A198" s="107" t="s">
         <v>599</v>
       </c>
-      <c r="B196" s="109"/>
-      <c r="C196"/>
-    </row>
-    <row r="197" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A197" s="107" t="s">
+      <c r="B198" s="107"/>
+      <c r="C198"/>
+    </row>
+    <row r="199" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A199" s="108" t="s">
         <v>601</v>
       </c>
-      <c r="B197" s="108"/>
-    </row>
-    <row r="198" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A198" s="57" t="s">
-        <v>602</v>
-      </c>
-      <c r="B198" s="100" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A199" s="57" t="s">
-        <v>604</v>
-      </c>
-      <c r="B199" s="100" t="s">
-        <v>606</v>
-      </c>
+      <c r="B199" s="109"/>
     </row>
     <row r="200" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A200" s="57" t="s">
+        <v>602</v>
+      </c>
+      <c r="B200" s="100" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A201" s="57" t="s">
+        <v>604</v>
+      </c>
+      <c r="B201" s="100" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A202" s="57" t="s">
         <v>605</v>
       </c>
-      <c r="B200" s="100" t="s">
+      <c r="B202" s="100" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A201" s="57" t="s">
+    <row r="203" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A203" s="57" t="s">
         <v>609</v>
       </c>
-      <c r="B201" s="101" t="s">
+      <c r="B203" s="101" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A202" s="57" t="s">
+    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="57" t="s">
         <v>611</v>
       </c>
-      <c r="B202" s="100" t="s">
+      <c r="B204" s="100" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="57"/>
-      <c r="B203" s="99"/>
-    </row>
-    <row r="204" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A204" s="107" t="s">
+    <row r="205" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A205" s="57"/>
+      <c r="B205" s="99"/>
+    </row>
+    <row r="206" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A206" s="108" t="s">
         <v>612</v>
       </c>
-      <c r="B204" s="108"/>
-    </row>
-    <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A205" s="57" t="s">
+      <c r="B206" s="109"/>
+    </row>
+    <row r="207" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A207" s="57" t="s">
         <v>613</v>
       </c>
-      <c r="B205" s="76" t="s">
+      <c r="B207" s="76" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="57"/>
-      <c r="B206" s="76"/>
-    </row>
-    <row r="207" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A207" s="57"/>
-      <c r="B207" s="76"/>
     </row>
     <row r="208" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A208" s="57"/>
@@ -12828,556 +12885,559 @@
       <c r="A212" s="57"/>
       <c r="B212" s="76"/>
     </row>
-    <row r="213" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A213" s="107" t="s">
+    <row r="213" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A213" s="57"/>
+      <c r="B213" s="76"/>
+    </row>
+    <row r="214" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A214" s="57"/>
+      <c r="B214" s="76"/>
+    </row>
+    <row r="215" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A215" s="108" t="s">
         <v>614</v>
       </c>
-      <c r="B213" s="108"/>
-    </row>
-    <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A214" s="72" t="s">
+      <c r="B215" s="109"/>
+    </row>
+    <row r="216" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A216" s="72" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="76" t="s">
+      <c r="B216" s="76" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A215" s="107" t="s">
+    <row r="217" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A217" s="108" t="s">
         <v>618</v>
       </c>
-      <c r="B215" s="108"/>
-    </row>
-    <row r="216" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A216" s="57" t="s">
+      <c r="B217" s="109"/>
+    </row>
+    <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A218" s="57" t="s">
         <v>619</v>
       </c>
-      <c r="B216" s="76" t="s">
+      <c r="B218" s="76" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A217" s="57" t="s">
+    <row r="219" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A219" s="57" t="s">
         <v>622</v>
       </c>
-      <c r="B217" s="76" t="s">
+      <c r="B219" s="76" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A218" s="107" t="s">
+    <row r="220" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A220" s="108" t="s">
         <v>617</v>
       </c>
-      <c r="B218" s="108"/>
-    </row>
-    <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A219" s="57" t="s">
+      <c r="B220" s="109"/>
+    </row>
+    <row r="221" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A221" s="57" t="s">
         <v>600</v>
       </c>
-      <c r="B219" s="80" t="s">
+      <c r="B221" s="80" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A220" s="57" t="s">
+    <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A222" s="57" t="s">
         <v>623</v>
       </c>
-      <c r="B220" s="76" t="s">
+      <c r="B222" s="76" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A221" s="57" t="s">
+    <row r="223" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A223" s="57" t="s">
         <v>624</v>
       </c>
-      <c r="B221" s="76" t="s">
+      <c r="B223" s="76" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A222" s="57" t="s">
+    <row r="224" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A224" s="57" t="s">
         <v>628</v>
       </c>
-      <c r="B222" s="76" t="s">
+      <c r="B224" s="76" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="109" t="s">
+    <row r="225" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A225" s="107" t="s">
         <v>633</v>
       </c>
-      <c r="B223" s="109"/>
-    </row>
-    <row r="224" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A224" s="107" t="s">
+      <c r="B225" s="107"/>
+    </row>
+    <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A226" s="108" t="s">
         <v>635</v>
       </c>
-      <c r="B224" s="108"/>
-    </row>
-    <row r="225" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A225" s="107" t="s">
+      <c r="B226" s="109"/>
+    </row>
+    <row r="227" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A227" s="108" t="s">
         <v>634</v>
       </c>
-      <c r="B225" s="108"/>
-    </row>
-    <row r="226" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A226" s="57" t="s">
+      <c r="B227" s="109"/>
+    </row>
+    <row r="228" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A228" s="57" t="s">
         <v>636</v>
       </c>
-      <c r="B226" s="76" t="s">
+      <c r="B228" s="76" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A227" s="107" t="s">
+    <row r="229" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A229" s="108" t="s">
         <v>638</v>
       </c>
-      <c r="B227" s="108"/>
-    </row>
-    <row r="228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A228" s="57" t="s">
+      <c r="B229" s="109"/>
+    </row>
+    <row r="230" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A230" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="B228" s="76" t="s">
+      <c r="B230" s="76" t="s">
         <v>639</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A229" s="57" t="s">
-        <v>640</v>
-      </c>
-      <c r="B229" s="76" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A230" s="57" t="s">
-        <v>642</v>
-      </c>
-      <c r="B230" s="76" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="57" t="s">
+        <v>640</v>
+      </c>
+      <c r="B231" s="76" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A232" s="57" t="s">
+        <v>642</v>
+      </c>
+      <c r="B232" s="76" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A233" s="57" t="s">
         <v>644</v>
       </c>
-      <c r="B231" s="76" t="s">
+      <c r="B233" s="76" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A232" s="57" t="s">
+    <row r="234" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A234" s="57" t="s">
         <v>646</v>
       </c>
-      <c r="B232" s="76" t="s">
+      <c r="B234" s="76" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A233" s="107" t="s">
+    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A235" s="108" t="s">
         <v>648</v>
       </c>
-      <c r="B233" s="108"/>
-    </row>
-    <row r="234" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A234" s="57" t="s">
+      <c r="B235" s="109"/>
+    </row>
+    <row r="236" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A236" s="57" t="s">
         <v>649</v>
       </c>
-      <c r="B234" s="76" t="s">
+      <c r="B236" s="76" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="107" t="s">
+    <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A237" s="108" t="s">
         <v>651</v>
       </c>
-      <c r="B235" s="108"/>
-    </row>
-    <row r="236" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A236" s="57" t="s">
+      <c r="B237" s="109"/>
+    </row>
+    <row r="238" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A238" s="57" t="s">
         <v>653</v>
       </c>
-      <c r="B236" s="76"/>
-    </row>
-    <row r="237" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A237" s="57" t="s">
-        <v>652</v>
-      </c>
-      <c r="B237" s="76" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A238" s="107" t="s">
-        <v>655</v>
-      </c>
-      <c r="B238" s="108"/>
+      <c r="B238" s="76"/>
     </row>
     <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="57" t="s">
+        <v>652</v>
+      </c>
+      <c r="B239" s="76" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A240" s="108" t="s">
+        <v>655</v>
+      </c>
+      <c r="B240" s="109"/>
+    </row>
+    <row r="241" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A241" s="57" t="s">
         <v>656</v>
       </c>
-      <c r="B239" s="76" t="s">
+      <c r="B241" s="76" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A240" s="57" t="s">
+    <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A242" s="57" t="s">
         <v>658</v>
       </c>
-      <c r="B240" s="76" t="s">
+      <c r="B242" s="76" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A241" s="57" t="s">
+    <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A243" s="57" t="s">
         <v>660</v>
       </c>
-      <c r="B241" s="76" t="s">
+      <c r="B243" s="76" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A242" s="57" t="s">
+    <row r="244" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A244" s="57" t="s">
         <v>662</v>
       </c>
-      <c r="B242" s="76" t="s">
+      <c r="B244" s="76" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A243" s="57" t="s">
+    <row r="245" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A245" s="57" t="s">
         <v>664</v>
       </c>
-      <c r="B243" s="76" t="s">
+      <c r="B245" s="76" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A244" s="57" t="s">
+    <row r="246" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A246" s="57" t="s">
         <v>666</v>
       </c>
-      <c r="B244" s="76" t="s">
+      <c r="B246" s="76" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A245" s="57" t="s">
+    <row r="247" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A247" s="57" t="s">
         <v>668</v>
       </c>
-      <c r="B245" s="76" t="s">
+      <c r="B247" s="76" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A246" s="57" t="s">
+    <row r="248" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A248" s="57" t="s">
         <v>670</v>
       </c>
-      <c r="B246" s="76" t="s">
+      <c r="B248" s="76" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A247" s="57" t="s">
+    <row r="249" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A249" s="57" t="s">
         <v>672</v>
       </c>
-      <c r="B247" s="76" t="s">
+      <c r="B249" s="76" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A248" s="57" t="s">
+    <row r="250" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A250" s="57" t="s">
         <v>674</v>
       </c>
-      <c r="B248" s="76" t="s">
+      <c r="B250" s="76" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="57" t="s">
+    <row r="251" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A251" s="57" t="s">
         <v>676</v>
       </c>
-      <c r="B249" s="76" t="s">
+      <c r="B251" s="76" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A250" s="57" t="s">
+    <row r="252" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A252" s="57" t="s">
         <v>678</v>
       </c>
-      <c r="B250" s="76" t="s">
+      <c r="B252" s="76" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A251" s="57" t="s">
+    <row r="253" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A253" s="57" t="s">
         <v>680</v>
       </c>
-      <c r="B251" s="76" t="s">
+      <c r="B253" s="76" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A252" s="57" t="s">
+    <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A254" s="57" t="s">
         <v>682</v>
       </c>
-      <c r="B252" s="76" t="s">
+      <c r="B254" s="76" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A253" s="57" t="s">
+    <row r="255" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A255" s="57" t="s">
         <v>684</v>
       </c>
-      <c r="B253" s="76" t="s">
+      <c r="B255" s="76" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A254" s="57" t="s">
+    <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A256" s="57" t="s">
         <v>686</v>
       </c>
-      <c r="B254" s="76" t="s">
+      <c r="B256" s="76" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A255" s="57" t="s">
+    <row r="257" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A257" s="57" t="s">
         <v>688</v>
       </c>
-      <c r="B255" s="76" t="s">
+      <c r="B257" s="76" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A256" s="57" t="s">
+    <row r="258" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A258" s="57" t="s">
         <v>690</v>
       </c>
-      <c r="B256" s="76" t="s">
+      <c r="B258" s="76" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A257" s="107" t="s">
+    <row r="259" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A259" s="108" t="s">
         <v>692</v>
       </c>
-      <c r="B257" s="108"/>
-    </row>
-    <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A258" s="57" t="s">
+      <c r="B259" s="109"/>
+    </row>
+    <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A260" s="57" t="s">
         <v>693</v>
       </c>
-      <c r="B258" s="76" t="s">
+      <c r="B260" s="76" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A259" s="57" t="s">
+    <row r="261" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A261" s="57" t="s">
         <v>695</v>
       </c>
-      <c r="B259" s="76" t="s">
+      <c r="B261" s="76" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A260" s="57" t="s">
+    <row r="262" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A262" s="57" t="s">
         <v>698</v>
       </c>
-      <c r="B260" s="76" t="s">
+      <c r="B262" s="76" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A261" s="107" t="s">
+    <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A263" s="108" t="s">
         <v>700</v>
       </c>
-      <c r="B261" s="108"/>
-    </row>
-    <row r="262" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A262" s="57" t="s">
+      <c r="B263" s="109"/>
+    </row>
+    <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A264" s="57" t="s">
         <v>701</v>
       </c>
-      <c r="B262" s="76" t="s">
+      <c r="B264" s="76" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="109" t="s">
+    <row r="265" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A265" s="107" t="s">
         <v>703</v>
       </c>
-      <c r="B263" s="109"/>
-    </row>
-    <row r="264" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A264" s="107" t="s">
+      <c r="B265" s="107"/>
+    </row>
+    <row r="266" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A266" s="108" t="s">
         <v>704</v>
       </c>
-      <c r="B264" s="108"/>
-    </row>
-    <row r="265" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A265" s="57" t="s">
-        <v>704</v>
-      </c>
-      <c r="B265" s="76" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A266" s="57" t="s">
-        <v>707</v>
-      </c>
-      <c r="B266" s="104" t="s">
-        <v>708</v>
-      </c>
+      <c r="B266" s="109"/>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A267" s="57" t="s">
+        <v>704</v>
+      </c>
+      <c r="B267" s="76" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A268" s="57" t="s">
+        <v>707</v>
+      </c>
+      <c r="B268" s="104" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A269" s="57" t="s">
         <v>709</v>
       </c>
-      <c r="B267" s="104" t="s">
+      <c r="B269" s="104" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A268" s="57" t="s">
+    <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A270" s="57" t="s">
         <v>711</v>
       </c>
-      <c r="B268" s="76" t="s">
+      <c r="B270" s="76" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A269" s="107" t="s">
+    <row r="271" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A271" s="108" t="s">
         <v>713</v>
       </c>
-      <c r="B269" s="108"/>
-    </row>
-    <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A270" s="57" t="s">
-        <v>714</v>
-      </c>
-      <c r="B270" s="104" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A271" s="57" t="s">
-        <v>716</v>
-      </c>
-      <c r="B271" s="104" t="s">
-        <v>717</v>
-      </c>
+      <c r="B271" s="109"/>
     </row>
     <row r="272" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A272" s="57" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B272" s="104" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A273" s="57" t="s">
+        <v>716</v>
+      </c>
+      <c r="B273" s="104" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A274" s="57" t="s">
+        <v>718</v>
+      </c>
+      <c r="B274" s="104" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A275" s="57" t="s">
         <v>720</v>
       </c>
-      <c r="B273" s="104" t="s">
+      <c r="B275" s="104" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="274" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A274" s="107" t="s">
+    <row r="276" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A276" s="108" t="s">
         <v>705</v>
       </c>
-      <c r="B274" s="108"/>
-    </row>
-    <row r="275" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A275" s="57" t="s">
+      <c r="B276" s="109"/>
+    </row>
+    <row r="277" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A277" s="57" t="s">
         <v>722</v>
       </c>
-      <c r="B275" s="105" t="s">
+      <c r="B277" s="105" t="s">
         <v>723</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A276" s="57" t="s">
-        <v>724</v>
-      </c>
-      <c r="B276" s="76" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A277" s="57" t="s">
-        <v>726</v>
-      </c>
-      <c r="B277" s="76" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A278" s="57" t="s">
+        <v>724</v>
+      </c>
+      <c r="B278" s="76" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A279" s="57" t="s">
+        <v>726</v>
+      </c>
+      <c r="B279" s="76" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A280" s="57" t="s">
         <v>728</v>
       </c>
-      <c r="B278" s="76" t="s">
+      <c r="B280" s="76" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A279" s="57" t="s">
+    <row r="281" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A281" s="57" t="s">
         <v>730</v>
       </c>
-      <c r="B279" s="105" t="s">
+      <c r="B281" s="126" t="s">
         <v>731</v>
       </c>
-      <c r="C279" s="106" t="s">
+      <c r="C281" s="106" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A280" s="57" t="s">
+    <row r="282" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A282" s="57" t="s">
         <v>732</v>
       </c>
-      <c r="B280" s="76" t="s">
+      <c r="B282" s="76" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A281" s="107" t="s">
+      <c r="C282" s="94" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A283" s="108" t="s">
         <v>734</v>
       </c>
-      <c r="B281" s="108"/>
-    </row>
-    <row r="282" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A282" s="57" t="s">
+      <c r="B283" s="109"/>
+    </row>
+    <row r="284" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A284" s="57" t="s">
         <v>735</v>
       </c>
-      <c r="B282" s="104" t="s">
+      <c r="B284" s="104" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A283" s="57" t="s">
+    <row r="285" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A285" s="57" t="s">
         <v>737</v>
       </c>
-      <c r="B283" s="76" t="s">
+      <c r="B285" s="76" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A284" s="57" t="s">
+    <row r="286" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A286" s="57" t="s">
         <v>739</v>
       </c>
-      <c r="B284" s="104" t="s">
+      <c r="B286" s="104" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A285" s="57"/>
-      <c r="B285" s="76"/>
-    </row>
-    <row r="286" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A286" s="57"/>
-      <c r="B286" s="76"/>
     </row>
     <row r="287" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A287" s="57"/>
@@ -13399,69 +13459,77 @@
       <c r="A291" s="57"/>
       <c r="B291" s="76"/>
     </row>
+    <row r="292" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A292" s="57"/>
+      <c r="B292" s="76"/>
+    </row>
+    <row r="293" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A293" s="57"/>
+      <c r="B293" s="76"/>
+    </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A266:B266"/>
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="A276:B276"/>
+    <mergeCell ref="A283:B283"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A227:B227"/>
+    <mergeCell ref="A229:B229"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="A265:B265"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A240:B240"/>
+    <mergeCell ref="A259:B259"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A76:A87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A75:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="A269:B269"/>
-    <mergeCell ref="A274:B274"/>
-    <mergeCell ref="A281:B281"/>
-    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="A198:B198"/>
+    <mergeCell ref="A193:B193"/>
     <mergeCell ref="A225:B225"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A233:B233"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="A206:B206"/>
+    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="A220:B220"/>
+    <mergeCell ref="A217:B217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# DB - 13.09.2019 - Exam Preparation
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="753">
   <si>
     <t>Операция</t>
   </si>
@@ -2545,9 +2545,6 @@
     <t>Data Types in SQL Server</t>
   </si>
   <si>
-    <t>BIT (1-bit), INT (32-bit), BIGINT (64-bit)</t>
-  </si>
-  <si>
     <t>MONEY – for money (precise) operations</t>
   </si>
   <si>
@@ -2627,32 +2624,6 @@
     <t xml:space="preserve"> 2.12</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Изтриване на PRIMARY KEY -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ALTER TABLE Users
-DROP CONSTRAINT PK__Users__3214EC07AD8DD30C</t>
-    </r>
-  </si>
-  <si>
     <t>USE Users</t>
   </si>
   <si>
@@ -2660,57 +2631,6 @@
   </si>
   <si>
     <t>Добавяне на FOREIGN KEY</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">DirectorId </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>INT FOREIGN KEY REFERENCES</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Directors(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>SELECT Name FROM Departments
@@ -7345,17 +7265,126 @@
   <si>
     <t>Обновяване на повече от един запис</t>
   </si>
+  <si>
+    <t>BIT (1-bit),TINYINT(8-bit) INT (32-bit), BIGINT (64-bit)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ДОБАВЯНЕ ПРОВЕРКА ПРИ ЗЪЗДАВАНЕ НА ТАБЛИЦАТА:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CREATE TABLE Students(
+Id INT PRIMARY KEY IDENTITY,
+Age INT CHECK (Age &gt; 0) NOT NULL)</t>
+    </r>
+  </si>
+  <si>
+    <t>Добавяне на FOREIGN KEY при създаване на таблица</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CREATE TABLE Exams
+(Id INT PRIMARY KEY IDENTITY NOT NULL,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubjectId INT FOREIGN KEY REFERENCES Subjects(Id))</t>
+    </r>
+  </si>
+  <si>
+    <t>DirectorId INT FOREIGN KEY REFERENCES Directors(Id)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DELETE - Изтриване на PRIMARY KEY -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ALTER TABLE Users
+DROP CONSTRAINT PK__Users__3214EC07AD8DD30C</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ISNULL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replaces NULL with the specified replacement value:
+SELECT AVG(ISNULL(Weight, 50))  
+FROM Production.Product;  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8139,42 +8168,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8189,91 +8218,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8288,73 +8317,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8363,55 +8392,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8423,89 +8446,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11237,10 +11263,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C293"/>
+  <dimension ref="A1:C296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11252,128 +11278,128 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B1" s="59" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="107" t="s">
-        <v>341</v>
-      </c>
-      <c r="B2" s="112"/>
+      <c r="A2" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="121"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="114" t="s">
-        <v>505</v>
-      </c>
-      <c r="B3" s="113"/>
+      <c r="A3" s="123" t="s">
+        <v>502</v>
+      </c>
+      <c r="B3" s="122"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="113" t="s">
-        <v>517</v>
-      </c>
-      <c r="B7" s="111"/>
+      <c r="A7" s="122" t="s">
+        <v>514</v>
+      </c>
+      <c r="B7" s="120"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
-        <v>518</v>
-      </c>
-      <c r="B8" s="103" t="s">
-        <v>699</v>
+        <v>515</v>
+      </c>
+      <c r="B8" s="101" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>522</v>
-      </c>
-      <c r="B9" s="93" t="s">
-        <v>523</v>
+        <v>519</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>524</v>
-      </c>
-      <c r="B10" s="103" t="s">
-        <v>525</v>
+        <v>521</v>
+      </c>
+      <c r="B10" s="101" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="113" t="s">
-        <v>519</v>
-      </c>
-      <c r="B11" s="111"/>
+      <c r="A11" s="122" t="s">
+        <v>516</v>
+      </c>
+      <c r="B11" s="120"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B12" s="89" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113" t="s">
-        <v>387</v>
-      </c>
-      <c r="B13" s="113"/>
+      <c r="A13" s="122" t="s">
+        <v>384</v>
+      </c>
+      <c r="B13" s="122"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B17" s="81" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -11386,344 +11412,344 @@
     </row>
     <row r="19" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="113" t="s">
-        <v>502</v>
-      </c>
-      <c r="B21" s="113"/>
+      <c r="A21" s="122" t="s">
+        <v>499</v>
+      </c>
+      <c r="B21" s="122"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="113" t="s">
-        <v>386</v>
-      </c>
-      <c r="B23" s="113"/>
+      <c r="A23" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="B23" s="122"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>382</v>
-      </c>
-      <c r="C24" s="94"/>
+        <v>379</v>
+      </c>
+      <c r="C24" s="92"/>
     </row>
     <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="127" t="s">
-        <v>747</v>
-      </c>
-      <c r="B25" s="128" t="s">
-        <v>746</v>
-      </c>
-      <c r="C25" s="94"/>
+      <c r="A25" s="107" t="s">
+        <v>744</v>
+      </c>
+      <c r="B25" s="108" t="s">
+        <v>743</v>
+      </c>
+      <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="113" t="s">
-        <v>351</v>
-      </c>
-      <c r="B26" s="113"/>
+      <c r="A26" s="122" t="s">
+        <v>348</v>
+      </c>
+      <c r="B26" s="122"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B28" s="81" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B29" s="81" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="113" t="s">
-        <v>351</v>
-      </c>
-      <c r="B30" s="113"/>
+      <c r="A30" s="122" t="s">
+        <v>348</v>
+      </c>
+      <c r="B30" s="122"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B31" s="74" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B32" s="74" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B33" s="74" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="111" t="s">
-        <v>361</v>
-      </c>
-      <c r="B34" s="111"/>
+      <c r="A34" s="120" t="s">
+        <v>358</v>
+      </c>
+      <c r="B34" s="120"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="72" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B36" s="74" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="57" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B37" s="74" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="113" t="s">
-        <v>358</v>
-      </c>
-      <c r="B38" s="113"/>
+      <c r="A38" s="122" t="s">
+        <v>355</v>
+      </c>
+      <c r="B38" s="122"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B39" s="74" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A40" s="72" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B40" s="74" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A41" s="57" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="111" t="s">
-        <v>362</v>
-      </c>
-      <c r="B42" s="111"/>
+      <c r="A42" s="120" t="s">
+        <v>359</v>
+      </c>
+      <c r="B42" s="120"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B43" s="74" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B44" s="74" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="113" t="s">
-        <v>512</v>
-      </c>
-      <c r="B45" s="111"/>
+      <c r="A45" s="122" t="s">
+        <v>509</v>
+      </c>
+      <c r="B45" s="120"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B46" s="74" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="57" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B47" s="74" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" s="57" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B48" s="74" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="107" t="s">
-        <v>372</v>
-      </c>
-      <c r="B49" s="107"/>
+      <c r="A49" s="111" t="s">
+        <v>369</v>
+      </c>
+      <c r="B49" s="111"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="110" t="s">
+      <c r="A50" s="112" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="109"/>
+      <c r="B50" s="110"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="118" t="s">
+      <c r="A51" s="117" t="s">
+        <v>320</v>
+      </c>
+      <c r="B51" s="62" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="118"/>
+      <c r="B52" s="62" t="s">
+        <v>587</v>
+      </c>
+      <c r="C52" s="66" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="119"/>
+      <c r="B53" s="62" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="117" t="s">
         <v>321</v>
       </c>
-      <c r="B51" s="62" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="119"/>
-      <c r="B52" s="62" t="s">
-        <v>590</v>
-      </c>
-      <c r="C52" s="66" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="120"/>
-      <c r="B53" s="62" t="s">
+      <c r="B54" s="62" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="118" t="s">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="118"/>
+      <c r="B55" s="62" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="118"/>
+      <c r="B56" s="62" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="119"/>
+      <c r="B57" s="62" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="117" t="s">
         <v>322</v>
       </c>
-      <c r="B54" s="62" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="119"/>
-      <c r="B55" s="62" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="119"/>
-      <c r="B56" s="62" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="120"/>
-      <c r="B57" s="62" t="s">
+      <c r="B58" s="62" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="118" t="s">
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="119"/>
+      <c r="B59" s="62" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="117" t="s">
         <v>323</v>
       </c>
-      <c r="B58" s="62" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="120"/>
-      <c r="B59" s="62" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="118" t="s">
+      <c r="B60" s="62" t="s">
         <v>324</v>
       </c>
-      <c r="B60" s="62" t="s">
+      <c r="C60" s="66" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="118"/>
+      <c r="B61" s="62" t="s">
+        <v>524</v>
+      </c>
+      <c r="C61" s="68" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="118"/>
+      <c r="B62" s="62" t="s">
+        <v>584</v>
+      </c>
+      <c r="C62" s="68"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="119"/>
+      <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="C60" s="66" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="119"/>
-      <c r="B61" s="62" t="s">
-        <v>527</v>
-      </c>
-      <c r="C61" s="68" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="119"/>
-      <c r="B62" s="62" t="s">
-        <v>587</v>
-      </c>
-      <c r="C62" s="68"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="120"/>
-      <c r="B63" s="62" t="s">
-        <v>326</v>
-      </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="102" t="s">
-        <v>631</v>
+      <c r="A64" s="100" t="s">
+        <v>628</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11739,23 +11765,23 @@
         <v>285</v>
       </c>
       <c r="B66" s="62" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A67" s="57" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A68" s="57" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B68" s="62" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -11767,7 +11793,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="115" t="s">
+      <c r="A70" s="114" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -11775,1107 +11801,1119 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="116"/>
+      <c r="A71" s="115"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="116"/>
+      <c r="A72" s="115"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="116"/>
+      <c r="A73" s="115"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="116"/>
+    <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="115"/>
       <c r="B74" s="62" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="117"/>
+        <v>746</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="115"/>
       <c r="B75" s="62" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="116"/>
+      <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="115" t="s">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="114" t="s">
         <v>291</v>
       </c>
-      <c r="B76" s="62" t="s">
+      <c r="B77" s="62" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="116"/>
-      <c r="B77" s="62" t="s">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="115"/>
+      <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="C77" s="67"/>
-    </row>
-    <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="116"/>
-      <c r="B78" s="62" t="s">
+      <c r="C78" s="67"/>
+    </row>
+    <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="115"/>
+      <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="116"/>
-      <c r="B79" s="62" t="s">
+    <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="115"/>
+      <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="116"/>
-      <c r="B80" s="81" t="s">
+    <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="115"/>
+      <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="116"/>
-      <c r="B81" s="81" t="s">
+    <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="115"/>
+      <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="116"/>
-      <c r="B82" s="81" t="s">
+    <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="115"/>
+      <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
-      <c r="B83" s="81" t="s">
+    <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="115"/>
+      <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A84" s="116"/>
-      <c r="B84" s="81" t="s">
+    <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A85" s="115"/>
+      <c r="B85" s="81" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="115"/>
+      <c r="B86" s="81" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="115"/>
+      <c r="B87" s="81" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="116"/>
+      <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="116"/>
-      <c r="B85" s="81" t="s">
+    <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="114" t="s">
+        <v>292</v>
+      </c>
+      <c r="B89" s="82" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="115"/>
+      <c r="B90" s="83" t="s">
+        <v>307</v>
+      </c>
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="115"/>
+      <c r="B91" s="83" t="s">
+        <v>308</v>
+      </c>
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="116"/>
+      <c r="B92" s="82" t="s">
+        <v>542</v>
+      </c>
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="114" t="s">
+        <v>309</v>
+      </c>
+      <c r="B93" s="84" t="s">
+        <v>310</v>
+      </c>
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A94" s="116"/>
+      <c r="B94" s="84" t="s">
+        <v>311</v>
+      </c>
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A95" s="105" t="s">
+        <v>747</v>
+      </c>
+      <c r="B95" s="84" t="s">
+        <v>748</v>
+      </c>
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="69" t="s">
+        <v>333</v>
+      </c>
+      <c r="B96" s="83" t="s">
+        <v>749</v>
+      </c>
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="65" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="116"/>
-      <c r="B86" s="81" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="117"/>
-      <c r="B87" s="81" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="115" t="s">
-        <v>292</v>
-      </c>
-      <c r="B88" s="82" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="116"/>
-      <c r="B89" s="83" t="s">
-        <v>307</v>
-      </c>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="116"/>
-      <c r="B90" s="83" t="s">
-        <v>308</v>
-      </c>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="117"/>
-      <c r="B91" s="82" t="s">
-        <v>545</v>
-      </c>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="115" t="s">
-        <v>309</v>
-      </c>
-      <c r="B92" s="84" t="s">
-        <v>310</v>
-      </c>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A93" s="117"/>
-      <c r="B93" s="84" t="s">
-        <v>311</v>
-      </c>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A94" s="69" t="s">
-        <v>335</v>
-      </c>
-      <c r="B94" s="83" t="s">
-        <v>336</v>
-      </c>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="65" t="s">
-        <v>334</v>
-      </c>
-      <c r="B95" s="84" t="s">
-        <v>333</v>
-      </c>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A96" s="61" t="s">
+      <c r="B97" s="84" t="s">
+        <v>331</v>
+      </c>
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="61" t="s">
+        <v>382</v>
+      </c>
+      <c r="B98" s="85" t="s">
+        <v>327</v>
+      </c>
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="71" t="s">
+        <v>370</v>
+      </c>
+      <c r="B99" s="84" t="s">
+        <v>528</v>
+      </c>
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="90" t="s">
+        <v>525</v>
+      </c>
+      <c r="B100" s="81" t="s">
+        <v>739</v>
+      </c>
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="73" t="s">
+        <v>372</v>
+      </c>
+      <c r="B101" s="81" t="s">
+        <v>371</v>
+      </c>
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="111" t="s">
         <v>385</v>
       </c>
-      <c r="B96" s="85" t="s">
-        <v>328</v>
-      </c>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="71" t="s">
-        <v>373</v>
-      </c>
-      <c r="B97" s="84" t="s">
-        <v>531</v>
-      </c>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="90" t="s">
-        <v>528</v>
-      </c>
-      <c r="B98" s="81" t="s">
-        <v>742</v>
-      </c>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="73" t="s">
-        <v>375</v>
-      </c>
-      <c r="B99" s="81" t="s">
-        <v>374</v>
-      </c>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="107" t="s">
+      <c r="B102" s="111"/>
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A103" s="112" t="s">
+        <v>386</v>
+      </c>
+      <c r="B103" s="110"/>
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="70" t="s">
+        <v>387</v>
+      </c>
+      <c r="B104" s="60" t="s">
         <v>388</v>
       </c>
-      <c r="B100" s="107"/>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A101" s="110" t="s">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="70" t="s">
         <v>389</v>
       </c>
-      <c r="B101" s="109"/>
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="70" t="s">
+      <c r="B105" s="76" t="s">
         <v>390</v>
       </c>
-      <c r="B102" s="60" t="s">
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="70" t="s">
         <v>391</v>
       </c>
-      <c r="C102"/>
-    </row>
-    <row r="103" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="70" t="s">
+      <c r="B106" s="76" t="s">
         <v>392</v>
       </c>
-      <c r="B103" s="76" t="s">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A107" s="112" t="s">
         <v>393</v>
       </c>
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="70" t="s">
+      <c r="B107" s="110"/>
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A108" s="57" t="s">
+        <v>395</v>
+      </c>
+      <c r="B108" s="80" t="s">
         <v>394</v>
       </c>
-      <c r="B104" s="76" t="s">
-        <v>395</v>
-      </c>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A105" s="110" t="s">
+      <c r="C108"/>
+    </row>
+    <row r="109" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="57" t="s">
         <v>396</v>
       </c>
-      <c r="B105" s="109"/>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A106" s="57" t="s">
+      <c r="B109" s="80" t="s">
+        <v>397</v>
+      </c>
+      <c r="C109"/>
+    </row>
+    <row r="110" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A110" s="72" t="s">
         <v>398</v>
       </c>
-      <c r="B106" s="80" t="s">
-        <v>397</v>
-      </c>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="57" t="s">
+      <c r="B110" s="80" t="s">
         <v>399</v>
       </c>
-      <c r="B107" s="80" t="s">
+      <c r="C110"/>
+    </row>
+    <row r="111" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="57" t="s">
         <v>400</v>
       </c>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A108" s="72" t="s">
+      <c r="B111" s="80" t="s">
         <v>401</v>
       </c>
-      <c r="B108" s="80" t="s">
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="57" t="s">
         <v>402</v>
       </c>
-      <c r="C108"/>
-    </row>
-    <row r="109" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A109" s="57" t="s">
+      <c r="B112" s="80" t="s">
         <v>403</v>
       </c>
-      <c r="B109" s="80" t="s">
+      <c r="C112"/>
+    </row>
+    <row r="113" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="C109"/>
-    </row>
-    <row r="110" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="57" t="s">
+      <c r="B113" s="79" t="s">
         <v>405</v>
       </c>
-      <c r="B110" s="80" t="s">
+      <c r="C113"/>
+    </row>
+    <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="57" t="s">
         <v>406</v>
       </c>
-      <c r="C110"/>
-    </row>
-    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
+      <c r="B114" s="79" t="s">
         <v>407</v>
       </c>
-      <c r="B111" s="79" t="s">
+      <c r="C114"/>
+    </row>
+    <row r="115" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A115" s="57" t="s">
         <v>408</v>
       </c>
-      <c r="C111"/>
-    </row>
-    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="57" t="s">
+      <c r="B115" s="86" t="s">
         <v>409</v>
       </c>
-      <c r="B112" s="79" t="s">
+      <c r="C115"/>
+    </row>
+    <row r="116" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="B116" s="80" t="s">
         <v>410</v>
-      </c>
-      <c r="C112"/>
-    </row>
-    <row r="113" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A113" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B113" s="86" t="s">
-        <v>412</v>
-      </c>
-      <c r="C113"/>
-    </row>
-    <row r="114" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="B114" s="80" t="s">
-        <v>413</v>
-      </c>
-      <c r="C114"/>
-    </row>
-    <row r="115" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
-        <v>420</v>
-      </c>
-      <c r="B115" s="79" t="s">
-        <v>414</v>
-      </c>
-      <c r="C115"/>
-    </row>
-    <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="B116" s="79" t="s">
-        <v>415</v>
       </c>
       <c r="C116"/>
     </row>
     <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B117" s="79" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C117"/>
     </row>
     <row r="118" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B118" s="79" t="s">
+        <v>412</v>
+      </c>
+      <c r="C118"/>
+    </row>
+    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="57" t="s">
+        <v>413</v>
+      </c>
+      <c r="B119" s="79" t="s">
+        <v>414</v>
+      </c>
+      <c r="C119"/>
+    </row>
+    <row r="120" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="57" t="s">
+        <v>415</v>
+      </c>
+      <c r="B120" s="79" t="s">
+        <v>419</v>
+      </c>
+      <c r="C120"/>
+    </row>
+    <row r="121" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A121" s="57" t="s">
+        <v>420</v>
+      </c>
+      <c r="B121" s="79" t="s">
+        <v>421</v>
+      </c>
+      <c r="C121"/>
+    </row>
+    <row r="122" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="72" t="s">
         <v>422</v>
       </c>
-      <c r="C118"/>
-    </row>
-    <row r="119" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
+      <c r="B122" s="80" t="s">
         <v>423</v>
       </c>
-      <c r="B119" s="79" t="s">
+      <c r="C122"/>
+    </row>
+    <row r="123" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="57" t="s">
+        <v>751</v>
+      </c>
+      <c r="B123" s="80" t="s">
+        <v>752</v>
+      </c>
+      <c r="C123"/>
+    </row>
+    <row r="124" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="57" t="s">
+        <v>531</v>
+      </c>
+      <c r="B124" s="80" t="s">
+        <v>532</v>
+      </c>
+      <c r="C124"/>
+    </row>
+    <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A125" s="112" t="s">
         <v>424</v>
       </c>
-      <c r="C119"/>
-    </row>
-    <row r="120" spans="1:3" ht="81.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="72" t="s">
-        <v>425</v>
-      </c>
-      <c r="B120" s="80" t="s">
-        <v>426</v>
-      </c>
-      <c r="C120"/>
-    </row>
-    <row r="121" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A121" s="92" t="s">
-        <v>534</v>
-      </c>
-      <c r="B121" s="91" t="s">
-        <v>535</v>
-      </c>
-      <c r="C121"/>
-    </row>
-    <row r="122" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A122" s="110" t="s">
-        <v>427</v>
-      </c>
-      <c r="B122" s="109"/>
-      <c r="C122"/>
-    </row>
-    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
-        <v>432</v>
-      </c>
-      <c r="B123" s="79" t="s">
-        <v>431</v>
-      </c>
-      <c r="C123"/>
-    </row>
-    <row r="124" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
-        <v>433</v>
-      </c>
-      <c r="B124" s="79" t="s">
-        <v>430</v>
-      </c>
-      <c r="C124"/>
-    </row>
-    <row r="125" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="57" t="s">
-        <v>434</v>
-      </c>
-      <c r="B125" s="79" t="s">
-        <v>429</v>
-      </c>
+      <c r="B125" s="110"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="B126" s="79" t="s">
         <v>428</v>
       </c>
       <c r="C126"/>
     </row>
-    <row r="127" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A127" s="70" t="s">
+    <row r="127" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="57" t="s">
+        <v>430</v>
+      </c>
+      <c r="B127" s="79" t="s">
+        <v>427</v>
+      </c>
+      <c r="C127"/>
+    </row>
+    <row r="128" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="57" t="s">
+        <v>431</v>
+      </c>
+      <c r="B128" s="79" t="s">
+        <v>426</v>
+      </c>
+      <c r="C128"/>
+    </row>
+    <row r="129" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="57" t="s">
+        <v>432</v>
+      </c>
+      <c r="B129" s="79" t="s">
+        <v>425</v>
+      </c>
+      <c r="C129"/>
+    </row>
+    <row r="130" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="70" t="s">
+        <v>436</v>
+      </c>
+      <c r="B130" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="C130"/>
+    </row>
+    <row r="131" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A131" s="57" t="s">
+        <v>435</v>
+      </c>
+      <c r="B131" s="79" t="s">
+        <v>434</v>
+      </c>
+      <c r="C131"/>
+    </row>
+    <row r="132" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A132" s="70" t="s">
+        <v>437</v>
+      </c>
+      <c r="B132" s="80" t="s">
+        <v>438</v>
+      </c>
+      <c r="C132"/>
+    </row>
+    <row r="133" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="57" t="s">
         <v>439</v>
       </c>
-      <c r="B127" s="79" t="s">
-        <v>436</v>
-      </c>
-      <c r="C127"/>
-    </row>
-    <row r="128" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A128" s="57" t="s">
-        <v>438</v>
-      </c>
-      <c r="B128" s="79" t="s">
-        <v>437</v>
-      </c>
-      <c r="C128"/>
-    </row>
-    <row r="129" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A129" s="70" t="s">
+      <c r="B133" s="79" t="s">
         <v>440</v>
       </c>
-      <c r="B129" s="80" t="s">
+      <c r="C133"/>
+    </row>
+    <row r="134" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A134" s="57" t="s">
         <v>441</v>
       </c>
-      <c r="C129"/>
-    </row>
-    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="57" t="s">
+      <c r="B134" s="80" t="s">
         <v>442</v>
       </c>
-      <c r="B130" s="79" t="s">
+      <c r="C134"/>
+    </row>
+    <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A135" s="112" t="s">
+        <v>496</v>
+      </c>
+      <c r="B135" s="110"/>
+      <c r="C135"/>
+    </row>
+    <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A136" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="C130"/>
-    </row>
-    <row r="131" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
+      <c r="B136" s="80" t="s">
+        <v>495</v>
+      </c>
+      <c r="C136"/>
+    </row>
+    <row r="137" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A137" s="57" t="s">
         <v>444</v>
       </c>
-      <c r="B131" s="80" t="s">
+      <c r="B137" s="80" t="s">
         <v>445</v>
       </c>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A132" s="110" t="s">
-        <v>499</v>
-      </c>
-      <c r="B132" s="109"/>
-      <c r="C132"/>
-    </row>
-    <row r="133" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A133" s="57" t="s">
+      <c r="C137"/>
+    </row>
+    <row r="138" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="57" t="s">
         <v>446</v>
       </c>
-      <c r="B133" s="80" t="s">
-        <v>498</v>
-      </c>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A134" s="57" t="s">
+      <c r="B138" s="79" t="s">
         <v>447</v>
       </c>
-      <c r="B134" s="80" t="s">
+      <c r="C138"/>
+    </row>
+    <row r="139" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="57" t="s">
         <v>448</v>
       </c>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="57" t="s">
+      <c r="B139" s="79" t="s">
         <v>449</v>
       </c>
-      <c r="B135" s="79" t="s">
+      <c r="C139"/>
+    </row>
+    <row r="140" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="70" t="s">
         <v>450</v>
       </c>
-      <c r="C135"/>
-    </row>
-    <row r="136" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="57" t="s">
+      <c r="B140" s="79" t="s">
         <v>451</v>
       </c>
-      <c r="B136" s="79" t="s">
+      <c r="C140"/>
+    </row>
+    <row r="141" spans="1:3" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="77" t="s">
+        <v>453</v>
+      </c>
+      <c r="B141" s="80" t="s">
         <v>452</v>
       </c>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A137" s="70" t="s">
-        <v>453</v>
-      </c>
-      <c r="B137" s="79" t="s">
+      <c r="C141"/>
+    </row>
+    <row r="142" spans="1:3" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="A142" s="78" t="s">
         <v>454</v>
       </c>
-      <c r="C137"/>
-    </row>
-    <row r="138" spans="1:3" ht="103.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="77" t="s">
+      <c r="B142" s="95" t="s">
+        <v>455</v>
+      </c>
+      <c r="C142"/>
+    </row>
+    <row r="143" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A143" s="78" t="s">
         <v>456</v>
       </c>
-      <c r="B138" s="80" t="s">
-        <v>455</v>
-      </c>
-      <c r="C138"/>
-    </row>
-    <row r="139" spans="1:3" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="A139" s="78" t="s">
+      <c r="B143" s="95" t="s">
+        <v>547</v>
+      </c>
+      <c r="C143"/>
+    </row>
+    <row r="144" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
+      <c r="A144" s="78" t="s">
         <v>457</v>
       </c>
-      <c r="B139" s="97" t="s">
+      <c r="B144" s="95" t="s">
+        <v>546</v>
+      </c>
+      <c r="C144"/>
+    </row>
+    <row r="145" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
+      <c r="A145" s="78" t="s">
         <v>458</v>
       </c>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A140" s="78" t="s">
+      <c r="B145" s="95" t="s">
+        <v>545</v>
+      </c>
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A146" s="109" t="s">
         <v>459</v>
       </c>
-      <c r="B140" s="97" t="s">
-        <v>550</v>
-      </c>
-      <c r="C140"/>
-    </row>
-    <row r="141" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
-      <c r="A141" s="78" t="s">
+      <c r="B146" s="110"/>
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A147" s="78" t="s">
+        <v>461</v>
+      </c>
+      <c r="B147" s="80" t="s">
         <v>460</v>
       </c>
-      <c r="B141" s="97" t="s">
-        <v>549</v>
-      </c>
-      <c r="C141"/>
-    </row>
-    <row r="142" spans="1:3" ht="127.5" x14ac:dyDescent="0.3">
-      <c r="A142" s="78" t="s">
-        <v>461</v>
-      </c>
-      <c r="B142" s="97" t="s">
-        <v>548</v>
-      </c>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="108" t="s">
+      <c r="C147"/>
+    </row>
+    <row r="148" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A148" s="70" t="s">
         <v>462</v>
       </c>
-      <c r="B143" s="109"/>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A144" s="78" t="s">
+      <c r="B148" s="86" t="s">
+        <v>465</v>
+      </c>
+      <c r="C148"/>
+    </row>
+    <row r="149" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A149" s="78" t="s">
+        <v>463</v>
+      </c>
+      <c r="B149" s="80" t="s">
         <v>464</v>
       </c>
-      <c r="B144" s="80" t="s">
-        <v>463</v>
-      </c>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A145" s="70" t="s">
-        <v>465</v>
-      </c>
-      <c r="B145" s="86" t="s">
+      <c r="C149"/>
+    </row>
+    <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="109" t="s">
+        <v>467</v>
+      </c>
+      <c r="B150" s="110"/>
+      <c r="C150"/>
+    </row>
+    <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A151" s="70" t="s">
+        <v>466</v>
+      </c>
+      <c r="B151" s="87" t="s">
         <v>468</v>
       </c>
-      <c r="C145"/>
-    </row>
-    <row r="146" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A146" s="78" t="s">
-        <v>466</v>
-      </c>
-      <c r="B146" s="80" t="s">
-        <v>467</v>
-      </c>
-      <c r="C146"/>
-    </row>
-    <row r="147" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A147" s="108" t="s">
-        <v>470</v>
-      </c>
-      <c r="B147" s="109"/>
-      <c r="C147"/>
-    </row>
-    <row r="148" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A148" s="70" t="s">
+      <c r="C151"/>
+    </row>
+    <row r="152" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A152" s="57" t="s">
+        <v>535</v>
+      </c>
+      <c r="B152" s="87" t="s">
+        <v>536</v>
+      </c>
+      <c r="C152"/>
+    </row>
+    <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A153" s="109" t="s">
+        <v>537</v>
+      </c>
+      <c r="B153" s="110"/>
+      <c r="C153"/>
+    </row>
+    <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A154" s="57" t="s">
+        <v>538</v>
+      </c>
+      <c r="B154" s="80" t="s">
+        <v>541</v>
+      </c>
+      <c r="C154" s="11" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A155" s="57" t="s">
+        <v>539</v>
+      </c>
+      <c r="B155" s="76" t="s">
+        <v>540</v>
+      </c>
+      <c r="C155"/>
+    </row>
+    <row r="156" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A156" s="57" t="s">
+        <v>593</v>
+      </c>
+      <c r="B156" s="96" t="s">
+        <v>592</v>
+      </c>
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="57" t="s">
+        <v>741</v>
+      </c>
+      <c r="B157" s="96" t="s">
+        <v>742</v>
+      </c>
+      <c r="C157"/>
+    </row>
+    <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A158" s="111" t="s">
         <v>469</v>
       </c>
-      <c r="B148" s="87" t="s">
-        <v>471</v>
-      </c>
-      <c r="C148"/>
-    </row>
-    <row r="149" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A149" s="57" t="s">
-        <v>538</v>
-      </c>
-      <c r="B149" s="87" t="s">
-        <v>539</v>
-      </c>
-      <c r="C149"/>
-    </row>
-    <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="108" t="s">
-        <v>540</v>
-      </c>
-      <c r="B150" s="109"/>
-      <c r="C150"/>
-    </row>
-    <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A151" s="57" t="s">
-        <v>541</v>
-      </c>
-      <c r="B151" s="80" t="s">
-        <v>544</v>
-      </c>
-      <c r="C151" s="11" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A152" s="57" t="s">
-        <v>542</v>
-      </c>
-      <c r="B152" s="76" t="s">
-        <v>543</v>
-      </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A153" s="57" t="s">
-        <v>596</v>
-      </c>
-      <c r="B153" s="98" t="s">
-        <v>595</v>
-      </c>
-      <c r="C153"/>
-    </row>
-    <row r="154" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="57" t="s">
-        <v>744</v>
-      </c>
-      <c r="B154" s="98" t="s">
-        <v>745</v>
-      </c>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A155" s="107" t="s">
+      <c r="B158" s="111"/>
+      <c r="C158"/>
+    </row>
+    <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A159" s="112" t="s">
         <v>472</v>
       </c>
-      <c r="B155" s="107"/>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A156" s="110" t="s">
+      <c r="B159" s="110"/>
+      <c r="C159"/>
+    </row>
+    <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A160" s="57" t="s">
+        <v>534</v>
+      </c>
+      <c r="B160" s="76" t="s">
+        <v>533</v>
+      </c>
+      <c r="C160"/>
+    </row>
+    <row r="161" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="A161" s="57" t="s">
+        <v>526</v>
+      </c>
+      <c r="B161" s="80" t="s">
+        <v>527</v>
+      </c>
+      <c r="C161"/>
+    </row>
+    <row r="162" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="57"/>
+      <c r="B162" s="80"/>
+      <c r="C162"/>
+    </row>
+    <row r="163" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="57"/>
+      <c r="B163" s="80"/>
+      <c r="C163"/>
+    </row>
+    <row r="164" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="70"/>
+      <c r="C164"/>
+    </row>
+    <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A165" s="109" t="s">
         <v>475</v>
       </c>
-      <c r="B156" s="109"/>
-      <c r="C156"/>
-    </row>
-    <row r="157" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A157" s="57" t="s">
-        <v>537</v>
-      </c>
-      <c r="B157" s="76" t="s">
-        <v>536</v>
-      </c>
-      <c r="C157"/>
-    </row>
-    <row r="158" spans="1:3" ht="50.25" x14ac:dyDescent="0.25">
-      <c r="A158" s="57" t="s">
-        <v>529</v>
-      </c>
-      <c r="B158" s="80" t="s">
-        <v>530</v>
-      </c>
-      <c r="C158"/>
-    </row>
-    <row r="159" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="57"/>
-      <c r="B159" s="80"/>
-      <c r="C159"/>
-    </row>
-    <row r="160" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="57"/>
-      <c r="B160" s="80"/>
-      <c r="C160"/>
-    </row>
-    <row r="161" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="70"/>
-      <c r="C161"/>
-    </row>
-    <row r="162" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A162" s="108" t="s">
-        <v>478</v>
-      </c>
-      <c r="B162" s="121"/>
-      <c r="C162"/>
-    </row>
-    <row r="163" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A163" s="57" t="s">
-        <v>477</v>
-      </c>
-      <c r="B163" s="76" t="s">
-        <v>476</v>
-      </c>
-      <c r="C163"/>
-    </row>
-    <row r="164" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A164" s="57" t="s">
-        <v>483</v>
-      </c>
-      <c r="B164" s="76" t="s">
-        <v>479</v>
-      </c>
-      <c r="C164"/>
-    </row>
-    <row r="165" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A165" s="57" t="s">
-        <v>481</v>
-      </c>
-      <c r="B165" s="76" t="s">
-        <v>480</v>
-      </c>
+      <c r="B165" s="113"/>
       <c r="C165"/>
     </row>
-    <row r="166" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A166" s="57" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B166" s="76" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C166"/>
     </row>
     <row r="167" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A167" s="57" t="s">
+        <v>480</v>
+      </c>
+      <c r="B167" s="76" t="s">
+        <v>476</v>
+      </c>
+      <c r="C167"/>
+    </row>
+    <row r="168" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A168" s="57" t="s">
+        <v>478</v>
+      </c>
+      <c r="B168" s="76" t="s">
+        <v>477</v>
+      </c>
+      <c r="C168"/>
+    </row>
+    <row r="169" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A169" s="57" t="s">
+        <v>479</v>
+      </c>
+      <c r="B169" s="76" t="s">
+        <v>473</v>
+      </c>
+      <c r="C169"/>
+    </row>
+    <row r="170" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A170" s="57" t="s">
+        <v>481</v>
+      </c>
+      <c r="B170" s="76" t="s">
+        <v>482</v>
+      </c>
+      <c r="C170"/>
+    </row>
+    <row r="171" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A171" s="57" t="s">
+        <v>483</v>
+      </c>
+      <c r="B171" s="76" t="s">
         <v>484</v>
       </c>
-      <c r="B167" s="76" t="s">
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A172" s="57" t="s">
+        <v>493</v>
+      </c>
+      <c r="B172" s="88" t="s">
+        <v>494</v>
+      </c>
+      <c r="C172"/>
+    </row>
+    <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A173" s="112" t="s">
+        <v>470</v>
+      </c>
+      <c r="B173" s="110"/>
+      <c r="C173"/>
+    </row>
+    <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A174" s="57" t="s">
         <v>485</v>
       </c>
-      <c r="C167"/>
-    </row>
-    <row r="168" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A168" s="57" t="s">
+      <c r="B174" s="76" t="s">
         <v>486</v>
       </c>
-      <c r="B168" s="76" t="s">
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A175" s="57" t="s">
+        <v>488</v>
+      </c>
+      <c r="B175" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="C168"/>
-    </row>
-    <row r="169" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A169" s="57" t="s">
-        <v>496</v>
-      </c>
-      <c r="B169" s="88" t="s">
-        <v>497</v>
-      </c>
-      <c r="C169"/>
-    </row>
-    <row r="170" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A170" s="110" t="s">
-        <v>473</v>
-      </c>
-      <c r="B170" s="109"/>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A171" s="57" t="s">
-        <v>488</v>
-      </c>
-      <c r="B171" s="76" t="s">
+      <c r="C175"/>
+    </row>
+    <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A176" s="112" t="s">
+        <v>471</v>
+      </c>
+      <c r="B176" s="110"/>
+      <c r="C176"/>
+    </row>
+    <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A177" s="57" t="s">
         <v>489</v>
       </c>
-      <c r="C171"/>
-    </row>
-    <row r="172" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A172" s="57" t="s">
+      <c r="B177" s="76" t="s">
+        <v>490</v>
+      </c>
+      <c r="C177"/>
+    </row>
+    <row r="178" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A178" s="57" t="s">
         <v>491</v>
       </c>
-      <c r="B172" s="76" t="s">
-        <v>490</v>
-      </c>
-      <c r="C172"/>
-    </row>
-    <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="110" t="s">
-        <v>474</v>
-      </c>
-      <c r="B173" s="109"/>
-      <c r="C173"/>
-    </row>
-    <row r="174" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A174" s="57" t="s">
+      <c r="B178" s="76" t="s">
         <v>492</v>
       </c>
-      <c r="B174" s="76" t="s">
-        <v>493</v>
-      </c>
-      <c r="C174"/>
-    </row>
-    <row r="175" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A175" s="57" t="s">
-        <v>494</v>
-      </c>
-      <c r="B175" s="76" t="s">
-        <v>495</v>
-      </c>
-      <c r="C175"/>
-    </row>
-    <row r="176" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A176" s="107" t="s">
+      <c r="C178"/>
+    </row>
+    <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A179" s="111" t="s">
+        <v>548</v>
+      </c>
+      <c r="B179" s="111"/>
+      <c r="C179"/>
+    </row>
+    <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A180" s="112" t="s">
+        <v>549</v>
+      </c>
+      <c r="B180" s="110"/>
+      <c r="C180"/>
+    </row>
+    <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A181" s="57" t="s">
+        <v>550</v>
+      </c>
+      <c r="B181" s="76" t="s">
         <v>551</v>
       </c>
-      <c r="B176" s="107"/>
-      <c r="C176"/>
-    </row>
-    <row r="177" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A177" s="110" t="s">
+    </row>
+    <row r="182" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A182" s="57"/>
+      <c r="B182" s="76"/>
+    </row>
+    <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A183" s="112" t="s">
+        <v>548</v>
+      </c>
+      <c r="B183" s="110"/>
+      <c r="C183"/>
+    </row>
+    <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A184" s="57" t="s">
         <v>552</v>
       </c>
-      <c r="B177" s="109"/>
-      <c r="C177"/>
-    </row>
-    <row r="178" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A178" s="57" t="s">
+      <c r="B184" s="76" t="s">
         <v>553</v>
       </c>
-      <c r="B178" s="76" t="s">
+    </row>
+    <row r="185" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A185" s="57" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A179" s="57"/>
-      <c r="B179" s="76"/>
-    </row>
-    <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="110" t="s">
-        <v>551</v>
-      </c>
-      <c r="B180" s="109"/>
-      <c r="C180"/>
-    </row>
-    <row r="181" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A181" s="57" t="s">
+      <c r="B185" s="76" t="s">
         <v>555</v>
       </c>
-      <c r="B181" s="76" t="s">
+    </row>
+    <row r="186" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A186" s="57" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A182" s="57" t="s">
+      <c r="B186" s="76" t="s">
         <v>557</v>
       </c>
-      <c r="B182" s="76" t="s">
+    </row>
+    <row r="187" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A187" s="57" t="s">
+        <v>559</v>
+      </c>
+      <c r="B187" s="76" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A183" s="57" t="s">
-        <v>559</v>
-      </c>
-      <c r="B183" s="76" t="s">
+    <row r="188" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="57" t="s">
+        <v>561</v>
+      </c>
+      <c r="B188" s="76" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A184" s="57" t="s">
+    <row r="189" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
+      <c r="A189" s="57" t="s">
         <v>562</v>
       </c>
-      <c r="B184" s="76" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="57" t="s">
+      <c r="B189" s="80" t="s">
+        <v>563</v>
+      </c>
+      <c r="C189" s="93" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
+      <c r="A190" s="57" t="s">
         <v>564</v>
       </c>
-      <c r="B185" s="76" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="108.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="57" t="s">
+      <c r="B190" s="80" t="s">
         <v>565</v>
       </c>
-      <c r="B186" s="80" t="s">
+      <c r="C190" s="93" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A191" s="57" t="s">
         <v>566</v>
       </c>
-      <c r="C186" s="95" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="205.5" x14ac:dyDescent="0.25">
-      <c r="A187" s="57" t="s">
+      <c r="B191" s="76" t="s">
         <v>567</v>
       </c>
-      <c r="B187" s="80" t="s">
-        <v>568</v>
-      </c>
-      <c r="C187" s="95" t="s">
+      <c r="C191" s="92" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A192" s="57"/>
+      <c r="B192" s="76"/>
+    </row>
+    <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A193" s="112" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A188" s="57" t="s">
-        <v>569</v>
-      </c>
-      <c r="B188" s="76" t="s">
-        <v>570</v>
-      </c>
-      <c r="C188" s="94" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="57"/>
-      <c r="B189" s="76"/>
-    </row>
-    <row r="190" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A190" s="110" t="s">
-        <v>574</v>
-      </c>
-      <c r="B190" s="109"/>
-      <c r="C190"/>
-    </row>
-    <row r="191" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A191" s="57" t="s">
-        <v>575</v>
-      </c>
-      <c r="B191" s="76" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A192" s="57"/>
-      <c r="B192" s="76" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A193" s="108" t="s">
-        <v>578</v>
-      </c>
-      <c r="B193" s="109"/>
+      <c r="B193" s="110"/>
+      <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A194" s="57" t="s">
+        <v>572</v>
+      </c>
+      <c r="B194" s="76" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A195" s="57"/>
+      <c r="B195" s="76" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A196" s="109" t="s">
+        <v>575</v>
+      </c>
+      <c r="B196" s="110"/>
+    </row>
+    <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A197" s="57" t="s">
+        <v>576</v>
+      </c>
+      <c r="B197" s="76" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A198" s="57" t="s">
+        <v>578</v>
+      </c>
+      <c r="B198" s="76" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A199" s="57" t="s">
+        <v>582</v>
+      </c>
+      <c r="B199" s="94" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A200" s="57" t="s">
+        <v>580</v>
+      </c>
+      <c r="B200" s="94" t="s">
         <v>579</v>
       </c>
-      <c r="B194" s="76" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A195" s="57" t="s">
-        <v>581</v>
-      </c>
-      <c r="B195" s="76" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A196" s="57" t="s">
-        <v>585</v>
-      </c>
-      <c r="B196" s="96" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A197" s="57" t="s">
-        <v>583</v>
-      </c>
-      <c r="B197" s="96" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A198" s="107" t="s">
+    </row>
+    <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A201" s="111" t="s">
+        <v>596</v>
+      </c>
+      <c r="B201" s="111"/>
+      <c r="C201"/>
+    </row>
+    <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A202" s="109" t="s">
+        <v>598</v>
+      </c>
+      <c r="B202" s="110"/>
+    </row>
+    <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A203" s="57" t="s">
         <v>599</v>
       </c>
-      <c r="B198" s="107"/>
-      <c r="C198"/>
-    </row>
-    <row r="199" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A199" s="108" t="s">
+      <c r="B203" s="98" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A204" s="57" t="s">
         <v>601</v>
       </c>
-      <c r="B199" s="109"/>
-    </row>
-    <row r="200" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A200" s="57" t="s">
+      <c r="B204" s="98" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A205" s="57" t="s">
         <v>602</v>
       </c>
-      <c r="B200" s="100" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A201" s="57" t="s">
+      <c r="B205" s="98" t="s">
         <v>604</v>
       </c>
-      <c r="B201" s="100" t="s">
+    </row>
+    <row r="206" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A206" s="57" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A202" s="57" t="s">
+      <c r="B206" s="99" t="s">
         <v>605</v>
       </c>
-      <c r="B202" s="100" t="s">
+    </row>
+    <row r="207" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="57" t="s">
+        <v>608</v>
+      </c>
+      <c r="B207" s="98" t="s">
         <v>607</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A203" s="57" t="s">
-        <v>609</v>
-      </c>
-      <c r="B203" s="101" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A204" s="57" t="s">
-        <v>611</v>
-      </c>
-      <c r="B204" s="100" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A205" s="57"/>
-      <c r="B205" s="99"/>
-    </row>
-    <row r="206" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A206" s="108" t="s">
-        <v>612</v>
-      </c>
-      <c r="B206" s="109"/>
-    </row>
-    <row r="207" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A207" s="57" t="s">
-        <v>613</v>
-      </c>
-      <c r="B207" s="76" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A208" s="57"/>
-      <c r="B208" s="76"/>
-    </row>
-    <row r="209" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="57"/>
-      <c r="B209" s="76"/>
-    </row>
-    <row r="210" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="57"/>
-      <c r="B210" s="76"/>
+      <c r="B208" s="97"/>
+    </row>
+    <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A209" s="109" t="s">
+        <v>609</v>
+      </c>
+      <c r="B209" s="110"/>
+    </row>
+    <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A210" s="57" t="s">
+        <v>610</v>
+      </c>
+      <c r="B210" s="76" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="211" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A211" s="57"/>
@@ -12893,563 +12931,563 @@
       <c r="A214" s="57"/>
       <c r="B214" s="76"/>
     </row>
-    <row r="215" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A215" s="108" t="s">
-        <v>614</v>
-      </c>
-      <c r="B215" s="109"/>
-    </row>
-    <row r="216" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A216" s="72" t="s">
+    <row r="215" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A215" s="57"/>
+      <c r="B215" s="76"/>
+    </row>
+    <row r="216" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A216" s="57"/>
+      <c r="B216" s="76"/>
+    </row>
+    <row r="217" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A217" s="57"/>
+      <c r="B217" s="76"/>
+    </row>
+    <row r="218" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A218" s="109" t="s">
+        <v>611</v>
+      </c>
+      <c r="B218" s="110"/>
+    </row>
+    <row r="219" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A219" s="72" t="s">
+        <v>612</v>
+      </c>
+      <c r="B219" s="76" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A220" s="109" t="s">
         <v>615</v>
       </c>
-      <c r="B216" s="76" t="s">
+      <c r="B220" s="110"/>
+    </row>
+    <row r="221" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A221" s="57" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A217" s="108" t="s">
-        <v>618</v>
-      </c>
-      <c r="B217" s="109"/>
-    </row>
-    <row r="218" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A218" s="57" t="s">
-        <v>619</v>
-      </c>
-      <c r="B218" s="76" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A219" s="57" t="s">
-        <v>622</v>
-      </c>
-      <c r="B219" s="76" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A220" s="108" t="s">
+      <c r="B221" s="76" t="s">
         <v>617</v>
-      </c>
-      <c r="B220" s="109"/>
-    </row>
-    <row r="221" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A221" s="57" t="s">
-        <v>600</v>
-      </c>
-      <c r="B221" s="80" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A222" s="57" t="s">
+        <v>619</v>
+      </c>
+      <c r="B222" s="76" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A223" s="109" t="s">
+        <v>614</v>
+      </c>
+      <c r="B223" s="110"/>
+    </row>
+    <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A224" s="57" t="s">
+        <v>597</v>
+      </c>
+      <c r="B224" s="80" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A225" s="57" t="s">
+        <v>620</v>
+      </c>
+      <c r="B225" s="76" t="s">
         <v>623</v>
       </c>
-      <c r="B222" s="76" t="s">
+    </row>
+    <row r="226" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A226" s="57" t="s">
+        <v>621</v>
+      </c>
+      <c r="B226" s="76" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A227" s="57" t="s">
+        <v>625</v>
+      </c>
+      <c r="B227" s="76" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A223" s="57" t="s">
-        <v>624</v>
-      </c>
-      <c r="B223" s="76" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A224" s="57" t="s">
-        <v>628</v>
-      </c>
-      <c r="B224" s="76" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A225" s="107" t="s">
+    <row r="228" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A228" s="111" t="s">
+        <v>630</v>
+      </c>
+      <c r="B228" s="111"/>
+    </row>
+    <row r="229" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A229" s="109" t="s">
+        <v>632</v>
+      </c>
+      <c r="B229" s="110"/>
+    </row>
+    <row r="230" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A230" s="109" t="s">
+        <v>631</v>
+      </c>
+      <c r="B230" s="110"/>
+    </row>
+    <row r="231" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A231" s="57" t="s">
         <v>633</v>
       </c>
-      <c r="B225" s="107"/>
-    </row>
-    <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="108" t="s">
+      <c r="B231" s="76" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A232" s="109" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="109"/>
-    </row>
-    <row r="227" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A227" s="108" t="s">
-        <v>634</v>
-      </c>
-      <c r="B227" s="109"/>
-    </row>
-    <row r="228" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A228" s="57" t="s">
+      <c r="B232" s="110"/>
+    </row>
+    <row r="233" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A233" s="57" t="s">
+        <v>391</v>
+      </c>
+      <c r="B233" s="76" t="s">
         <v>636</v>
       </c>
-      <c r="B228" s="76" t="s">
+    </row>
+    <row r="234" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A234" s="57" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A229" s="108" t="s">
+      <c r="B234" s="76" t="s">
         <v>638</v>
       </c>
-      <c r="B229" s="109"/>
-    </row>
-    <row r="230" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A230" s="57" t="s">
-        <v>394</v>
-      </c>
-      <c r="B230" s="76" t="s">
+    </row>
+    <row r="235" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A235" s="57" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A231" s="57" t="s">
+      <c r="B235" s="76" t="s">
         <v>640</v>
       </c>
-      <c r="B231" s="76" t="s">
+    </row>
+    <row r="236" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A236" s="57" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A232" s="57" t="s">
+      <c r="B236" s="76" t="s">
         <v>642</v>
       </c>
-      <c r="B232" s="76" t="s">
+    </row>
+    <row r="237" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A237" s="57" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A233" s="57" t="s">
+      <c r="B237" s="76" t="s">
         <v>644</v>
       </c>
-      <c r="B233" s="76" t="s">
+    </row>
+    <row r="238" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A238" s="109" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A234" s="57" t="s">
+      <c r="B238" s="110"/>
+    </row>
+    <row r="239" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A239" s="57" t="s">
         <v>646</v>
       </c>
-      <c r="B234" s="76" t="s">
+      <c r="B239" s="76" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A235" s="108" t="s">
+    <row r="240" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A240" s="109" t="s">
         <v>648</v>
       </c>
-      <c r="B235" s="109"/>
-    </row>
-    <row r="236" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A236" s="57" t="s">
-        <v>649</v>
-      </c>
-      <c r="B236" s="76" t="s">
+      <c r="B240" s="110"/>
+    </row>
+    <row r="241" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A241" s="57" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="108" t="s">
-        <v>651</v>
-      </c>
-      <c r="B237" s="109"/>
-    </row>
-    <row r="238" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A238" s="57" t="s">
-        <v>653</v>
-      </c>
-      <c r="B238" s="76"/>
-    </row>
-    <row r="239" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A239" s="57" t="s">
-        <v>652</v>
-      </c>
-      <c r="B239" s="76" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A240" s="108" t="s">
-        <v>655</v>
-      </c>
-      <c r="B240" s="109"/>
-    </row>
-    <row r="241" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A241" s="57" t="s">
-        <v>656</v>
-      </c>
-      <c r="B241" s="76" t="s">
-        <v>657</v>
-      </c>
+      <c r="B241" s="76"/>
     </row>
     <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A242" s="57" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="B242" s="76" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A243" s="57" t="s">
-        <v>660</v>
-      </c>
-      <c r="B243" s="76" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A243" s="109" t="s">
+        <v>652</v>
+      </c>
+      <c r="B243" s="110"/>
+    </row>
+    <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A244" s="57" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="B244" s="76" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A245" s="57" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
       <c r="B245" s="76" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A246" s="57" t="s">
+        <v>657</v>
+      </c>
+      <c r="B246" s="76" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A247" s="57" t="s">
+        <v>659</v>
+      </c>
+      <c r="B247" s="76" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A248" s="57" t="s">
+        <v>661</v>
+      </c>
+      <c r="B248" s="76" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A249" s="57" t="s">
+        <v>663</v>
+      </c>
+      <c r="B249" s="76" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A250" s="57" t="s">
+        <v>665</v>
+      </c>
+      <c r="B250" s="76" t="s">
         <v>666</v>
-      </c>
-      <c r="B246" s="76" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A247" s="57" t="s">
-        <v>668</v>
-      </c>
-      <c r="B247" s="76" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A248" s="57" t="s">
-        <v>670</v>
-      </c>
-      <c r="B248" s="76" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A249" s="57" t="s">
-        <v>672</v>
-      </c>
-      <c r="B249" s="76" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A250" s="57" t="s">
-        <v>674</v>
-      </c>
-      <c r="B250" s="76" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A251" s="57" t="s">
-        <v>676</v>
+        <v>667</v>
       </c>
       <c r="B251" s="76" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A252" s="57" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
       <c r="B252" s="76" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A253" s="57" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="B253" s="76" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A254" s="57" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
       <c r="B254" s="76" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A255" s="57" t="s">
-        <v>684</v>
+        <v>675</v>
       </c>
       <c r="B255" s="76" t="s">
-        <v>685</v>
+        <v>676</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="57" t="s">
+        <v>677</v>
+      </c>
+      <c r="B256" s="76" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A257" s="57" t="s">
+        <v>679</v>
+      </c>
+      <c r="B257" s="76" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A258" s="57" t="s">
+        <v>681</v>
+      </c>
+      <c r="B258" s="76" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A259" s="57" t="s">
+        <v>683</v>
+      </c>
+      <c r="B259" s="76" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A260" s="57" t="s">
+        <v>685</v>
+      </c>
+      <c r="B260" s="76" t="s">
         <v>686</v>
       </c>
-      <c r="B256" s="76" t="s">
+    </row>
+    <row r="261" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A261" s="57" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A257" s="57" t="s">
+      <c r="B261" s="76" t="s">
         <v>688</v>
       </c>
-      <c r="B257" s="76" t="s">
+    </row>
+    <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A262" s="109" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A258" s="57" t="s">
+      <c r="B262" s="110"/>
+    </row>
+    <row r="263" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A263" s="57" t="s">
         <v>690</v>
       </c>
-      <c r="B258" s="76" t="s">
+      <c r="B263" s="76" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A259" s="108" t="s">
+    <row r="264" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A264" s="57" t="s">
         <v>692</v>
       </c>
-      <c r="B259" s="109"/>
-    </row>
-    <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A260" s="57" t="s">
+      <c r="B264" s="76" t="s">
         <v>693</v>
       </c>
-      <c r="B260" s="76" t="s">
+    </row>
+    <row r="265" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A265" s="57" t="s">
+        <v>695</v>
+      </c>
+      <c r="B265" s="76" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A261" s="57" t="s">
-        <v>695</v>
-      </c>
-      <c r="B261" s="76" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A262" s="57" t="s">
-        <v>698</v>
-      </c>
-      <c r="B262" s="76" t="s">
+    <row r="266" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A266" s="109" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="108" t="s">
-        <v>700</v>
-      </c>
-      <c r="B263" s="109"/>
-    </row>
-    <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A264" s="57" t="s">
-        <v>701</v>
-      </c>
-      <c r="B264" s="76" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A265" s="107" t="s">
-        <v>703</v>
-      </c>
-      <c r="B265" s="107"/>
-    </row>
-    <row r="266" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A266" s="108" t="s">
-        <v>704</v>
-      </c>
-      <c r="B266" s="109"/>
+      <c r="B266" s="110"/>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A267" s="57" t="s">
+        <v>698</v>
+      </c>
+      <c r="B267" s="76" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A268" s="111" t="s">
+        <v>700</v>
+      </c>
+      <c r="B268" s="111"/>
+    </row>
+    <row r="269" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A269" s="109" t="s">
+        <v>701</v>
+      </c>
+      <c r="B269" s="110"/>
+    </row>
+    <row r="270" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A270" s="57" t="s">
+        <v>701</v>
+      </c>
+      <c r="B270" s="76" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A271" s="57" t="s">
         <v>704</v>
       </c>
-      <c r="B267" s="76" t="s">
+      <c r="B271" s="102" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A272" s="57" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A268" s="57" t="s">
+      <c r="B272" s="102" t="s">
         <v>707</v>
       </c>
-      <c r="B268" s="104" t="s">
+    </row>
+    <row r="273" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A273" s="57" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A269" s="57" t="s">
+      <c r="B273" s="76" t="s">
         <v>709</v>
       </c>
-      <c r="B269" s="104" t="s">
+    </row>
+    <row r="274" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A274" s="109" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A270" s="57" t="s">
-        <v>711</v>
-      </c>
-      <c r="B270" s="76" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A271" s="108" t="s">
-        <v>713</v>
-      </c>
-      <c r="B271" s="109"/>
-    </row>
-    <row r="272" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A272" s="57" t="s">
-        <v>714</v>
-      </c>
-      <c r="B272" s="104" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A273" s="57" t="s">
-        <v>716</v>
-      </c>
-      <c r="B273" s="104" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A274" s="57" t="s">
-        <v>718</v>
-      </c>
-      <c r="B274" s="104" t="s">
-        <v>719</v>
-      </c>
+      <c r="B274" s="110"/>
     </row>
     <row r="275" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A275" s="57" t="s">
+        <v>711</v>
+      </c>
+      <c r="B275" s="102" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A276" s="57" t="s">
+        <v>713</v>
+      </c>
+      <c r="B276" s="102" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A277" s="57" t="s">
+        <v>715</v>
+      </c>
+      <c r="B277" s="102" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A278" s="57" t="s">
+        <v>717</v>
+      </c>
+      <c r="B278" s="102" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A279" s="109" t="s">
+        <v>702</v>
+      </c>
+      <c r="B279" s="110"/>
+    </row>
+    <row r="280" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A280" s="57" t="s">
+        <v>719</v>
+      </c>
+      <c r="B280" s="103" t="s">
         <v>720</v>
       </c>
-      <c r="B275" s="104" t="s">
+    </row>
+    <row r="281" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A281" s="57" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A276" s="108" t="s">
-        <v>705</v>
-      </c>
-      <c r="B276" s="109"/>
-    </row>
-    <row r="277" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A277" s="57" t="s">
+      <c r="B281" s="76" t="s">
         <v>722</v>
       </c>
-      <c r="B277" s="105" t="s">
+    </row>
+    <row r="282" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A282" s="57" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A278" s="57" t="s">
+      <c r="B282" s="76" t="s">
         <v>724</v>
       </c>
-      <c r="B278" s="76" t="s">
+    </row>
+    <row r="283" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A283" s="57" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A279" s="57" t="s">
+      <c r="B283" s="76" t="s">
         <v>726</v>
       </c>
-      <c r="B279" s="76" t="s">
+    </row>
+    <row r="284" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A284" s="57" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A280" s="57" t="s">
+      <c r="B284" s="106" t="s">
         <v>728</v>
       </c>
-      <c r="B280" s="76" t="s">
+      <c r="C284" s="104" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A285" s="57" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A281" s="57" t="s">
+      <c r="B285" s="76" t="s">
         <v>730</v>
       </c>
-      <c r="B281" s="126" t="s">
+      <c r="C285" s="92" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A286" s="109" t="s">
         <v>731</v>
       </c>
-      <c r="C281" s="106" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A282" s="57" t="s">
+      <c r="B286" s="110"/>
+    </row>
+    <row r="287" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A287" s="57" t="s">
         <v>732</v>
       </c>
-      <c r="B282" s="76" t="s">
+      <c r="B287" s="102" t="s">
         <v>733</v>
       </c>
-      <c r="C282" s="94" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A283" s="108" t="s">
+    </row>
+    <row r="288" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A288" s="57" t="s">
         <v>734</v>
       </c>
-      <c r="B283" s="109"/>
-    </row>
-    <row r="284" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A284" s="57" t="s">
+      <c r="B288" s="76" t="s">
         <v>735</v>
       </c>
-      <c r="B284" s="104" t="s">
+    </row>
+    <row r="289" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A289" s="57" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A285" s="57" t="s">
+      <c r="B289" s="102" t="s">
         <v>737</v>
       </c>
-      <c r="B285" s="76" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A286" s="57" t="s">
-        <v>739</v>
-      </c>
-      <c r="B286" s="104" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A287" s="57"/>
-      <c r="B287" s="76"/>
-    </row>
-    <row r="288" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A288" s="57"/>
-      <c r="B288" s="76"/>
-    </row>
-    <row r="289" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A289" s="57"/>
-      <c r="B289" s="76"/>
     </row>
     <row r="290" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A290" s="57"/>
@@ -13467,42 +13505,33 @@
       <c r="A293" s="57"/>
       <c r="B293" s="76"/>
     </row>
+    <row r="294" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A294" s="57"/>
+      <c r="B294" s="76"/>
+    </row>
+    <row r="295" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A295" s="57"/>
+      <c r="B295" s="76"/>
+    </row>
+    <row r="296" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A296" s="57"/>
+      <c r="B296" s="76"/>
+    </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A266:B266"/>
-    <mergeCell ref="A271:B271"/>
-    <mergeCell ref="A276:B276"/>
-    <mergeCell ref="A283:B283"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A229:B229"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="A265:B265"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A240:B240"/>
-    <mergeCell ref="A259:B259"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A76:A87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A228:B228"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A220:B220"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A2:B2"/>
@@ -13517,19 +13546,40 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
     <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="A198:B198"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A225:B225"/>
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="A206:B206"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A220:B220"/>
-    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A269:B269"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A279:B279"/>
+    <mergeCell ref="A286:B286"/>
+    <mergeCell ref="A229:B229"/>
+    <mergeCell ref="A230:B230"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A266:B266"/>
+    <mergeCell ref="A240:B240"/>
+    <mergeCell ref="A243:B243"/>
+    <mergeCell ref="A262:B262"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13951,7 +14001,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="124" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -13971,7 +14021,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123"/>
+      <c r="A2" s="125"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -14039,10 +14089,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="126" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="125"/>
+      <c r="C6" s="127"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB - 23.10.2019 - Update Folder Structure
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -7371,12 +7371,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8160,42 +8168,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8210,91 +8218,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8309,73 +8317,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8384,49 +8392,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8438,95 +8446,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11261,7 +11269,7 @@
   <dimension ref="A1:C290"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11283,13 +11291,13 @@
       <c r="A2" s="110" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="120"/>
+      <c r="B2" s="115"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="117" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="121"/>
+      <c r="B3" s="116"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11316,10 +11324,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="116" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="114"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11346,10 +11354,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="116" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="119"/>
+      <c r="B11" s="114"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11360,10 +11368,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="116" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="121"/>
+      <c r="B13" s="116"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11422,10 +11430,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="121" t="s">
+      <c r="A21" s="116" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="121"/>
+      <c r="B21" s="116"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11436,10 +11444,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="116" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="121"/>
+      <c r="B23" s="116"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11460,10 +11468,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="121" t="s">
+      <c r="A26" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="121"/>
+      <c r="B26" s="116"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -11490,10 +11498,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="121" t="s">
+      <c r="A30" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="121"/>
+      <c r="B30" s="116"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -11520,10 +11528,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="114" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="119"/>
+      <c r="B34" s="114"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -11550,10 +11558,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="121" t="s">
+      <c r="A38" s="116" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="121"/>
+      <c r="B38" s="116"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -11580,10 +11588,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="119" t="s">
+      <c r="A42" s="114" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="119"/>
+      <c r="B42" s="114"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -11602,10 +11610,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="121" t="s">
+      <c r="A45" s="116" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="119"/>
+      <c r="B45" s="114"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -11638,13 +11646,13 @@
       <c r="B49" s="110"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="111" t="s">
+      <c r="A50" s="113" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="109"/>
+      <c r="B50" s="112"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="116" t="s">
+      <c r="A51" s="121" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -11652,7 +11660,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="117"/>
+      <c r="A52" s="122"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -11661,13 +11669,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="118"/>
+      <c r="A53" s="123"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="116" t="s">
+      <c r="A54" s="121" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -11675,25 +11683,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="117"/>
+      <c r="A55" s="122"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="117"/>
+      <c r="A56" s="122"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="118"/>
+      <c r="A57" s="123"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="116" t="s">
+      <c r="A58" s="121" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -11701,13 +11709,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="118"/>
+      <c r="A59" s="123"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="116" t="s">
+      <c r="A60" s="121" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -11718,7 +11726,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="117"/>
+      <c r="A61" s="122"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -11727,14 +11735,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="117"/>
+      <c r="A62" s="122"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="118"/>
+      <c r="A63" s="123"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -11788,7 +11796,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="113" t="s">
+      <c r="A70" s="118" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -11796,43 +11804,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="114"/>
+      <c r="A71" s="119"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="114"/>
+      <c r="A72" s="119"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="114"/>
+      <c r="A73" s="119"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="114"/>
+      <c r="A74" s="119"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="114"/>
+      <c r="A75" s="119"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="115"/>
+      <c r="A76" s="120"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="113" t="s">
+      <c r="A77" s="118" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -11840,74 +11848,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="114"/>
+      <c r="A78" s="119"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="114"/>
+      <c r="A79" s="119"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="114"/>
+      <c r="A80" s="119"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="114"/>
+      <c r="A81" s="119"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="114"/>
+      <c r="A82" s="119"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="114"/>
+      <c r="A83" s="119"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="114"/>
+      <c r="A84" s="119"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="114"/>
+      <c r="A85" s="119"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="114"/>
+      <c r="A86" s="119"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="114"/>
+      <c r="A87" s="119"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="115"/>
+      <c r="A88" s="120"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="113" t="s">
+      <c r="A89" s="118" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -11915,28 +11923,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="114"/>
+      <c r="A90" s="119"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="114"/>
+      <c r="A91" s="119"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="115"/>
+      <c r="A92" s="120"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="113" t="s">
+      <c r="A93" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -11945,7 +11953,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="115"/>
+      <c r="A94" s="120"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -12022,10 +12030,10 @@
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="111" t="s">
+      <c r="A103" s="113" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="109"/>
+      <c r="B103" s="112"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -12056,10 +12064,10 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="111" t="s">
+      <c r="A107" s="113" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="109"/>
+      <c r="B107" s="112"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12129,7 +12137,7 @@
       <c r="A115" s="57" t="s">
         <v>408</v>
       </c>
-      <c r="B115" s="128" t="s">
+      <c r="B115" s="109" t="s">
         <v>409</v>
       </c>
       <c r="C115"/>
@@ -12216,10 +12224,10 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="111" t="s">
+      <c r="A125" s="113" t="s">
         <v>424</v>
       </c>
-      <c r="B125" s="109"/>
+      <c r="B125" s="112"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12304,10 +12312,10 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="111" t="s">
+      <c r="A135" s="113" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="109"/>
+      <c r="B135" s="112"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12401,10 +12409,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="108" t="s">
+      <c r="A146" s="111" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="109"/>
+      <c r="B146" s="112"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12435,10 +12443,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="108" t="s">
+      <c r="A150" s="111" t="s">
         <v>467</v>
       </c>
-      <c r="B150" s="109"/>
+      <c r="B150" s="112"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12460,10 +12468,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="108" t="s">
+      <c r="A153" s="111" t="s">
         <v>537</v>
       </c>
-      <c r="B153" s="109"/>
+      <c r="B153" s="112"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12512,10 +12520,10 @@
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="111" t="s">
+      <c r="A159" s="113" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="109"/>
+      <c r="B159" s="112"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12551,10 +12559,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="108" t="s">
+      <c r="A165" s="111" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="112"/>
+      <c r="B165" s="124"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12621,10 +12629,10 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="111" t="s">
+      <c r="A173" s="113" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="109"/>
+      <c r="B173" s="112"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12646,10 +12654,10 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="111" t="s">
+      <c r="A176" s="113" t="s">
         <v>471</v>
       </c>
-      <c r="B176" s="109"/>
+      <c r="B176" s="112"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12678,10 +12686,10 @@
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="111" t="s">
+      <c r="A180" s="113" t="s">
         <v>549</v>
       </c>
-      <c r="B180" s="109"/>
+      <c r="B180" s="112"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12697,10 +12705,10 @@
       <c r="B182" s="76"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="111" t="s">
+      <c r="A183" s="113" t="s">
         <v>548</v>
       </c>
-      <c r="B183" s="109"/>
+      <c r="B183" s="112"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12781,10 +12789,10 @@
       <c r="B192" s="76"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="111" t="s">
+      <c r="A193" s="113" t="s">
         <v>571</v>
       </c>
-      <c r="B193" s="109"/>
+      <c r="B193" s="112"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12802,10 +12810,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="108" t="s">
+      <c r="A196" s="111" t="s">
         <v>575</v>
       </c>
-      <c r="B196" s="109"/>
+      <c r="B196" s="112"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -12847,10 +12855,10 @@
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="108" t="s">
+      <c r="A202" s="111" t="s">
         <v>598</v>
       </c>
-      <c r="B202" s="109"/>
+      <c r="B202" s="112"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -12897,10 +12905,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="108" t="s">
+      <c r="A209" s="111" t="s">
         <v>609</v>
       </c>
-      <c r="B209" s="109"/>
+      <c r="B209" s="112"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -12915,10 +12923,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="108" t="s">
+      <c r="A212" s="111" t="s">
         <v>611</v>
       </c>
-      <c r="B212" s="109"/>
+      <c r="B212" s="112"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -12929,10 +12937,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="108" t="s">
+      <c r="A214" s="111" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="109"/>
+      <c r="B214" s="112"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -12951,10 +12959,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="108" t="s">
+      <c r="A217" s="111" t="s">
         <v>614</v>
       </c>
-      <c r="B217" s="109"/>
+      <c r="B217" s="112"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -12995,16 +13003,16 @@
       <c r="B222" s="110"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="108" t="s">
+      <c r="A223" s="111" t="s">
         <v>632</v>
       </c>
-      <c r="B223" s="109"/>
+      <c r="B223" s="112"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="108" t="s">
+      <c r="A224" s="111" t="s">
         <v>631</v>
       </c>
-      <c r="B224" s="109"/>
+      <c r="B224" s="112"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -13015,10 +13023,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="108" t="s">
+      <c r="A226" s="111" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="109"/>
+      <c r="B226" s="112"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -13061,10 +13069,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="108" t="s">
+      <c r="A232" s="111" t="s">
         <v>645</v>
       </c>
-      <c r="B232" s="109"/>
+      <c r="B232" s="112"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -13075,10 +13083,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="108" t="s">
+      <c r="A234" s="111" t="s">
         <v>648</v>
       </c>
-      <c r="B234" s="109"/>
+      <c r="B234" s="112"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -13095,10 +13103,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="108" t="s">
+      <c r="A237" s="111" t="s">
         <v>652</v>
       </c>
-      <c r="B237" s="109"/>
+      <c r="B237" s="112"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -13245,10 +13253,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="108" t="s">
+      <c r="A256" s="111" t="s">
         <v>689</v>
       </c>
-      <c r="B256" s="109"/>
+      <c r="B256" s="112"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -13275,10 +13283,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="108" t="s">
+      <c r="A260" s="111" t="s">
         <v>697</v>
       </c>
-      <c r="B260" s="109"/>
+      <c r="B260" s="112"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -13295,10 +13303,10 @@
       <c r="B262" s="110"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="108" t="s">
+      <c r="A263" s="111" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="109"/>
+      <c r="B263" s="112"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -13333,10 +13341,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="108" t="s">
+      <c r="A268" s="111" t="s">
         <v>710</v>
       </c>
-      <c r="B268" s="109"/>
+      <c r="B268" s="112"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -13371,10 +13379,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="108" t="s">
+      <c r="A273" s="111" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="109"/>
+      <c r="B273" s="112"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -13412,7 +13420,7 @@
       <c r="A278" s="57" t="s">
         <v>727</v>
       </c>
-      <c r="B278" s="127" t="s">
+      <c r="B278" s="108" t="s">
         <v>728</v>
       </c>
       <c r="C278" s="104" t="s">
@@ -13431,10 +13439,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="108" t="s">
+      <c r="A280" s="111" t="s">
         <v>731</v>
       </c>
-      <c r="B280" s="109"/>
+      <c r="B280" s="112"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -13490,18 +13498,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -13518,39 +13547,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13972,7 +13980,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -13992,7 +14000,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124"/>
+      <c r="A2" s="126"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -14060,10 +14068,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="127" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="126"/>
+      <c r="C6" s="128"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework - 01.Fetching Resultsets With ADO.NET
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="631" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
-    <sheet name="DB-SQL" sheetId="11" r:id="rId2"/>
-    <sheet name="DB" sheetId="4" r:id="rId3"/>
-    <sheet name="Regex" sheetId="2" r:id="rId4"/>
-    <sheet name="Solidity" sheetId="5" r:id="rId5"/>
-    <sheet name="Git" sheetId="6" r:id="rId6"/>
-    <sheet name="Comparators" sheetId="7" r:id="rId7"/>
-    <sheet name="ShortCuts" sheetId="3" r:id="rId8"/>
-    <sheet name="OOP" sheetId="8" r:id="rId9"/>
-    <sheet name="SOLID" sheetId="12" r:id="rId10"/>
-    <sheet name="Reflection" sheetId="9" r:id="rId11"/>
-    <sheet name="UnitTesting" sheetId="10" r:id="rId12"/>
+    <sheet name="DB-EF" sheetId="13" r:id="rId2"/>
+    <sheet name="DB-SQL" sheetId="11" r:id="rId3"/>
+    <sheet name="DB" sheetId="4" r:id="rId4"/>
+    <sheet name="Regex" sheetId="2" r:id="rId5"/>
+    <sheet name="Solidity" sheetId="5" r:id="rId6"/>
+    <sheet name="Git" sheetId="6" r:id="rId7"/>
+    <sheet name="Comparators" sheetId="7" r:id="rId8"/>
+    <sheet name="ShortCuts" sheetId="3" r:id="rId9"/>
+    <sheet name="OOP" sheetId="8" r:id="rId10"/>
+    <sheet name="SOLID" sheetId="12" r:id="rId11"/>
+    <sheet name="Reflection" sheetId="9" r:id="rId12"/>
+    <sheet name="UnitTesting" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -8479,29 +8480,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8521,8 +8513,17 @@
     <xf numFmtId="0" fontId="40" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -11076,6 +11077,154 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11133,7 +11282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -11208,7 +11357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11266,9 +11415,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
@@ -11288,16 +11451,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="112" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="122"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="124" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="116"/>
+      <c r="B3" s="123"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11324,10 +11487,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="123" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="114"/>
+      <c r="B7" s="121"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11354,10 +11517,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="123" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="114"/>
+      <c r="B11" s="121"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11368,10 +11531,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="123" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="116"/>
+      <c r="B13" s="123"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11430,10 +11593,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="123" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="116"/>
+      <c r="B21" s="123"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11444,10 +11607,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="123" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="116"/>
+      <c r="B23" s="123"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11468,10 +11631,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="116"/>
+      <c r="B26" s="123"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -11498,10 +11661,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="116"/>
+      <c r="B30" s="123"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -11528,10 +11691,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="114" t="s">
+      <c r="A34" s="121" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="114"/>
+      <c r="B34" s="121"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -11558,10 +11721,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="116" t="s">
+      <c r="A38" s="123" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="116"/>
+      <c r="B38" s="123"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -11588,10 +11751,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="121" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="114"/>
+      <c r="B42" s="121"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -11610,10 +11773,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="116" t="s">
+      <c r="A45" s="123" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="114"/>
+      <c r="B45" s="121"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -11640,19 +11803,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="110" t="s">
+      <c r="A49" s="112" t="s">
         <v>369</v>
       </c>
-      <c r="B49" s="110"/>
+      <c r="B49" s="112"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A50" s="113" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="112"/>
+      <c r="B50" s="111"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="121" t="s">
+      <c r="A51" s="118" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -11660,7 +11823,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="122"/>
+      <c r="A52" s="119"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -11669,13 +11832,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="123"/>
+      <c r="A53" s="120"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="121" t="s">
+      <c r="A54" s="118" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -11683,25 +11846,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="122"/>
+      <c r="A55" s="119"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="122"/>
+      <c r="A56" s="119"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="123"/>
+      <c r="A57" s="120"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="121" t="s">
+      <c r="A58" s="118" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -11709,13 +11872,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="123"/>
+      <c r="A59" s="120"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="121" t="s">
+      <c r="A60" s="118" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -11726,7 +11889,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="122"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -11735,14 +11898,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="122"/>
+      <c r="A62" s="119"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="123"/>
+      <c r="A63" s="120"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -11796,7 +11959,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="115" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -11804,43 +11967,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="119"/>
+      <c r="A71" s="116"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="119"/>
+      <c r="A72" s="116"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="119"/>
+      <c r="A73" s="116"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="119"/>
+      <c r="A74" s="116"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="119"/>
+      <c r="A75" s="116"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="120"/>
+      <c r="A76" s="117"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="118" t="s">
+      <c r="A77" s="115" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -11848,74 +12011,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="119"/>
+      <c r="A78" s="116"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="119"/>
+      <c r="A79" s="116"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="119"/>
+      <c r="A80" s="116"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="119"/>
+      <c r="A81" s="116"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="119"/>
+      <c r="A82" s="116"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="119"/>
+      <c r="A83" s="116"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="119"/>
+      <c r="A84" s="116"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="119"/>
+      <c r="A85" s="116"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="119"/>
+      <c r="A86" s="116"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="119"/>
+      <c r="A87" s="116"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="120"/>
+      <c r="A88" s="117"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="118" t="s">
+      <c r="A89" s="115" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -11923,28 +12086,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="119"/>
+      <c r="A90" s="116"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="119"/>
+      <c r="A91" s="116"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="120"/>
+      <c r="A92" s="117"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="118" t="s">
+      <c r="A93" s="115" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -11953,7 +12116,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="120"/>
+      <c r="A94" s="117"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -12023,17 +12186,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="110" t="s">
+      <c r="A102" s="112" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="110"/>
+      <c r="B102" s="112"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A103" s="113" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="112"/>
+      <c r="B103" s="111"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -12067,7 +12230,7 @@
       <c r="A107" s="113" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="112"/>
+      <c r="B107" s="111"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12227,7 +12390,7 @@
       <c r="A125" s="113" t="s">
         <v>424</v>
       </c>
-      <c r="B125" s="112"/>
+      <c r="B125" s="111"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12315,7 +12478,7 @@
       <c r="A135" s="113" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="112"/>
+      <c r="B135" s="111"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12409,10 +12572,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="111" t="s">
+      <c r="A146" s="110" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="112"/>
+      <c r="B146" s="111"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12443,10 +12606,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="111" t="s">
+      <c r="A150" s="110" t="s">
         <v>467</v>
       </c>
-      <c r="B150" s="112"/>
+      <c r="B150" s="111"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12468,10 +12631,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="111" t="s">
+      <c r="A153" s="110" t="s">
         <v>537</v>
       </c>
-      <c r="B153" s="112"/>
+      <c r="B153" s="111"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12513,17 +12676,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="110" t="s">
+      <c r="A158" s="112" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="110"/>
+      <c r="B158" s="112"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A159" s="113" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="112"/>
+      <c r="B159" s="111"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12559,10 +12722,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="111" t="s">
+      <c r="A165" s="110" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="124"/>
+      <c r="B165" s="114"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12632,7 +12795,7 @@
       <c r="A173" s="113" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="112"/>
+      <c r="B173" s="111"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12657,7 +12820,7 @@
       <c r="A176" s="113" t="s">
         <v>471</v>
       </c>
-      <c r="B176" s="112"/>
+      <c r="B176" s="111"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12679,17 +12842,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="110" t="s">
+      <c r="A179" s="112" t="s">
         <v>548</v>
       </c>
-      <c r="B179" s="110"/>
+      <c r="B179" s="112"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A180" s="113" t="s">
         <v>549</v>
       </c>
-      <c r="B180" s="112"/>
+      <c r="B180" s="111"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12708,7 +12871,7 @@
       <c r="A183" s="113" t="s">
         <v>548</v>
       </c>
-      <c r="B183" s="112"/>
+      <c r="B183" s="111"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12792,7 +12955,7 @@
       <c r="A193" s="113" t="s">
         <v>571</v>
       </c>
-      <c r="B193" s="112"/>
+      <c r="B193" s="111"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12810,10 +12973,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="111" t="s">
+      <c r="A196" s="110" t="s">
         <v>575</v>
       </c>
-      <c r="B196" s="112"/>
+      <c r="B196" s="111"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -12848,17 +13011,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="110" t="s">
+      <c r="A201" s="112" t="s">
         <v>596</v>
       </c>
-      <c r="B201" s="110"/>
+      <c r="B201" s="112"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="111" t="s">
+      <c r="A202" s="110" t="s">
         <v>598</v>
       </c>
-      <c r="B202" s="112"/>
+      <c r="B202" s="111"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -12905,10 +13068,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="111" t="s">
+      <c r="A209" s="110" t="s">
         <v>609</v>
       </c>
-      <c r="B209" s="112"/>
+      <c r="B209" s="111"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -12923,10 +13086,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="111" t="s">
+      <c r="A212" s="110" t="s">
         <v>611</v>
       </c>
-      <c r="B212" s="112"/>
+      <c r="B212" s="111"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -12937,10 +13100,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="111" t="s">
+      <c r="A214" s="110" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="112"/>
+      <c r="B214" s="111"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -12959,10 +13122,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="111" t="s">
+      <c r="A217" s="110" t="s">
         <v>614</v>
       </c>
-      <c r="B217" s="112"/>
+      <c r="B217" s="111"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -12997,22 +13160,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="110" t="s">
+      <c r="A222" s="112" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="110"/>
+      <c r="B222" s="112"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="111" t="s">
+      <c r="A223" s="110" t="s">
         <v>632</v>
       </c>
-      <c r="B223" s="112"/>
+      <c r="B223" s="111"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="111" t="s">
+      <c r="A224" s="110" t="s">
         <v>631</v>
       </c>
-      <c r="B224" s="112"/>
+      <c r="B224" s="111"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -13023,10 +13186,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="111" t="s">
+      <c r="A226" s="110" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="112"/>
+      <c r="B226" s="111"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -13069,10 +13232,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="111" t="s">
+      <c r="A232" s="110" t="s">
         <v>645</v>
       </c>
-      <c r="B232" s="112"/>
+      <c r="B232" s="111"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -13083,10 +13246,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="111" t="s">
+      <c r="A234" s="110" t="s">
         <v>648</v>
       </c>
-      <c r="B234" s="112"/>
+      <c r="B234" s="111"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -13103,10 +13266,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="111" t="s">
+      <c r="A237" s="110" t="s">
         <v>652</v>
       </c>
-      <c r="B237" s="112"/>
+      <c r="B237" s="111"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -13253,10 +13416,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="111" t="s">
+      <c r="A256" s="110" t="s">
         <v>689</v>
       </c>
-      <c r="B256" s="112"/>
+      <c r="B256" s="111"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -13283,10 +13446,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="111" t="s">
+      <c r="A260" s="110" t="s">
         <v>697</v>
       </c>
-      <c r="B260" s="112"/>
+      <c r="B260" s="111"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -13297,16 +13460,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="110" t="s">
+      <c r="A262" s="112" t="s">
         <v>700</v>
       </c>
-      <c r="B262" s="110"/>
+      <c r="B262" s="112"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="111" t="s">
+      <c r="A263" s="110" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="112"/>
+      <c r="B263" s="111"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -13341,10 +13504,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="111" t="s">
+      <c r="A268" s="110" t="s">
         <v>710</v>
       </c>
-      <c r="B268" s="112"/>
+      <c r="B268" s="111"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -13379,10 +13542,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="111" t="s">
+      <c r="A273" s="110" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="112"/>
+      <c r="B273" s="111"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -13439,10 +13602,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="111" t="s">
+      <c r="A280" s="110" t="s">
         <v>731</v>
       </c>
-      <c r="B280" s="112"/>
+      <c r="B280" s="111"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -13498,39 +13661,18 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -13547,25 +13689,46 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -13659,7 +13822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -13957,7 +14120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -14103,7 +14266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -14222,7 +14385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -14265,7 +14428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -14313,152 +14476,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="42" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>255</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>241</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>254</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
-        <v>224</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>222</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>227</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>225</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
-        <v>262</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>269</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework - 02.ORM-Fundamentals-MiniORM-Exercise
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -8480,20 +8480,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8513,17 +8522,8 @@
     <xf numFmtId="0" fontId="40" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -11451,16 +11451,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="110" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="122"/>
+      <c r="B2" s="115"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="117" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="123"/>
+      <c r="B3" s="116"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11487,10 +11487,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="116" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="121"/>
+      <c r="B7" s="114"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11517,10 +11517,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="116" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="121"/>
+      <c r="B11" s="114"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11531,10 +11531,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="116" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="116"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11593,10 +11593,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="123" t="s">
+      <c r="A21" s="116" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="123"/>
+      <c r="B21" s="116"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11607,10 +11607,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="116" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="123"/>
+      <c r="B23" s="116"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11631,10 +11631,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="123" t="s">
+      <c r="A26" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="123"/>
+      <c r="B26" s="116"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -11661,10 +11661,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="123"/>
+      <c r="B30" s="116"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -11691,10 +11691,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="121" t="s">
+      <c r="A34" s="114" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="121"/>
+      <c r="B34" s="114"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -11721,10 +11721,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="123" t="s">
+      <c r="A38" s="116" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="123"/>
+      <c r="B38" s="116"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -11751,10 +11751,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="121" t="s">
+      <c r="A42" s="114" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="121"/>
+      <c r="B42" s="114"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -11773,10 +11773,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="123" t="s">
+      <c r="A45" s="116" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="121"/>
+      <c r="B45" s="114"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -11803,19 +11803,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="112" t="s">
+      <c r="A49" s="110" t="s">
         <v>369</v>
       </c>
-      <c r="B49" s="112"/>
+      <c r="B49" s="110"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A50" s="113" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="111"/>
+      <c r="B50" s="112"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="118" t="s">
+      <c r="A51" s="121" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -11823,7 +11823,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="119"/>
+      <c r="A52" s="122"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -11832,13 +11832,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="120"/>
+      <c r="A53" s="123"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="118" t="s">
+      <c r="A54" s="121" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -11846,25 +11846,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="119"/>
+      <c r="A55" s="122"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="119"/>
+      <c r="A56" s="122"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="120"/>
+      <c r="A57" s="123"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="118" t="s">
+      <c r="A58" s="121" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -11872,13 +11872,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="120"/>
+      <c r="A59" s="123"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="118" t="s">
+      <c r="A60" s="121" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -11889,7 +11889,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="119"/>
+      <c r="A61" s="122"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -11898,14 +11898,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="119"/>
+      <c r="A62" s="122"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="120"/>
+      <c r="A63" s="123"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -11959,7 +11959,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="115" t="s">
+      <c r="A70" s="118" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -11967,43 +11967,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="116"/>
+      <c r="A71" s="119"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="116"/>
+      <c r="A72" s="119"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="116"/>
+      <c r="A73" s="119"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="116"/>
+      <c r="A74" s="119"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="116"/>
+      <c r="A75" s="119"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="117"/>
+      <c r="A76" s="120"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="115" t="s">
+      <c r="A77" s="118" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -12011,74 +12011,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="116"/>
+      <c r="A78" s="119"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="116"/>
+      <c r="A79" s="119"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="116"/>
+      <c r="A80" s="119"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="116"/>
+      <c r="A81" s="119"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="116"/>
+      <c r="A82" s="119"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
+      <c r="A83" s="119"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="116"/>
+      <c r="A84" s="119"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="116"/>
+      <c r="A85" s="119"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="116"/>
+      <c r="A86" s="119"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="116"/>
+      <c r="A87" s="119"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="117"/>
+      <c r="A88" s="120"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="115" t="s">
+      <c r="A89" s="118" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -12086,28 +12086,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="116"/>
+      <c r="A90" s="119"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="116"/>
+      <c r="A91" s="119"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="117"/>
+      <c r="A92" s="120"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="115" t="s">
+      <c r="A93" s="118" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -12116,7 +12116,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="117"/>
+      <c r="A94" s="120"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -12186,17 +12186,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="112" t="s">
+      <c r="A102" s="110" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="112"/>
+      <c r="B102" s="110"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A103" s="113" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="111"/>
+      <c r="B103" s="112"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -12230,7 +12230,7 @@
       <c r="A107" s="113" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="111"/>
+      <c r="B107" s="112"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12390,7 +12390,7 @@
       <c r="A125" s="113" t="s">
         <v>424</v>
       </c>
-      <c r="B125" s="111"/>
+      <c r="B125" s="112"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12478,7 +12478,7 @@
       <c r="A135" s="113" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="111"/>
+      <c r="B135" s="112"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12572,10 +12572,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="110" t="s">
+      <c r="A146" s="111" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="111"/>
+      <c r="B146" s="112"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12606,10 +12606,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="110" t="s">
+      <c r="A150" s="111" t="s">
         <v>467</v>
       </c>
-      <c r="B150" s="111"/>
+      <c r="B150" s="112"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12631,10 +12631,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="110" t="s">
+      <c r="A153" s="111" t="s">
         <v>537</v>
       </c>
-      <c r="B153" s="111"/>
+      <c r="B153" s="112"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12676,17 +12676,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="112" t="s">
+      <c r="A158" s="110" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="112"/>
+      <c r="B158" s="110"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A159" s="113" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="111"/>
+      <c r="B159" s="112"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12722,10 +12722,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="110" t="s">
+      <c r="A165" s="111" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="114"/>
+      <c r="B165" s="124"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12795,7 +12795,7 @@
       <c r="A173" s="113" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="111"/>
+      <c r="B173" s="112"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12820,7 +12820,7 @@
       <c r="A176" s="113" t="s">
         <v>471</v>
       </c>
-      <c r="B176" s="111"/>
+      <c r="B176" s="112"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12842,17 +12842,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="112" t="s">
+      <c r="A179" s="110" t="s">
         <v>548</v>
       </c>
-      <c r="B179" s="112"/>
+      <c r="B179" s="110"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A180" s="113" t="s">
         <v>549</v>
       </c>
-      <c r="B180" s="111"/>
+      <c r="B180" s="112"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
       <c r="A183" s="113" t="s">
         <v>548</v>
       </c>
-      <c r="B183" s="111"/>
+      <c r="B183" s="112"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12955,7 +12955,7 @@
       <c r="A193" s="113" t="s">
         <v>571</v>
       </c>
-      <c r="B193" s="111"/>
+      <c r="B193" s="112"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12973,10 +12973,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="110" t="s">
+      <c r="A196" s="111" t="s">
         <v>575</v>
       </c>
-      <c r="B196" s="111"/>
+      <c r="B196" s="112"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -13011,17 +13011,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="112" t="s">
+      <c r="A201" s="110" t="s">
         <v>596</v>
       </c>
-      <c r="B201" s="112"/>
+      <c r="B201" s="110"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="110" t="s">
+      <c r="A202" s="111" t="s">
         <v>598</v>
       </c>
-      <c r="B202" s="111"/>
+      <c r="B202" s="112"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -13068,10 +13068,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="110" t="s">
+      <c r="A209" s="111" t="s">
         <v>609</v>
       </c>
-      <c r="B209" s="111"/>
+      <c r="B209" s="112"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -13086,10 +13086,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="110" t="s">
+      <c r="A212" s="111" t="s">
         <v>611</v>
       </c>
-      <c r="B212" s="111"/>
+      <c r="B212" s="112"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -13100,10 +13100,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="110" t="s">
+      <c r="A214" s="111" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="111"/>
+      <c r="B214" s="112"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -13122,10 +13122,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="110" t="s">
+      <c r="A217" s="111" t="s">
         <v>614</v>
       </c>
-      <c r="B217" s="111"/>
+      <c r="B217" s="112"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -13160,22 +13160,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="112" t="s">
+      <c r="A222" s="110" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="112"/>
+      <c r="B222" s="110"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="110" t="s">
+      <c r="A223" s="111" t="s">
         <v>632</v>
       </c>
-      <c r="B223" s="111"/>
+      <c r="B223" s="112"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="110" t="s">
+      <c r="A224" s="111" t="s">
         <v>631</v>
       </c>
-      <c r="B224" s="111"/>
+      <c r="B224" s="112"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -13186,10 +13186,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="110" t="s">
+      <c r="A226" s="111" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="111"/>
+      <c r="B226" s="112"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -13232,10 +13232,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="110" t="s">
+      <c r="A232" s="111" t="s">
         <v>645</v>
       </c>
-      <c r="B232" s="111"/>
+      <c r="B232" s="112"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -13246,10 +13246,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="110" t="s">
+      <c r="A234" s="111" t="s">
         <v>648</v>
       </c>
-      <c r="B234" s="111"/>
+      <c r="B234" s="112"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -13266,10 +13266,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="110" t="s">
+      <c r="A237" s="111" t="s">
         <v>652</v>
       </c>
-      <c r="B237" s="111"/>
+      <c r="B237" s="112"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -13416,10 +13416,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="110" t="s">
+      <c r="A256" s="111" t="s">
         <v>689</v>
       </c>
-      <c r="B256" s="111"/>
+      <c r="B256" s="112"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -13446,10 +13446,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="110" t="s">
+      <c r="A260" s="111" t="s">
         <v>697</v>
       </c>
-      <c r="B260" s="111"/>
+      <c r="B260" s="112"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -13460,16 +13460,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="112" t="s">
+      <c r="A262" s="110" t="s">
         <v>700</v>
       </c>
-      <c r="B262" s="112"/>
+      <c r="B262" s="110"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="110" t="s">
+      <c r="A263" s="111" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="111"/>
+      <c r="B263" s="112"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -13504,10 +13504,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="110" t="s">
+      <c r="A268" s="111" t="s">
         <v>710</v>
       </c>
-      <c r="B268" s="111"/>
+      <c r="B268" s="112"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -13542,10 +13542,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="110" t="s">
+      <c r="A273" s="111" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="111"/>
+      <c r="B273" s="112"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -13602,10 +13602,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="110" t="s">
+      <c r="A280" s="111" t="s">
         <v>731</v>
       </c>
-      <c r="B280" s="111"/>
+      <c r="B280" s="112"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -13661,18 +13661,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -13689,39 +13710,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework -03.Introduction-to-EntityFramework-Exercise
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
-    <sheet name="DB-EF" sheetId="13" r:id="rId2"/>
+    <sheet name="DB-EF-Databas First" sheetId="13" r:id="rId2"/>
     <sheet name="DB-SQL" sheetId="11" r:id="rId3"/>
     <sheet name="DB" sheetId="4" r:id="rId4"/>
     <sheet name="Regex" sheetId="2" r:id="rId5"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="759">
   <si>
     <t>Операция</t>
   </si>
@@ -7366,6 +7366,42 @@
     <t xml:space="preserve">Replaces NULL with the specified replacement value:
 SELECT AVG(ISNULL(Weight, 50))  
 FROM Production.Product;  </t>
+  </si>
+  <si>
+    <t>Install Needed packeges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install-Package Microsoft.EntityFrameworkCore.Tools –v 2.2.0
+Install-Package Microsoft.EntityFrameworkCore.SqlServer –v 2.2.0
+Install-Package Microsoft.EntityFrameworkCore.SqlServer.Design
+</t>
+  </si>
+  <si>
+    <t>Scaffold-DbContext -Connection "Server=.;Database=SoftUni;Integrated Security=True;" -Provider Microsoft.EntityFrameworkCore.SqlServer -OutputDir Data/Models</t>
+  </si>
+  <si>
+    <r>
+      <t>scaffold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /Command to generate entities/</t>
+    </r>
+  </si>
+  <si>
+    <t>CleanUp packages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uninstall-Package Microsoft.EntityFrameworkCore.Tools -r
+Uninstall-Package Microsoft.EntityFrameworkCore.SqlServer.Design -RemoveDependencies
+</t>
   </si>
 </sst>
 </file>
@@ -8175,7 +8211,7 @@
     <xf numFmtId="0" fontId="39" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8480,29 +8516,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8522,8 +8549,17 @@
     <xf numFmtId="0" fontId="40" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8536,6 +8572,15 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11415,15 +11460,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23" style="129" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.28515625" style="129" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="130" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1" s="129" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="130" t="s">
+        <v>756</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="130" t="s">
+        <v>757</v>
+      </c>
+      <c r="B3" s="131" t="s">
+        <v>758</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11451,16 +11526,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="112" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="122"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="124" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="116"/>
+      <c r="B3" s="123"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11487,10 +11562,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="123" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="114"/>
+      <c r="B7" s="121"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11517,10 +11592,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="123" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="114"/>
+      <c r="B11" s="121"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11531,10 +11606,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="123" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="116"/>
+      <c r="B13" s="123"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11593,10 +11668,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="123" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="116"/>
+      <c r="B21" s="123"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11607,10 +11682,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="123" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="116"/>
+      <c r="B23" s="123"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11631,10 +11706,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="116"/>
+      <c r="B26" s="123"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -11661,10 +11736,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="116"/>
+      <c r="B30" s="123"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -11691,10 +11766,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="114" t="s">
+      <c r="A34" s="121" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="114"/>
+      <c r="B34" s="121"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -11721,10 +11796,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="116" t="s">
+      <c r="A38" s="123" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="116"/>
+      <c r="B38" s="123"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -11751,10 +11826,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="121" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="114"/>
+      <c r="B42" s="121"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -11773,10 +11848,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="116" t="s">
+      <c r="A45" s="123" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="114"/>
+      <c r="B45" s="121"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -11803,19 +11878,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="110" t="s">
+      <c r="A49" s="112" t="s">
         <v>369</v>
       </c>
-      <c r="B49" s="110"/>
+      <c r="B49" s="112"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A50" s="113" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="112"/>
+      <c r="B50" s="111"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="121" t="s">
+      <c r="A51" s="118" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -11823,7 +11898,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="122"/>
+      <c r="A52" s="119"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -11832,13 +11907,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="123"/>
+      <c r="A53" s="120"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="121" t="s">
+      <c r="A54" s="118" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -11846,25 +11921,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="122"/>
+      <c r="A55" s="119"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="122"/>
+      <c r="A56" s="119"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="123"/>
+      <c r="A57" s="120"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="121" t="s">
+      <c r="A58" s="118" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -11872,13 +11947,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="123"/>
+      <c r="A59" s="120"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="121" t="s">
+      <c r="A60" s="118" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -11889,7 +11964,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="122"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -11898,14 +11973,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="122"/>
+      <c r="A62" s="119"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="123"/>
+      <c r="A63" s="120"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -11959,7 +12034,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="115" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -11967,43 +12042,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="119"/>
+      <c r="A71" s="116"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="119"/>
+      <c r="A72" s="116"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="119"/>
+      <c r="A73" s="116"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="119"/>
+      <c r="A74" s="116"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="119"/>
+      <c r="A75" s="116"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="120"/>
+      <c r="A76" s="117"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="118" t="s">
+      <c r="A77" s="115" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -12011,74 +12086,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="119"/>
+      <c r="A78" s="116"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="119"/>
+      <c r="A79" s="116"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="119"/>
+      <c r="A80" s="116"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="119"/>
+      <c r="A81" s="116"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="119"/>
+      <c r="A82" s="116"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="119"/>
+      <c r="A83" s="116"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="119"/>
+      <c r="A84" s="116"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="119"/>
+      <c r="A85" s="116"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="119"/>
+      <c r="A86" s="116"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="119"/>
+      <c r="A87" s="116"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="120"/>
+      <c r="A88" s="117"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="118" t="s">
+      <c r="A89" s="115" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -12086,28 +12161,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="119"/>
+      <c r="A90" s="116"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="119"/>
+      <c r="A91" s="116"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="120"/>
+      <c r="A92" s="117"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="118" t="s">
+      <c r="A93" s="115" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -12116,7 +12191,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="120"/>
+      <c r="A94" s="117"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -12186,17 +12261,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="110" t="s">
+      <c r="A102" s="112" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="110"/>
+      <c r="B102" s="112"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A103" s="113" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="112"/>
+      <c r="B103" s="111"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -12230,7 +12305,7 @@
       <c r="A107" s="113" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="112"/>
+      <c r="B107" s="111"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12390,7 +12465,7 @@
       <c r="A125" s="113" t="s">
         <v>424</v>
       </c>
-      <c r="B125" s="112"/>
+      <c r="B125" s="111"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12478,7 +12553,7 @@
       <c r="A135" s="113" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="112"/>
+      <c r="B135" s="111"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12572,10 +12647,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="111" t="s">
+      <c r="A146" s="110" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="112"/>
+      <c r="B146" s="111"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12606,10 +12681,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="111" t="s">
+      <c r="A150" s="110" t="s">
         <v>467</v>
       </c>
-      <c r="B150" s="112"/>
+      <c r="B150" s="111"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12631,10 +12706,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="111" t="s">
+      <c r="A153" s="110" t="s">
         <v>537</v>
       </c>
-      <c r="B153" s="112"/>
+      <c r="B153" s="111"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12676,17 +12751,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="110" t="s">
+      <c r="A158" s="112" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="110"/>
+      <c r="B158" s="112"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A159" s="113" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="112"/>
+      <c r="B159" s="111"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12722,10 +12797,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="111" t="s">
+      <c r="A165" s="110" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="124"/>
+      <c r="B165" s="114"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12795,7 +12870,7 @@
       <c r="A173" s="113" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="112"/>
+      <c r="B173" s="111"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12820,7 +12895,7 @@
       <c r="A176" s="113" t="s">
         <v>471</v>
       </c>
-      <c r="B176" s="112"/>
+      <c r="B176" s="111"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12842,17 +12917,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="110" t="s">
+      <c r="A179" s="112" t="s">
         <v>548</v>
       </c>
-      <c r="B179" s="110"/>
+      <c r="B179" s="112"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A180" s="113" t="s">
         <v>549</v>
       </c>
-      <c r="B180" s="112"/>
+      <c r="B180" s="111"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12871,7 +12946,7 @@
       <c r="A183" s="113" t="s">
         <v>548</v>
       </c>
-      <c r="B183" s="112"/>
+      <c r="B183" s="111"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12955,7 +13030,7 @@
       <c r="A193" s="113" t="s">
         <v>571</v>
       </c>
-      <c r="B193" s="112"/>
+      <c r="B193" s="111"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12973,10 +13048,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="111" t="s">
+      <c r="A196" s="110" t="s">
         <v>575</v>
       </c>
-      <c r="B196" s="112"/>
+      <c r="B196" s="111"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -13011,17 +13086,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="110" t="s">
+      <c r="A201" s="112" t="s">
         <v>596</v>
       </c>
-      <c r="B201" s="110"/>
+      <c r="B201" s="112"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="111" t="s">
+      <c r="A202" s="110" t="s">
         <v>598</v>
       </c>
-      <c r="B202" s="112"/>
+      <c r="B202" s="111"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -13068,10 +13143,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="111" t="s">
+      <c r="A209" s="110" t="s">
         <v>609</v>
       </c>
-      <c r="B209" s="112"/>
+      <c r="B209" s="111"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -13086,10 +13161,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="111" t="s">
+      <c r="A212" s="110" t="s">
         <v>611</v>
       </c>
-      <c r="B212" s="112"/>
+      <c r="B212" s="111"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -13100,10 +13175,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="111" t="s">
+      <c r="A214" s="110" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="112"/>
+      <c r="B214" s="111"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -13122,10 +13197,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="111" t="s">
+      <c r="A217" s="110" t="s">
         <v>614</v>
       </c>
-      <c r="B217" s="112"/>
+      <c r="B217" s="111"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -13160,22 +13235,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="110" t="s">
+      <c r="A222" s="112" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="110"/>
+      <c r="B222" s="112"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="111" t="s">
+      <c r="A223" s="110" t="s">
         <v>632</v>
       </c>
-      <c r="B223" s="112"/>
+      <c r="B223" s="111"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="111" t="s">
+      <c r="A224" s="110" t="s">
         <v>631</v>
       </c>
-      <c r="B224" s="112"/>
+      <c r="B224" s="111"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -13186,10 +13261,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="111" t="s">
+      <c r="A226" s="110" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="112"/>
+      <c r="B226" s="111"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -13232,10 +13307,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="111" t="s">
+      <c r="A232" s="110" t="s">
         <v>645</v>
       </c>
-      <c r="B232" s="112"/>
+      <c r="B232" s="111"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -13246,10 +13321,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="111" t="s">
+      <c r="A234" s="110" t="s">
         <v>648</v>
       </c>
-      <c r="B234" s="112"/>
+      <c r="B234" s="111"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -13266,10 +13341,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="111" t="s">
+      <c r="A237" s="110" t="s">
         <v>652</v>
       </c>
-      <c r="B237" s="112"/>
+      <c r="B237" s="111"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -13416,10 +13491,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="111" t="s">
+      <c r="A256" s="110" t="s">
         <v>689</v>
       </c>
-      <c r="B256" s="112"/>
+      <c r="B256" s="111"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -13446,10 +13521,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="111" t="s">
+      <c r="A260" s="110" t="s">
         <v>697</v>
       </c>
-      <c r="B260" s="112"/>
+      <c r="B260" s="111"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -13460,16 +13535,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="110" t="s">
+      <c r="A262" s="112" t="s">
         <v>700</v>
       </c>
-      <c r="B262" s="110"/>
+      <c r="B262" s="112"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="111" t="s">
+      <c r="A263" s="110" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="112"/>
+      <c r="B263" s="111"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -13504,10 +13579,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="111" t="s">
+      <c r="A268" s="110" t="s">
         <v>710</v>
       </c>
-      <c r="B268" s="112"/>
+      <c r="B268" s="111"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -13542,10 +13617,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="111" t="s">
+      <c r="A273" s="110" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="112"/>
+      <c r="B273" s="111"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -13602,10 +13677,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="111" t="s">
+      <c r="A280" s="110" t="s">
         <v>731</v>
       </c>
-      <c r="B280" s="112"/>
+      <c r="B280" s="111"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -13661,39 +13736,18 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -13710,18 +13764,39 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework -03.Introduction-to-EntityFramework-Exercise-Complete
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -7408,12 +7408,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="55" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8205,42 +8213,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8255,91 +8263,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8354,73 +8362,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8429,49 +8437,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8483,104 +8491,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11468,31 +11476,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="129" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.28515625" style="129" customWidth="1"/>
+    <col min="1" max="1" width="23" style="110" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.28515625" style="110" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="111" t="s">
         <v>753</v>
       </c>
-      <c r="B1" s="129" t="s">
+      <c r="B1" s="110" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="111" t="s">
         <v>756</v>
       </c>
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="110" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="111" t="s">
         <v>757</v>
       </c>
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="112" t="s">
         <v>758</v>
       </c>
     </row>
@@ -11526,16 +11534,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="113" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="122"/>
+      <c r="B2" s="118"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="120" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="123"/>
+      <c r="B3" s="119"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11562,10 +11570,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="119" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="121"/>
+      <c r="B7" s="117"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11592,10 +11600,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="119" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="121"/>
+      <c r="B11" s="117"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11606,10 +11614,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="119" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="119"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11668,10 +11676,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="123" t="s">
+      <c r="A21" s="119" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="123"/>
+      <c r="B21" s="119"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11682,10 +11690,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="119" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="123"/>
+      <c r="B23" s="119"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11706,10 +11714,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="123" t="s">
+      <c r="A26" s="119" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="123"/>
+      <c r="B26" s="119"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -11736,10 +11744,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="119" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="123"/>
+      <c r="B30" s="119"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -11766,10 +11774,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="121" t="s">
+      <c r="A34" s="117" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="121"/>
+      <c r="B34" s="117"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -11796,10 +11804,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="123" t="s">
+      <c r="A38" s="119" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="123"/>
+      <c r="B38" s="119"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -11826,10 +11834,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="121" t="s">
+      <c r="A42" s="117" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="121"/>
+      <c r="B42" s="117"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -11848,10 +11856,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="123" t="s">
+      <c r="A45" s="119" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="121"/>
+      <c r="B45" s="117"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -11878,19 +11886,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="112" t="s">
+      <c r="A49" s="113" t="s">
         <v>369</v>
       </c>
-      <c r="B49" s="112"/>
+      <c r="B49" s="113"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="113" t="s">
+      <c r="A50" s="116" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="111"/>
+      <c r="B50" s="115"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="118" t="s">
+      <c r="A51" s="124" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -11898,7 +11906,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="119"/>
+      <c r="A52" s="125"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -11907,13 +11915,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="120"/>
+      <c r="A53" s="126"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="118" t="s">
+      <c r="A54" s="124" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -11921,25 +11929,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="119"/>
+      <c r="A55" s="125"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="119"/>
+      <c r="A56" s="125"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="120"/>
+      <c r="A57" s="126"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="118" t="s">
+      <c r="A58" s="124" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -11947,13 +11955,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="120"/>
+      <c r="A59" s="126"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="118" t="s">
+      <c r="A60" s="124" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -11964,7 +11972,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="119"/>
+      <c r="A61" s="125"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -11973,14 +11981,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="119"/>
+      <c r="A62" s="125"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="120"/>
+      <c r="A63" s="126"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -12034,7 +12042,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="115" t="s">
+      <c r="A70" s="121" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -12042,43 +12050,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="116"/>
+      <c r="A71" s="122"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="116"/>
+      <c r="A72" s="122"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="116"/>
+      <c r="A73" s="122"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="116"/>
+      <c r="A74" s="122"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="116"/>
+      <c r="A75" s="122"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="117"/>
+      <c r="A76" s="123"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="115" t="s">
+      <c r="A77" s="121" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -12086,74 +12094,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="116"/>
+      <c r="A78" s="122"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="116"/>
+      <c r="A79" s="122"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="116"/>
+      <c r="A80" s="122"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="116"/>
+      <c r="A81" s="122"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="116"/>
+      <c r="A82" s="122"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
+      <c r="A83" s="122"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="116"/>
+      <c r="A84" s="122"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="116"/>
+      <c r="A85" s="122"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="116"/>
+      <c r="A86" s="122"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="116"/>
+      <c r="A87" s="122"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="117"/>
+      <c r="A88" s="123"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="115" t="s">
+      <c r="A89" s="121" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -12161,28 +12169,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="116"/>
+      <c r="A90" s="122"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="116"/>
+      <c r="A91" s="122"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="117"/>
+      <c r="A92" s="123"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="115" t="s">
+      <c r="A93" s="121" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -12191,7 +12199,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="117"/>
+      <c r="A94" s="123"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -12261,17 +12269,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="112" t="s">
+      <c r="A102" s="113" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="112"/>
+      <c r="B102" s="113"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="113" t="s">
+      <c r="A103" s="116" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="111"/>
+      <c r="B103" s="115"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -12302,10 +12310,10 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="113" t="s">
+      <c r="A107" s="116" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="111"/>
+      <c r="B107" s="115"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12462,10 +12470,10 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="113" t="s">
+      <c r="A125" s="116" t="s">
         <v>424</v>
       </c>
-      <c r="B125" s="111"/>
+      <c r="B125" s="115"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12550,10 +12558,10 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="113" t="s">
+      <c r="A135" s="116" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="111"/>
+      <c r="B135" s="115"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12647,10 +12655,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="110" t="s">
+      <c r="A146" s="114" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="111"/>
+      <c r="B146" s="115"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12681,10 +12689,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="110" t="s">
+      <c r="A150" s="114" t="s">
         <v>467</v>
       </c>
-      <c r="B150" s="111"/>
+      <c r="B150" s="115"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12706,10 +12714,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="110" t="s">
+      <c r="A153" s="114" t="s">
         <v>537</v>
       </c>
-      <c r="B153" s="111"/>
+      <c r="B153" s="115"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12751,17 +12759,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="112" t="s">
+      <c r="A158" s="113" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="112"/>
+      <c r="B158" s="113"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="113" t="s">
+      <c r="A159" s="116" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="111"/>
+      <c r="B159" s="115"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12797,10 +12805,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="110" t="s">
+      <c r="A165" s="114" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="114"/>
+      <c r="B165" s="127"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12867,10 +12875,10 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="113" t="s">
+      <c r="A173" s="116" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="111"/>
+      <c r="B173" s="115"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12892,10 +12900,10 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="113" t="s">
+      <c r="A176" s="116" t="s">
         <v>471</v>
       </c>
-      <c r="B176" s="111"/>
+      <c r="B176" s="115"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12917,17 +12925,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="112" t="s">
+      <c r="A179" s="113" t="s">
         <v>548</v>
       </c>
-      <c r="B179" s="112"/>
+      <c r="B179" s="113"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="113" t="s">
+      <c r="A180" s="116" t="s">
         <v>549</v>
       </c>
-      <c r="B180" s="111"/>
+      <c r="B180" s="115"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12943,10 +12951,10 @@
       <c r="B182" s="76"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="113" t="s">
+      <c r="A183" s="116" t="s">
         <v>548</v>
       </c>
-      <c r="B183" s="111"/>
+      <c r="B183" s="115"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -13027,10 +13035,10 @@
       <c r="B192" s="76"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="113" t="s">
+      <c r="A193" s="116" t="s">
         <v>571</v>
       </c>
-      <c r="B193" s="111"/>
+      <c r="B193" s="115"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -13048,10 +13056,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="110" t="s">
+      <c r="A196" s="114" t="s">
         <v>575</v>
       </c>
-      <c r="B196" s="111"/>
+      <c r="B196" s="115"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -13086,17 +13094,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="112" t="s">
+      <c r="A201" s="113" t="s">
         <v>596</v>
       </c>
-      <c r="B201" s="112"/>
+      <c r="B201" s="113"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="110" t="s">
+      <c r="A202" s="114" t="s">
         <v>598</v>
       </c>
-      <c r="B202" s="111"/>
+      <c r="B202" s="115"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -13143,10 +13151,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="110" t="s">
+      <c r="A209" s="114" t="s">
         <v>609</v>
       </c>
-      <c r="B209" s="111"/>
+      <c r="B209" s="115"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -13161,10 +13169,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="110" t="s">
+      <c r="A212" s="114" t="s">
         <v>611</v>
       </c>
-      <c r="B212" s="111"/>
+      <c r="B212" s="115"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -13175,10 +13183,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="110" t="s">
+      <c r="A214" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="111"/>
+      <c r="B214" s="115"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -13197,10 +13205,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="110" t="s">
+      <c r="A217" s="114" t="s">
         <v>614</v>
       </c>
-      <c r="B217" s="111"/>
+      <c r="B217" s="115"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -13235,22 +13243,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="112" t="s">
+      <c r="A222" s="113" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="112"/>
+      <c r="B222" s="113"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="110" t="s">
+      <c r="A223" s="114" t="s">
         <v>632</v>
       </c>
-      <c r="B223" s="111"/>
+      <c r="B223" s="115"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="110" t="s">
+      <c r="A224" s="114" t="s">
         <v>631</v>
       </c>
-      <c r="B224" s="111"/>
+      <c r="B224" s="115"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -13261,10 +13269,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="110" t="s">
+      <c r="A226" s="114" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="111"/>
+      <c r="B226" s="115"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -13307,10 +13315,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="110" t="s">
+      <c r="A232" s="114" t="s">
         <v>645</v>
       </c>
-      <c r="B232" s="111"/>
+      <c r="B232" s="115"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -13321,10 +13329,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="110" t="s">
+      <c r="A234" s="114" t="s">
         <v>648</v>
       </c>
-      <c r="B234" s="111"/>
+      <c r="B234" s="115"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -13341,10 +13349,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="110" t="s">
+      <c r="A237" s="114" t="s">
         <v>652</v>
       </c>
-      <c r="B237" s="111"/>
+      <c r="B237" s="115"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -13491,10 +13499,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="110" t="s">
+      <c r="A256" s="114" t="s">
         <v>689</v>
       </c>
-      <c r="B256" s="111"/>
+      <c r="B256" s="115"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -13521,10 +13529,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="110" t="s">
+      <c r="A260" s="114" t="s">
         <v>697</v>
       </c>
-      <c r="B260" s="111"/>
+      <c r="B260" s="115"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -13535,16 +13543,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="112" t="s">
+      <c r="A262" s="113" t="s">
         <v>700</v>
       </c>
-      <c r="B262" s="112"/>
+      <c r="B262" s="113"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="110" t="s">
+      <c r="A263" s="114" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="111"/>
+      <c r="B263" s="115"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -13579,10 +13587,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="110" t="s">
+      <c r="A268" s="114" t="s">
         <v>710</v>
       </c>
-      <c r="B268" s="111"/>
+      <c r="B268" s="115"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -13617,10 +13625,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="110" t="s">
+      <c r="A273" s="114" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="111"/>
+      <c r="B273" s="115"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -13677,10 +13685,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="110" t="s">
+      <c r="A280" s="114" t="s">
         <v>731</v>
       </c>
-      <c r="B280" s="111"/>
+      <c r="B280" s="115"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -13736,18 +13744,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -13764,39 +13793,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14218,7 +14226,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="128" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -14238,7 +14246,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="126"/>
+      <c r="A2" s="129"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -14306,10 +14314,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="130" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="128"/>
+      <c r="C6" s="131"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
DB EF - Database First
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="631" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
-    <sheet name="DB-EF-Databas First" sheetId="13" r:id="rId2"/>
-    <sheet name="DB-SQL" sheetId="11" r:id="rId3"/>
-    <sheet name="DB" sheetId="4" r:id="rId4"/>
-    <sheet name="Regex" sheetId="2" r:id="rId5"/>
-    <sheet name="Solidity" sheetId="5" r:id="rId6"/>
-    <sheet name="Git" sheetId="6" r:id="rId7"/>
-    <sheet name="Comparators" sheetId="7" r:id="rId8"/>
-    <sheet name="ShortCuts" sheetId="3" r:id="rId9"/>
-    <sheet name="OOP" sheetId="8" r:id="rId10"/>
-    <sheet name="SOLID" sheetId="12" r:id="rId11"/>
-    <sheet name="Reflection" sheetId="9" r:id="rId12"/>
-    <sheet name="UnitTesting" sheetId="10" r:id="rId13"/>
+    <sheet name="EF-ORM" sheetId="14" r:id="rId2"/>
+    <sheet name="ADO. NET" sheetId="13" r:id="rId3"/>
+    <sheet name="DB-SQL" sheetId="11" r:id="rId4"/>
+    <sheet name="DB" sheetId="4" r:id="rId5"/>
+    <sheet name="Regex" sheetId="2" r:id="rId6"/>
+    <sheet name="Solidity" sheetId="5" r:id="rId7"/>
+    <sheet name="Git" sheetId="6" r:id="rId8"/>
+    <sheet name="Comparators" sheetId="7" r:id="rId9"/>
+    <sheet name="ShortCuts" sheetId="3" r:id="rId10"/>
+    <sheet name="OOP" sheetId="8" r:id="rId11"/>
+    <sheet name="SOLID" sheetId="12" r:id="rId12"/>
+    <sheet name="Reflection" sheetId="9" r:id="rId13"/>
+    <sheet name="UnitTesting" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -31,7 +32,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="855">
   <si>
     <t>Операция</t>
   </si>
@@ -7399,15 +7400,796 @@
     <t>CleanUp packages</t>
   </si>
   <si>
-    <t xml:space="preserve">Uninstall-Package Microsoft.EntityFrameworkCore.Tools -r
-Uninstall-Package Microsoft.EntityFrameworkCore.SqlServer.Design -RemoveDependencies
+    <t>Data Access Models
+Connecting to a DB through C#</t>
+  </si>
+  <si>
+    <t>Connected data access model</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Applicable to an environment where the database is constantly available:
+- Connected data access model (SqlClient)
 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Benefits:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Concurrency control is easier to maintain
+     - Better chance to work with the most recent version of the data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Drawbacks:
+     - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Needs a constant reliable network
+     - Problems when scalability is an issue</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ADO.NET </t>
+  </si>
+  <si>
+    <t>What Is ADO.NET?</t>
+  </si>
+  <si>
+    <t>ADO.NET is a standard .NET class library for accessing  databases, processing data and XML
+Supports connected, disconnected and ORM data access  models
+     - Excellent integration with LINQ
+     - Allows executing SQL in RDBMS systems
+     - Allows accessing data in the ORM approach</t>
+  </si>
+  <si>
+    <t>Data Providers in ADO.NET</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Providers are collections of classes that provide access to various databases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - For different RDBMS systems different Data Providers are  available
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Several common objects are defined</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Connection – to connect to the database
+     - Command – to run an SQL command
+     - DataReader – to retrieve data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Several standard ADO.NET Data Providers come as part of  .NET Framework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - SqlClient – accessing SQL Server
+     - OleDB – accessing standard OLE DB data sources
+     - Odbc – accessing standard ODBC data sources
+     - Oracle – accessing Oracle databases</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Third party Data Providers are available for:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - MySQL, PostgreSQL, Interbase, DB2, SQLite
+     - Other RDBMS systems and data sources (SQL Azure, Salesforce CRM, Amazon SimpleDB, …)</t>
+    </r>
+  </si>
+  <si>
+    <t>SqlClient and ADO.NET Connected Model</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Retrieving data in connected model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Open a connection (SqlConnection)
+     - Execute command (SqlCommand)
+     - Process the result set of the query by using a reader (SqlDataReader)
+     - Close the reader
+     - Close the connection</t>
+    </r>
+  </si>
+  <si>
+    <t>ORM Model</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ORM data access model (Entity Framework Core)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Maps database tables to classes and objects
+     - Objects can be automatically persisted in the database
+     - Can operate in both connected and disconnected modes</t>
+    </r>
+  </si>
+  <si>
+    <t>ORM Model – Benefits and Problems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ORM model benefits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Less code
+     - Use objects with associations instead of tables and SQL
+     - Integrated object query mechanism
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ORM model drawbacks:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Less flexibility
+     - SQL is automatically generated
+     - Performance issues (sometimes)</t>
+    </r>
+  </si>
+  <si>
+    <t>ADO.NET: Entity Framework Core</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entity Framework Core is a generic ORM framework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     - Create entity data model mapping the database
+     - Open an object context
+     - Retrieve data with LINQ / modify the tables in the object  context
+     - Persist the object context changes into the DB
+     - Connection is automatically managed</t>
+    </r>
+  </si>
+  <si>
+    <t>SQL Client Data Provider</t>
+  </si>
+  <si>
+    <t>SqlConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Establish database connection to SQL Server </t>
+  </si>
+  <si>
+    <t>SqlCommand</t>
+  </si>
+  <si>
+    <t>SqlDataReader</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Executes SQL commands on the SQL Server through an established  connection
+ - Could accept parameters (SQLParameter)</t>
+  </si>
+  <si>
+    <t>Retrieves data (record set) from SQL Server as a result of SQL query execution</t>
+  </si>
+  <si>
+    <t>The SqlConnection Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SqlConnection establishes a connection to SQL Server database
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Requires a valid connection string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Connection string example:</t>
+  </si>
+  <si>
+    <t>Connecting to SQL Server:</t>
+  </si>
+  <si>
+    <t>Data Source=(local)\SQLEXPRESS;Initial Catalog=SoftUni;Integrated Security=true;</t>
+  </si>
+  <si>
+    <t>SqlConnection con = new SqlConnection(
+ @"Server=.;
+   Database=SoftUni;
+   Integrated Security=true");
+con.Open();</t>
+  </si>
+  <si>
+    <t>Creating and opening connection to SQL Server  (database SoftUni)</t>
+  </si>
+  <si>
+    <t>SqlConnection dbCon = new SqlConnection(
+    "Server=.\\SQLEXPRESS; " +
+    "Database=SoftUni; " +
+    "Integrated Security=true");
+dbCon.Open();
+using (dbCon)
+{
+ //TODO: Use the connection to execute SQL commands here …
+}</t>
+  </si>
+  <si>
+    <t>DB Connection String</t>
+  </si>
+  <si>
+    <t>Database connection string</t>
+  </si>
+  <si>
+    <t>Defines the parameters needed to establish the connection to the database</t>
+  </si>
+  <si>
+    <t>Settings for SQL Server connections:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Data Source / Server – server name / IP address + database  instance name
+     - Database / Initial Catalog – database name
+     - User ID / Password – credentials
+     - Integrated Security – false if credentials are provided</t>
+  </si>
+  <si>
+    <t>Working with SqlConnection</t>
+  </si>
+  <si>
+    <t>Explicitly opening and closing a connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Open() and Close() methods
+     - Works through the connection pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB connections are IDisposable objects
+</t>
+  </si>
+  <si>
+    <t>Always use the using construct in C#!</t>
+  </si>
+  <si>
+    <t>The SqlCommand Class
+(More important methods)</t>
+  </si>
+  <si>
+    <t>ExecuteScalar()</t>
+  </si>
+  <si>
+    <t>ExecuteReader()</t>
+  </si>
+  <si>
+    <t>ExecuteNonQuery()</t>
+  </si>
+  <si>
+    <t>Returns a single value - the value in the first column of the first row of the result set (as System.Object)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Returns a SqlDataReader - It is a cursor over the returned records (result set)
+     - CommandBehavior – assigns some options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Used for non-query SQL commands, e.g. INSERT
+     - Returns the number of affected rows (int)</t>
+  </si>
+  <si>
+    <t>SqlCommand – Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SqlConnection dbCon = new SqlConnection(
+  "Server=.; " +
+  "Database=SoftUni; " +
+  "Integrated Security=true");
+dbCon.Open();
+using(dbCon)
+{
+  SqlCommand command = new SqlCommand(
+    "SELECT COUNT(*) FROM Employees", dbCon);
+  int employeesCount = (int) command.ExecuteScalar();
+  Console.WriteLine("Employees count: {0} ", employeesCount);
+}
+</t>
+  </si>
+  <si>
+    <t>The SqlDataReader Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SqlDataReader </t>
+  </si>
+  <si>
+    <t>SqlDataReader retrieves a sequence of records (cursor) returned  as result of an SQL command
+     - Data is available for reading only (can't be changed)
+     - Forward-only row processing (no move back)</t>
+  </si>
+  <si>
+    <t>Important properties and methods:</t>
+  </si>
+  <si>
+    <t>Close() – closes the cursor and releases resources</t>
+  </si>
+  <si>
+    <t>Read() – moves the cursor forward and returns false if there is no next record</t>
+  </si>
+  <si>
+    <t>Indexer[] – retrieves the value in the current record by given column name or index</t>
+  </si>
+  <si>
+    <t>Uninstall-Package Microsoft.EntityFrameworkCore.Tools -r
+Uninstall-Package Microsoft.EntityFrameworkCore.SqlServer.Design -RemoveDependencies</t>
+  </si>
+  <si>
+    <t>SqlDataReader – Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SqlConnection dbCon = new SqlConnection(…);
+dbCon.Open();
+using(dbCon)
+{
+  SqlCommand command = new SqlCommand("SELECT * FROM Employees", dbCon);
+  SqlDataReader reader = command.ExecuteReader();
+  using (reader)
+  {
+    while (reader.Read())
+    {
+      string firstName = (string)reader["FirstName"];
+      string lastName = (string)reader["LastName"];
+      decimal salary = (decimal)reader["Salary"];
+      Console.WriteLine("{0} {1} - {2}", firstName, lastName, salary);
+    }
+  }
+}
+</t>
+  </si>
+  <si>
+    <t>SQL Injection - What is SQL Injection? How to Prevent It?</t>
+  </si>
+  <si>
+    <t>What is SQL Injection?</t>
+  </si>
+  <si>
+    <t>How Does SQL Injection Work?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bool IsPasswordValid(string username, string password)
+{
+  string sql = 
+    $"SELECT COUNT(*) FROM Users " +
+    $"WHERE UserName = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">'{username}' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">AND" +
+    $"PasswordHash = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'{CalcSHA1(password)}'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>";
+  SqlCommand cmd = new SqlCommand(sql, dbConnection);
+  int matchedUsersCount = (int)cmd.ExecuteScalar();
+  return matchedUsersCount &gt; 0;
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bool normalLogin =
+  IsPasswordValid("peter", "qwerty123"); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>// true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+bool sqlInjectedLogin = 
+  IsPasswordValid(" ' or 1=1 --", "qwerty123"); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>// true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+bool evilHackerCreatesNewUser = 
+  IsPasswordValid("' INSERT INTO Users VALUES('hacker','') --",
+  "qwerty123");
+</t>
+    </r>
+  </si>
+  <si>
+    <t>The following SQL commands are executed:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usual password check (no SQL injection):
+</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM Users WHERE UserName = 'peter’ AND PasswordHash = 'XOwXWxZePV5iyeE86Ejvb+rIG/8='</t>
+  </si>
+  <si>
+    <t>SQL-injected password check:</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM Users WHERE UserName = ' ' or 1=1 -- ‘ AND PasswordHash = 'XOwXWxZePV5iyeE86Ejvb+rIG/8='</t>
+  </si>
+  <si>
+    <t>SQL-injected INSERT command:</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) FROM Users WHERE UserName = '' INSERT INTO Users VALUES('hacker','') --’ AND PasswordHash = 'XOwXWxZePV5iyeE86Ejvb+rIG/8='</t>
+  </si>
+  <si>
+    <t>SQL Injection - What is SQL Injection? How to Prevent It?
+Ways to prevent the SQL injection:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL-escape all data coming from the user:
+</t>
+  </si>
+  <si>
+    <t>string escapedUsername = username.Replace("'", "''");
+string sql = 
+    "SELECT COUNT(*) FROM Users " +
+    "WHERE UserName = '" + escapedUsername + "' and " +
+    "PasswordHash = '" + CalcSHA1(password) + "'";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not recommended: use as last resort only!
+</t>
+  </si>
+  <si>
+    <t>Preferred approach:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Use parameterized queries
+     - Separate the SQL command from its arguments</t>
+  </si>
+  <si>
+    <t>The SqlParameter Class</t>
+  </si>
+  <si>
+    <t>What are SqlParameters?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - SQL queries and stored procedures can have input and output  parameters
+     - Accessed through the Parameters property of the SqlCommand  class</t>
+  </si>
+  <si>
+    <t>Properties of SqlParameter:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - ParameterName – name of the parameter
+     - DbType – SQL type (NVarChar, Timestamp, …)
+     - Size – size of the type (if applicable)
+     - Direction – input / output</t>
+  </si>
+  <si>
+    <t>Parameterized Commands – Example</t>
+  </si>
+  <si>
+    <t>void InsertProject(string name, string description, DateTime startDate)
+{
+  SqlCommand cmd = new SqlCommand(
+    "INSERT INTO Projects " + 
+    "(Name, Description, StartDate, EndDate) VALUES " +
+    "(@name, @desc, @start, @end)", dbCon);
+  cmd.Parameters.AddWithValue("@name", name);
+  cmd.Parameters.AddWithValue("@desc", description);
+  cmd.Parameters.AddWithValue("@start", startDate);
+  cmd.ExecuteNonQuery();
+}</t>
+  </si>
+  <si>
+    <t>Connecting to Non-Microsoft Databases
+ADO.NET supports accessing various databases via their  Data Providers:</t>
+  </si>
+  <si>
+    <t>OLE DB – supported internally in ADO.NET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Access any OLE DB-compliant data source
+     - E.g. MS Access, MS Excel, MS Project, MS Exchange,  Windows Active Directory, text files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Supported internally in ADO.NET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Third party extension</t>
+  </si>
+  <si>
+    <t>Entity Framework - Database First</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7866,7 +8648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7896,6 +8678,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8219,7 +9007,7 @@
     <xf numFmtId="0" fontId="40" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8527,11 +9315,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -8539,14 +9324,20 @@
     <xf numFmtId="0" fontId="42" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="42" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8566,17 +9357,8 @@
     <xf numFmtId="0" fontId="41" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8588,6 +9370,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8683,7 +9504,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -8691,17 +9512,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -8755,7 +9565,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8790,7 +9600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11130,6 +11940,56 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11276,7 +12136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -11335,7 +12195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -11410,7 +12270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11468,49 +12328,554 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="110" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.28515625" style="110" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="87.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="130" t="s">
+        <v>854</v>
+      </c>
+      <c r="B1" s="130"/>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="131" t="s">
         <v>753</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B2" s="132" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="111" t="s">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="131" t="s">
         <v>756</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B3" s="132" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="111" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="131" t="s">
         <v>757</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B4" s="134" t="s">
+        <v>819</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" style="110" customWidth="1"/>
+    <col min="2" max="2" width="85.28515625" style="110" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="130" t="s">
+        <v>761</v>
+      </c>
+      <c r="B1" s="130"/>
+    </row>
+    <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="141" t="s">
         <v>758</v>
       </c>
+      <c r="B2" s="142"/>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="131" t="s">
+        <v>762</v>
+      </c>
+      <c r="B3" s="132" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="131" t="s">
+        <v>759</v>
+      </c>
+      <c r="B4" s="132" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="136" t="s">
+        <v>764</v>
+      </c>
+      <c r="B5" s="134" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="139"/>
+      <c r="B6" s="134" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="139"/>
+      <c r="B7" s="134" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="137"/>
+      <c r="B8" s="134" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="135" t="s">
+        <v>769</v>
+      </c>
+      <c r="B9" s="134" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="135" t="s">
+        <v>771</v>
+      </c>
+      <c r="B10" s="134" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="135" t="s">
+        <v>773</v>
+      </c>
+      <c r="B11" s="134" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="135" t="s">
+        <v>775</v>
+      </c>
+      <c r="B12" s="134" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="140" t="s">
+        <v>777</v>
+      </c>
+      <c r="B13" s="140"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="135" t="s">
+        <v>778</v>
+      </c>
+      <c r="B14" s="134" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="135" t="s">
+        <v>780</v>
+      </c>
+      <c r="B15" s="134" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="135" t="s">
+        <v>781</v>
+      </c>
+      <c r="B16" s="134" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="140" t="s">
+        <v>784</v>
+      </c>
+      <c r="B17" s="140"/>
+    </row>
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="135" t="s">
+        <v>785</v>
+      </c>
+      <c r="B18" s="134" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="135" t="s">
+        <v>787</v>
+      </c>
+      <c r="B19" s="134" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="135" t="s">
+        <v>788</v>
+      </c>
+      <c r="B20" s="134" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="135" t="s">
+        <v>791</v>
+      </c>
+      <c r="B21" s="134" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="140" t="s">
+        <v>793</v>
+      </c>
+      <c r="B22" s="140"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="135" t="s">
+        <v>794</v>
+      </c>
+      <c r="B23" s="134" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="135" t="s">
+        <v>796</v>
+      </c>
+      <c r="B24" s="134" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="140" t="s">
+        <v>798</v>
+      </c>
+      <c r="B25" s="140"/>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="135" t="s">
+        <v>799</v>
+      </c>
+      <c r="B26" s="134" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="135" t="s">
+        <v>801</v>
+      </c>
+      <c r="B27" s="134" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="140" t="s">
+        <v>803</v>
+      </c>
+      <c r="B28" s="140"/>
+    </row>
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="135" t="s">
+        <v>804</v>
+      </c>
+      <c r="B29" s="132" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="135" t="s">
+        <v>805</v>
+      </c>
+      <c r="B30" s="132" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="135" t="s">
+        <v>806</v>
+      </c>
+      <c r="B31" s="132" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="140" t="s">
+        <v>810</v>
+      </c>
+      <c r="B32" s="140"/>
+    </row>
+    <row r="33" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A33" s="135"/>
+      <c r="B33" s="132" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="140" t="s">
+        <v>812</v>
+      </c>
+      <c r="B34" s="140"/>
+    </row>
+    <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="135" t="s">
+        <v>813</v>
+      </c>
+      <c r="B35" s="132" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="136" t="s">
+        <v>815</v>
+      </c>
+      <c r="B36" s="132" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="139"/>
+      <c r="B37" s="132" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="137"/>
+      <c r="B38" s="132" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="140" t="s">
+        <v>820</v>
+      </c>
+      <c r="B39" s="140"/>
+    </row>
+    <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A40" s="138"/>
+      <c r="B40" s="132" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="140" t="s">
+        <v>822</v>
+      </c>
+      <c r="B41" s="140"/>
+    </row>
+    <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A42" s="136" t="s">
+        <v>823</v>
+      </c>
+      <c r="B42" s="132" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A43" s="137"/>
+      <c r="B43" s="132" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="138" t="s">
+        <v>824</v>
+      </c>
+      <c r="B44" s="132" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="138" t="s">
+        <v>828</v>
+      </c>
+      <c r="B45" s="132" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="138" t="s">
+        <v>830</v>
+      </c>
+      <c r="B46" s="132" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="135" t="s">
+        <v>832</v>
+      </c>
+      <c r="B47" s="132" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="140" t="s">
+        <v>834</v>
+      </c>
+      <c r="B48" s="140"/>
+    </row>
+    <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="131" t="s">
+        <v>835</v>
+      </c>
+      <c r="B49" s="132" t="s">
+        <v>836</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="131" t="s">
+        <v>838</v>
+      </c>
+      <c r="B50" s="132" t="s">
+        <v>839</v>
+      </c>
+      <c r="C50" s="35"/>
+    </row>
+    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="140" t="s">
+        <v>840</v>
+      </c>
+      <c r="B51" s="140"/>
+      <c r="C51" s="35"/>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="131" t="s">
+        <v>841</v>
+      </c>
+      <c r="B52" s="132" t="s">
+        <v>842</v>
+      </c>
+      <c r="C52" s="35"/>
+    </row>
+    <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="131" t="s">
+        <v>843</v>
+      </c>
+      <c r="B53" s="132" t="s">
+        <v>844</v>
+      </c>
+      <c r="C53" s="35"/>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="140" t="s">
+        <v>845</v>
+      </c>
+      <c r="B54" s="140"/>
+      <c r="C54" s="35"/>
+    </row>
+    <row r="55" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A55" s="131"/>
+      <c r="B55" s="132" t="s">
+        <v>846</v>
+      </c>
+      <c r="C55" s="35"/>
+    </row>
+    <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="140" t="s">
+        <v>847</v>
+      </c>
+      <c r="B56" s="140"/>
+      <c r="C56" s="35"/>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="131" t="s">
+        <v>848</v>
+      </c>
+      <c r="B57" s="132" t="s">
+        <v>849</v>
+      </c>
+      <c r="C57" s="35"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="131" t="s">
+        <v>850</v>
+      </c>
+      <c r="B58" s="132" t="s">
+        <v>851</v>
+      </c>
+      <c r="C58" s="35"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="131" t="s">
+        <v>852</v>
+      </c>
+      <c r="B59" s="132" t="s">
+        <v>853</v>
+      </c>
+      <c r="C59" s="35"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="131"/>
+      <c r="B60" s="132"/>
+      <c r="C60" s="35"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="131"/>
+      <c r="B61" s="132"/>
+      <c r="C61" s="35"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="131"/>
+      <c r="B62" s="132"/>
+      <c r="C62" s="35"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="131"/>
+      <c r="B63" s="133"/>
     </row>
   </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
@@ -11534,16 +12899,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="125"/>
+      <c r="B2" s="116"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="118" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="126"/>
+      <c r="B3" s="117"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -11570,10 +12935,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="117" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="124"/>
+      <c r="B7" s="115"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -11600,10 +12965,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="126" t="s">
+      <c r="A11" s="117" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="124"/>
+      <c r="B11" s="115"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -11614,10 +12979,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="117" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="126"/>
+      <c r="B13" s="117"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -11676,10 +13041,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="126" t="s">
+      <c r="A21" s="117" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="126"/>
+      <c r="B21" s="117"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -11690,10 +13055,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="126" t="s">
+      <c r="A23" s="117" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="126"/>
+      <c r="B23" s="117"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -11714,10 +13079,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="126" t="s">
+      <c r="A26" s="117" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="126"/>
+      <c r="B26" s="117"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -11744,10 +13109,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="126" t="s">
+      <c r="A30" s="117" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="126"/>
+      <c r="B30" s="117"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -11774,10 +13139,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="124" t="s">
+      <c r="A34" s="115" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="124"/>
+      <c r="B34" s="115"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -11804,10 +13169,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="126" t="s">
+      <c r="A38" s="117" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="126"/>
+      <c r="B38" s="117"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -11834,10 +13199,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="124" t="s">
+      <c r="A42" s="115" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="124"/>
+      <c r="B42" s="115"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -11856,10 +13221,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="126" t="s">
+      <c r="A45" s="117" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="124"/>
+      <c r="B45" s="115"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -11886,19 +13251,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="115" t="s">
+      <c r="A49" s="111" t="s">
         <v>369</v>
       </c>
-      <c r="B49" s="115"/>
+      <c r="B49" s="111"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="116" t="s">
+      <c r="A50" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="114"/>
+      <c r="B50" s="113"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="121" t="s">
+      <c r="A51" s="122" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -11906,7 +13271,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="122"/>
+      <c r="A52" s="123"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -11915,13 +13280,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="123"/>
+      <c r="A53" s="124"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="121" t="s">
+      <c r="A54" s="122" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -11929,25 +13294,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="122"/>
+      <c r="A55" s="123"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="122"/>
+      <c r="A56" s="123"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="123"/>
+      <c r="A57" s="124"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="121" t="s">
+      <c r="A58" s="122" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -11955,13 +13320,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="123"/>
+      <c r="A59" s="124"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="121" t="s">
+      <c r="A60" s="122" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -11972,7 +13337,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="122"/>
+      <c r="A61" s="123"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -11981,14 +13346,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="122"/>
+      <c r="A62" s="123"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="123"/>
+      <c r="A63" s="124"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -12042,7 +13407,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="119" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -12050,43 +13415,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="119"/>
+      <c r="A71" s="120"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="119"/>
+      <c r="A72" s="120"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="119"/>
+      <c r="A73" s="120"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="119"/>
+      <c r="A74" s="120"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="119"/>
+      <c r="A75" s="120"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="120"/>
+      <c r="A76" s="121"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="118" t="s">
+      <c r="A77" s="119" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -12094,74 +13459,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="119"/>
+      <c r="A78" s="120"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="119"/>
+      <c r="A79" s="120"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="119"/>
+      <c r="A80" s="120"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="119"/>
+      <c r="A81" s="120"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="119"/>
+      <c r="A82" s="120"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="119"/>
+      <c r="A83" s="120"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="119"/>
+      <c r="A84" s="120"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="119"/>
+      <c r="A85" s="120"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="119"/>
+      <c r="A86" s="120"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="119"/>
+      <c r="A87" s="120"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="120"/>
+      <c r="A88" s="121"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="118" t="s">
+      <c r="A89" s="119" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -12169,28 +13534,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="119"/>
+      <c r="A90" s="120"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="119"/>
+      <c r="A91" s="120"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="120"/>
+      <c r="A92" s="121"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="118" t="s">
+      <c r="A93" s="119" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -12199,7 +13564,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="120"/>
+      <c r="A94" s="121"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -12269,17 +13634,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="115" t="s">
+      <c r="A102" s="111" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="115"/>
+      <c r="B102" s="111"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="116" t="s">
+      <c r="A103" s="114" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="114"/>
+      <c r="B103" s="113"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -12310,10 +13675,10 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="116" t="s">
+      <c r="A107" s="114" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="114"/>
+      <c r="B107" s="113"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12470,10 +13835,10 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="116" t="s">
+      <c r="A125" s="114" t="s">
         <v>424</v>
       </c>
-      <c r="B125" s="114"/>
+      <c r="B125" s="113"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -12558,10 +13923,10 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="116" t="s">
+      <c r="A135" s="114" t="s">
         <v>496</v>
       </c>
-      <c r="B135" s="114"/>
+      <c r="B135" s="113"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12655,10 +14020,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="113" t="s">
+      <c r="A146" s="112" t="s">
         <v>459</v>
       </c>
-      <c r="B146" s="114"/>
+      <c r="B146" s="113"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -12689,10 +14054,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="113" t="s">
+      <c r="A150" s="112" t="s">
         <v>467</v>
       </c>
-      <c r="B150" s="114"/>
+      <c r="B150" s="113"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -12714,10 +14079,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="113" t="s">
+      <c r="A153" s="112" t="s">
         <v>537</v>
       </c>
-      <c r="B153" s="114"/>
+      <c r="B153" s="113"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -12759,17 +14124,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="115" t="s">
+      <c r="A158" s="111" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="115"/>
+      <c r="B158" s="111"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="116" t="s">
+      <c r="A159" s="114" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="114"/>
+      <c r="B159" s="113"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -12805,10 +14170,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="113" t="s">
+      <c r="A165" s="112" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="117"/>
+      <c r="B165" s="125"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12875,10 +14240,10 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="116" t="s">
+      <c r="A173" s="114" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="114"/>
+      <c r="B173" s="113"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -12900,10 +14265,10 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="116" t="s">
+      <c r="A176" s="114" t="s">
         <v>471</v>
       </c>
-      <c r="B176" s="114"/>
+      <c r="B176" s="113"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -12925,17 +14290,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="115" t="s">
+      <c r="A179" s="111" t="s">
         <v>548</v>
       </c>
-      <c r="B179" s="115"/>
+      <c r="B179" s="111"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="116" t="s">
+      <c r="A180" s="114" t="s">
         <v>549</v>
       </c>
-      <c r="B180" s="114"/>
+      <c r="B180" s="113"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -12951,10 +14316,10 @@
       <c r="B182" s="76"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="116" t="s">
+      <c r="A183" s="114" t="s">
         <v>548</v>
       </c>
-      <c r="B183" s="114"/>
+      <c r="B183" s="113"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -13035,10 +14400,10 @@
       <c r="B192" s="76"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="116" t="s">
+      <c r="A193" s="114" t="s">
         <v>571</v>
       </c>
-      <c r="B193" s="114"/>
+      <c r="B193" s="113"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -13056,10 +14421,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="113" t="s">
+      <c r="A196" s="112" t="s">
         <v>575</v>
       </c>
-      <c r="B196" s="114"/>
+      <c r="B196" s="113"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -13094,17 +14459,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="115" t="s">
+      <c r="A201" s="111" t="s">
         <v>596</v>
       </c>
-      <c r="B201" s="115"/>
+      <c r="B201" s="111"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="113" t="s">
+      <c r="A202" s="112" t="s">
         <v>598</v>
       </c>
-      <c r="B202" s="114"/>
+      <c r="B202" s="113"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -13151,10 +14516,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="113" t="s">
+      <c r="A209" s="112" t="s">
         <v>609</v>
       </c>
-      <c r="B209" s="114"/>
+      <c r="B209" s="113"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -13169,10 +14534,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="113" t="s">
+      <c r="A212" s="112" t="s">
         <v>611</v>
       </c>
-      <c r="B212" s="114"/>
+      <c r="B212" s="113"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -13183,10 +14548,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="113" t="s">
+      <c r="A214" s="112" t="s">
         <v>615</v>
       </c>
-      <c r="B214" s="114"/>
+      <c r="B214" s="113"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -13205,10 +14570,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="113" t="s">
+      <c r="A217" s="112" t="s">
         <v>614</v>
       </c>
-      <c r="B217" s="114"/>
+      <c r="B217" s="113"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -13243,22 +14608,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="115" t="s">
+      <c r="A222" s="111" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="115"/>
+      <c r="B222" s="111"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="113" t="s">
+      <c r="A223" s="112" t="s">
         <v>632</v>
       </c>
-      <c r="B223" s="114"/>
+      <c r="B223" s="113"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="113" t="s">
+      <c r="A224" s="112" t="s">
         <v>631</v>
       </c>
-      <c r="B224" s="114"/>
+      <c r="B224" s="113"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -13269,10 +14634,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="113" t="s">
+      <c r="A226" s="112" t="s">
         <v>635</v>
       </c>
-      <c r="B226" s="114"/>
+      <c r="B226" s="113"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -13315,10 +14680,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="113" t="s">
+      <c r="A232" s="112" t="s">
         <v>645</v>
       </c>
-      <c r="B232" s="114"/>
+      <c r="B232" s="113"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -13329,10 +14694,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="113" t="s">
+      <c r="A234" s="112" t="s">
         <v>648</v>
       </c>
-      <c r="B234" s="114"/>
+      <c r="B234" s="113"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -13349,10 +14714,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="113" t="s">
+      <c r="A237" s="112" t="s">
         <v>652</v>
       </c>
-      <c r="B237" s="114"/>
+      <c r="B237" s="113"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -13499,10 +14864,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="113" t="s">
+      <c r="A256" s="112" t="s">
         <v>689</v>
       </c>
-      <c r="B256" s="114"/>
+      <c r="B256" s="113"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -13529,10 +14894,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="113" t="s">
+      <c r="A260" s="112" t="s">
         <v>697</v>
       </c>
-      <c r="B260" s="114"/>
+      <c r="B260" s="113"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -13543,16 +14908,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="115" t="s">
+      <c r="A262" s="111" t="s">
         <v>700</v>
       </c>
-      <c r="B262" s="115"/>
+      <c r="B262" s="111"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="113" t="s">
+      <c r="A263" s="112" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="114"/>
+      <c r="B263" s="113"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -13587,10 +14952,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="113" t="s">
+      <c r="A268" s="112" t="s">
         <v>710</v>
       </c>
-      <c r="B268" s="114"/>
+      <c r="B268" s="113"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -13625,10 +14990,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="113" t="s">
+      <c r="A273" s="112" t="s">
         <v>702</v>
       </c>
-      <c r="B273" s="114"/>
+      <c r="B273" s="113"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -13685,10 +15050,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="113" t="s">
+      <c r="A280" s="112" t="s">
         <v>731</v>
       </c>
-      <c r="B280" s="114"/>
+      <c r="B280" s="113"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -13744,18 +15109,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -13772,46 +15158,25 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -13905,7 +15270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -14203,7 +15568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -14226,7 +15591,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="126" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -14246,7 +15611,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="129"/>
+      <c r="A2" s="127"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -14314,10 +15679,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="128" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="131"/>
+      <c r="C6" s="129"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>
@@ -14349,7 +15714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -14468,7 +15833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -14509,54 +15874,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework -04.Code First
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686" activeTab="1"/>
@@ -23,7 +23,6 @@
     <sheet name="UnitTesting" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -33,7 +32,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="918">
   <si>
     <t>Операция</t>
   </si>
@@ -8202,9 +8201,6 @@
     <t>4. Добавяме DbContext + DbSet за всеки модел</t>
   </si>
   <si>
-    <t>5. OnConfiguring (Connection String) + OnModelCreating (Модели с релации)</t>
-  </si>
-  <si>
     <t>6.2. Many-to-Many - Две One-to-Many + .HasKey (sc =&gt; new 
 {
      sc.FirstKeyId, sc.SecondKeyId
@@ -8655,11 +8651,20 @@
     <t xml:space="preserve">Update-Database
 </t>
   </si>
+  <si>
+    <t>"Server=B5400\\SQLEXPRESS;Database=Hospital;Integrated Security=true;";</t>
+  </si>
+  <si>
+    <t>5.1. OnConfiguring (Connection String)</t>
+  </si>
+  <si>
+    <t>5.2. OnModelCreating (Модели с релации)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -9492,7 +9497,7 @@
     <xf numFmtId="0" fontId="41" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9824,13 +9829,16 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9848,29 +9856,20 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="43" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9890,8 +9889,17 @@
     <xf numFmtId="0" fontId="42" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9905,7 +9913,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10001,7 +10009,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -10009,6 +10017,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -10062,7 +10081,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10097,7 +10116,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -12825,10 +12844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12839,10 +12858,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="122" t="s">
         <v>854</v>
       </c>
-      <c r="B1" s="119"/>
+      <c r="B1" s="122"/>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
@@ -12869,10 +12888,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="122" t="s">
         <v>855</v>
       </c>
-      <c r="B8" s="119"/>
+      <c r="B8" s="122"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="110" t="s">
@@ -12889,290 +12908,299 @@
         <v>858</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="110" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="110" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+        <v>916</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
-        <v>866</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>865</v>
-      </c>
+        <v>917</v>
+      </c>
+      <c r="B14" s="35"/>
     </row>
     <row r="15" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="110" t="s">
+        <v>865</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="110" t="s">
+        <v>860</v>
+      </c>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="110" t="s">
+        <v>866</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="110" t="s">
         <v>861</v>
-      </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="110" t="s">
-        <v>867</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="110" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="110" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="110" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="120" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="110" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="120" t="s">
+        <v>868</v>
+      </c>
+      <c r="B21" s="121"/>
+    </row>
+    <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="117" t="s">
         <v>869</v>
       </c>
-      <c r="B20" s="121"/>
-    </row>
-    <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="117" t="s">
+      <c r="B22" s="35" t="s">
         <v>870</v>
       </c>
-      <c r="B21" s="35" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="123" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="122" t="s">
+      <c r="B23" t="s">
         <v>872</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="123"/>
+      <c r="B24" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="122"/>
-      <c r="B23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="123"/>
+      <c r="B25" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
-      <c r="B24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="123"/>
+      <c r="B26" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="122"/>
-      <c r="B25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="123"/>
+      <c r="B27" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="122"/>
-      <c r="B26" t="s">
+    <row r="29" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="120" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="120" t="s">
+      <c r="B29" s="121"/>
+    </row>
+    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="120" t="s">
+        <v>879</v>
+      </c>
+      <c r="B30" s="121"/>
+    </row>
+    <row r="31" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A31" s="110" t="s">
         <v>878</v>
       </c>
-      <c r="B28" s="121"/>
-    </row>
-    <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="120" t="s">
+      <c r="B31" s="11" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="110" t="s">
         <v>880</v>
       </c>
-      <c r="B29" s="121"/>
-    </row>
-    <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" s="110" t="s">
-        <v>879</v>
-      </c>
-      <c r="B30" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="110" t="s">
-        <v>881</v>
-      </c>
-      <c r="B31" s="11" t="s">
+    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="120" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="120" t="s">
-        <v>884</v>
-      </c>
-      <c r="B32" s="121"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="110" t="s">
-        <v>885</v>
-      </c>
+      <c r="B33" s="121"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="110" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="110" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="110" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="110" t="s">
+      <c r="B36" s="119" t="s">
+        <v>888</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>887</v>
       </c>
-      <c r="B35" s="146" t="s">
+    </row>
+    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="120" t="s">
         <v>889</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="120" t="s">
+      <c r="B40" s="121"/>
+    </row>
+    <row r="41" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A41" s="110" t="s">
+        <v>889</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>890</v>
       </c>
-      <c r="B39" s="121"/>
-    </row>
-    <row r="40" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A40" s="110" t="s">
-        <v>890</v>
-      </c>
-      <c r="B40" s="11" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A42" s="110" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A41" s="110" t="s">
+      <c r="B42" s="11" t="s">
         <v>892</v>
       </c>
-      <c r="B41" s="11" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="120" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="120" t="s">
+      <c r="B44" s="121"/>
+    </row>
+    <row r="45" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="B43" s="121"/>
-    </row>
-    <row r="44" spans="1:3" ht="225" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="120" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="120" t="s">
+      <c r="B47" s="121"/>
+    </row>
+    <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="118" t="s">
         <v>896</v>
       </c>
-      <c r="B46" s="121"/>
-    </row>
-    <row r="47" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="118" t="s">
+      <c r="B48" s="11" t="s">
         <v>897</v>
       </c>
-      <c r="B47" s="11" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="120" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="120" t="s">
+      <c r="B50" s="121"/>
+    </row>
+    <row r="51" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="118" t="s">
         <v>899</v>
       </c>
-      <c r="B49" s="121"/>
-    </row>
-    <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="118" t="s">
+      <c r="B51" s="11" t="s">
         <v>900</v>
       </c>
-      <c r="B50" s="11" t="s">
+    </row>
+    <row r="52" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="118" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="118" t="s">
+      <c r="B52" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="B51" s="11" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="120" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="120" t="s">
+      <c r="B54" s="121"/>
+    </row>
+    <row r="55" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A55" s="118" t="s">
         <v>904</v>
       </c>
-      <c r="B53" s="121"/>
-    </row>
-    <row r="54" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A54" s="118" t="s">
+      <c r="B55" s="11" t="s">
         <v>905</v>
       </c>
-      <c r="B54" s="11" t="s">
+    </row>
+    <row r="57" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="120" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="120" t="s">
+      <c r="B57" s="121"/>
+    </row>
+    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="118" t="s">
         <v>907</v>
       </c>
-      <c r="B56" s="121"/>
-    </row>
-    <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="118" t="s">
+      <c r="B58" s="110" t="s">
         <v>908</v>
       </c>
-      <c r="B57" s="110" t="s">
+    </row>
+    <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="118" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="118" t="s">
+      <c r="B59" s="110" t="s">
         <v>910</v>
       </c>
-      <c r="B58" s="110" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="118" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="118" t="s">
+      <c r="B60" s="110" t="s">
         <v>912</v>
       </c>
-      <c r="B59" s="110" t="s">
+    </row>
+    <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="118" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="118" t="s">
+      <c r="B61" s="110" t="s">
         <v>914</v>
-      </c>
-      <c r="B60" s="110" t="s">
-        <v>915</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A50:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13183,8 +13211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13195,10 +13223,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="122" t="s">
         <v>761</v>
       </c>
-      <c r="B1" s="119"/>
+      <c r="B1" s="122"/>
     </row>
     <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="120" t="s">
@@ -13223,7 +13251,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>764</v>
       </c>
       <c r="B5" s="114" t="s">
@@ -13231,19 +13259,19 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="125"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="114" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="125"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="114" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="126"/>
+      <c r="A8" s="127"/>
       <c r="B8" s="114" t="s">
         <v>768</v>
       </c>
@@ -13281,10 +13309,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="124" t="s">
         <v>777</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="124"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="115" t="s">
@@ -13311,10 +13339,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="123" t="s">
+      <c r="A17" s="124" t="s">
         <v>784</v>
       </c>
-      <c r="B17" s="123"/>
+      <c r="B17" s="124"/>
     </row>
     <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="115" t="s">
@@ -13344,15 +13372,15 @@
       <c r="A21" s="115" t="s">
         <v>791</v>
       </c>
-      <c r="B21" s="114" t="s">
+      <c r="B21" s="147" t="s">
         <v>792</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="123" t="s">
+      <c r="A22" s="124" t="s">
         <v>793</v>
       </c>
-      <c r="B22" s="123"/>
+      <c r="B22" s="124"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="115" t="s">
@@ -13371,10 +13399,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="123" t="s">
+      <c r="A25" s="124" t="s">
         <v>798</v>
       </c>
-      <c r="B25" s="123"/>
+      <c r="B25" s="124"/>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="115" t="s">
@@ -13393,10 +13421,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="123" t="s">
+      <c r="A28" s="124" t="s">
         <v>803</v>
       </c>
-      <c r="B28" s="123"/>
+      <c r="B28" s="124"/>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="115" t="s">
@@ -13423,10 +13451,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="124" t="s">
         <v>810</v>
       </c>
-      <c r="B32" s="123"/>
+      <c r="B32" s="124"/>
     </row>
     <row r="33" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
@@ -13435,10 +13463,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="124" t="s">
         <v>812</v>
       </c>
-      <c r="B34" s="123"/>
+      <c r="B34" s="124"/>
     </row>
     <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="115" t="s">
@@ -13449,7 +13477,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="124" t="s">
+      <c r="A36" s="125" t="s">
         <v>815</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -13457,22 +13485,22 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="125"/>
+      <c r="A37" s="126"/>
       <c r="B37" s="112" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="126"/>
+      <c r="A38" s="127"/>
       <c r="B38" s="112" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="123" t="s">
+      <c r="A39" s="124" t="s">
         <v>820</v>
       </c>
-      <c r="B39" s="123"/>
+      <c r="B39" s="124"/>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="116"/>
@@ -13481,13 +13509,13 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="123" t="s">
+      <c r="A41" s="124" t="s">
         <v>822</v>
       </c>
-      <c r="B41" s="123"/>
+      <c r="B41" s="124"/>
     </row>
     <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A42" s="124" t="s">
+      <c r="A42" s="125" t="s">
         <v>823</v>
       </c>
       <c r="B42" s="112" t="s">
@@ -13495,7 +13523,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A43" s="126"/>
+      <c r="A43" s="127"/>
       <c r="B43" s="112" t="s">
         <v>826</v>
       </c>
@@ -13533,10 +13561,10 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="123" t="s">
+      <c r="A48" s="124" t="s">
         <v>834</v>
       </c>
-      <c r="B48" s="123"/>
+      <c r="B48" s="124"/>
     </row>
     <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="111" t="s">
@@ -13559,10 +13587,10 @@
       <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="123" t="s">
+      <c r="A51" s="124" t="s">
         <v>840</v>
       </c>
-      <c r="B51" s="123"/>
+      <c r="B51" s="124"/>
       <c r="C51" s="35"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -13584,10 +13612,10 @@
       <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="123" t="s">
+      <c r="A54" s="124" t="s">
         <v>845</v>
       </c>
-      <c r="B54" s="123"/>
+      <c r="B54" s="124"/>
       <c r="C54" s="35"/>
     </row>
     <row r="55" spans="1:3" ht="195" x14ac:dyDescent="0.25">
@@ -13598,10 +13626,10 @@
       <c r="C55" s="35"/>
     </row>
     <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="123" t="s">
+      <c r="A56" s="124" t="s">
         <v>847</v>
       </c>
-      <c r="B56" s="123"/>
+      <c r="B56" s="124"/>
       <c r="C56" s="35"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -13652,6 +13680,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A56:B56"/>
@@ -13662,14 +13698,6 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13680,7 +13708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
@@ -13700,16 +13728,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="130" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="140"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="134" t="s">
+      <c r="A3" s="142" t="s">
         <v>502</v>
       </c>
-      <c r="B3" s="133"/>
+      <c r="B3" s="141"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -13736,10 +13764,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="141" t="s">
         <v>514</v>
       </c>
-      <c r="B7" s="131"/>
+      <c r="B7" s="139"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -13766,10 +13794,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="141" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="131"/>
+      <c r="B11" s="139"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -13780,10 +13808,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="141" t="s">
         <v>384</v>
       </c>
-      <c r="B13" s="133"/>
+      <c r="B13" s="141"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -13842,10 +13870,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="133" t="s">
+      <c r="A21" s="141" t="s">
         <v>499</v>
       </c>
-      <c r="B21" s="133"/>
+      <c r="B21" s="141"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -13856,10 +13884,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="133" t="s">
+      <c r="A23" s="141" t="s">
         <v>383</v>
       </c>
-      <c r="B23" s="133"/>
+      <c r="B23" s="141"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -13880,10 +13908,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="133" t="s">
+      <c r="A26" s="141" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="133"/>
+      <c r="B26" s="141"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -13910,10 +13938,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="133" t="s">
+      <c r="A30" s="141" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="133"/>
+      <c r="B30" s="141"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -13940,10 +13968,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="131" t="s">
+      <c r="A34" s="139" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="131"/>
+      <c r="B34" s="139"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -13970,10 +13998,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="133" t="s">
+      <c r="A38" s="141" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="133"/>
+      <c r="B38" s="141"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -14000,10 +14028,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="131" t="s">
+      <c r="A42" s="139" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="131"/>
+      <c r="B42" s="139"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -14022,10 +14050,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="133" t="s">
+      <c r="A45" s="141" t="s">
         <v>509</v>
       </c>
-      <c r="B45" s="131"/>
+      <c r="B45" s="139"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -14052,19 +14080,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="127" t="s">
+      <c r="A49" s="130" t="s">
         <v>369</v>
       </c>
-      <c r="B49" s="127"/>
+      <c r="B49" s="130"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="130" t="s">
+      <c r="A50" s="131" t="s">
         <v>312</v>
       </c>
       <c r="B50" s="129"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="138" t="s">
+      <c r="A51" s="136" t="s">
         <v>320</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -14072,7 +14100,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="139"/>
+      <c r="A52" s="137"/>
       <c r="B52" s="62" t="s">
         <v>587</v>
       </c>
@@ -14081,13 +14109,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="140"/>
+      <c r="A53" s="138"/>
       <c r="B53" s="62" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="138" t="s">
+      <c r="A54" s="136" t="s">
         <v>321</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -14095,25 +14123,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="139"/>
+      <c r="A55" s="137"/>
       <c r="B55" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="139"/>
+      <c r="A56" s="137"/>
       <c r="B56" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="140"/>
+      <c r="A57" s="138"/>
       <c r="B57" s="62" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="138" t="s">
+      <c r="A58" s="136" t="s">
         <v>322</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -14121,13 +14149,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="140"/>
+      <c r="A59" s="138"/>
       <c r="B59" s="62" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="138" t="s">
+      <c r="A60" s="136" t="s">
         <v>323</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -14138,7 +14166,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="139"/>
+      <c r="A61" s="137"/>
       <c r="B61" s="62" t="s">
         <v>524</v>
       </c>
@@ -14147,14 +14175,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="139"/>
+      <c r="A62" s="137"/>
       <c r="B62" s="62" t="s">
         <v>584</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="140"/>
+      <c r="A63" s="138"/>
       <c r="B63" s="62" t="s">
         <v>325</v>
       </c>
@@ -14208,7 +14236,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="135" t="s">
+      <c r="A70" s="133" t="s">
         <v>290</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -14216,43 +14244,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="136"/>
+      <c r="A71" s="134"/>
       <c r="B71" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="136"/>
+      <c r="A72" s="134"/>
       <c r="B72" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="136"/>
+      <c r="A73" s="134"/>
       <c r="B73" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="136"/>
+      <c r="A74" s="134"/>
       <c r="B74" s="62" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="136"/>
+      <c r="A75" s="134"/>
       <c r="B75" s="62" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="137"/>
+      <c r="A76" s="135"/>
       <c r="B76" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="135" t="s">
+      <c r="A77" s="133" t="s">
         <v>291</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -14260,74 +14288,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="136"/>
+      <c r="A78" s="134"/>
       <c r="B78" s="62" t="s">
         <v>299</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="136"/>
+      <c r="A79" s="134"/>
       <c r="B79" s="62" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="136"/>
+      <c r="A80" s="134"/>
       <c r="B80" s="62" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="136"/>
+      <c r="A81" s="134"/>
       <c r="B81" s="81" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="136"/>
+      <c r="A82" s="134"/>
       <c r="B82" s="81" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="136"/>
+      <c r="A83" s="134"/>
       <c r="B83" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="136"/>
+      <c r="A84" s="134"/>
       <c r="B84" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="136"/>
+      <c r="A85" s="134"/>
       <c r="B85" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="136"/>
+      <c r="A86" s="134"/>
       <c r="B86" s="81" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="136"/>
+      <c r="A87" s="134"/>
       <c r="B87" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="137"/>
+      <c r="A88" s="135"/>
       <c r="B88" s="81" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="135" t="s">
+      <c r="A89" s="133" t="s">
         <v>292</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -14335,28 +14363,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="136"/>
+      <c r="A90" s="134"/>
       <c r="B90" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="136"/>
+      <c r="A91" s="134"/>
       <c r="B91" s="83" t="s">
         <v>308</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="137"/>
+      <c r="A92" s="135"/>
       <c r="B92" s="82" t="s">
         <v>542</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="135" t="s">
+      <c r="A93" s="133" t="s">
         <v>309</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -14365,7 +14393,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="137"/>
+      <c r="A94" s="135"/>
       <c r="B94" s="84" t="s">
         <v>311</v>
       </c>
@@ -14435,14 +14463,14 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="127" t="s">
+      <c r="A102" s="130" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="127"/>
+      <c r="B102" s="130"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="130" t="s">
+      <c r="A103" s="131" t="s">
         <v>386</v>
       </c>
       <c r="B103" s="129"/>
@@ -14476,7 +14504,7 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="130" t="s">
+      <c r="A107" s="131" t="s">
         <v>393</v>
       </c>
       <c r="B107" s="129"/>
@@ -14636,7 +14664,7 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="130" t="s">
+      <c r="A125" s="131" t="s">
         <v>424</v>
       </c>
       <c r="B125" s="129"/>
@@ -14724,7 +14752,7 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="130" t="s">
+      <c r="A135" s="131" t="s">
         <v>496</v>
       </c>
       <c r="B135" s="129"/>
@@ -14925,14 +14953,14 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="127" t="s">
+      <c r="A158" s="130" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="127"/>
+      <c r="B158" s="130"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="130" t="s">
+      <c r="A159" s="131" t="s">
         <v>472</v>
       </c>
       <c r="B159" s="129"/>
@@ -14974,7 +15002,7 @@
       <c r="A165" s="128" t="s">
         <v>475</v>
       </c>
-      <c r="B165" s="141"/>
+      <c r="B165" s="132"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -15041,7 +15069,7 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="130" t="s">
+      <c r="A173" s="131" t="s">
         <v>470</v>
       </c>
       <c r="B173" s="129"/>
@@ -15066,7 +15094,7 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="130" t="s">
+      <c r="A176" s="131" t="s">
         <v>471</v>
       </c>
       <c r="B176" s="129"/>
@@ -15091,14 +15119,14 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="127" t="s">
+      <c r="A179" s="130" t="s">
         <v>548</v>
       </c>
-      <c r="B179" s="127"/>
+      <c r="B179" s="130"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="130" t="s">
+      <c r="A180" s="131" t="s">
         <v>549</v>
       </c>
       <c r="B180" s="129"/>
@@ -15117,7 +15145,7 @@
       <c r="B182" s="76"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="130" t="s">
+      <c r="A183" s="131" t="s">
         <v>548</v>
       </c>
       <c r="B183" s="129"/>
@@ -15201,7 +15229,7 @@
       <c r="B192" s="76"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="130" t="s">
+      <c r="A193" s="131" t="s">
         <v>571</v>
       </c>
       <c r="B193" s="129"/>
@@ -15260,10 +15288,10 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="127" t="s">
+      <c r="A201" s="130" t="s">
         <v>596</v>
       </c>
-      <c r="B201" s="127"/>
+      <c r="B201" s="130"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -15409,10 +15437,10 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="127" t="s">
+      <c r="A222" s="130" t="s">
         <v>630</v>
       </c>
-      <c r="B222" s="127"/>
+      <c r="B222" s="130"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A223" s="128" t="s">
@@ -15709,10 +15737,10 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="127" t="s">
+      <c r="A262" s="130" t="s">
         <v>700</v>
       </c>
-      <c r="B262" s="127"/>
+      <c r="B262" s="130"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A263" s="128" t="s">
@@ -15910,39 +15938,18 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -15959,18 +15966,39 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16392,7 +16420,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -16412,7 +16440,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="143"/>
+      <c r="A2" s="144"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -16480,10 +16508,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="145" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="145"/>
+      <c r="C6" s="146"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework -04.Code First - Complete
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686" activeTab="1"/>
@@ -32,7 +32,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -9319,13 +9319,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="60" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="61" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10168,42 +10176,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10218,91 +10226,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10317,73 +10325,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10392,49 +10400,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10446,166 +10454,166 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -10699,7 +10707,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -10707,6 +10715,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -10760,7 +10779,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10795,7 +10814,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13526,7 +13545,7 @@
   <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13537,10 +13556,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="129" t="s">
         <v>919</v>
       </c>
-      <c r="B1" s="125"/>
+      <c r="B1" s="129"/>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
@@ -13566,17 +13585,17 @@
         <v>818</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>920</v>
       </c>
       <c r="B5" s="58"/>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="123" t="s">
+      <c r="A6" s="127" t="s">
         <v>921</v>
       </c>
-      <c r="B6" s="124"/>
+      <c r="B6" s="128"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
@@ -13615,10 +13634,10 @@
       <c r="B12" s="58"/>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="127" t="s">
         <v>928</v>
       </c>
-      <c r="B13" s="124"/>
+      <c r="B13" s="128"/>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="112" t="s">
@@ -13629,10 +13648,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="123" t="s">
+      <c r="A15" s="127" t="s">
         <v>853</v>
       </c>
-      <c r="B15" s="124"/>
+      <c r="B15" s="128"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="121" t="s">
@@ -13657,10 +13676,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="123" t="s">
+      <c r="A19" s="127" t="s">
         <v>936</v>
       </c>
-      <c r="B19" s="124"/>
+      <c r="B19" s="128"/>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="118" t="s">
@@ -13695,30 +13714,30 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="123" t="s">
+      <c r="A24" s="127" t="s">
         <v>945</v>
       </c>
-      <c r="B24" s="124"/>
+      <c r="B24" s="128"/>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="123" t="s">
+      <c r="A25" s="127" t="s">
         <v>888</v>
       </c>
-      <c r="B25" s="124"/>
+      <c r="B25" s="128"/>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="120" t="s">
         <v>946</v>
       </c>
-      <c r="B26" s="150" t="s">
+      <c r="B26" s="122" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="123" t="s">
+      <c r="A27" s="127" t="s">
         <v>951</v>
       </c>
-      <c r="B27" s="124"/>
+      <c r="B27" s="128"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="112" t="s">
@@ -13743,10 +13762,10 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="123" t="s">
+      <c r="A31" s="127" t="s">
         <v>951</v>
       </c>
-      <c r="B31" s="124"/>
+      <c r="B31" s="128"/>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="120" t="s">
@@ -13787,10 +13806,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="127" t="s">
         <v>964</v>
       </c>
-      <c r="B36" s="124"/>
+      <c r="B36" s="128"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="120" t="s">
@@ -13857,16 +13876,16 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="123" t="s">
+      <c r="A45" s="127" t="s">
         <v>964</v>
       </c>
-      <c r="B45" s="124"/>
+      <c r="B45" s="128"/>
     </row>
     <row r="46" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="120" t="s">
         <v>981</v>
       </c>
-      <c r="B46" s="151" t="s">
+      <c r="B46" s="123" t="s">
         <v>982</v>
       </c>
     </row>
@@ -13874,15 +13893,15 @@
       <c r="A47" s="120" t="s">
         <v>983</v>
       </c>
-      <c r="B47" s="152" t="s">
+      <c r="B47" s="124" t="s">
         <v>984</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="123" t="s">
+      <c r="A48" s="127" t="s">
         <v>985</v>
       </c>
-      <c r="B48" s="124"/>
+      <c r="B48" s="128"/>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="120" t="s">
@@ -13896,15 +13915,15 @@
       <c r="A50" s="120" t="s">
         <v>988</v>
       </c>
-      <c r="B50" s="150" t="s">
+      <c r="B50" s="122" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="123" t="s">
+      <c r="A51" s="127" t="s">
         <v>990</v>
       </c>
-      <c r="B51" s="124"/>
+      <c r="B51" s="128"/>
     </row>
     <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="120" t="s">
@@ -13923,10 +13942,10 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="123" t="s">
+      <c r="A54" s="127" t="s">
         <v>995</v>
       </c>
-      <c r="B54" s="124"/>
+      <c r="B54" s="128"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="120" t="s">
@@ -13947,10 +13966,10 @@
       <c r="B57" s="58"/>
     </row>
     <row r="58" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="125" t="s">
+      <c r="A58" s="129" t="s">
         <v>854</v>
       </c>
-      <c r="B58" s="125"/>
+      <c r="B58" s="129"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="112" t="s">
@@ -14033,10 +14052,10 @@
       <c r="B70" s="58"/>
     </row>
     <row r="71" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="122" t="s">
+      <c r="A71" s="130" t="s">
         <v>867</v>
       </c>
-      <c r="B71" s="122"/>
+      <c r="B71" s="130"/>
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="111" t="s">
@@ -14047,7 +14066,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="126" t="s">
+      <c r="A73" s="125" t="s">
         <v>870</v>
       </c>
       <c r="B73" s="58" t="s">
@@ -14055,25 +14074,25 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="126"/>
+      <c r="A74" s="125"/>
       <c r="B74" s="58" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="126"/>
+      <c r="A75" s="125"/>
       <c r="B75" s="58" t="s">
         <v>873</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="126"/>
+      <c r="A76" s="125"/>
       <c r="B76" s="58" t="s">
         <v>874</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="126"/>
+      <c r="A77" s="125"/>
       <c r="B77" s="58" t="s">
         <v>875</v>
       </c>
@@ -14083,16 +14102,16 @@
       <c r="B78" s="58"/>
     </row>
     <row r="79" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="127" t="s">
+      <c r="A79" s="126" t="s">
         <v>876</v>
       </c>
-      <c r="B79" s="127"/>
+      <c r="B79" s="126"/>
     </row>
     <row r="80" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="122" t="s">
+      <c r="A80" s="130" t="s">
         <v>878</v>
       </c>
-      <c r="B80" s="122"/>
+      <c r="B80" s="130"/>
     </row>
     <row r="81" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" s="112" t="s">
@@ -14111,10 +14130,10 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="122" t="s">
+      <c r="A83" s="130" t="s">
         <v>882</v>
       </c>
-      <c r="B83" s="122"/>
+      <c r="B83" s="130"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="112" t="s">
@@ -14152,10 +14171,10 @@
       <c r="B89" s="58"/>
     </row>
     <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="122" t="s">
+      <c r="A90" s="130" t="s">
         <v>888</v>
       </c>
-      <c r="B90" s="122"/>
+      <c r="B90" s="130"/>
     </row>
     <row r="91" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A91" s="112" t="s">
@@ -14178,10 +14197,10 @@
       <c r="B93" s="58"/>
     </row>
     <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="122" t="s">
+      <c r="A94" s="130" t="s">
         <v>892</v>
       </c>
-      <c r="B94" s="122"/>
+      <c r="B94" s="130"/>
     </row>
     <row r="95" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A95" s="112"/>
@@ -14194,10 +14213,10 @@
       <c r="B96" s="58"/>
     </row>
     <row r="97" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="122" t="s">
+      <c r="A97" s="130" t="s">
         <v>894</v>
       </c>
-      <c r="B97" s="122"/>
+      <c r="B97" s="130"/>
     </row>
     <row r="98" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="111" t="s">
@@ -14212,10 +14231,10 @@
       <c r="B99" s="58"/>
     </row>
     <row r="100" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="122" t="s">
+      <c r="A100" s="130" t="s">
         <v>897</v>
       </c>
-      <c r="B100" s="122"/>
+      <c r="B100" s="130"/>
     </row>
     <row r="101" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="111" t="s">
@@ -14238,10 +14257,10 @@
       <c r="B103" s="58"/>
     </row>
     <row r="104" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="122" t="s">
+      <c r="A104" s="130" t="s">
         <v>902</v>
       </c>
-      <c r="B104" s="122"/>
+      <c r="B104" s="130"/>
     </row>
     <row r="105" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A105" s="111" t="s">
@@ -14256,10 +14275,10 @@
       <c r="B106" s="58"/>
     </row>
     <row r="107" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="122" t="s">
+      <c r="A107" s="130" t="s">
         <v>905</v>
       </c>
-      <c r="B107" s="122"/>
+      <c r="B107" s="130"/>
     </row>
     <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="111" t="s">
@@ -14295,6 +14314,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A100:B100"/>
     <mergeCell ref="A73:A77"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A6:B6"/>
@@ -14310,17 +14340,6 @@
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A100:B100"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1"/>
@@ -14346,16 +14365,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="129" t="s">
         <v>760</v>
       </c>
-      <c r="B1" s="125"/>
+      <c r="B1" s="129"/>
     </row>
     <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="127" t="s">
         <v>757</v>
       </c>
-      <c r="B2" s="124"/>
+      <c r="B2" s="128"/>
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="111" t="s">
@@ -14374,7 +14393,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="128" t="s">
+      <c r="A5" s="131" t="s">
         <v>763</v>
       </c>
       <c r="B5" s="114" t="s">
@@ -14382,19 +14401,19 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="129"/>
+      <c r="A6" s="132"/>
       <c r="B6" s="114" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
+      <c r="A7" s="132"/>
       <c r="B7" s="114" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
+      <c r="A8" s="133"/>
       <c r="B8" s="114" t="s">
         <v>767</v>
       </c>
@@ -14432,10 +14451,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="130" t="s">
         <v>776</v>
       </c>
-      <c r="B13" s="122"/>
+      <c r="B13" s="130"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="115" t="s">
@@ -14462,10 +14481,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="130" t="s">
         <v>783</v>
       </c>
-      <c r="B17" s="122"/>
+      <c r="B17" s="130"/>
     </row>
     <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="115" t="s">
@@ -14500,10 +14519,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="122" t="s">
+      <c r="A22" s="130" t="s">
         <v>792</v>
       </c>
-      <c r="B22" s="122"/>
+      <c r="B22" s="130"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="115" t="s">
@@ -14522,10 +14541,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="122" t="s">
+      <c r="A25" s="130" t="s">
         <v>797</v>
       </c>
-      <c r="B25" s="122"/>
+      <c r="B25" s="130"/>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="115" t="s">
@@ -14544,10 +14563,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="122" t="s">
+      <c r="A28" s="130" t="s">
         <v>802</v>
       </c>
-      <c r="B28" s="122"/>
+      <c r="B28" s="130"/>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="115" t="s">
@@ -14574,10 +14593,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="122" t="s">
+      <c r="A32" s="130" t="s">
         <v>809</v>
       </c>
-      <c r="B32" s="122"/>
+      <c r="B32" s="130"/>
     </row>
     <row r="33" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
@@ -14586,10 +14605,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="122" t="s">
+      <c r="A34" s="130" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="122"/>
+      <c r="B34" s="130"/>
     </row>
     <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="115" t="s">
@@ -14600,7 +14619,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="128" t="s">
+      <c r="A36" s="131" t="s">
         <v>814</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -14608,22 +14627,22 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="129"/>
+      <c r="A37" s="132"/>
       <c r="B37" s="112" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="130"/>
+      <c r="A38" s="133"/>
       <c r="B38" s="112" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="122" t="s">
+      <c r="A39" s="130" t="s">
         <v>819</v>
       </c>
-      <c r="B39" s="122"/>
+      <c r="B39" s="130"/>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="116"/>
@@ -14632,13 +14651,13 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="122" t="s">
+      <c r="A41" s="130" t="s">
         <v>821</v>
       </c>
-      <c r="B41" s="122"/>
+      <c r="B41" s="130"/>
     </row>
     <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A42" s="128" t="s">
+      <c r="A42" s="131" t="s">
         <v>822</v>
       </c>
       <c r="B42" s="112" t="s">
@@ -14646,7 +14665,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A43" s="130"/>
+      <c r="A43" s="133"/>
       <c r="B43" s="112" t="s">
         <v>825</v>
       </c>
@@ -14684,10 +14703,10 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="122" t="s">
+      <c r="A48" s="130" t="s">
         <v>833</v>
       </c>
-      <c r="B48" s="122"/>
+      <c r="B48" s="130"/>
     </row>
     <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="111" t="s">
@@ -14710,10 +14729,10 @@
       <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="122" t="s">
+      <c r="A51" s="130" t="s">
         <v>839</v>
       </c>
-      <c r="B51" s="122"/>
+      <c r="B51" s="130"/>
       <c r="C51" s="35"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14735,10 +14754,10 @@
       <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="122" t="s">
+      <c r="A54" s="130" t="s">
         <v>844</v>
       </c>
-      <c r="B54" s="122"/>
+      <c r="B54" s="130"/>
       <c r="C54" s="35"/>
     </row>
     <row r="55" spans="1:3" ht="195" x14ac:dyDescent="0.25">
@@ -14749,10 +14768,10 @@
       <c r="C55" s="35"/>
     </row>
     <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="122" t="s">
+      <c r="A56" s="130" t="s">
         <v>846</v>
       </c>
-      <c r="B56" s="122"/>
+      <c r="B56" s="130"/>
       <c r="C56" s="35"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14803,14 +14822,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A56:B56"/>
@@ -14821,6 +14832,14 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14851,16 +14870,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="134" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="143"/>
+      <c r="B2" s="139"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="141" t="s">
         <v>501</v>
       </c>
-      <c r="B3" s="144"/>
+      <c r="B3" s="140"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -14887,10 +14906,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="140" t="s">
         <v>513</v>
       </c>
-      <c r="B7" s="142"/>
+      <c r="B7" s="138"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -14917,10 +14936,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="140" t="s">
         <v>515</v>
       </c>
-      <c r="B11" s="142"/>
+      <c r="B11" s="138"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -14931,10 +14950,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="140" t="s">
         <v>383</v>
       </c>
-      <c r="B13" s="144"/>
+      <c r="B13" s="140"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -14993,10 +15012,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="144" t="s">
+      <c r="A21" s="140" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="144"/>
+      <c r="B21" s="140"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -15007,10 +15026,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="144" t="s">
+      <c r="A23" s="140" t="s">
         <v>382</v>
       </c>
-      <c r="B23" s="144"/>
+      <c r="B23" s="140"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -15031,10 +15050,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="144" t="s">
+      <c r="A26" s="140" t="s">
         <v>347</v>
       </c>
-      <c r="B26" s="144"/>
+      <c r="B26" s="140"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -15061,10 +15080,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="144" t="s">
+      <c r="A30" s="140" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="144"/>
+      <c r="B30" s="140"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -15091,10 +15110,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="142" t="s">
+      <c r="A34" s="138" t="s">
         <v>357</v>
       </c>
-      <c r="B34" s="142"/>
+      <c r="B34" s="138"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -15121,10 +15140,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="140" t="s">
         <v>354</v>
       </c>
-      <c r="B38" s="144"/>
+      <c r="B38" s="140"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -15151,10 +15170,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="142" t="s">
+      <c r="A42" s="138" t="s">
         <v>358</v>
       </c>
-      <c r="B42" s="142"/>
+      <c r="B42" s="138"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -15173,10 +15192,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="144" t="s">
+      <c r="A45" s="140" t="s">
         <v>508</v>
       </c>
-      <c r="B45" s="142"/>
+      <c r="B45" s="138"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -15203,19 +15222,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="133" t="s">
+      <c r="A49" s="134" t="s">
         <v>368</v>
       </c>
-      <c r="B49" s="133"/>
+      <c r="B49" s="134"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="134" t="s">
+      <c r="A50" s="137" t="s">
         <v>311</v>
       </c>
-      <c r="B50" s="132"/>
+      <c r="B50" s="136"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="139" t="s">
+      <c r="A51" s="145" t="s">
         <v>319</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -15223,7 +15242,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="140"/>
+      <c r="A52" s="146"/>
       <c r="B52" s="62" t="s">
         <v>586</v>
       </c>
@@ -15232,13 +15251,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="141"/>
+      <c r="A53" s="147"/>
       <c r="B53" s="62" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="139" t="s">
+      <c r="A54" s="145" t="s">
         <v>320</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -15246,25 +15265,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="140"/>
+      <c r="A55" s="146"/>
       <c r="B55" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="140"/>
+      <c r="A56" s="146"/>
       <c r="B56" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="141"/>
+      <c r="A57" s="147"/>
       <c r="B57" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="139" t="s">
+      <c r="A58" s="145" t="s">
         <v>321</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -15272,13 +15291,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="141"/>
+      <c r="A59" s="147"/>
       <c r="B59" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="139" t="s">
+      <c r="A60" s="145" t="s">
         <v>322</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -15289,7 +15308,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="140"/>
+      <c r="A61" s="146"/>
       <c r="B61" s="62" t="s">
         <v>523</v>
       </c>
@@ -15298,14 +15317,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="140"/>
+      <c r="A62" s="146"/>
       <c r="B62" s="62" t="s">
         <v>583</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="141"/>
+      <c r="A63" s="147"/>
       <c r="B63" s="62" t="s">
         <v>324</v>
       </c>
@@ -15359,7 +15378,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="136" t="s">
+      <c r="A70" s="142" t="s">
         <v>289</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -15367,43 +15386,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="137"/>
+      <c r="A71" s="143"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="137"/>
+      <c r="A72" s="143"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="137"/>
+      <c r="A73" s="143"/>
       <c r="B73" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="137"/>
+      <c r="A74" s="143"/>
       <c r="B74" s="62" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="137"/>
+      <c r="A75" s="143"/>
       <c r="B75" s="62" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="138"/>
+      <c r="A76" s="144"/>
       <c r="B76" s="62" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="136" t="s">
+      <c r="A77" s="142" t="s">
         <v>290</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -15411,74 +15430,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="137"/>
+      <c r="A78" s="143"/>
       <c r="B78" s="62" t="s">
         <v>298</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="137"/>
+      <c r="A79" s="143"/>
       <c r="B79" s="62" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="137"/>
+      <c r="A80" s="143"/>
       <c r="B80" s="62" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="137"/>
+      <c r="A81" s="143"/>
       <c r="B81" s="81" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="137"/>
+      <c r="A82" s="143"/>
       <c r="B82" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="137"/>
+      <c r="A83" s="143"/>
       <c r="B83" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="137"/>
+      <c r="A84" s="143"/>
       <c r="B84" s="81" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="137"/>
+      <c r="A85" s="143"/>
       <c r="B85" s="81" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="137"/>
+      <c r="A86" s="143"/>
       <c r="B86" s="81" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="137"/>
+      <c r="A87" s="143"/>
       <c r="B87" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="138"/>
+      <c r="A88" s="144"/>
       <c r="B88" s="81" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="136" t="s">
+      <c r="A89" s="142" t="s">
         <v>291</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -15486,28 +15505,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="137"/>
+      <c r="A90" s="143"/>
       <c r="B90" s="83" t="s">
         <v>306</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="137"/>
+      <c r="A91" s="143"/>
       <c r="B91" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="138"/>
+      <c r="A92" s="144"/>
       <c r="B92" s="82" t="s">
         <v>541</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="136" t="s">
+      <c r="A93" s="142" t="s">
         <v>308</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -15516,7 +15535,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="138"/>
+      <c r="A94" s="144"/>
       <c r="B94" s="84" t="s">
         <v>310</v>
       </c>
@@ -15586,17 +15605,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="133" t="s">
+      <c r="A102" s="134" t="s">
         <v>384</v>
       </c>
-      <c r="B102" s="133"/>
+      <c r="B102" s="134"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="134" t="s">
+      <c r="A103" s="137" t="s">
         <v>385</v>
       </c>
-      <c r="B103" s="132"/>
+      <c r="B103" s="136"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -15627,10 +15646,10 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="134" t="s">
+      <c r="A107" s="137" t="s">
         <v>392</v>
       </c>
-      <c r="B107" s="132"/>
+      <c r="B107" s="136"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -15787,10 +15806,10 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="134" t="s">
+      <c r="A125" s="137" t="s">
         <v>423</v>
       </c>
-      <c r="B125" s="132"/>
+      <c r="B125" s="136"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -15875,10 +15894,10 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="134" t="s">
+      <c r="A135" s="137" t="s">
         <v>495</v>
       </c>
-      <c r="B135" s="132"/>
+      <c r="B135" s="136"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -15972,10 +15991,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="131" t="s">
+      <c r="A146" s="135" t="s">
         <v>458</v>
       </c>
-      <c r="B146" s="132"/>
+      <c r="B146" s="136"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -16006,10 +16025,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="131" t="s">
+      <c r="A150" s="135" t="s">
         <v>466</v>
       </c>
-      <c r="B150" s="132"/>
+      <c r="B150" s="136"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16031,10 +16050,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="131" t="s">
+      <c r="A153" s="135" t="s">
         <v>536</v>
       </c>
-      <c r="B153" s="132"/>
+      <c r="B153" s="136"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -16076,17 +16095,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="133" t="s">
+      <c r="A158" s="134" t="s">
         <v>468</v>
       </c>
-      <c r="B158" s="133"/>
+      <c r="B158" s="134"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="134" t="s">
+      <c r="A159" s="137" t="s">
         <v>471</v>
       </c>
-      <c r="B159" s="132"/>
+      <c r="B159" s="136"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -16122,10 +16141,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="131" t="s">
+      <c r="A165" s="135" t="s">
         <v>474</v>
       </c>
-      <c r="B165" s="135"/>
+      <c r="B165" s="148"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -16192,10 +16211,10 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="134" t="s">
+      <c r="A173" s="137" t="s">
         <v>469</v>
       </c>
-      <c r="B173" s="132"/>
+      <c r="B173" s="136"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -16217,10 +16236,10 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="134" t="s">
+      <c r="A176" s="137" t="s">
         <v>470</v>
       </c>
-      <c r="B176" s="132"/>
+      <c r="B176" s="136"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -16242,17 +16261,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="133" t="s">
+      <c r="A179" s="134" t="s">
         <v>547</v>
       </c>
-      <c r="B179" s="133"/>
+      <c r="B179" s="134"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="134" t="s">
+      <c r="A180" s="137" t="s">
         <v>548</v>
       </c>
-      <c r="B180" s="132"/>
+      <c r="B180" s="136"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16268,10 +16287,10 @@
       <c r="B182" s="76"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="134" t="s">
+      <c r="A183" s="137" t="s">
         <v>547</v>
       </c>
-      <c r="B183" s="132"/>
+      <c r="B183" s="136"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16352,10 +16371,10 @@
       <c r="B192" s="76"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="134" t="s">
+      <c r="A193" s="137" t="s">
         <v>570</v>
       </c>
-      <c r="B193" s="132"/>
+      <c r="B193" s="136"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16373,10 +16392,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="131" t="s">
+      <c r="A196" s="135" t="s">
         <v>574</v>
       </c>
-      <c r="B196" s="132"/>
+      <c r="B196" s="136"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -16411,17 +16430,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="133" t="s">
+      <c r="A201" s="134" t="s">
         <v>595</v>
       </c>
-      <c r="B201" s="133"/>
+      <c r="B201" s="134"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="131" t="s">
+      <c r="A202" s="135" t="s">
         <v>597</v>
       </c>
-      <c r="B202" s="132"/>
+      <c r="B202" s="136"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -16468,10 +16487,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="131" t="s">
+      <c r="A209" s="135" t="s">
         <v>608</v>
       </c>
-      <c r="B209" s="132"/>
+      <c r="B209" s="136"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -16486,10 +16505,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="131" t="s">
+      <c r="A212" s="135" t="s">
         <v>610</v>
       </c>
-      <c r="B212" s="132"/>
+      <c r="B212" s="136"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -16500,10 +16519,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="131" t="s">
+      <c r="A214" s="135" t="s">
         <v>614</v>
       </c>
-      <c r="B214" s="132"/>
+      <c r="B214" s="136"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -16522,10 +16541,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="131" t="s">
+      <c r="A217" s="135" t="s">
         <v>613</v>
       </c>
-      <c r="B217" s="132"/>
+      <c r="B217" s="136"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -16560,22 +16579,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="133" t="s">
+      <c r="A222" s="134" t="s">
         <v>629</v>
       </c>
-      <c r="B222" s="133"/>
+      <c r="B222" s="134"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="131" t="s">
+      <c r="A223" s="135" t="s">
         <v>631</v>
       </c>
-      <c r="B223" s="132"/>
+      <c r="B223" s="136"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="131" t="s">
+      <c r="A224" s="135" t="s">
         <v>630</v>
       </c>
-      <c r="B224" s="132"/>
+      <c r="B224" s="136"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -16586,10 +16605,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="131" t="s">
+      <c r="A226" s="135" t="s">
         <v>634</v>
       </c>
-      <c r="B226" s="132"/>
+      <c r="B226" s="136"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -16632,10 +16651,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="131" t="s">
+      <c r="A232" s="135" t="s">
         <v>644</v>
       </c>
-      <c r="B232" s="132"/>
+      <c r="B232" s="136"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -16646,10 +16665,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="131" t="s">
+      <c r="A234" s="135" t="s">
         <v>647</v>
       </c>
-      <c r="B234" s="132"/>
+      <c r="B234" s="136"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -16666,10 +16685,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="131" t="s">
+      <c r="A237" s="135" t="s">
         <v>651</v>
       </c>
-      <c r="B237" s="132"/>
+      <c r="B237" s="136"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -16816,10 +16835,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="131" t="s">
+      <c r="A256" s="135" t="s">
         <v>688</v>
       </c>
-      <c r="B256" s="132"/>
+      <c r="B256" s="136"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -16846,10 +16865,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="131" t="s">
+      <c r="A260" s="135" t="s">
         <v>696</v>
       </c>
-      <c r="B260" s="132"/>
+      <c r="B260" s="136"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -16860,16 +16879,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="133" t="s">
+      <c r="A262" s="134" t="s">
         <v>699</v>
       </c>
-      <c r="B262" s="133"/>
+      <c r="B262" s="134"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="131" t="s">
+      <c r="A263" s="135" t="s">
         <v>700</v>
       </c>
-      <c r="B263" s="132"/>
+      <c r="B263" s="136"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -16904,10 +16923,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="131" t="s">
+      <c r="A268" s="135" t="s">
         <v>709</v>
       </c>
-      <c r="B268" s="132"/>
+      <c r="B268" s="136"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -16942,10 +16961,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="131" t="s">
+      <c r="A273" s="135" t="s">
         <v>701</v>
       </c>
-      <c r="B273" s="132"/>
+      <c r="B273" s="136"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -17002,10 +17021,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="131" t="s">
+      <c r="A280" s="135" t="s">
         <v>730</v>
       </c>
-      <c r="B280" s="132"/>
+      <c r="B280" s="136"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -17061,18 +17080,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -17089,39 +17129,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17543,7 +17562,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="149" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -17563,7 +17582,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
+      <c r="A2" s="150"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -17631,10 +17650,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="151" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="149"/>
+      <c r="C6" s="152"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework -05.Entity-Relations
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -8567,12 +8567,6 @@
     <t>One way to connect is to create a Configuration class with your  connection string:</t>
   </si>
   <si>
-    <t>public static class Configuration
-{
-  public const string ConnectionString = "Server=.;Database=…;";
-}</t>
-  </si>
-  <si>
     <t>Then add the connection string in the OnConfiguring method in  the DbContext class</t>
   </si>
   <si>
@@ -9314,6 +9308,12 @@
       </rPr>
       <t xml:space="preserve"> - Execute the SQL DELETE command</t>
     </r>
+  </si>
+  <si>
+    <t>public static class Configuration
+{
+  public const string ConnectionString = "Server=.\\SQLEXPRESS;Database=Hospital;Integrated Security=true;";
+}</t>
   </si>
 </sst>
 </file>
@@ -10530,6 +10530,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -10542,12 +10548,6 @@
     <xf numFmtId="0" fontId="51" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10557,29 +10557,20 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10599,8 +10590,17 @@
     <xf numFmtId="0" fontId="45" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -13544,8 +13544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13556,10 +13556,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
-        <v>919</v>
-      </c>
-      <c r="B1" s="129"/>
+      <c r="A1" s="125" t="s">
+        <v>918</v>
+      </c>
+      <c r="B1" s="125"/>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
@@ -13587,378 +13587,378 @@
     </row>
     <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
+        <v>919</v>
+      </c>
+      <c r="B5" s="58"/>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="129" t="s">
         <v>920</v>
       </c>
-      <c r="B5" s="58"/>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="127" t="s">
-        <v>921</v>
-      </c>
-      <c r="B6" s="128"/>
+      <c r="B6" s="130"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B7" s="58"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B8" s="58"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B9" s="58"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="112" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B10" s="58"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="112" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B11" s="58"/>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="112" t="s">
+        <v>926</v>
+      </c>
+      <c r="B12" s="58"/>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="129" t="s">
         <v>927</v>
       </c>
-      <c r="B12" s="58"/>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="127" t="s">
-        <v>928</v>
-      </c>
-      <c r="B13" s="128"/>
+      <c r="B13" s="130"/>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="112" t="s">
+        <v>928</v>
+      </c>
+      <c r="B14" s="76" t="s">
         <v>929</v>
       </c>
-      <c r="B14" s="76" t="s">
-        <v>930</v>
-      </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="127" t="s">
+      <c r="A15" s="129" t="s">
         <v>853</v>
       </c>
-      <c r="B15" s="128"/>
+      <c r="B15" s="130"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="121" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B16" s="58"/>
     </row>
     <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="118" t="s">
+        <v>931</v>
+      </c>
+      <c r="B17" s="76" t="s">
         <v>932</v>
-      </c>
-      <c r="B17" s="76" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="118" t="s">
+        <v>933</v>
+      </c>
+      <c r="B18" s="76" t="s">
         <v>934</v>
       </c>
-      <c r="B18" s="76" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="129" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="127" t="s">
-        <v>936</v>
-      </c>
-      <c r="B19" s="128"/>
+      <c r="B19" s="130"/>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="118" t="s">
+        <v>936</v>
+      </c>
+      <c r="B20" s="76" t="s">
         <v>937</v>
-      </c>
-      <c r="B20" s="76" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="118" t="s">
+        <v>938</v>
+      </c>
+      <c r="B21" s="76" t="s">
         <v>939</v>
-      </c>
-      <c r="B21" s="76" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="118" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B22" s="76" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="118" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B23" s="76" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="129" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="127" t="s">
-        <v>945</v>
-      </c>
-      <c r="B24" s="128"/>
+      <c r="B24" s="130"/>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="127" t="s">
+      <c r="A25" s="129" t="s">
         <v>888</v>
       </c>
-      <c r="B25" s="128"/>
+      <c r="B25" s="130"/>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="120" t="s">
+        <v>945</v>
+      </c>
+      <c r="B26" s="122" t="s">
         <v>946</v>
       </c>
-      <c r="B26" s="122" t="s">
-        <v>947</v>
-      </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="127" t="s">
-        <v>951</v>
-      </c>
-      <c r="B27" s="128"/>
+      <c r="A27" s="129" t="s">
+        <v>950</v>
+      </c>
+      <c r="B27" s="130"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="112" t="s">
+        <v>947</v>
+      </c>
+      <c r="B28" s="76" t="s">
         <v>948</v>
-      </c>
-      <c r="B28" s="76" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="112" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B29" s="58"/>
     </row>
     <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="112" t="s">
+        <v>951</v>
+      </c>
+      <c r="B30" s="76" t="s">
         <v>952</v>
       </c>
-      <c r="B30" s="76" t="s">
-        <v>953</v>
-      </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="127" t="s">
-        <v>951</v>
-      </c>
-      <c r="B31" s="128"/>
+      <c r="A31" s="129" t="s">
+        <v>950</v>
+      </c>
+      <c r="B31" s="130"/>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="120" t="s">
+        <v>953</v>
+      </c>
+      <c r="B32" s="76" t="s">
         <v>954</v>
-      </c>
-      <c r="B32" s="76" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="120" t="s">
+        <v>955</v>
+      </c>
+      <c r="B33" s="76" t="s">
         <v>956</v>
       </c>
-      <c r="B33" s="76" t="s">
-        <v>957</v>
-      </c>
       <c r="C33" s="35" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="120" t="s">
+        <v>957</v>
+      </c>
+      <c r="B34" s="76" t="s">
         <v>958</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="C34" s="46" t="s">
         <v>959</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="120" t="s">
+        <v>961</v>
+      </c>
+      <c r="B35" s="76" t="s">
         <v>962</v>
       </c>
-      <c r="B35" s="76" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="129" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="127" t="s">
-        <v>964</v>
-      </c>
-      <c r="B36" s="128"/>
+      <c r="B36" s="130"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="120" t="s">
+        <v>964</v>
+      </c>
+      <c r="B37" s="58" t="s">
         <v>965</v>
-      </c>
-      <c r="B37" s="58" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="120" t="s">
+        <v>966</v>
+      </c>
+      <c r="B38" s="76" t="s">
         <v>967</v>
-      </c>
-      <c r="B38" s="76" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="120" t="s">
+        <v>968</v>
+      </c>
+      <c r="B39" s="76" t="s">
         <v>969</v>
-      </c>
-      <c r="B39" s="76" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="120" t="s">
+        <v>970</v>
+      </c>
+      <c r="B40" s="58" t="s">
         <v>971</v>
-      </c>
-      <c r="B40" s="58" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="120" t="s">
+        <v>972</v>
+      </c>
+      <c r="B41" s="58" t="s">
         <v>973</v>
-      </c>
-      <c r="B41" s="58" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="120" t="s">
+        <v>974</v>
+      </c>
+      <c r="B42" s="58" t="s">
         <v>975</v>
-      </c>
-      <c r="B42" s="58" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="120" t="s">
+        <v>976</v>
+      </c>
+      <c r="B43" s="58" t="s">
         <v>977</v>
-      </c>
-      <c r="B43" s="58" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="120" t="s">
+        <v>978</v>
+      </c>
+      <c r="B44" s="58" t="s">
         <v>979</v>
       </c>
-      <c r="B44" s="58" t="s">
-        <v>980</v>
-      </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="127" t="s">
-        <v>964</v>
-      </c>
-      <c r="B45" s="128"/>
+      <c r="A45" s="129" t="s">
+        <v>963</v>
+      </c>
+      <c r="B45" s="130"/>
     </row>
     <row r="46" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="120" t="s">
+        <v>980</v>
+      </c>
+      <c r="B46" s="123" t="s">
         <v>981</v>
-      </c>
-      <c r="B46" s="123" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="120" t="s">
+        <v>982</v>
+      </c>
+      <c r="B47" s="124" t="s">
         <v>983</v>
       </c>
-      <c r="B47" s="124" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="129" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="127" t="s">
-        <v>985</v>
-      </c>
-      <c r="B48" s="128"/>
+      <c r="B48" s="130"/>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="120" t="s">
+        <v>985</v>
+      </c>
+      <c r="B49" s="76" t="s">
         <v>986</v>
-      </c>
-      <c r="B49" s="76" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="120" t="s">
+        <v>987</v>
+      </c>
+      <c r="B50" s="122" t="s">
         <v>988</v>
       </c>
-      <c r="B50" s="122" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="129" t="s">
         <v>989</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="127" t="s">
-        <v>990</v>
-      </c>
-      <c r="B51" s="128"/>
+      <c r="B51" s="130"/>
     </row>
     <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="120" t="s">
+        <v>990</v>
+      </c>
+      <c r="B52" s="58" t="s">
         <v>991</v>
-      </c>
-      <c r="B52" s="58" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="120" t="s">
+        <v>992</v>
+      </c>
+      <c r="B53" s="76" t="s">
         <v>993</v>
       </c>
-      <c r="B53" s="76" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="129" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="127" t="s">
-        <v>995</v>
-      </c>
-      <c r="B54" s="128"/>
+      <c r="B54" s="130"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="120" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B55" s="58"/>
     </row>
     <row r="56" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="120" t="s">
+        <v>996</v>
+      </c>
+      <c r="B56" s="76" t="s">
         <v>997</v>
-      </c>
-      <c r="B56" s="76" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -13966,10 +13966,10 @@
       <c r="B57" s="58"/>
     </row>
     <row r="58" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="129" t="s">
+      <c r="A58" s="125" t="s">
         <v>854</v>
       </c>
-      <c r="B58" s="129"/>
+      <c r="B58" s="125"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="112" t="s">
@@ -13997,15 +13997,15 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="112" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B63" s="87" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="112" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B64" s="87"/>
     </row>
@@ -14022,7 +14022,7 @@
         <v>859</v>
       </c>
       <c r="B66" s="76" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -14052,10 +14052,10 @@
       <c r="B70" s="58"/>
     </row>
     <row r="71" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="130" t="s">
+      <c r="A71" s="126" t="s">
         <v>867</v>
       </c>
-      <c r="B71" s="130"/>
+      <c r="B71" s="126"/>
     </row>
     <row r="72" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="111" t="s">
@@ -14066,7 +14066,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="125" t="s">
+      <c r="A73" s="127" t="s">
         <v>870</v>
       </c>
       <c r="B73" s="58" t="s">
@@ -14074,25 +14074,25 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="125"/>
+      <c r="A74" s="127"/>
       <c r="B74" s="58" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="125"/>
+      <c r="A75" s="127"/>
       <c r="B75" s="58" t="s">
         <v>873</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="125"/>
+      <c r="A76" s="127"/>
       <c r="B76" s="58" t="s">
         <v>874</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="125"/>
+      <c r="A77" s="127"/>
       <c r="B77" s="58" t="s">
         <v>875</v>
       </c>
@@ -14102,16 +14102,16 @@
       <c r="B78" s="58"/>
     </row>
     <row r="79" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="126" t="s">
+      <c r="A79" s="128" t="s">
         <v>876</v>
       </c>
-      <c r="B79" s="126"/>
+      <c r="B79" s="128"/>
     </row>
     <row r="80" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="130" t="s">
+      <c r="A80" s="126" t="s">
         <v>878</v>
       </c>
-      <c r="B80" s="130"/>
+      <c r="B80" s="126"/>
     </row>
     <row r="81" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" s="112" t="s">
@@ -14130,10 +14130,10 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="130" t="s">
+      <c r="A83" s="126" t="s">
         <v>882</v>
       </c>
-      <c r="B83" s="130"/>
+      <c r="B83" s="126"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="112" t="s">
@@ -14171,10 +14171,10 @@
       <c r="B89" s="58"/>
     </row>
     <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="130" t="s">
+      <c r="A90" s="126" t="s">
         <v>888</v>
       </c>
-      <c r="B90" s="130"/>
+      <c r="B90" s="126"/>
     </row>
     <row r="91" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A91" s="112" t="s">
@@ -14197,10 +14197,10 @@
       <c r="B93" s="58"/>
     </row>
     <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="130" t="s">
+      <c r="A94" s="126" t="s">
         <v>892</v>
       </c>
-      <c r="B94" s="130"/>
+      <c r="B94" s="126"/>
     </row>
     <row r="95" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A95" s="112"/>
@@ -14213,10 +14213,10 @@
       <c r="B96" s="58"/>
     </row>
     <row r="97" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="130" t="s">
+      <c r="A97" s="126" t="s">
         <v>894</v>
       </c>
-      <c r="B97" s="130"/>
+      <c r="B97" s="126"/>
     </row>
     <row r="98" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="111" t="s">
@@ -14231,25 +14231,25 @@
       <c r="B99" s="58"/>
     </row>
     <row r="100" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="130" t="s">
+      <c r="A100" s="126" t="s">
         <v>897</v>
       </c>
-      <c r="B100" s="130"/>
-    </row>
-    <row r="101" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B100" s="126"/>
+    </row>
+    <row r="101" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="111" t="s">
         <v>898</v>
       </c>
       <c r="B101" s="76" t="s">
-        <v>899</v>
+        <v>998</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A102" s="111" t="s">
+        <v>899</v>
+      </c>
+      <c r="B102" s="76" t="s">
         <v>900</v>
-      </c>
-      <c r="B102" s="76" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -14257,17 +14257,17 @@
       <c r="B103" s="58"/>
     </row>
     <row r="104" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="130" t="s">
-        <v>902</v>
-      </c>
-      <c r="B104" s="130"/>
+      <c r="A104" s="126" t="s">
+        <v>901</v>
+      </c>
+      <c r="B104" s="126"/>
     </row>
     <row r="105" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A105" s="111" t="s">
+        <v>902</v>
+      </c>
+      <c r="B105" s="76" t="s">
         <v>903</v>
-      </c>
-      <c r="B105" s="76" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -14275,45 +14275,55 @@
       <c r="B106" s="58"/>
     </row>
     <row r="107" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="130" t="s">
-        <v>905</v>
-      </c>
-      <c r="B107" s="130"/>
+      <c r="A107" s="126" t="s">
+        <v>904</v>
+      </c>
+      <c r="B107" s="126"/>
     </row>
     <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="111" t="s">
+        <v>905</v>
+      </c>
+      <c r="B108" s="112" t="s">
         <v>906</v>
-      </c>
-      <c r="B108" s="112" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="111" t="s">
+        <v>907</v>
+      </c>
+      <c r="B109" s="112" t="s">
         <v>908</v>
-      </c>
-      <c r="B109" s="112" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="111" t="s">
+        <v>909</v>
+      </c>
+      <c r="B110" s="112" t="s">
         <v>910</v>
-      </c>
-      <c r="B110" s="112" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="111" t="s">
+        <v>911</v>
+      </c>
+      <c r="B111" s="112" t="s">
         <v>912</v>
-      </c>
-      <c r="B111" s="112" t="s">
-        <v>913</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A71:B71"/>
@@ -14330,16 +14340,6 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1"/>
@@ -14365,16 +14365,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="125" t="s">
         <v>760</v>
       </c>
-      <c r="B1" s="129"/>
+      <c r="B1" s="125"/>
     </row>
     <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="129" t="s">
         <v>757</v>
       </c>
-      <c r="B2" s="128"/>
+      <c r="B2" s="130"/>
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="111" t="s">
@@ -14451,10 +14451,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="130" t="s">
+      <c r="A13" s="126" t="s">
         <v>776</v>
       </c>
-      <c r="B13" s="130"/>
+      <c r="B13" s="126"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="115" t="s">
@@ -14481,10 +14481,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="126" t="s">
         <v>783</v>
       </c>
-      <c r="B17" s="130"/>
+      <c r="B17" s="126"/>
     </row>
     <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="115" t="s">
@@ -14519,10 +14519,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="130" t="s">
+      <c r="A22" s="126" t="s">
         <v>792</v>
       </c>
-      <c r="B22" s="130"/>
+      <c r="B22" s="126"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="115" t="s">
@@ -14541,10 +14541,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="130" t="s">
+      <c r="A25" s="126" t="s">
         <v>797</v>
       </c>
-      <c r="B25" s="130"/>
+      <c r="B25" s="126"/>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="115" t="s">
@@ -14563,10 +14563,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="130" t="s">
+      <c r="A28" s="126" t="s">
         <v>802</v>
       </c>
-      <c r="B28" s="130"/>
+      <c r="B28" s="126"/>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="115" t="s">
@@ -14593,10 +14593,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="130" t="s">
+      <c r="A32" s="126" t="s">
         <v>809</v>
       </c>
-      <c r="B32" s="130"/>
+      <c r="B32" s="126"/>
     </row>
     <row r="33" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
@@ -14605,10 +14605,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="130" t="s">
+      <c r="A34" s="126" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="130"/>
+      <c r="B34" s="126"/>
     </row>
     <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="115" t="s">
@@ -14639,10 +14639,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="130" t="s">
+      <c r="A39" s="126" t="s">
         <v>819</v>
       </c>
-      <c r="B39" s="130"/>
+      <c r="B39" s="126"/>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="116"/>
@@ -14651,10 +14651,10 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="130" t="s">
+      <c r="A41" s="126" t="s">
         <v>821</v>
       </c>
-      <c r="B41" s="130"/>
+      <c r="B41" s="126"/>
     </row>
     <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="131" t="s">
@@ -14703,10 +14703,10 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="130" t="s">
+      <c r="A48" s="126" t="s">
         <v>833</v>
       </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="126"/>
     </row>
     <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="111" t="s">
@@ -14729,10 +14729,10 @@
       <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="130" t="s">
+      <c r="A51" s="126" t="s">
         <v>839</v>
       </c>
-      <c r="B51" s="130"/>
+      <c r="B51" s="126"/>
       <c r="C51" s="35"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14754,10 +14754,10 @@
       <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="130" t="s">
+      <c r="A54" s="126" t="s">
         <v>844</v>
       </c>
-      <c r="B54" s="130"/>
+      <c r="B54" s="126"/>
       <c r="C54" s="35"/>
     </row>
     <row r="55" spans="1:3" ht="195" x14ac:dyDescent="0.25">
@@ -14768,10 +14768,10 @@
       <c r="C55" s="35"/>
     </row>
     <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="130" t="s">
+      <c r="A56" s="126" t="s">
         <v>846</v>
       </c>
-      <c r="B56" s="130"/>
+      <c r="B56" s="126"/>
       <c r="C56" s="35"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14822,6 +14822,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A56:B56"/>
@@ -14832,14 +14840,6 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14870,16 +14870,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="136" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="139"/>
+      <c r="B2" s="146"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="148" t="s">
         <v>501</v>
       </c>
-      <c r="B3" s="140"/>
+      <c r="B3" s="147"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -14906,10 +14906,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="140" t="s">
+      <c r="A7" s="147" t="s">
         <v>513</v>
       </c>
-      <c r="B7" s="138"/>
+      <c r="B7" s="145"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -14936,10 +14936,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="140" t="s">
+      <c r="A11" s="147" t="s">
         <v>515</v>
       </c>
-      <c r="B11" s="138"/>
+      <c r="B11" s="145"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -14950,10 +14950,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140" t="s">
+      <c r="A13" s="147" t="s">
         <v>383</v>
       </c>
-      <c r="B13" s="140"/>
+      <c r="B13" s="147"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -15012,10 +15012,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="140" t="s">
+      <c r="A21" s="147" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="140"/>
+      <c r="B21" s="147"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -15026,10 +15026,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="140" t="s">
+      <c r="A23" s="147" t="s">
         <v>382</v>
       </c>
-      <c r="B23" s="140"/>
+      <c r="B23" s="147"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -15050,10 +15050,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="140" t="s">
+      <c r="A26" s="147" t="s">
         <v>347</v>
       </c>
-      <c r="B26" s="140"/>
+      <c r="B26" s="147"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -15080,10 +15080,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="140" t="s">
+      <c r="A30" s="147" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="140"/>
+      <c r="B30" s="147"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -15110,10 +15110,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="138" t="s">
+      <c r="A34" s="145" t="s">
         <v>357</v>
       </c>
-      <c r="B34" s="138"/>
+      <c r="B34" s="145"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -15140,10 +15140,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="140" t="s">
+      <c r="A38" s="147" t="s">
         <v>354</v>
       </c>
-      <c r="B38" s="140"/>
+      <c r="B38" s="147"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -15170,10 +15170,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="138" t="s">
+      <c r="A42" s="145" t="s">
         <v>358</v>
       </c>
-      <c r="B42" s="138"/>
+      <c r="B42" s="145"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -15192,10 +15192,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="140" t="s">
+      <c r="A45" s="147" t="s">
         <v>508</v>
       </c>
-      <c r="B45" s="138"/>
+      <c r="B45" s="145"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -15222,19 +15222,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="134" t="s">
+      <c r="A49" s="136" t="s">
         <v>368</v>
       </c>
-      <c r="B49" s="134"/>
+      <c r="B49" s="136"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A50" s="137" t="s">
         <v>311</v>
       </c>
-      <c r="B50" s="136"/>
+      <c r="B50" s="135"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="145" t="s">
+      <c r="A51" s="142" t="s">
         <v>319</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -15242,7 +15242,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="146"/>
+      <c r="A52" s="143"/>
       <c r="B52" s="62" t="s">
         <v>586</v>
       </c>
@@ -15251,13 +15251,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="147"/>
+      <c r="A53" s="144"/>
       <c r="B53" s="62" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="145" t="s">
+      <c r="A54" s="142" t="s">
         <v>320</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -15265,25 +15265,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="146"/>
+      <c r="A55" s="143"/>
       <c r="B55" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="146"/>
+      <c r="A56" s="143"/>
       <c r="B56" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="147"/>
+      <c r="A57" s="144"/>
       <c r="B57" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="145" t="s">
+      <c r="A58" s="142" t="s">
         <v>321</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -15291,13 +15291,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="147"/>
+      <c r="A59" s="144"/>
       <c r="B59" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="145" t="s">
+      <c r="A60" s="142" t="s">
         <v>322</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -15308,7 +15308,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="146"/>
+      <c r="A61" s="143"/>
       <c r="B61" s="62" t="s">
         <v>523</v>
       </c>
@@ -15317,14 +15317,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="146"/>
+      <c r="A62" s="143"/>
       <c r="B62" s="62" t="s">
         <v>583</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="147"/>
+      <c r="A63" s="144"/>
       <c r="B63" s="62" t="s">
         <v>324</v>
       </c>
@@ -15378,7 +15378,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="142" t="s">
+      <c r="A70" s="139" t="s">
         <v>289</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -15386,43 +15386,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="143"/>
+      <c r="A71" s="140"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="143"/>
+      <c r="A72" s="140"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="143"/>
+      <c r="A73" s="140"/>
       <c r="B73" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="143"/>
+      <c r="A74" s="140"/>
       <c r="B74" s="62" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="143"/>
+      <c r="A75" s="140"/>
       <c r="B75" s="62" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="144"/>
+      <c r="A76" s="141"/>
       <c r="B76" s="62" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="142" t="s">
+      <c r="A77" s="139" t="s">
         <v>290</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -15430,74 +15430,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="143"/>
+      <c r="A78" s="140"/>
       <c r="B78" s="62" t="s">
         <v>298</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="143"/>
+      <c r="A79" s="140"/>
       <c r="B79" s="62" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="143"/>
+      <c r="A80" s="140"/>
       <c r="B80" s="62" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="143"/>
+      <c r="A81" s="140"/>
       <c r="B81" s="81" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="143"/>
+      <c r="A82" s="140"/>
       <c r="B82" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="143"/>
+      <c r="A83" s="140"/>
       <c r="B83" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="143"/>
+      <c r="A84" s="140"/>
       <c r="B84" s="81" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="143"/>
+      <c r="A85" s="140"/>
       <c r="B85" s="81" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="143"/>
+      <c r="A86" s="140"/>
       <c r="B86" s="81" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="143"/>
+      <c r="A87" s="140"/>
       <c r="B87" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="144"/>
+      <c r="A88" s="141"/>
       <c r="B88" s="81" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="142" t="s">
+      <c r="A89" s="139" t="s">
         <v>291</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -15505,28 +15505,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="143"/>
+      <c r="A90" s="140"/>
       <c r="B90" s="83" t="s">
         <v>306</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="143"/>
+      <c r="A91" s="140"/>
       <c r="B91" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="144"/>
+      <c r="A92" s="141"/>
       <c r="B92" s="82" t="s">
         <v>541</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="142" t="s">
+      <c r="A93" s="139" t="s">
         <v>308</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -15535,7 +15535,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="144"/>
+      <c r="A94" s="141"/>
       <c r="B94" s="84" t="s">
         <v>310</v>
       </c>
@@ -15605,17 +15605,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="134" t="s">
+      <c r="A102" s="136" t="s">
         <v>384</v>
       </c>
-      <c r="B102" s="134"/>
+      <c r="B102" s="136"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A103" s="137" t="s">
         <v>385</v>
       </c>
-      <c r="B103" s="136"/>
+      <c r="B103" s="135"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -15649,7 +15649,7 @@
       <c r="A107" s="137" t="s">
         <v>392</v>
       </c>
-      <c r="B107" s="136"/>
+      <c r="B107" s="135"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -15809,7 +15809,7 @@
       <c r="A125" s="137" t="s">
         <v>423</v>
       </c>
-      <c r="B125" s="136"/>
+      <c r="B125" s="135"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -15897,7 +15897,7 @@
       <c r="A135" s="137" t="s">
         <v>495</v>
       </c>
-      <c r="B135" s="136"/>
+      <c r="B135" s="135"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -15991,10 +15991,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="135" t="s">
+      <c r="A146" s="134" t="s">
         <v>458</v>
       </c>
-      <c r="B146" s="136"/>
+      <c r="B146" s="135"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -16025,10 +16025,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="135" t="s">
+      <c r="A150" s="134" t="s">
         <v>466</v>
       </c>
-      <c r="B150" s="136"/>
+      <c r="B150" s="135"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16050,10 +16050,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="135" t="s">
+      <c r="A153" s="134" t="s">
         <v>536</v>
       </c>
-      <c r="B153" s="136"/>
+      <c r="B153" s="135"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -16095,17 +16095,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="134" t="s">
+      <c r="A158" s="136" t="s">
         <v>468</v>
       </c>
-      <c r="B158" s="134"/>
+      <c r="B158" s="136"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A159" s="137" t="s">
         <v>471</v>
       </c>
-      <c r="B159" s="136"/>
+      <c r="B159" s="135"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -16141,10 +16141,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="135" t="s">
+      <c r="A165" s="134" t="s">
         <v>474</v>
       </c>
-      <c r="B165" s="148"/>
+      <c r="B165" s="138"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -16214,7 +16214,7 @@
       <c r="A173" s="137" t="s">
         <v>469</v>
       </c>
-      <c r="B173" s="136"/>
+      <c r="B173" s="135"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -16239,7 +16239,7 @@
       <c r="A176" s="137" t="s">
         <v>470</v>
       </c>
-      <c r="B176" s="136"/>
+      <c r="B176" s="135"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -16261,17 +16261,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="134" t="s">
+      <c r="A179" s="136" t="s">
         <v>547</v>
       </c>
-      <c r="B179" s="134"/>
+      <c r="B179" s="136"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A180" s="137" t="s">
         <v>548</v>
       </c>
-      <c r="B180" s="136"/>
+      <c r="B180" s="135"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16290,7 +16290,7 @@
       <c r="A183" s="137" t="s">
         <v>547</v>
       </c>
-      <c r="B183" s="136"/>
+      <c r="B183" s="135"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16374,7 +16374,7 @@
       <c r="A193" s="137" t="s">
         <v>570</v>
       </c>
-      <c r="B193" s="136"/>
+      <c r="B193" s="135"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16392,10 +16392,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="135" t="s">
+      <c r="A196" s="134" t="s">
         <v>574</v>
       </c>
-      <c r="B196" s="136"/>
+      <c r="B196" s="135"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -16430,17 +16430,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="134" t="s">
+      <c r="A201" s="136" t="s">
         <v>595</v>
       </c>
-      <c r="B201" s="134"/>
+      <c r="B201" s="136"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="135" t="s">
+      <c r="A202" s="134" t="s">
         <v>597</v>
       </c>
-      <c r="B202" s="136"/>
+      <c r="B202" s="135"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -16487,10 +16487,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="135" t="s">
+      <c r="A209" s="134" t="s">
         <v>608</v>
       </c>
-      <c r="B209" s="136"/>
+      <c r="B209" s="135"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -16505,10 +16505,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="135" t="s">
+      <c r="A212" s="134" t="s">
         <v>610</v>
       </c>
-      <c r="B212" s="136"/>
+      <c r="B212" s="135"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -16519,10 +16519,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="135" t="s">
+      <c r="A214" s="134" t="s">
         <v>614</v>
       </c>
-      <c r="B214" s="136"/>
+      <c r="B214" s="135"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -16541,10 +16541,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="135" t="s">
+      <c r="A217" s="134" t="s">
         <v>613</v>
       </c>
-      <c r="B217" s="136"/>
+      <c r="B217" s="135"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -16579,22 +16579,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="134" t="s">
+      <c r="A222" s="136" t="s">
         <v>629</v>
       </c>
-      <c r="B222" s="134"/>
+      <c r="B222" s="136"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="135" t="s">
+      <c r="A223" s="134" t="s">
         <v>631</v>
       </c>
-      <c r="B223" s="136"/>
+      <c r="B223" s="135"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="135" t="s">
+      <c r="A224" s="134" t="s">
         <v>630</v>
       </c>
-      <c r="B224" s="136"/>
+      <c r="B224" s="135"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -16605,10 +16605,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="135" t="s">
+      <c r="A226" s="134" t="s">
         <v>634</v>
       </c>
-      <c r="B226" s="136"/>
+      <c r="B226" s="135"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -16651,10 +16651,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="135" t="s">
+      <c r="A232" s="134" t="s">
         <v>644</v>
       </c>
-      <c r="B232" s="136"/>
+      <c r="B232" s="135"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -16665,10 +16665,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="135" t="s">
+      <c r="A234" s="134" t="s">
         <v>647</v>
       </c>
-      <c r="B234" s="136"/>
+      <c r="B234" s="135"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -16685,10 +16685,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="135" t="s">
+      <c r="A237" s="134" t="s">
         <v>651</v>
       </c>
-      <c r="B237" s="136"/>
+      <c r="B237" s="135"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -16835,10 +16835,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="135" t="s">
+      <c r="A256" s="134" t="s">
         <v>688</v>
       </c>
-      <c r="B256" s="136"/>
+      <c r="B256" s="135"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -16865,10 +16865,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="135" t="s">
+      <c r="A260" s="134" t="s">
         <v>696</v>
       </c>
-      <c r="B260" s="136"/>
+      <c r="B260" s="135"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -16879,16 +16879,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="134" t="s">
+      <c r="A262" s="136" t="s">
         <v>699</v>
       </c>
-      <c r="B262" s="134"/>
+      <c r="B262" s="136"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="135" t="s">
+      <c r="A263" s="134" t="s">
         <v>700</v>
       </c>
-      <c r="B263" s="136"/>
+      <c r="B263" s="135"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -16923,10 +16923,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="135" t="s">
+      <c r="A268" s="134" t="s">
         <v>709</v>
       </c>
-      <c r="B268" s="136"/>
+      <c r="B268" s="135"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -16961,10 +16961,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="135" t="s">
+      <c r="A273" s="134" t="s">
         <v>701</v>
       </c>
-      <c r="B273" s="136"/>
+      <c r="B273" s="135"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -17021,10 +17021,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="135" t="s">
+      <c r="A280" s="134" t="s">
         <v>730</v>
       </c>
-      <c r="B280" s="136"/>
+      <c r="B280" s="135"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -17080,39 +17080,18 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -17129,18 +17108,39 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17183,7 +17183,7 @@
         <v>143</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C3" t="s">
         <v>197</v>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework -05.Entity-Relations - Complete
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -13610,8 +13610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DB EF - Database - Advanced-Querying
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="1010">
   <si>
     <t>Операция</t>
   </si>
@@ -9378,17 +9378,64 @@
   <si>
     <t>public DbSet&lt;Employee&gt; Employees { get; set; }</t>
   </si>
+  <si>
+    <t>ENUM PARSE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var bookTitles = context
+                .Books
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                .Where(b =&gt; b.AgeRestriction.ToString().ToLower() == command.ToLower())</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                .OrderBy(b=&gt;b.Title)
+                .Select(b =&gt; b.Title)
+                .ToList();</t>
+    </r>
+  </si>
+  <si>
+    <t>Парсване на enum в заявка</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="61" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="62" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10239,42 +10286,42 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10289,91 +10336,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10388,73 +10435,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10463,49 +10510,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10517,168 +10564,168 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="59" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -10773,7 +10820,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -10781,17 +10828,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -10845,7 +10881,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10880,7 +10916,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11091,8 +11127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C394"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -11356,10 +11392,16 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+    <row r="24" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>1008</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
@@ -13610,8 +13652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13622,10 +13664,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="128" t="s">
         <v>917</v>
       </c>
-      <c r="B1" s="125"/>
+      <c r="B1" s="128"/>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
@@ -13658,10 +13700,10 @@
       <c r="B5" s="58"/>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="129" t="s">
+      <c r="A6" s="126" t="s">
         <v>919</v>
       </c>
-      <c r="B6" s="130"/>
+      <c r="B6" s="127"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
@@ -13700,10 +13742,10 @@
       <c r="B12" s="58"/>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="126" t="s">
         <v>926</v>
       </c>
-      <c r="B13" s="130"/>
+      <c r="B13" s="127"/>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="112" t="s">
@@ -13714,10 +13756,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="126" t="s">
         <v>853</v>
       </c>
-      <c r="B15" s="130"/>
+      <c r="B15" s="127"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="121" t="s">
@@ -13742,10 +13784,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="126" t="s">
         <v>934</v>
       </c>
-      <c r="B19" s="130"/>
+      <c r="B19" s="127"/>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="118" t="s">
@@ -13780,16 +13822,16 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="129" t="s">
+      <c r="A24" s="126" t="s">
         <v>943</v>
       </c>
-      <c r="B24" s="130"/>
+      <c r="B24" s="127"/>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="129" t="s">
+      <c r="A25" s="126" t="s">
         <v>887</v>
       </c>
-      <c r="B25" s="130"/>
+      <c r="B25" s="127"/>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="120" t="s">
@@ -13800,10 +13842,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="129" t="s">
+      <c r="A27" s="126" t="s">
         <v>949</v>
       </c>
-      <c r="B27" s="130"/>
+      <c r="B27" s="127"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="112" t="s">
@@ -13828,10 +13870,10 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="129" t="s">
+      <c r="A31" s="126" t="s">
         <v>949</v>
       </c>
-      <c r="B31" s="130"/>
+      <c r="B31" s="127"/>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="120" t="s">
@@ -13872,10 +13914,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="129" t="s">
+      <c r="A36" s="126" t="s">
         <v>962</v>
       </c>
-      <c r="B36" s="130"/>
+      <c r="B36" s="127"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="120" t="s">
@@ -13942,10 +13984,10 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="129" t="s">
+      <c r="A45" s="126" t="s">
         <v>962</v>
       </c>
-      <c r="B45" s="130"/>
+      <c r="B45" s="127"/>
     </row>
     <row r="46" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="120" t="s">
@@ -13964,10 +14006,10 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="129" t="s">
+      <c r="A48" s="126" t="s">
         <v>983</v>
       </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="127"/>
     </row>
     <row r="49" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="120" t="s">
@@ -13986,10 +14028,10 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="129" t="s">
+      <c r="A51" s="126" t="s">
         <v>988</v>
       </c>
-      <c r="B51" s="130"/>
+      <c r="B51" s="127"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="120" t="s">
@@ -14008,10 +14050,10 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="129" t="s">
+      <c r="A54" s="126" t="s">
         <v>993</v>
       </c>
-      <c r="B54" s="130"/>
+      <c r="B54" s="127"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="120" t="s">
@@ -14032,10 +14074,10 @@
       <c r="B57" s="58"/>
     </row>
     <row r="58" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="125" t="s">
+      <c r="A58" s="128" t="s">
         <v>854</v>
       </c>
-      <c r="B58" s="125"/>
+      <c r="B58" s="128"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="112" t="s">
@@ -14099,7 +14141,7 @@
       <c r="B66" s="76" t="s">
         <v>914</v>
       </c>
-      <c r="C66" s="153" t="s">
+      <c r="C66" s="125" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -14142,10 +14184,10 @@
       <c r="B71" s="58"/>
     </row>
     <row r="72" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="126" t="s">
+      <c r="A72" s="129" t="s">
         <v>866</v>
       </c>
-      <c r="B72" s="126"/>
+      <c r="B72" s="129"/>
     </row>
     <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="111" t="s">
@@ -14156,7 +14198,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="127" t="s">
+      <c r="A74" s="130" t="s">
         <v>869</v>
       </c>
       <c r="B74" s="58" t="s">
@@ -14164,25 +14206,25 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="127"/>
+      <c r="A75" s="130"/>
       <c r="B75" s="58" t="s">
         <v>871</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="127"/>
+      <c r="A76" s="130"/>
       <c r="B76" s="58" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="127"/>
+      <c r="A77" s="130"/>
       <c r="B77" s="58" t="s">
         <v>873</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="127"/>
+      <c r="A78" s="130"/>
       <c r="B78" s="58" t="s">
         <v>874</v>
       </c>
@@ -14192,16 +14234,16 @@
       <c r="B79" s="58"/>
     </row>
     <row r="80" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="128" t="s">
+      <c r="A80" s="131" t="s">
         <v>875</v>
       </c>
-      <c r="B80" s="128"/>
+      <c r="B80" s="131"/>
     </row>
     <row r="81" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="126" t="s">
+      <c r="A81" s="129" t="s">
         <v>877</v>
       </c>
-      <c r="B81" s="126"/>
+      <c r="B81" s="129"/>
     </row>
     <row r="82" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="112" t="s">
@@ -14220,10 +14262,10 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="126" t="s">
+      <c r="A84" s="129" t="s">
         <v>881</v>
       </c>
-      <c r="B84" s="126"/>
+      <c r="B84" s="129"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="112" t="s">
@@ -14261,10 +14303,10 @@
       <c r="B90" s="58"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="126" t="s">
+      <c r="A91" s="129" t="s">
         <v>887</v>
       </c>
-      <c r="B91" s="126"/>
+      <c r="B91" s="129"/>
     </row>
     <row r="92" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="112" t="s">
@@ -14287,10 +14329,10 @@
       <c r="B94" s="58"/>
     </row>
     <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="126" t="s">
+      <c r="A95" s="129" t="s">
         <v>891</v>
       </c>
-      <c r="B95" s="126"/>
+      <c r="B95" s="129"/>
     </row>
     <row r="96" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A96" s="112"/>
@@ -14303,10 +14345,10 @@
       <c r="B97" s="58"/>
     </row>
     <row r="98" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="126" t="s">
+      <c r="A98" s="129" t="s">
         <v>893</v>
       </c>
-      <c r="B98" s="126"/>
+      <c r="B98" s="129"/>
     </row>
     <row r="99" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="111" t="s">
@@ -14321,10 +14363,10 @@
       <c r="B100" s="58"/>
     </row>
     <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="126" t="s">
+      <c r="A101" s="129" t="s">
         <v>896</v>
       </c>
-      <c r="B101" s="126"/>
+      <c r="B101" s="129"/>
     </row>
     <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A102" s="111" t="s">
@@ -14347,10 +14389,10 @@
       <c r="B104" s="58"/>
     </row>
     <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="126" t="s">
+      <c r="A105" s="129" t="s">
         <v>900</v>
       </c>
-      <c r="B105" s="126"/>
+      <c r="B105" s="129"/>
     </row>
     <row r="106" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A106" s="111" t="s">
@@ -14365,10 +14407,10 @@
       <c r="B107" s="58"/>
     </row>
     <row r="108" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="126" t="s">
+      <c r="A108" s="129" t="s">
         <v>903</v>
       </c>
-      <c r="B108" s="126"/>
+      <c r="B108" s="129"/>
     </row>
     <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="111" t="s">
@@ -14404,16 +14446,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A72:B72"/>
@@ -14430,6 +14462,16 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A45:B45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1"/>
@@ -14455,16 +14497,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="128" t="s">
         <v>760</v>
       </c>
-      <c r="B1" s="125"/>
+      <c r="B1" s="128"/>
     </row>
     <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="126" t="s">
         <v>757</v>
       </c>
-      <c r="B2" s="130"/>
+      <c r="B2" s="127"/>
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="111" t="s">
@@ -14483,7 +14525,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="131" t="s">
+      <c r="A5" s="132" t="s">
         <v>763</v>
       </c>
       <c r="B5" s="114" t="s">
@@ -14491,19 +14533,19 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="132"/>
+      <c r="A6" s="133"/>
       <c r="B6" s="114" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="132"/>
+      <c r="A7" s="133"/>
       <c r="B7" s="114" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="133"/>
+      <c r="A8" s="134"/>
       <c r="B8" s="114" t="s">
         <v>767</v>
       </c>
@@ -14541,10 +14583,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="129" t="s">
         <v>776</v>
       </c>
-      <c r="B13" s="126"/>
+      <c r="B13" s="129"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="115" t="s">
@@ -14571,10 +14613,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="129" t="s">
         <v>783</v>
       </c>
-      <c r="B17" s="126"/>
+      <c r="B17" s="129"/>
     </row>
     <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="115" t="s">
@@ -14609,10 +14651,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="126" t="s">
+      <c r="A22" s="129" t="s">
         <v>792</v>
       </c>
-      <c r="B22" s="126"/>
+      <c r="B22" s="129"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="115" t="s">
@@ -14631,10 +14673,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="126" t="s">
+      <c r="A25" s="129" t="s">
         <v>797</v>
       </c>
-      <c r="B25" s="126"/>
+      <c r="B25" s="129"/>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="115" t="s">
@@ -14653,10 +14695,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="126" t="s">
+      <c r="A28" s="129" t="s">
         <v>802</v>
       </c>
-      <c r="B28" s="126"/>
+      <c r="B28" s="129"/>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="115" t="s">
@@ -14683,10 +14725,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="126" t="s">
+      <c r="A32" s="129" t="s">
         <v>809</v>
       </c>
-      <c r="B32" s="126"/>
+      <c r="B32" s="129"/>
     </row>
     <row r="33" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
@@ -14695,10 +14737,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="126" t="s">
+      <c r="A34" s="129" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="126"/>
+      <c r="B34" s="129"/>
     </row>
     <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="115" t="s">
@@ -14709,7 +14751,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="131" t="s">
+      <c r="A36" s="132" t="s">
         <v>814</v>
       </c>
       <c r="B36" s="112" t="s">
@@ -14717,22 +14759,22 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="132"/>
+      <c r="A37" s="133"/>
       <c r="B37" s="112" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="133"/>
+      <c r="A38" s="134"/>
       <c r="B38" s="112" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="126" t="s">
+      <c r="A39" s="129" t="s">
         <v>819</v>
       </c>
-      <c r="B39" s="126"/>
+      <c r="B39" s="129"/>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="116"/>
@@ -14741,13 +14783,13 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="126" t="s">
+      <c r="A41" s="129" t="s">
         <v>821</v>
       </c>
-      <c r="B41" s="126"/>
+      <c r="B41" s="129"/>
     </row>
     <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A42" s="131" t="s">
+      <c r="A42" s="132" t="s">
         <v>822</v>
       </c>
       <c r="B42" s="112" t="s">
@@ -14755,7 +14797,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A43" s="133"/>
+      <c r="A43" s="134"/>
       <c r="B43" s="112" t="s">
         <v>825</v>
       </c>
@@ -14793,10 +14835,10 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="126" t="s">
+      <c r="A48" s="129" t="s">
         <v>833</v>
       </c>
-      <c r="B48" s="126"/>
+      <c r="B48" s="129"/>
     </row>
     <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="111" t="s">
@@ -14819,10 +14861,10 @@
       <c r="C50" s="35"/>
     </row>
     <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="126" t="s">
+      <c r="A51" s="129" t="s">
         <v>839</v>
       </c>
-      <c r="B51" s="126"/>
+      <c r="B51" s="129"/>
       <c r="C51" s="35"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14844,10 +14886,10 @@
       <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="126" t="s">
+      <c r="A54" s="129" t="s">
         <v>844</v>
       </c>
-      <c r="B54" s="126"/>
+      <c r="B54" s="129"/>
       <c r="C54" s="35"/>
     </row>
     <row r="55" spans="1:3" ht="195" x14ac:dyDescent="0.25">
@@ -14858,10 +14900,10 @@
       <c r="C55" s="35"/>
     </row>
     <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="126" t="s">
+      <c r="A56" s="129" t="s">
         <v>846</v>
       </c>
-      <c r="B56" s="126"/>
+      <c r="B56" s="129"/>
       <c r="C56" s="35"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14912,14 +14954,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A56:B56"/>
@@ -14930,6 +14964,14 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14960,16 +15002,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="135" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="140"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="142" t="s">
         <v>501</v>
       </c>
-      <c r="B3" s="147"/>
+      <c r="B3" s="141"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -14996,10 +15038,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="141" t="s">
         <v>513</v>
       </c>
-      <c r="B7" s="145"/>
+      <c r="B7" s="139"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
@@ -15026,10 +15068,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="147" t="s">
+      <c r="A11" s="141" t="s">
         <v>515</v>
       </c>
-      <c r="B11" s="145"/>
+      <c r="B11" s="139"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
@@ -15040,10 +15082,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="147" t="s">
+      <c r="A13" s="141" t="s">
         <v>383</v>
       </c>
-      <c r="B13" s="147"/>
+      <c r="B13" s="141"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
@@ -15102,10 +15144,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="147" t="s">
+      <c r="A21" s="141" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="147"/>
+      <c r="B21" s="141"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
@@ -15116,10 +15158,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="147" t="s">
+      <c r="A23" s="141" t="s">
         <v>382</v>
       </c>
-      <c r="B23" s="147"/>
+      <c r="B23" s="141"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
@@ -15140,10 +15182,10 @@
       <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="141" t="s">
         <v>347</v>
       </c>
-      <c r="B26" s="147"/>
+      <c r="B26" s="141"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
@@ -15170,10 +15212,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="147" t="s">
+      <c r="A30" s="141" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="147"/>
+      <c r="B30" s="141"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
@@ -15200,10 +15242,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="145" t="s">
+      <c r="A34" s="139" t="s">
         <v>357</v>
       </c>
-      <c r="B34" s="145"/>
+      <c r="B34" s="139"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="72" t="s">
@@ -15230,10 +15272,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="147" t="s">
+      <c r="A38" s="141" t="s">
         <v>354</v>
       </c>
-      <c r="B38" s="147"/>
+      <c r="B38" s="141"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="72" t="s">
@@ -15260,10 +15302,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="145" t="s">
+      <c r="A42" s="139" t="s">
         <v>358</v>
       </c>
-      <c r="B42" s="145"/>
+      <c r="B42" s="139"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
@@ -15282,10 +15324,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="147" t="s">
+      <c r="A45" s="141" t="s">
         <v>508</v>
       </c>
-      <c r="B45" s="145"/>
+      <c r="B45" s="139"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -15312,19 +15354,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="136" t="s">
+      <c r="A49" s="135" t="s">
         <v>368</v>
       </c>
-      <c r="B49" s="136"/>
+      <c r="B49" s="135"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="137" t="s">
+      <c r="A50" s="138" t="s">
         <v>311</v>
       </c>
-      <c r="B50" s="135"/>
+      <c r="B50" s="137"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="142" t="s">
+      <c r="A51" s="146" t="s">
         <v>319</v>
       </c>
       <c r="B51" s="62" t="s">
@@ -15332,7 +15374,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="143"/>
+      <c r="A52" s="147"/>
       <c r="B52" s="62" t="s">
         <v>586</v>
       </c>
@@ -15341,13 +15383,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="144"/>
+      <c r="A53" s="148"/>
       <c r="B53" s="62" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="142" t="s">
+      <c r="A54" s="146" t="s">
         <v>320</v>
       </c>
       <c r="B54" s="62" t="s">
@@ -15355,25 +15397,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="143"/>
+      <c r="A55" s="147"/>
       <c r="B55" s="62" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="143"/>
+      <c r="A56" s="147"/>
       <c r="B56" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="144"/>
+      <c r="A57" s="148"/>
       <c r="B57" s="62" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="142" t="s">
+      <c r="A58" s="146" t="s">
         <v>321</v>
       </c>
       <c r="B58" s="62" t="s">
@@ -15381,13 +15423,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="144"/>
+      <c r="A59" s="148"/>
       <c r="B59" s="62" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="142" t="s">
+      <c r="A60" s="146" t="s">
         <v>322</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -15398,7 +15440,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="143"/>
+      <c r="A61" s="147"/>
       <c r="B61" s="62" t="s">
         <v>523</v>
       </c>
@@ -15407,14 +15449,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="143"/>
+      <c r="A62" s="147"/>
       <c r="B62" s="62" t="s">
         <v>583</v>
       </c>
       <c r="C62" s="68"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="144"/>
+      <c r="A63" s="148"/>
       <c r="B63" s="62" t="s">
         <v>324</v>
       </c>
@@ -15468,7 +15510,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="139" t="s">
+      <c r="A70" s="143" t="s">
         <v>289</v>
       </c>
       <c r="B70" s="62" t="s">
@@ -15476,43 +15518,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="140"/>
+      <c r="A71" s="144"/>
       <c r="B71" s="62" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="140"/>
+      <c r="A72" s="144"/>
       <c r="B72" s="62" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="140"/>
+      <c r="A73" s="144"/>
       <c r="B73" s="62" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="140"/>
+      <c r="A74" s="144"/>
       <c r="B74" s="62" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="140"/>
+      <c r="A75" s="144"/>
       <c r="B75" s="62" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="141"/>
+      <c r="A76" s="145"/>
       <c r="B76" s="62" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="139" t="s">
+      <c r="A77" s="143" t="s">
         <v>290</v>
       </c>
       <c r="B77" s="62" t="s">
@@ -15520,74 +15562,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="140"/>
+      <c r="A78" s="144"/>
       <c r="B78" s="62" t="s">
         <v>298</v>
       </c>
       <c r="C78" s="67"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="140"/>
+      <c r="A79" s="144"/>
       <c r="B79" s="62" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="140"/>
+      <c r="A80" s="144"/>
       <c r="B80" s="62" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="140"/>
+      <c r="A81" s="144"/>
       <c r="B81" s="81" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="140"/>
+      <c r="A82" s="144"/>
       <c r="B82" s="81" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="140"/>
+      <c r="A83" s="144"/>
       <c r="B83" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="140"/>
+      <c r="A84" s="144"/>
       <c r="B84" s="81" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="140"/>
+      <c r="A85" s="144"/>
       <c r="B85" s="81" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="140"/>
+      <c r="A86" s="144"/>
       <c r="B86" s="81" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="140"/>
+      <c r="A87" s="144"/>
       <c r="B87" s="81" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="141"/>
+      <c r="A88" s="145"/>
       <c r="B88" s="81" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="139" t="s">
+      <c r="A89" s="143" t="s">
         <v>291</v>
       </c>
       <c r="B89" s="82" t="s">
@@ -15595,28 +15637,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="140"/>
+      <c r="A90" s="144"/>
       <c r="B90" s="83" t="s">
         <v>306</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="140"/>
+      <c r="A91" s="144"/>
       <c r="B91" s="83" t="s">
         <v>307</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="141"/>
+      <c r="A92" s="145"/>
       <c r="B92" s="82" t="s">
         <v>541</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="139" t="s">
+      <c r="A93" s="143" t="s">
         <v>308</v>
       </c>
       <c r="B93" s="84" t="s">
@@ -15625,7 +15667,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="141"/>
+      <c r="A94" s="145"/>
       <c r="B94" s="84" t="s">
         <v>310</v>
       </c>
@@ -15695,17 +15737,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="136" t="s">
+      <c r="A102" s="135" t="s">
         <v>384</v>
       </c>
-      <c r="B102" s="136"/>
+      <c r="B102" s="135"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="137" t="s">
+      <c r="A103" s="138" t="s">
         <v>385</v>
       </c>
-      <c r="B103" s="135"/>
+      <c r="B103" s="137"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -15736,10 +15778,10 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="137" t="s">
+      <c r="A107" s="138" t="s">
         <v>392</v>
       </c>
-      <c r="B107" s="135"/>
+      <c r="B107" s="137"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -15896,10 +15938,10 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="137" t="s">
+      <c r="A125" s="138" t="s">
         <v>423</v>
       </c>
-      <c r="B125" s="135"/>
+      <c r="B125" s="137"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -15984,10 +16026,10 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="137" t="s">
+      <c r="A135" s="138" t="s">
         <v>495</v>
       </c>
-      <c r="B135" s="135"/>
+      <c r="B135" s="137"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16081,10 +16123,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="134" t="s">
+      <c r="A146" s="136" t="s">
         <v>458</v>
       </c>
-      <c r="B146" s="135"/>
+      <c r="B146" s="137"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -16115,10 +16157,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="134" t="s">
+      <c r="A150" s="136" t="s">
         <v>466</v>
       </c>
-      <c r="B150" s="135"/>
+      <c r="B150" s="137"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16140,10 +16182,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="134" t="s">
+      <c r="A153" s="136" t="s">
         <v>536</v>
       </c>
-      <c r="B153" s="135"/>
+      <c r="B153" s="137"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -16185,17 +16227,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="136" t="s">
+      <c r="A158" s="135" t="s">
         <v>468</v>
       </c>
-      <c r="B158" s="136"/>
+      <c r="B158" s="135"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="137" t="s">
+      <c r="A159" s="138" t="s">
         <v>471</v>
       </c>
-      <c r="B159" s="135"/>
+      <c r="B159" s="137"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -16231,10 +16273,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="134" t="s">
+      <c r="A165" s="136" t="s">
         <v>474</v>
       </c>
-      <c r="B165" s="138"/>
+      <c r="B165" s="149"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -16301,10 +16343,10 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="137" t="s">
+      <c r="A173" s="138" t="s">
         <v>469</v>
       </c>
-      <c r="B173" s="135"/>
+      <c r="B173" s="137"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -16326,10 +16368,10 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="137" t="s">
+      <c r="A176" s="138" t="s">
         <v>470</v>
       </c>
-      <c r="B176" s="135"/>
+      <c r="B176" s="137"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -16351,17 +16393,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="136" t="s">
+      <c r="A179" s="135" t="s">
         <v>547</v>
       </c>
-      <c r="B179" s="136"/>
+      <c r="B179" s="135"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="137" t="s">
+      <c r="A180" s="138" t="s">
         <v>548</v>
       </c>
-      <c r="B180" s="135"/>
+      <c r="B180" s="137"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16377,10 +16419,10 @@
       <c r="B182" s="76"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="137" t="s">
+      <c r="A183" s="138" t="s">
         <v>547</v>
       </c>
-      <c r="B183" s="135"/>
+      <c r="B183" s="137"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16461,10 +16503,10 @@
       <c r="B192" s="76"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="137" t="s">
+      <c r="A193" s="138" t="s">
         <v>570</v>
       </c>
-      <c r="B193" s="135"/>
+      <c r="B193" s="137"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16482,10 +16524,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="134" t="s">
+      <c r="A196" s="136" t="s">
         <v>574</v>
       </c>
-      <c r="B196" s="135"/>
+      <c r="B196" s="137"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="57" t="s">
@@ -16520,17 +16562,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="136" t="s">
+      <c r="A201" s="135" t="s">
         <v>595</v>
       </c>
-      <c r="B201" s="136"/>
+      <c r="B201" s="135"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="134" t="s">
+      <c r="A202" s="136" t="s">
         <v>597</v>
       </c>
-      <c r="B202" s="135"/>
+      <c r="B202" s="137"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="57" t="s">
@@ -16577,10 +16619,10 @@
       <c r="B208" s="97"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="134" t="s">
+      <c r="A209" s="136" t="s">
         <v>608</v>
       </c>
-      <c r="B209" s="135"/>
+      <c r="B209" s="137"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="57" t="s">
@@ -16595,10 +16637,10 @@
       <c r="B211" s="76"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="134" t="s">
+      <c r="A212" s="136" t="s">
         <v>610</v>
       </c>
-      <c r="B212" s="135"/>
+      <c r="B212" s="137"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="72" t="s">
@@ -16609,10 +16651,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="134" t="s">
+      <c r="A214" s="136" t="s">
         <v>614</v>
       </c>
-      <c r="B214" s="135"/>
+      <c r="B214" s="137"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="57" t="s">
@@ -16631,10 +16673,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="134" t="s">
+      <c r="A217" s="136" t="s">
         <v>613</v>
       </c>
-      <c r="B217" s="135"/>
+      <c r="B217" s="137"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="57" t="s">
@@ -16669,22 +16711,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="136" t="s">
+      <c r="A222" s="135" t="s">
         <v>629</v>
       </c>
-      <c r="B222" s="136"/>
+      <c r="B222" s="135"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="134" t="s">
+      <c r="A223" s="136" t="s">
         <v>631</v>
       </c>
-      <c r="B223" s="135"/>
+      <c r="B223" s="137"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="134" t="s">
+      <c r="A224" s="136" t="s">
         <v>630</v>
       </c>
-      <c r="B224" s="135"/>
+      <c r="B224" s="137"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="57" t="s">
@@ -16695,10 +16737,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="134" t="s">
+      <c r="A226" s="136" t="s">
         <v>634</v>
       </c>
-      <c r="B226" s="135"/>
+      <c r="B226" s="137"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="57" t="s">
@@ -16741,10 +16783,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="134" t="s">
+      <c r="A232" s="136" t="s">
         <v>644</v>
       </c>
-      <c r="B232" s="135"/>
+      <c r="B232" s="137"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="57" t="s">
@@ -16755,10 +16797,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="134" t="s">
+      <c r="A234" s="136" t="s">
         <v>647</v>
       </c>
-      <c r="B234" s="135"/>
+      <c r="B234" s="137"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="57" t="s">
@@ -16775,10 +16817,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="134" t="s">
+      <c r="A237" s="136" t="s">
         <v>651</v>
       </c>
-      <c r="B237" s="135"/>
+      <c r="B237" s="137"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="57" t="s">
@@ -16925,10 +16967,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="134" t="s">
+      <c r="A256" s="136" t="s">
         <v>688</v>
       </c>
-      <c r="B256" s="135"/>
+      <c r="B256" s="137"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="57" t="s">
@@ -16955,10 +16997,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="134" t="s">
+      <c r="A260" s="136" t="s">
         <v>696</v>
       </c>
-      <c r="B260" s="135"/>
+      <c r="B260" s="137"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="57" t="s">
@@ -16969,16 +17011,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="136" t="s">
+      <c r="A262" s="135" t="s">
         <v>699</v>
       </c>
-      <c r="B262" s="136"/>
+      <c r="B262" s="135"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="134" t="s">
+      <c r="A263" s="136" t="s">
         <v>700</v>
       </c>
-      <c r="B263" s="135"/>
+      <c r="B263" s="137"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="57" t="s">
@@ -17013,10 +17055,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="134" t="s">
+      <c r="A268" s="136" t="s">
         <v>709</v>
       </c>
-      <c r="B268" s="135"/>
+      <c r="B268" s="137"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="57" t="s">
@@ -17051,10 +17093,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="134" t="s">
+      <c r="A273" s="136" t="s">
         <v>701</v>
       </c>
-      <c r="B273" s="135"/>
+      <c r="B273" s="137"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="57" t="s">
@@ -17111,10 +17153,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="134" t="s">
+      <c r="A280" s="136" t="s">
         <v>730</v>
       </c>
-      <c r="B280" s="135"/>
+      <c r="B280" s="137"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="57" t="s">
@@ -17170,18 +17212,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -17198,39 +17261,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17652,7 +17694,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="150" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -17672,7 +17714,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
+      <c r="A2" s="151"/>
       <c r="B2" s="23" t="s">
         <v>172</v>
       </c>
@@ -17740,10 +17782,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25"/>
-      <c r="B6" s="151" t="s">
+      <c r="B6" s="152" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="152"/>
+      <c r="C6" s="153"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>

</xml_diff>

<commit_message>
DB EF - Database - 11.JSON-Processing
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13740" tabRatio="686" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="C#" sheetId="1" r:id="rId1"/>
@@ -7788,9 +7788,6 @@
     <t>Connecting to SQL Server:</t>
   </si>
   <si>
-    <t>Data Source=(local)\SQLEXPRESS;Initial Catalog=SoftUni;Integrated Security=true;</t>
-  </si>
-  <si>
     <t>SqlConnection con = new SqlConnection(
  @"Server=.;
    Database=SoftUni;
@@ -9801,17 +9798,28 @@
 });</t>
     </r>
   </si>
+  <si>
+    <t>Data Source=.\SQLEXPRESS;Initial Catalog=SoftUni;Integrated Security=true;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="63" x14ac:knownFonts="1">
+  <fonts count="64" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10679,131 +10687,131 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="44" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10818,73 +10826,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10893,49 +10901,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="58" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10947,200 +10955,203 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11542,7 +11553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C394"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -11809,13 +11820,13 @@
     </row>
     <row r="24" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>1007</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -14122,10 +14133,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
-        <v>917</v>
-      </c>
-      <c r="B1" s="122"/>
+      <c r="A1" s="133" t="s">
+        <v>916</v>
+      </c>
+      <c r="B1" s="133"/>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="107" t="s">
@@ -14148,383 +14159,383 @@
         <v>756</v>
       </c>
       <c r="B4" s="110" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="108" t="s">
+        <v>917</v>
+      </c>
+      <c r="B5" s="54"/>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="131" t="s">
         <v>918</v>
       </c>
-      <c r="B5" s="54"/>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="126" t="s">
-        <v>919</v>
-      </c>
-      <c r="B6" s="127"/>
+      <c r="B6" s="132"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="108" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B7" s="54"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="108" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B8" s="54"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B9" s="54"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="108" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B10" s="54"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="108" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B11" s="54"/>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="108" t="s">
+        <v>924</v>
+      </c>
+      <c r="B12" s="54"/>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="131" t="s">
         <v>925</v>
       </c>
-      <c r="B12" s="54"/>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
-        <v>926</v>
-      </c>
-      <c r="B13" s="127"/>
+      <c r="B13" s="132"/>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="108" t="s">
+        <v>926</v>
+      </c>
+      <c r="B14" s="72" t="s">
         <v>927</v>
       </c>
-      <c r="B14" s="72" t="s">
-        <v>928</v>
-      </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="126" t="s">
-        <v>853</v>
-      </c>
-      <c r="B15" s="127"/>
+      <c r="A15" s="131" t="s">
+        <v>852</v>
+      </c>
+      <c r="B15" s="132"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="117" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B16" s="54"/>
     </row>
     <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="114" t="s">
+        <v>929</v>
+      </c>
+      <c r="B17" s="72" t="s">
         <v>930</v>
-      </c>
-      <c r="B17" s="72" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="114" t="s">
+        <v>931</v>
+      </c>
+      <c r="B18" s="72" t="s">
         <v>932</v>
       </c>
-      <c r="B18" s="72" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="131" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="126" t="s">
-        <v>934</v>
-      </c>
-      <c r="B19" s="127"/>
+      <c r="B19" s="132"/>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="114" t="s">
+        <v>934</v>
+      </c>
+      <c r="B20" s="72" t="s">
         <v>935</v>
-      </c>
-      <c r="B20" s="72" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="114" t="s">
+        <v>936</v>
+      </c>
+      <c r="B21" s="72" t="s">
         <v>937</v>
-      </c>
-      <c r="B21" s="72" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="114" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B22" s="72" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="114" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B23" s="72" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="131" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="126" t="s">
-        <v>943</v>
-      </c>
-      <c r="B24" s="127"/>
+      <c r="B24" s="132"/>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="126" t="s">
-        <v>887</v>
-      </c>
-      <c r="B25" s="127"/>
+      <c r="A25" s="131" t="s">
+        <v>886</v>
+      </c>
+      <c r="B25" s="132"/>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="116" t="s">
+        <v>943</v>
+      </c>
+      <c r="B26" s="118" t="s">
         <v>944</v>
       </c>
-      <c r="B26" s="118" t="s">
-        <v>945</v>
-      </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="126" t="s">
-        <v>949</v>
-      </c>
-      <c r="B27" s="127"/>
+      <c r="A27" s="131" t="s">
+        <v>948</v>
+      </c>
+      <c r="B27" s="132"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="108" t="s">
+        <v>945</v>
+      </c>
+      <c r="B28" s="72" t="s">
         <v>946</v>
-      </c>
-      <c r="B28" s="72" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="108" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B29" s="54"/>
     </row>
     <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="108" t="s">
+        <v>949</v>
+      </c>
+      <c r="B30" s="72" t="s">
         <v>950</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="126" t="s">
-        <v>949</v>
-      </c>
-      <c r="B31" s="127"/>
+      <c r="A31" s="131" t="s">
+        <v>948</v>
+      </c>
+      <c r="B31" s="132"/>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="116" t="s">
+        <v>951</v>
+      </c>
+      <c r="B32" s="72" t="s">
         <v>952</v>
-      </c>
-      <c r="B32" s="72" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="116" t="s">
+        <v>953</v>
+      </c>
+      <c r="B33" s="72" t="s">
         <v>954</v>
       </c>
-      <c r="B33" s="72" t="s">
-        <v>955</v>
-      </c>
       <c r="C33" s="31" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="116" t="s">
+        <v>955</v>
+      </c>
+      <c r="B34" s="72" t="s">
         <v>956</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="C34" s="42" t="s">
         <v>957</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="116" t="s">
+        <v>959</v>
+      </c>
+      <c r="B35" s="72" t="s">
         <v>960</v>
       </c>
-      <c r="B35" s="72" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="131" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="126" t="s">
-        <v>962</v>
-      </c>
-      <c r="B36" s="127"/>
+      <c r="B36" s="132"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="116" t="s">
+        <v>962</v>
+      </c>
+      <c r="B37" s="54" t="s">
         <v>963</v>
-      </c>
-      <c r="B37" s="54" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="116" t="s">
+        <v>964</v>
+      </c>
+      <c r="B38" s="72" t="s">
         <v>965</v>
-      </c>
-      <c r="B38" s="72" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="116" t="s">
+        <v>966</v>
+      </c>
+      <c r="B39" s="72" t="s">
         <v>967</v>
-      </c>
-      <c r="B39" s="72" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="116" t="s">
+        <v>968</v>
+      </c>
+      <c r="B40" s="54" t="s">
         <v>969</v>
-      </c>
-      <c r="B40" s="54" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="116" t="s">
+        <v>970</v>
+      </c>
+      <c r="B41" s="54" t="s">
         <v>971</v>
-      </c>
-      <c r="B41" s="54" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="116" t="s">
+        <v>972</v>
+      </c>
+      <c r="B42" s="54" t="s">
         <v>973</v>
-      </c>
-      <c r="B42" s="54" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="116" t="s">
+        <v>974</v>
+      </c>
+      <c r="B43" s="54" t="s">
         <v>975</v>
-      </c>
-      <c r="B43" s="54" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="116" t="s">
+        <v>976</v>
+      </c>
+      <c r="B44" s="54" t="s">
         <v>977</v>
       </c>
-      <c r="B44" s="54" t="s">
-        <v>978</v>
-      </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="126" t="s">
-        <v>962</v>
-      </c>
-      <c r="B45" s="127"/>
+      <c r="A45" s="131" t="s">
+        <v>961</v>
+      </c>
+      <c r="B45" s="132"/>
     </row>
     <row r="46" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="116" t="s">
+        <v>978</v>
+      </c>
+      <c r="B46" s="119" t="s">
         <v>979</v>
-      </c>
-      <c r="B46" s="119" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="116" t="s">
+        <v>980</v>
+      </c>
+      <c r="B47" s="120" t="s">
         <v>981</v>
       </c>
-      <c r="B47" s="120" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="131" t="s">
         <v>982</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="126" t="s">
-        <v>983</v>
-      </c>
-      <c r="B48" s="127"/>
+      <c r="B48" s="132"/>
     </row>
     <row r="49" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="116" t="s">
+        <v>983</v>
+      </c>
+      <c r="B49" s="72" t="s">
         <v>984</v>
-      </c>
-      <c r="B49" s="72" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="116" t="s">
+        <v>985</v>
+      </c>
+      <c r="B50" s="118" t="s">
         <v>986</v>
       </c>
-      <c r="B50" s="118" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="131" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="126" t="s">
-        <v>988</v>
-      </c>
-      <c r="B51" s="127"/>
+      <c r="B51" s="132"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="116" t="s">
+        <v>988</v>
+      </c>
+      <c r="B52" s="54" t="s">
         <v>989</v>
-      </c>
-      <c r="B52" s="54" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="116" t="s">
+        <v>990</v>
+      </c>
+      <c r="B53" s="72" t="s">
         <v>991</v>
       </c>
-      <c r="B53" s="72" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="131" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="126" t="s">
-        <v>993</v>
-      </c>
-      <c r="B54" s="127"/>
+      <c r="B54" s="132"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="116" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B55" s="54"/>
     </row>
     <row r="56" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="116" t="s">
+        <v>994</v>
+      </c>
+      <c r="B56" s="72" t="s">
         <v>995</v>
-      </c>
-      <c r="B56" s="72" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -14532,159 +14543,159 @@
       <c r="B57" s="54"/>
     </row>
     <row r="58" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="122" t="s">
-        <v>854</v>
-      </c>
-      <c r="B58" s="122"/>
+      <c r="A58" s="133" t="s">
+        <v>853</v>
+      </c>
+      <c r="B58" s="133"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="108" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B59" s="54" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="108" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B60" s="54" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="108" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B61" s="54"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="108" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B62" s="54" t="s">
         <v>1005</v>
-      </c>
-      <c r="B62" s="54" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="108" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B63" s="83" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="108" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B64" s="83"/>
     </row>
     <row r="65" spans="1:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="108" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B65" s="72" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="108" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B66" s="72" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C66" s="121" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="108" t="s">
+        <v>863</v>
+      </c>
+      <c r="B67" s="72" t="s">
         <v>864</v>
       </c>
-      <c r="B67" s="72" t="s">
-        <v>865</v>
-      </c>
       <c r="C67" s="46" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="108" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B68" s="72"/>
       <c r="C68" s="46" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="108" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B69" s="54"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="108" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B70" s="54"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="108" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B71" s="54"/>
     </row>
     <row r="72" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="123" t="s">
-        <v>866</v>
-      </c>
-      <c r="B72" s="123"/>
+      <c r="A72" s="134" t="s">
+        <v>865</v>
+      </c>
+      <c r="B72" s="134"/>
     </row>
     <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="107" t="s">
+        <v>866</v>
+      </c>
+      <c r="B73" s="83" t="s">
         <v>867</v>
       </c>
-      <c r="B73" s="83" t="s">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="135" t="s">
         <v>868</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="124" t="s">
+      <c r="B74" s="54" t="s">
         <v>869</v>
       </c>
-      <c r="B74" s="54" t="s">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="135"/>
+      <c r="B75" s="54" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="124"/>
-      <c r="B75" s="54" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="135"/>
+      <c r="B76" s="54" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="124"/>
-      <c r="B76" s="54" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="135"/>
+      <c r="B77" s="54" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="124"/>
-      <c r="B77" s="54" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="135"/>
+      <c r="B78" s="54" t="s">
         <v>873</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="124"/>
-      <c r="B78" s="54" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -14692,60 +14703,60 @@
       <c r="B79" s="54"/>
     </row>
     <row r="80" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="125" t="s">
-        <v>875</v>
-      </c>
-      <c r="B80" s="125"/>
+      <c r="A80" s="136" t="s">
+        <v>874</v>
+      </c>
+      <c r="B80" s="136"/>
     </row>
     <row r="81" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="123" t="s">
-        <v>877</v>
-      </c>
-      <c r="B81" s="123"/>
+      <c r="A81" s="134" t="s">
+        <v>876</v>
+      </c>
+      <c r="B81" s="134"/>
     </row>
     <row r="82" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="108" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B82" s="72" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="108" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B83" s="72" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="134" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="123" t="s">
-        <v>881</v>
-      </c>
-      <c r="B84" s="123"/>
+      <c r="B84" s="134"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="108" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B85" s="54"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="108" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B86" s="54"/>
     </row>
     <row r="87" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="108" t="s">
+        <v>883</v>
+      </c>
+      <c r="B87" s="115" t="s">
+        <v>885</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>884</v>
-      </c>
-      <c r="B87" s="115" t="s">
-        <v>886</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -14761,25 +14772,25 @@
       <c r="B90" s="54"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="123" t="s">
-        <v>887</v>
-      </c>
-      <c r="B91" s="123"/>
+      <c r="A91" s="134" t="s">
+        <v>886</v>
+      </c>
+      <c r="B91" s="134"/>
     </row>
     <row r="92" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="108" t="s">
+        <v>886</v>
+      </c>
+      <c r="B92" s="72" t="s">
         <v>887</v>
-      </c>
-      <c r="B92" s="72" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A93" s="108" t="s">
+        <v>888</v>
+      </c>
+      <c r="B93" s="72" t="s">
         <v>889</v>
-      </c>
-      <c r="B93" s="72" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -14787,15 +14798,15 @@
       <c r="B94" s="54"/>
     </row>
     <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="123" t="s">
-        <v>891</v>
-      </c>
-      <c r="B95" s="123"/>
+      <c r="A95" s="134" t="s">
+        <v>890</v>
+      </c>
+      <c r="B95" s="134"/>
     </row>
     <row r="96" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A96" s="108"/>
       <c r="B96" s="72" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -14803,17 +14814,17 @@
       <c r="B97" s="54"/>
     </row>
     <row r="98" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="123" t="s">
-        <v>893</v>
-      </c>
-      <c r="B98" s="123"/>
+      <c r="A98" s="134" t="s">
+        <v>892</v>
+      </c>
+      <c r="B98" s="134"/>
     </row>
     <row r="99" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="107" t="s">
+        <v>893</v>
+      </c>
+      <c r="B99" s="72" t="s">
         <v>894</v>
-      </c>
-      <c r="B99" s="72" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -14821,25 +14832,25 @@
       <c r="B100" s="54"/>
     </row>
     <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="123" t="s">
-        <v>896</v>
-      </c>
-      <c r="B101" s="123"/>
+      <c r="A101" s="134" t="s">
+        <v>895</v>
+      </c>
+      <c r="B101" s="134"/>
     </row>
     <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A102" s="107" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B102" s="72" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="107" t="s">
+        <v>897</v>
+      </c>
+      <c r="B103" s="72" t="s">
         <v>898</v>
-      </c>
-      <c r="B103" s="72" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -14847,17 +14858,17 @@
       <c r="B104" s="54"/>
     </row>
     <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="123" t="s">
-        <v>900</v>
-      </c>
-      <c r="B105" s="123"/>
+      <c r="A105" s="134" t="s">
+        <v>899</v>
+      </c>
+      <c r="B105" s="134"/>
     </row>
     <row r="106" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A106" s="107" t="s">
+        <v>900</v>
+      </c>
+      <c r="B106" s="72" t="s">
         <v>901</v>
-      </c>
-      <c r="B106" s="72" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -14865,55 +14876,45 @@
       <c r="B107" s="54"/>
     </row>
     <row r="108" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="123" t="s">
-        <v>903</v>
-      </c>
-      <c r="B108" s="123"/>
+      <c r="A108" s="134" t="s">
+        <v>902</v>
+      </c>
+      <c r="B108" s="134"/>
     </row>
     <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="107" t="s">
+        <v>903</v>
+      </c>
+      <c r="B109" s="108" t="s">
         <v>904</v>
-      </c>
-      <c r="B109" s="108" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="107" t="s">
+        <v>905</v>
+      </c>
+      <c r="B110" s="108" t="s">
         <v>906</v>
-      </c>
-      <c r="B110" s="108" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="107" t="s">
+        <v>907</v>
+      </c>
+      <c r="B111" s="108" t="s">
         <v>908</v>
-      </c>
-      <c r="B111" s="108" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="107" t="s">
+        <v>909</v>
+      </c>
+      <c r="B112" s="108" t="s">
         <v>910</v>
-      </c>
-      <c r="B112" s="108" t="s">
-        <v>911</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A72:B72"/>
@@ -14930,6 +14931,16 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A45:B45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1"/>
@@ -14943,7 +14954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -14955,160 +14966,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="137" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1" s="137"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="126" t="s">
         <v>1011</v>
       </c>
-      <c r="B1" s="155"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="156" t="s">
+      <c r="B2" s="72" t="s">
         <v>1012</v>
       </c>
-      <c r="B2" s="72" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="137" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="155" t="s">
+      <c r="B3" s="137"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="127" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B4" s="72" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="126" t="s">
         <v>1014</v>
       </c>
-      <c r="B3" s="155"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="157" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B4" s="72" t="s">
+      <c r="B5" s="72" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="156" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B5" s="72" t="s">
+    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A6" s="137" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A6" s="155" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B6" s="155"/>
+      <c r="B6" s="137"/>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="85" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B7" s="72" t="s">
         <v>1020</v>
       </c>
-      <c r="B7" s="72" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="126" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="156" t="s">
+      <c r="B8" s="72" t="s">
         <v>1022</v>
       </c>
-      <c r="B8" s="72" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="137" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="155" t="s">
+      <c r="B9" s="137"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="127" t="s">
         <v>1024</v>
       </c>
-      <c r="B9" s="155"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="157" t="s">
+      <c r="B10" s="54"/>
+    </row>
+    <row r="11" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A11" s="128" t="s">
         <v>1025</v>
       </c>
-      <c r="B10" s="54"/>
-    </row>
-    <row r="11" spans="1:3" ht="225" x14ac:dyDescent="0.25">
-      <c r="A11" s="158" t="s">
+      <c r="B11" s="76" t="s">
         <v>1026</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="C11" s="38" t="s">
         <v>1027</v>
       </c>
-      <c r="C11" s="38" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="128" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A12" s="158" t="s">
+      <c r="B12" s="72" t="s">
         <v>1029</v>
       </c>
-      <c r="B12" s="72" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A13" s="137" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A13" s="155" t="s">
+      <c r="B13" s="137"/>
+    </row>
+    <row r="14" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" s="138" t="s">
         <v>1031</v>
       </c>
-      <c r="B13" s="155"/>
-    </row>
-    <row r="14" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="159" t="s">
+      <c r="B14" s="129" t="s">
         <v>1032</v>
       </c>
-      <c r="B14" s="160" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A15" s="138"/>
+      <c r="B15" s="129" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="137" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B16" s="137"/>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="138" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A15" s="159"/>
-      <c r="B15" s="160" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A16" s="155" t="s">
+      <c r="B17" s="129" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="138"/>
+      <c r="B18" s="129" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="138"/>
+      <c r="B19" s="127" t="s">
         <v>1042</v>
       </c>
-      <c r="B16" s="155"/>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="159" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B17" s="160" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="160" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A20" s="130" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B20" s="72" t="s">
         <v>1036</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="157" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A20" s="161" t="s">
+    <row r="21" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A21" s="137" t="s">
         <v>1040</v>
       </c>
-      <c r="B20" s="72" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A21" s="155" t="s">
-        <v>1041</v>
-      </c>
-      <c r="B21" s="155"/>
+      <c r="B21" s="137"/>
     </row>
     <row r="22" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B22" s="72" t="s">
         <v>1038</v>
-      </c>
-      <c r="B22" s="72" t="s">
-        <v>1039</v>
       </c>
     </row>
   </sheetData>
@@ -15132,7 +15143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -15144,16 +15155,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="133" t="s">
         <v>760</v>
       </c>
-      <c r="B1" s="122"/>
+      <c r="B1" s="133"/>
     </row>
     <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="131" t="s">
         <v>757</v>
       </c>
-      <c r="B2" s="127"/>
+      <c r="B2" s="132"/>
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="107" t="s">
@@ -15172,7 +15183,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="128" t="s">
+      <c r="A5" s="139" t="s">
         <v>763</v>
       </c>
       <c r="B5" s="110" t="s">
@@ -15180,19 +15191,19 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="129"/>
+      <c r="A6" s="140"/>
       <c r="B6" s="110" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
+      <c r="A7" s="140"/>
       <c r="B7" s="110" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
+      <c r="A8" s="141"/>
       <c r="B8" s="110" t="s">
         <v>767</v>
       </c>
@@ -15230,10 +15241,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="134"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="111" t="s">
@@ -15260,10 +15271,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="123" t="s">
+      <c r="A17" s="134" t="s">
         <v>783</v>
       </c>
-      <c r="B17" s="123"/>
+      <c r="B17" s="134"/>
     </row>
     <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="111" t="s">
@@ -15277,8 +15288,8 @@
       <c r="A19" s="111" t="s">
         <v>786</v>
       </c>
-      <c r="B19" s="110" t="s">
-        <v>788</v>
+      <c r="B19" s="162" t="s">
+        <v>1044</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -15286,297 +15297,297 @@
         <v>787</v>
       </c>
       <c r="B20" s="110" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="111" t="s">
+        <v>789</v>
+      </c>
+      <c r="B21" s="113" t="s">
         <v>790</v>
       </c>
-      <c r="B21" s="113" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="134" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="123" t="s">
-        <v>792</v>
-      </c>
-      <c r="B22" s="123"/>
+      <c r="B22" s="134"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="111" t="s">
+        <v>792</v>
+      </c>
+      <c r="B23" s="110" t="s">
         <v>793</v>
-      </c>
-      <c r="B23" s="110" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="111" t="s">
+        <v>794</v>
+      </c>
+      <c r="B24" s="110" t="s">
         <v>795</v>
       </c>
-      <c r="B24" s="110" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="134" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="123" t="s">
-        <v>797</v>
-      </c>
-      <c r="B25" s="123"/>
+      <c r="B25" s="134"/>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="111" t="s">
+        <v>797</v>
+      </c>
+      <c r="B26" s="110" t="s">
         <v>798</v>
-      </c>
-      <c r="B26" s="110" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="111" t="s">
+        <v>799</v>
+      </c>
+      <c r="B27" s="110" t="s">
         <v>800</v>
       </c>
-      <c r="B27" s="110" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="134" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="123" t="s">
-        <v>802</v>
-      </c>
-      <c r="B28" s="123"/>
+      <c r="B28" s="134"/>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="111" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B29" s="108" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="111" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B30" s="108" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="111" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B31" s="108" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="134" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="123" t="s">
-        <v>809</v>
-      </c>
-      <c r="B32" s="123"/>
+      <c r="B32" s="134"/>
     </row>
     <row r="33" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="111"/>
       <c r="B33" s="108" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="134" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="123" t="s">
-        <v>811</v>
-      </c>
-      <c r="B34" s="123"/>
+      <c r="B34" s="134"/>
     </row>
     <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="111" t="s">
+        <v>811</v>
+      </c>
+      <c r="B35" s="108" t="s">
         <v>812</v>
       </c>
-      <c r="B35" s="108" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="139" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="128" t="s">
+      <c r="B36" s="108" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="140"/>
+      <c r="B37" s="108" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="141"/>
+      <c r="B38" s="108" t="s">
         <v>814</v>
       </c>
-      <c r="B36" s="108" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="129"/>
-      <c r="B37" s="108" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="130"/>
-      <c r="B38" s="108" t="s">
-        <v>815</v>
-      </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="123" t="s">
-        <v>819</v>
-      </c>
-      <c r="B39" s="123"/>
+      <c r="A39" s="134" t="s">
+        <v>818</v>
+      </c>
+      <c r="B39" s="134"/>
     </row>
     <row r="40" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" s="112"/>
       <c r="B40" s="108" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="134" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="123" t="s">
+      <c r="B41" s="134"/>
+    </row>
+    <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A42" s="139" t="s">
         <v>821</v>
       </c>
-      <c r="B41" s="123"/>
-    </row>
-    <row r="42" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A42" s="128" t="s">
-        <v>822</v>
-      </c>
       <c r="B42" s="108" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A43" s="141"/>
+      <c r="B43" s="108" t="s">
         <v>824</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A43" s="130"/>
-      <c r="B43" s="108" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="112" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B44" s="108" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="112" t="s">
+        <v>826</v>
+      </c>
+      <c r="B45" s="108" t="s">
         <v>827</v>
-      </c>
-      <c r="B45" s="108" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="112" t="s">
+        <v>828</v>
+      </c>
+      <c r="B46" s="108" t="s">
         <v>829</v>
-      </c>
-      <c r="B46" s="108" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="111" t="s">
+        <v>830</v>
+      </c>
+      <c r="B47" s="108" t="s">
         <v>831</v>
       </c>
-      <c r="B47" s="108" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="134" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="123" t="s">
-        <v>833</v>
-      </c>
-      <c r="B48" s="123"/>
+      <c r="B48" s="134"/>
     </row>
     <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="107" t="s">
+        <v>833</v>
+      </c>
+      <c r="B49" s="108" t="s">
         <v>834</v>
       </c>
-      <c r="B49" s="108" t="s">
+      <c r="C49" s="31" t="s">
         <v>835</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="107" t="s">
+        <v>836</v>
+      </c>
+      <c r="B50" s="108" t="s">
         <v>837</v>
       </c>
-      <c r="B50" s="108" t="s">
+      <c r="C50" s="31"/>
+    </row>
+    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="134" t="s">
         <v>838</v>
       </c>
-      <c r="C50" s="31"/>
-    </row>
-    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="123" t="s">
-        <v>839</v>
-      </c>
-      <c r="B51" s="123"/>
+      <c r="B51" s="134"/>
       <c r="C51" s="31"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="107" t="s">
+        <v>839</v>
+      </c>
+      <c r="B52" s="108" t="s">
         <v>840</v>
-      </c>
-      <c r="B52" s="108" t="s">
-        <v>841</v>
       </c>
       <c r="C52" s="31"/>
     </row>
     <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="107" t="s">
+        <v>841</v>
+      </c>
+      <c r="B53" s="108" t="s">
         <v>842</v>
       </c>
-      <c r="B53" s="108" t="s">
+      <c r="C53" s="31"/>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="134" t="s">
         <v>843</v>
       </c>
-      <c r="C53" s="31"/>
-    </row>
-    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="123" t="s">
-        <v>844</v>
-      </c>
-      <c r="B54" s="123"/>
+      <c r="B54" s="134"/>
       <c r="C54" s="31"/>
     </row>
     <row r="55" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A55" s="107"/>
       <c r="B55" s="108" t="s">
+        <v>844</v>
+      </c>
+      <c r="C55" s="31"/>
+    </row>
+    <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="134" t="s">
         <v>845</v>
       </c>
-      <c r="C55" s="31"/>
-    </row>
-    <row r="56" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="123" t="s">
-        <v>846</v>
-      </c>
-      <c r="B56" s="123"/>
+      <c r="B56" s="134"/>
       <c r="C56" s="31"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="107" t="s">
+        <v>846</v>
+      </c>
+      <c r="B57" s="108" t="s">
         <v>847</v>
-      </c>
-      <c r="B57" s="108" t="s">
-        <v>848</v>
       </c>
       <c r="C57" s="31"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="107" t="s">
+        <v>848</v>
+      </c>
+      <c r="B58" s="108" t="s">
         <v>849</v>
-      </c>
-      <c r="B58" s="108" t="s">
-        <v>850</v>
       </c>
       <c r="C58" s="31"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="107" t="s">
+        <v>850</v>
+      </c>
+      <c r="B59" s="108" t="s">
         <v>851</v>
-      </c>
-      <c r="B59" s="108" t="s">
-        <v>852</v>
       </c>
       <c r="C59" s="31"/>
     </row>
@@ -15601,14 +15612,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A56:B56"/>
@@ -15619,6 +15622,14 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15649,16 +15660,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="142" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="143"/>
+      <c r="B2" s="147"/>
     </row>
     <row r="3" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="149" t="s">
         <v>501</v>
       </c>
-      <c r="B3" s="144"/>
+      <c r="B3" s="148"/>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
@@ -15685,10 +15696,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="148" t="s">
         <v>513</v>
       </c>
-      <c r="B7" s="142"/>
+      <c r="B7" s="146"/>
     </row>
     <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
@@ -15715,10 +15726,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="148" t="s">
         <v>515</v>
       </c>
-      <c r="B11" s="142"/>
+      <c r="B11" s="146"/>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
@@ -15729,10 +15740,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="148" t="s">
         <v>383</v>
       </c>
-      <c r="B13" s="144"/>
+      <c r="B13" s="148"/>
     </row>
     <row r="14" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
@@ -15791,10 +15802,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="144" t="s">
+      <c r="A21" s="148" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="144"/>
+      <c r="B21" s="148"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
@@ -15805,10 +15816,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="144" t="s">
+      <c r="A23" s="148" t="s">
         <v>382</v>
       </c>
-      <c r="B23" s="144"/>
+      <c r="B23" s="148"/>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
@@ -15829,10 +15840,10 @@
       <c r="C25" s="88"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="144" t="s">
+      <c r="A26" s="148" t="s">
         <v>347</v>
       </c>
-      <c r="B26" s="144"/>
+      <c r="B26" s="148"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
@@ -15859,10 +15870,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="144" t="s">
+      <c r="A30" s="148" t="s">
         <v>347</v>
       </c>
-      <c r="B30" s="144"/>
+      <c r="B30" s="148"/>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="68" t="s">
@@ -15889,10 +15900,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="142" t="s">
+      <c r="A34" s="146" t="s">
         <v>357</v>
       </c>
-      <c r="B34" s="142"/>
+      <c r="B34" s="146"/>
     </row>
     <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="68" t="s">
@@ -15919,10 +15930,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="148" t="s">
         <v>354</v>
       </c>
-      <c r="B38" s="144"/>
+      <c r="B38" s="148"/>
     </row>
     <row r="39" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="68" t="s">
@@ -15949,10 +15960,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="142" t="s">
+      <c r="A42" s="146" t="s">
         <v>358</v>
       </c>
-      <c r="B42" s="142"/>
+      <c r="B42" s="146"/>
     </row>
     <row r="43" spans="1:2" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A43" s="53" t="s">
@@ -15971,10 +15982,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="144" t="s">
+      <c r="A45" s="148" t="s">
         <v>508</v>
       </c>
-      <c r="B45" s="142"/>
+      <c r="B45" s="146"/>
     </row>
     <row r="46" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="53" t="s">
@@ -16001,19 +16012,19 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="133" t="s">
+      <c r="A49" s="142" t="s">
         <v>368</v>
       </c>
-      <c r="B49" s="133"/>
+      <c r="B49" s="142"/>
     </row>
     <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="134" t="s">
+      <c r="A50" s="145" t="s">
         <v>311</v>
       </c>
-      <c r="B50" s="132"/>
+      <c r="B50" s="144"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="139" t="s">
+      <c r="A51" s="153" t="s">
         <v>319</v>
       </c>
       <c r="B51" s="58" t="s">
@@ -16021,7 +16032,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="140"/>
+      <c r="A52" s="154"/>
       <c r="B52" s="58" t="s">
         <v>586</v>
       </c>
@@ -16030,13 +16041,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="141"/>
+      <c r="A53" s="155"/>
       <c r="B53" s="58" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="139" t="s">
+      <c r="A54" s="153" t="s">
         <v>320</v>
       </c>
       <c r="B54" s="58" t="s">
@@ -16044,25 +16055,25 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="140"/>
+      <c r="A55" s="154"/>
       <c r="B55" s="58" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="140"/>
+      <c r="A56" s="154"/>
       <c r="B56" s="58" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="141"/>
+      <c r="A57" s="155"/>
       <c r="B57" s="58" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="139" t="s">
+      <c r="A58" s="153" t="s">
         <v>321</v>
       </c>
       <c r="B58" s="58" t="s">
@@ -16070,13 +16081,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="141"/>
+      <c r="A59" s="155"/>
       <c r="B59" s="58" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="139" t="s">
+      <c r="A60" s="153" t="s">
         <v>322</v>
       </c>
       <c r="B60" s="58" t="s">
@@ -16087,7 +16098,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="140"/>
+      <c r="A61" s="154"/>
       <c r="B61" s="58" t="s">
         <v>523</v>
       </c>
@@ -16096,14 +16107,14 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="140"/>
+      <c r="A62" s="154"/>
       <c r="B62" s="58" t="s">
         <v>583</v>
       </c>
       <c r="C62" s="64"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="141"/>
+      <c r="A63" s="155"/>
       <c r="B63" s="58" t="s">
         <v>324</v>
       </c>
@@ -16157,7 +16168,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="136" t="s">
+      <c r="A70" s="150" t="s">
         <v>289</v>
       </c>
       <c r="B70" s="58" t="s">
@@ -16165,43 +16176,43 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="137"/>
+      <c r="A71" s="151"/>
       <c r="B71" s="58" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="137"/>
+      <c r="A72" s="151"/>
       <c r="B72" s="58" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="137"/>
+      <c r="A73" s="151"/>
       <c r="B73" s="58" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="137"/>
+      <c r="A74" s="151"/>
       <c r="B74" s="58" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="137"/>
+      <c r="A75" s="151"/>
       <c r="B75" s="58" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="138"/>
+      <c r="A76" s="152"/>
       <c r="B76" s="58" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="136" t="s">
+      <c r="A77" s="150" t="s">
         <v>290</v>
       </c>
       <c r="B77" s="58" t="s">
@@ -16209,74 +16220,74 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="137"/>
+      <c r="A78" s="151"/>
       <c r="B78" s="58" t="s">
         <v>298</v>
       </c>
       <c r="C78" s="63"/>
     </row>
     <row r="79" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="137"/>
+      <c r="A79" s="151"/>
       <c r="B79" s="58" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="137"/>
+      <c r="A80" s="151"/>
       <c r="B80" s="58" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="137"/>
+      <c r="A81" s="151"/>
       <c r="B81" s="77" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="137"/>
+      <c r="A82" s="151"/>
       <c r="B82" s="77" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="137"/>
+      <c r="A83" s="151"/>
       <c r="B83" s="77" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="137"/>
+      <c r="A84" s="151"/>
       <c r="B84" s="77" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="137"/>
+      <c r="A85" s="151"/>
       <c r="B85" s="77" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="137"/>
+      <c r="A86" s="151"/>
       <c r="B86" s="77" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="137"/>
+      <c r="A87" s="151"/>
       <c r="B87" s="77" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="138"/>
+      <c r="A88" s="152"/>
       <c r="B88" s="77" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="136" t="s">
+      <c r="A89" s="150" t="s">
         <v>291</v>
       </c>
       <c r="B89" s="78" t="s">
@@ -16284,28 +16295,28 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="137"/>
+      <c r="A90" s="151"/>
       <c r="B90" s="79" t="s">
         <v>306</v>
       </c>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="137"/>
+      <c r="A91" s="151"/>
       <c r="B91" s="79" t="s">
         <v>307</v>
       </c>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="138"/>
+      <c r="A92" s="152"/>
       <c r="B92" s="78" t="s">
         <v>541</v>
       </c>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="136" t="s">
+      <c r="A93" s="150" t="s">
         <v>308</v>
       </c>
       <c r="B93" s="80" t="s">
@@ -16314,7 +16325,7 @@
       <c r="C93"/>
     </row>
     <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="138"/>
+      <c r="A94" s="152"/>
       <c r="B94" s="80" t="s">
         <v>310</v>
       </c>
@@ -16384,17 +16395,17 @@
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="133" t="s">
+      <c r="A102" s="142" t="s">
         <v>384</v>
       </c>
-      <c r="B102" s="133"/>
+      <c r="B102" s="142"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A103" s="134" t="s">
+      <c r="A103" s="145" t="s">
         <v>385</v>
       </c>
-      <c r="B103" s="132"/>
+      <c r="B103" s="144"/>
       <c r="C103"/>
     </row>
     <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -16425,10 +16436,10 @@
       <c r="C106"/>
     </row>
     <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A107" s="134" t="s">
+      <c r="A107" s="145" t="s">
         <v>392</v>
       </c>
-      <c r="B107" s="132"/>
+      <c r="B107" s="144"/>
       <c r="C107"/>
     </row>
     <row r="108" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -16585,10 +16596,10 @@
       <c r="C124"/>
     </row>
     <row r="125" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A125" s="134" t="s">
+      <c r="A125" s="145" t="s">
         <v>423</v>
       </c>
-      <c r="B125" s="132"/>
+      <c r="B125" s="144"/>
       <c r="C125"/>
     </row>
     <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -16673,10 +16684,10 @@
       <c r="C134"/>
     </row>
     <row r="135" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A135" s="134" t="s">
+      <c r="A135" s="145" t="s">
         <v>495</v>
       </c>
-      <c r="B135" s="132"/>
+      <c r="B135" s="144"/>
       <c r="C135"/>
     </row>
     <row r="136" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -16770,10 +16781,10 @@
       <c r="C145"/>
     </row>
     <row r="146" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="131" t="s">
+      <c r="A146" s="143" t="s">
         <v>458</v>
       </c>
-      <c r="B146" s="132"/>
+      <c r="B146" s="144"/>
       <c r="C146"/>
     </row>
     <row r="147" spans="1:3" ht="75" x14ac:dyDescent="0.3">
@@ -16804,10 +16815,10 @@
       <c r="C149"/>
     </row>
     <row r="150" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="131" t="s">
+      <c r="A150" s="143" t="s">
         <v>466</v>
       </c>
-      <c r="B150" s="132"/>
+      <c r="B150" s="144"/>
       <c r="C150"/>
     </row>
     <row r="151" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -16829,10 +16840,10 @@
       <c r="C152"/>
     </row>
     <row r="153" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="131" t="s">
+      <c r="A153" s="143" t="s">
         <v>536</v>
       </c>
-      <c r="B153" s="132"/>
+      <c r="B153" s="144"/>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -16874,17 +16885,17 @@
       <c r="C157"/>
     </row>
     <row r="158" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A158" s="133" t="s">
+      <c r="A158" s="142" t="s">
         <v>468</v>
       </c>
-      <c r="B158" s="133"/>
+      <c r="B158" s="142"/>
       <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A159" s="134" t="s">
+      <c r="A159" s="145" t="s">
         <v>471</v>
       </c>
-      <c r="B159" s="132"/>
+      <c r="B159" s="144"/>
       <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -16920,10 +16931,10 @@
       <c r="C164"/>
     </row>
     <row r="165" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="131" t="s">
+      <c r="A165" s="143" t="s">
         <v>474</v>
       </c>
-      <c r="B165" s="135"/>
+      <c r="B165" s="156"/>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -16990,10 +17001,10 @@
       <c r="C172"/>
     </row>
     <row r="173" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A173" s="134" t="s">
+      <c r="A173" s="145" t="s">
         <v>469</v>
       </c>
-      <c r="B173" s="132"/>
+      <c r="B173" s="144"/>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -17015,10 +17026,10 @@
       <c r="C175"/>
     </row>
     <row r="176" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A176" s="134" t="s">
+      <c r="A176" s="145" t="s">
         <v>470</v>
       </c>
-      <c r="B176" s="132"/>
+      <c r="B176" s="144"/>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -17040,17 +17051,17 @@
       <c r="C178"/>
     </row>
     <row r="179" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A179" s="133" t="s">
+      <c r="A179" s="142" t="s">
         <v>547</v>
       </c>
-      <c r="B179" s="133"/>
+      <c r="B179" s="142"/>
       <c r="C179"/>
     </row>
     <row r="180" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A180" s="134" t="s">
+      <c r="A180" s="145" t="s">
         <v>548</v>
       </c>
-      <c r="B180" s="132"/>
+      <c r="B180" s="144"/>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -17066,10 +17077,10 @@
       <c r="B182" s="72"/>
     </row>
     <row r="183" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A183" s="134" t="s">
+      <c r="A183" s="145" t="s">
         <v>547</v>
       </c>
-      <c r="B183" s="132"/>
+      <c r="B183" s="144"/>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -17150,10 +17161,10 @@
       <c r="B192" s="72"/>
     </row>
     <row r="193" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A193" s="134" t="s">
+      <c r="A193" s="145" t="s">
         <v>570</v>
       </c>
-      <c r="B193" s="132"/>
+      <c r="B193" s="144"/>
       <c r="C193"/>
     </row>
     <row r="194" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -17171,10 +17182,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A196" s="131" t="s">
+      <c r="A196" s="143" t="s">
         <v>574</v>
       </c>
-      <c r="B196" s="132"/>
+      <c r="B196" s="144"/>
     </row>
     <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A197" s="53" t="s">
@@ -17209,17 +17220,17 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A201" s="133" t="s">
+      <c r="A201" s="142" t="s">
         <v>595</v>
       </c>
-      <c r="B201" s="133"/>
+      <c r="B201" s="142"/>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A202" s="131" t="s">
+      <c r="A202" s="143" t="s">
         <v>597</v>
       </c>
-      <c r="B202" s="132"/>
+      <c r="B202" s="144"/>
     </row>
     <row r="203" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A203" s="53" t="s">
@@ -17266,10 +17277,10 @@
       <c r="B208" s="93"/>
     </row>
     <row r="209" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A209" s="131" t="s">
+      <c r="A209" s="143" t="s">
         <v>608</v>
       </c>
-      <c r="B209" s="132"/>
+      <c r="B209" s="144"/>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="53" t="s">
@@ -17284,10 +17295,10 @@
       <c r="B211" s="72"/>
     </row>
     <row r="212" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A212" s="131" t="s">
+      <c r="A212" s="143" t="s">
         <v>610</v>
       </c>
-      <c r="B212" s="132"/>
+      <c r="B212" s="144"/>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="68" t="s">
@@ -17298,10 +17309,10 @@
       </c>
     </row>
     <row r="214" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A214" s="131" t="s">
+      <c r="A214" s="143" t="s">
         <v>614</v>
       </c>
-      <c r="B214" s="132"/>
+      <c r="B214" s="144"/>
     </row>
     <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A215" s="53" t="s">
@@ -17320,10 +17331,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A217" s="131" t="s">
+      <c r="A217" s="143" t="s">
         <v>613</v>
       </c>
-      <c r="B217" s="132"/>
+      <c r="B217" s="144"/>
     </row>
     <row r="218" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A218" s="53" t="s">
@@ -17358,22 +17369,22 @@
       </c>
     </row>
     <row r="222" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A222" s="133" t="s">
+      <c r="A222" s="142" t="s">
         <v>629</v>
       </c>
-      <c r="B222" s="133"/>
+      <c r="B222" s="142"/>
     </row>
     <row r="223" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A223" s="131" t="s">
+      <c r="A223" s="143" t="s">
         <v>631</v>
       </c>
-      <c r="B223" s="132"/>
+      <c r="B223" s="144"/>
     </row>
     <row r="224" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="131" t="s">
+      <c r="A224" s="143" t="s">
         <v>630</v>
       </c>
-      <c r="B224" s="132"/>
+      <c r="B224" s="144"/>
     </row>
     <row r="225" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A225" s="53" t="s">
@@ -17384,10 +17395,10 @@
       </c>
     </row>
     <row r="226" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A226" s="131" t="s">
+      <c r="A226" s="143" t="s">
         <v>634</v>
       </c>
-      <c r="B226" s="132"/>
+      <c r="B226" s="144"/>
     </row>
     <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="53" t="s">
@@ -17430,10 +17441,10 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A232" s="131" t="s">
+      <c r="A232" s="143" t="s">
         <v>644</v>
       </c>
-      <c r="B232" s="132"/>
+      <c r="B232" s="144"/>
     </row>
     <row r="233" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="53" t="s">
@@ -17444,10 +17455,10 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A234" s="131" t="s">
+      <c r="A234" s="143" t="s">
         <v>647</v>
       </c>
-      <c r="B234" s="132"/>
+      <c r="B234" s="144"/>
     </row>
     <row r="235" spans="1:2" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A235" s="53" t="s">
@@ -17464,10 +17475,10 @@
       </c>
     </row>
     <row r="237" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A237" s="131" t="s">
+      <c r="A237" s="143" t="s">
         <v>651</v>
       </c>
-      <c r="B237" s="132"/>
+      <c r="B237" s="144"/>
     </row>
     <row r="238" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A238" s="53" t="s">
@@ -17614,10 +17625,10 @@
       </c>
     </row>
     <row r="256" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A256" s="131" t="s">
+      <c r="A256" s="143" t="s">
         <v>688</v>
       </c>
-      <c r="B256" s="132"/>
+      <c r="B256" s="144"/>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="53" t="s">
@@ -17644,10 +17655,10 @@
       </c>
     </row>
     <row r="260" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A260" s="131" t="s">
+      <c r="A260" s="143" t="s">
         <v>696</v>
       </c>
-      <c r="B260" s="132"/>
+      <c r="B260" s="144"/>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A261" s="53" t="s">
@@ -17658,16 +17669,16 @@
       </c>
     </row>
     <row r="262" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A262" s="133" t="s">
+      <c r="A262" s="142" t="s">
         <v>699</v>
       </c>
-      <c r="B262" s="133"/>
+      <c r="B262" s="142"/>
     </row>
     <row r="263" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A263" s="131" t="s">
+      <c r="A263" s="143" t="s">
         <v>700</v>
       </c>
-      <c r="B263" s="132"/>
+      <c r="B263" s="144"/>
     </row>
     <row r="264" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A264" s="53" t="s">
@@ -17702,10 +17713,10 @@
       </c>
     </row>
     <row r="268" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A268" s="131" t="s">
+      <c r="A268" s="143" t="s">
         <v>709</v>
       </c>
-      <c r="B268" s="132"/>
+      <c r="B268" s="144"/>
     </row>
     <row r="269" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A269" s="53" t="s">
@@ -17740,10 +17751,10 @@
       </c>
     </row>
     <row r="273" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A273" s="131" t="s">
+      <c r="A273" s="143" t="s">
         <v>701</v>
       </c>
-      <c r="B273" s="132"/>
+      <c r="B273" s="144"/>
     </row>
     <row r="274" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="53" t="s">
@@ -17800,10 +17811,10 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A280" s="131" t="s">
+      <c r="A280" s="143" t="s">
         <v>730</v>
       </c>
-      <c r="B280" s="132"/>
+      <c r="B280" s="144"/>
     </row>
     <row r="281" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A281" s="53" t="s">
@@ -17859,18 +17870,39 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A77:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A49:B49"/>
@@ -17887,39 +17919,18 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A77:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A214:B214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17962,7 +17973,7 @@
         <v>143</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C3" t="s">
         <v>197</v>
@@ -18036,17 +18047,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
+      <c r="A1" s="157" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="122" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="54" t="s">
@@ -18054,7 +18065,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="122" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="54" t="s">
@@ -18065,7 +18076,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="122" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="54" t="s">
@@ -18076,7 +18087,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="151" t="s">
+      <c r="A5" s="122" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="72" t="s">
@@ -18087,7 +18098,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="151" t="s">
+      <c r="A6" s="122" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="72" t="s">
@@ -18098,7 +18109,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="122" t="s">
         <v>91</v>
       </c>
       <c r="B7" s="54" t="s">
@@ -18109,7 +18120,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="122" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="54" t="s">
@@ -18120,7 +18131,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="151" t="s">
+      <c r="A9" s="122" t="s">
         <v>98</v>
       </c>
       <c r="B9" s="54" t="s">
@@ -18131,7 +18142,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="122" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="54" t="s">
@@ -18142,10 +18153,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="151" t="s">
+      <c r="A11" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="123" t="s">
         <v>100</v>
       </c>
       <c r="C11" s="119" t="s">
@@ -18153,7 +18164,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="122" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="54" t="s">
@@ -18164,7 +18175,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="122" t="s">
         <v>80</v>
       </c>
       <c r="B13" s="54" t="s">
@@ -18175,7 +18186,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="151" t="s">
+      <c r="A14" s="122" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="54" t="s">
@@ -18186,7 +18197,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="122" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="54" t="s">
@@ -18197,7 +18208,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="122" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="54" t="s">
@@ -18208,7 +18219,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="151" t="s">
+      <c r="A17" s="122" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="54" t="s">
@@ -18219,7 +18230,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="151" t="s">
+      <c r="A18" s="122" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="54" t="s">
@@ -18230,7 +18241,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="122" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="54" t="s">
@@ -18241,7 +18252,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="122" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="54" t="s">
@@ -18252,7 +18263,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="151" t="s">
+      <c r="A21" s="122" t="s">
         <v>116</v>
       </c>
       <c r="B21" s="54" t="s">
@@ -18263,7 +18274,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="151" t="s">
+      <c r="A22" s="122" t="s">
         <v>117</v>
       </c>
       <c r="B22" s="54" t="s">
@@ -18274,7 +18285,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="151" t="s">
+      <c r="A23" s="122" t="s">
         <v>122</v>
       </c>
       <c r="B23" s="54" t="s">
@@ -18285,18 +18296,18 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="151" t="s">
+      <c r="A24" s="122" t="s">
         <v>130</v>
       </c>
       <c r="B24" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="153" t="s">
+      <c r="C24" s="124" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="151" t="s">
+      <c r="A25" s="122" t="s">
         <v>177</v>
       </c>
       <c r="B25" s="54" t="s">
@@ -18305,31 +18316,31 @@
       <c r="C25" s="54"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="154"/>
+      <c r="A26" s="125"/>
       <c r="B26" s="54"/>
       <c r="C26" s="54"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="154"/>
+      <c r="A27" s="125"/>
       <c r="B27" s="54"/>
       <c r="C27" s="54"/>
     </row>
     <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="154"/>
+      <c r="A28" s="125"/>
       <c r="B28" s="72" t="s">
         <v>209</v>
       </c>
       <c r="C28" s="54"/>
     </row>
     <row r="29" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A29" s="154"/>
+      <c r="A29" s="125"/>
       <c r="B29" s="72" t="s">
         <v>210</v>
       </c>
       <c r="C29" s="54"/>
     </row>
     <row r="30" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="154"/>
+      <c r="A30" s="125"/>
       <c r="B30" s="72" t="s">
         <v>211</v>
       </c>
@@ -18368,7 +18379,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="158" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -18388,7 +18399,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
+      <c r="A2" s="159"/>
       <c r="B2" s="19" t="s">
         <v>172</v>
       </c>
@@ -18456,10 +18467,10 @@
     </row>
     <row r="6" spans="1:6" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="160" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="149"/>
+      <c r="C6" s="161"/>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
     </row>

</xml_diff>

<commit_message>
C# DB Advanced - Entity Framework - 10.XML-Processing
</commit_message>
<xml_diff>
--- a/C#-Hints.xlsx
+++ b/C#-Hints.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="1196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="1213">
   <si>
     <t>Операция</t>
   </si>
@@ -11021,17 +11021,136 @@
 }</t>
     </r>
   </si>
+  <si>
+    <t>Steps To Deserialize XML</t>
+  </si>
+  <si>
+    <t>Steps To Serialize XML</t>
+  </si>
+  <si>
+    <t>Mapper.Initialize(x =&gt; x.AddProfile&lt;ProductShopProfile&gt;());</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public ProductShopProfile()
+        {
+            this.CreateMap&lt;UserDto, User&gt;();
+        }</t>
+  </si>
+  <si>
+    <t>namespace ProductShop.Dtos.Import
+{    using System.Xml.Serialization;
+    [XmlType("User")]
+    public class UserDto
+    {
+        [XmlElement("firstName")]
+        public string FirstName { get; set; }
+        [XmlElement("age")]
+        public int Age { get; set; }    }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        //&lt;User&gt;
+        //    &lt;firstName&gt;Chrissy&lt;/firstName&gt;
+        //    &lt;lastName&gt;Falconbridge&lt;/lastName&gt;
+        //    &lt;age&gt;50&lt;/age&gt;
+        //&lt;/User&gt;</t>
+  </si>
+  <si>
+    <t>1.Create DTO</t>
+  </si>
+  <si>
+    <t>2.Create Map in - public class ProductShopProfile : Profile</t>
+  </si>
+  <si>
+    <t>public static string ImportUsers(ProductShopContext context, string inputXml)
+        {            XmlSerializer xmlSerializer = new XmlSerializer(typeof(UserDto[]), new XmlRootAttribute("Users"));
+            var usersDto = (UserDto[])xmlSerializer.Deserialize(new StringReader(inputXml));
+            var users = new List&lt;User&gt;();
+            foreach (var userDto in usersDto)
+            {
+                var user = Mapper.Map&lt;User&gt;(userDto);
+                users.Add(user);
+            }
+            context.Users.AddRange(users);
+            context.SaveChanges();
+            return $"Successfully imported {users.Count}"; ;
+        }</t>
+  </si>
+  <si>
+    <t>3.Mapper.Initialize in - Main
+Use DBContext, Create Databse if doesn’t exist and read XML File - In Main</t>
+  </si>
+  <si>
+    <t>using (ProductShopContext context = new ProductShopContext())
+{                context.Database.EnsureDeleted();
+context.Database.EnsureCreated();
+var usersXml = File.ReadAllText(@"Datasets\users.xml");
+Console.WriteLine(ImportUsers(context, usersXml));
+Console.WriteLine(GetProductsInRange(context));             }</t>
+  </si>
+  <si>
+    <t>namespace ProductShop.Dtos.Export
+{
+    using System.Xml.Serialization;
+    [XmlType("Product")]
+    public class ExportProductInRange
+    {
+        [XmlElement("name")]
+        public string Name { get; set; }
+        [XmlElement("price")]
+        public decimal price { get; set; }
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // &lt;Product&gt;
+        //  &lt;name&gt;TRAMADOL HYDROCHLORIDE&lt;/name&gt;
+        //  &lt;price&gt;516.48&lt;/price&gt;
+        //&lt;/Product&gt;</t>
+  </si>
+  <si>
+    <t>public ProductShopProfile()
+        {
+            this.CreateMap&lt;UserDto, User&gt;();
+        }</t>
+  </si>
+  <si>
+    <t>4.Export (or serialize)</t>
+  </si>
+  <si>
+    <t>4. Import (or deserialize) Users from readed file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public static string GetProductsInRange(ProductShopContext context)
+        {var products = context.Products.Take(10).Where(p =&gt; p.Price &gt;= 500 &amp;&amp; p.Price &lt;= 1000)
+                .Select(p =&gt; new ExportProductInRangeDto
+                {  Name = p.Name,Price = p.Price,Buyer = p.Buyer.FirstName + " " + p.Buyer.LastName}).OrderBy(p =&gt; p.Price).ToArray();
+            XmlSerializer serializer = new XmlSerializer(typeof(ExportProductInRangeDto[]), new XmlRootAttribute("Products"));
+            var sb = new StringBuilder();
+            var namespaces = new XmlSerializerNamespaces(new[]
+            {new XmlQualifiedName("","")});
+            serializer.Serialize(new StringWriter(sb), products, namespaces);
+            return sb.ToString().TrimEnd();}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="66" x14ac:knownFonts="1">
+  <fonts count="67" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11961,131 +12080,131 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="46" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="51" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -12100,73 +12219,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -12175,49 +12294,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -12229,285 +12348,297 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="22" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="2" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="2" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="2" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="5" borderId="22" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="5" borderId="22" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -12542,7 +12673,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2924175</xdr:colOff>
+      <xdr:colOff>2686050</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>2860302</xdr:rowOff>
     </xdr:to>
@@ -15705,10 +15836,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="143" t="s">
         <v>916</v>
       </c>
-      <c r="B1" s="136"/>
+      <c r="B1" s="143"/>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="107" t="s">
@@ -15741,10 +15872,10 @@
       <c r="B5" s="54"/>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="140" t="s">
+      <c r="A6" s="141" t="s">
         <v>918</v>
       </c>
-      <c r="B6" s="141"/>
+      <c r="B6" s="142"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="108" t="s">
@@ -15783,10 +15914,10 @@
       <c r="B12" s="54"/>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="140" t="s">
+      <c r="A13" s="141" t="s">
         <v>925</v>
       </c>
-      <c r="B13" s="141"/>
+      <c r="B13" s="142"/>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="108" t="s">
@@ -15797,10 +15928,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="140" t="s">
+      <c r="A15" s="141" t="s">
         <v>852</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="142"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="116" t="s">
@@ -15825,10 +15956,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="140" t="s">
+      <c r="A19" s="141" t="s">
         <v>933</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="142"/>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="113" t="s">
@@ -15863,16 +15994,16 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="140" t="s">
+      <c r="A24" s="141" t="s">
         <v>942</v>
       </c>
-      <c r="B24" s="141"/>
+      <c r="B24" s="142"/>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="140" t="s">
+      <c r="A25" s="141" t="s">
         <v>886</v>
       </c>
-      <c r="B25" s="141"/>
+      <c r="B25" s="142"/>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="115" t="s">
@@ -15883,10 +16014,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="140" t="s">
+      <c r="A27" s="141" t="s">
         <v>948</v>
       </c>
-      <c r="B27" s="141"/>
+      <c r="B27" s="142"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="108" t="s">
@@ -15911,10 +16042,10 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="140" t="s">
+      <c r="A31" s="141" t="s">
         <v>948</v>
       </c>
-      <c r="B31" s="141"/>
+      <c r="B31" s="142"/>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="115" t="s">
@@ -15955,10 +16086,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="140" t="s">
+      <c r="A36" s="141" t="s">
         <v>961</v>
       </c>
-      <c r="B36" s="141"/>
+      <c r="B36" s="142"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="115" t="s">
@@ -16025,10 +16156,10 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="140" t="s">
+      <c r="A45" s="141" t="s">
         <v>961</v>
       </c>
-      <c r="B45" s="141"/>
+      <c r="B45" s="142"/>
     </row>
     <row r="46" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="115" t="s">
@@ -16047,10 +16178,10 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="140" t="s">
+      <c r="A48" s="141" t="s">
         <v>982</v>
       </c>
-      <c r="B48" s="141"/>
+      <c r="B48" s="142"/>
     </row>
     <row r="49" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="115" t="s">
@@ -16069,10 +16200,10 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="140" t="s">
+      <c r="A51" s="141" t="s">
         <v>987</v>
       </c>
-      <c r="B51" s="141"/>
+      <c r="B51" s="142"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="115" t="s">
@@ -16091,10 +16222,10 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="140" t="s">
+      <c r="A54" s="141" t="s">
         <v>992</v>
       </c>
-      <c r="B54" s="141"/>
+      <c r="B54" s="142"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="115" t="s">
@@ -16115,10 +16246,10 @@
       <c r="B57" s="54"/>
     </row>
     <row r="58" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="136" t="s">
+      <c r="A58" s="143" t="s">
         <v>853</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="143"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="108" t="s">
@@ -16225,10 +16356,10 @@
       <c r="B71" s="54"/>
     </row>
     <row r="72" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="137" t="s">
+      <c r="A72" s="144" t="s">
         <v>865</v>
       </c>
-      <c r="B72" s="137"/>
+      <c r="B72" s="144"/>
     </row>
     <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="107" t="s">
@@ -16239,7 +16370,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="138" t="s">
+      <c r="A74" s="145" t="s">
         <v>868</v>
       </c>
       <c r="B74" s="54" t="s">
@@ -16247,25 +16378,25 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="138"/>
+      <c r="A75" s="145"/>
       <c r="B75" s="54" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="138"/>
+      <c r="A76" s="145"/>
       <c r="B76" s="54" t="s">
         <v>871</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="138"/>
+      <c r="A77" s="145"/>
       <c r="B77" s="54" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="138"/>
+      <c r="A78" s="145"/>
       <c r="B78" s="54" t="s">
         <v>873</v>
       </c>
@@ -16275,16 +16406,16 @@
       <c r="B79" s="54"/>
     </row>
     <row r="80" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="139" t="s">
+      <c r="A80" s="146" t="s">
         <v>874</v>
       </c>
-      <c r="B80" s="139"/>
+      <c r="B80" s="146"/>
     </row>
     <row r="81" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="137" t="s">
+      <c r="A81" s="144" t="s">
         <v>876</v>
       </c>
-      <c r="B81" s="137"/>
+      <c r="B81" s="144"/>
     </row>
     <row r="82" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="108" t="s">
@@ -16303,10 +16434,10 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="137" t="s">
+      <c r="A84" s="144" t="s">
         <v>880</v>
       </c>
-      <c r="B84" s="137"/>
+      <c r="B84" s="144"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="108" t="s">
@@ -16344,10 +16475,10 @@
       <c r="B90" s="54"/>
     </row>
     <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="137" t="s">
+      <c r="A91" s="144" t="s">
         <v>886</v>
       </c>
-      <c r="B91" s="137"/>
+      <c r="B91" s="144"/>
     </row>
     <row r="92" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A92" s="108" t="s">
@@ -16370,10 +16501,10 @@
       <c r="B94" s="54"/>
     </row>
     <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="137" t="s">
+      <c r="A95" s="144" t="s">
         <v>890</v>
       </c>
-      <c r="B95" s="137"/>
+      <c r="B95" s="144"/>
     </row>
     <row r="96" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A96" s="108"/>
@@ -16386,10 +16517,10 @@
       <c r="B97" s="54"/>
     </row>
     <row r="98" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="137" t="s">
+      <c r="A98" s="144" t="s">
         <v>892</v>
       </c>
-      <c r="B98" s="137"/>
+      <c r="B98" s="144"/>
     </row>
     <row r="99" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="107" t="s">
@@ -16404,10 +16535,10 @@
       <c r="B100" s="54"/>
     </row>
     <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="137" t="s">
+      <c r="A101" s="144" t="s">
         <v>895</v>
       </c>
-      <c r="B101" s="137"/>
+      <c r="B101" s="144"/>
     </row>
     <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A102" s="107" t="s">
@@ -16430,10 +16561,10 @@
       <c r="B104" s="54"/>
     </row>
     <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="137" t="s">
+      <c r="A105" s="144" t="s">
         <v>899</v>
       </c>
-      <c r="B105" s="137"/>
+      <c r="B105" s="144"/>
     </row>
     <row r="106" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A106" s="107" t="s">
@@ -16448,10 +16579,10 @@
       <c r="B107" s="54"/>
     </row>
     <row r="108" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="137" t="s">
+      <c r="A108" s="144" t="s">
         <v>902</v>
       </c>
-      <c r="B108" s="137"/>
+      <c r="B108" s="144"/>
     </row>
     <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="107" t="s">
@@ -16487,16 +16618,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A72:B72"/>
@@ -16513,6 +16634,16 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A45:B45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1"/>
@@ -16524,24 +16655,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="168" t="s">
         <v>1010</v>
       </c>
-      <c r="B1" s="142"/>
+      <c r="B1" s="168"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="125" t="s">
@@ -16552,10 +16683,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="143" t="s">
+      <c r="A3" s="147" t="s">
         <v>1013</v>
       </c>
-      <c r="B3" s="143"/>
+      <c r="B3" s="147"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="126" t="s">
@@ -16574,10 +16705,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="147" t="s">
         <v>1018</v>
       </c>
-      <c r="B6" s="143"/>
+      <c r="B6" s="147"/>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="85" t="s">
@@ -16596,10 +16727,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="143" t="s">
+      <c r="A9" s="147" t="s">
         <v>1023</v>
       </c>
-      <c r="B9" s="143"/>
+      <c r="B9" s="147"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="126" t="s">
@@ -16627,13 +16758,13 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="147" t="s">
         <v>1029</v>
       </c>
-      <c r="B13" s="143"/>
+      <c r="B13" s="147"/>
     </row>
     <row r="14" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="169" t="s">
         <v>1030</v>
       </c>
       <c r="B14" s="128" t="s">
@@ -16641,19 +16772,19 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
+      <c r="A15" s="169"/>
       <c r="B15" s="128" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A16" s="143" t="s">
+      <c r="A16" s="147" t="s">
         <v>1039</v>
       </c>
-      <c r="B16" s="143"/>
+      <c r="B16" s="147"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="169" t="s">
         <v>1032</v>
       </c>
       <c r="B17" s="128" t="s">
@@ -16661,13 +16792,13 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
+      <c r="A18" s="169"/>
       <c r="B18" s="128" t="s">
         <v>1034</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="144"/>
+      <c r="A19" s="169"/>
       <c r="B19" s="126" t="s">
         <v>1040</v>
       </c>
@@ -16681,10 +16812,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="147" t="s">
         <v>1038</v>
       </c>
-      <c r="B21" s="143"/>
+      <c r="B21" s="147"/>
     </row>
     <row r="22" spans="1:2" ht="240" x14ac:dyDescent="0.25">
